<commit_message>
Added 2018's RS and using that to complete this year's
</commit_message>
<xml_diff>
--- a/Weekly Planner.xlsx
+++ b/Weekly Planner.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\SoftwareProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F87D004-1780-439E-9501-488BC68AFBE0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D990BC-FA64-444A-A232-5EDDABBA4A77}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Weekly Planner" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1297" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="87">
   <si>
     <t>Monday</t>
   </si>
@@ -298,6 +298,9 @@
   </si>
   <si>
     <t>Data Application Dev - Python Tutorial</t>
+  </si>
+  <si>
+    <t>Software Project - Requirements Specifications</t>
   </si>
 </sst>
 </file>
@@ -851,7 +854,7 @@
     <xf numFmtId="0" fontId="11" fillId="10" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1029,10 +1032,31 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="8" xfId="8" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="15" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="16" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="10" xfId="9" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="17" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="19" xfId="9" applyBorder="1" applyAlignment="1">
@@ -1041,58 +1065,61 @@
     <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="29" xfId="9" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="20" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="15" xfId="9" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="6" fillId="8" borderId="4" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="17" xfId="9" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="30" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="16" xfId="9" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="24" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="9" fillId="6" borderId="11" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="31" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="6" fillId="8" borderId="11" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="8" xfId="8" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="8" xfId="8" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="8" xfId="8" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="29" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="4" fillId="5" borderId="24" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="6" fillId="8" borderId="4" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
@@ -1119,9 +1146,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="20" fontId="6" fillId="11" borderId="4" xfId="10" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1131,35 +1155,23 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="8" xfId="8" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="20" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="29" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="4" fillId="5" borderId="24" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="8" xfId="8" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="29" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="20" fontId="9" fillId="6" borderId="11" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="6" fillId="8" borderId="11" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1170,13 +1182,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="30" xfId="9" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="24" xfId="9" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="31" xfId="9" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1479,8 +1491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y507"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y66" sqref="Y66"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q95" sqref="Q95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1863,26 +1875,26 @@
       <c r="B13" s="57">
         <v>43724</v>
       </c>
-      <c r="C13" s="69" t="s">
+      <c r="C13" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="69"/>
-      <c r="E13" s="69"/>
-      <c r="F13" s="69"/>
-      <c r="G13" s="69"/>
-      <c r="H13" s="88" t="s">
+      <c r="D13" s="86"/>
+      <c r="E13" s="86"/>
+      <c r="F13" s="86"/>
+      <c r="G13" s="86"/>
+      <c r="H13" s="90" t="s">
         <v>39</v>
       </c>
-      <c r="I13" s="89"/>
-      <c r="J13" s="89"/>
-      <c r="K13" s="89"/>
-      <c r="L13" s="89"/>
-      <c r="M13" s="89"/>
-      <c r="N13" s="89"/>
-      <c r="O13" s="89"/>
-      <c r="P13" s="89"/>
-      <c r="Q13" s="89"/>
-      <c r="R13" s="90"/>
+      <c r="I13" s="98"/>
+      <c r="J13" s="98"/>
+      <c r="K13" s="98"/>
+      <c r="L13" s="98"/>
+      <c r="M13" s="98"/>
+      <c r="N13" s="98"/>
+      <c r="O13" s="98"/>
+      <c r="P13" s="98"/>
+      <c r="Q13" s="98"/>
+      <c r="R13" s="91"/>
       <c r="S13" s="51"/>
       <c r="T13" s="30" t="s">
         <v>22</v>
@@ -1895,26 +1907,26 @@
       <c r="B14" s="57">
         <v>43725</v>
       </c>
-      <c r="C14" s="69" t="s">
+      <c r="C14" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="69"/>
-      <c r="E14" s="69"/>
-      <c r="F14" s="69"/>
-      <c r="G14" s="69"/>
+      <c r="D14" s="86"/>
+      <c r="E14" s="86"/>
+      <c r="F14" s="86"/>
+      <c r="G14" s="86"/>
       <c r="H14" s="20"/>
       <c r="I14" s="20"/>
-      <c r="J14" s="91" t="s">
+      <c r="J14" s="99" t="s">
         <v>45</v>
       </c>
-      <c r="K14" s="92"/>
-      <c r="L14" s="92"/>
-      <c r="M14" s="92"/>
-      <c r="N14" s="93"/>
-      <c r="O14" s="88" t="s">
+      <c r="K14" s="100"/>
+      <c r="L14" s="100"/>
+      <c r="M14" s="100"/>
+      <c r="N14" s="101"/>
+      <c r="O14" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="P14" s="90"/>
+      <c r="P14" s="91"/>
       <c r="Q14" s="20"/>
       <c r="R14" s="20"/>
       <c r="S14" s="51"/>
@@ -1957,20 +1969,20 @@
       <c r="B16" s="57">
         <v>43727</v>
       </c>
-      <c r="C16" s="69" t="s">
+      <c r="C16" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="69"/>
-      <c r="E16" s="69"/>
-      <c r="F16" s="69"/>
-      <c r="G16" s="69"/>
-      <c r="H16" s="101" t="s">
+      <c r="D16" s="86"/>
+      <c r="E16" s="86"/>
+      <c r="F16" s="86"/>
+      <c r="G16" s="86"/>
+      <c r="H16" s="108" t="s">
         <v>47</v>
       </c>
-      <c r="I16" s="101"/>
-      <c r="J16" s="101"/>
-      <c r="K16" s="101"/>
-      <c r="L16" s="101"/>
+      <c r="I16" s="108"/>
+      <c r="J16" s="108"/>
+      <c r="K16" s="108"/>
+      <c r="L16" s="108"/>
       <c r="M16" s="20"/>
       <c r="N16" s="20"/>
       <c r="O16" s="20"/>
@@ -2175,26 +2187,26 @@
         <f>B13+7</f>
         <v>43731</v>
       </c>
-      <c r="C23" s="69" t="s">
+      <c r="C23" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="69"/>
-      <c r="E23" s="69"/>
-      <c r="F23" s="69"/>
-      <c r="G23" s="69"/>
-      <c r="H23" s="88" t="s">
+      <c r="D23" s="86"/>
+      <c r="E23" s="86"/>
+      <c r="F23" s="86"/>
+      <c r="G23" s="86"/>
+      <c r="H23" s="90" t="s">
         <v>39</v>
       </c>
-      <c r="I23" s="89"/>
-      <c r="J23" s="89"/>
-      <c r="K23" s="89"/>
-      <c r="L23" s="89"/>
-      <c r="M23" s="89"/>
-      <c r="N23" s="89"/>
-      <c r="O23" s="89"/>
-      <c r="P23" s="89"/>
-      <c r="Q23" s="89"/>
-      <c r="R23" s="90"/>
+      <c r="I23" s="98"/>
+      <c r="J23" s="98"/>
+      <c r="K23" s="98"/>
+      <c r="L23" s="98"/>
+      <c r="M23" s="98"/>
+      <c r="N23" s="98"/>
+      <c r="O23" s="98"/>
+      <c r="P23" s="98"/>
+      <c r="Q23" s="98"/>
+      <c r="R23" s="91"/>
       <c r="S23" s="51"/>
       <c r="T23" s="30" t="s">
         <v>22</v>
@@ -2208,30 +2220,30 @@
         <f t="shared" ref="B24:B29" si="0">B14+7</f>
         <v>43732</v>
       </c>
-      <c r="C24" s="69" t="s">
+      <c r="C24" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="69"/>
-      <c r="E24" s="69"/>
-      <c r="F24" s="69"/>
-      <c r="G24" s="69"/>
-      <c r="H24" s="88" t="s">
+      <c r="D24" s="86"/>
+      <c r="E24" s="86"/>
+      <c r="F24" s="86"/>
+      <c r="G24" s="86"/>
+      <c r="H24" s="90" t="s">
         <v>44</v>
       </c>
-      <c r="I24" s="102"/>
-      <c r="J24" s="86" t="s">
+      <c r="I24" s="109"/>
+      <c r="J24" s="71" t="s">
         <v>48</v>
       </c>
-      <c r="K24" s="87"/>
-      <c r="L24" s="99"/>
-      <c r="M24" s="86" t="s">
+      <c r="K24" s="72"/>
+      <c r="L24" s="95"/>
+      <c r="M24" s="71" t="s">
         <v>56</v>
       </c>
-      <c r="N24" s="99"/>
-      <c r="O24" s="91" t="s">
+      <c r="N24" s="95"/>
+      <c r="O24" s="99" t="s">
         <v>38</v>
       </c>
-      <c r="P24" s="93"/>
+      <c r="P24" s="101"/>
       <c r="Q24" s="20"/>
       <c r="R24" s="20"/>
       <c r="S24" s="51"/>
@@ -2276,20 +2288,20 @@
         <f t="shared" si="0"/>
         <v>43734</v>
       </c>
-      <c r="C26" s="69" t="s">
+      <c r="C26" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="D26" s="69"/>
-      <c r="E26" s="69"/>
-      <c r="F26" s="69"/>
-      <c r="G26" s="69"/>
-      <c r="H26" s="97" t="s">
+      <c r="D26" s="86"/>
+      <c r="E26" s="86"/>
+      <c r="F26" s="86"/>
+      <c r="G26" s="86"/>
+      <c r="H26" s="105" t="s">
         <v>57</v>
       </c>
-      <c r="I26" s="97"/>
-      <c r="J26" s="97"/>
-      <c r="K26" s="97"/>
-      <c r="L26" s="97"/>
+      <c r="I26" s="105"/>
+      <c r="J26" s="105"/>
+      <c r="K26" s="105"/>
+      <c r="L26" s="105"/>
       <c r="M26" s="20"/>
       <c r="N26" s="20"/>
       <c r="O26" s="20"/>
@@ -2471,12 +2483,12 @@
         <f>C22+1</f>
         <v>3</v>
       </c>
-      <c r="D32" s="100" t="s">
+      <c r="D32" s="107" t="s">
         <v>46</v>
       </c>
-      <c r="E32" s="100"/>
-      <c r="F32" s="100"/>
-      <c r="G32" s="100"/>
+      <c r="E32" s="107"/>
+      <c r="F32" s="107"/>
+      <c r="G32" s="107"/>
       <c r="H32" s="15"/>
       <c r="I32" s="15"/>
       <c r="J32" s="15"/>
@@ -2499,24 +2511,24 @@
         <f>B23+7</f>
         <v>43738</v>
       </c>
-      <c r="C33" s="69" t="s">
+      <c r="C33" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="D33" s="69"/>
-      <c r="E33" s="69"/>
-      <c r="F33" s="69"/>
-      <c r="G33" s="69"/>
-      <c r="H33" s="97" t="s">
+      <c r="D33" s="86"/>
+      <c r="E33" s="86"/>
+      <c r="F33" s="86"/>
+      <c r="G33" s="86"/>
+      <c r="H33" s="105" t="s">
         <v>14</v>
       </c>
-      <c r="I33" s="97"/>
-      <c r="J33" s="97"/>
-      <c r="K33" s="97"/>
-      <c r="L33" s="97"/>
-      <c r="M33" s="97"/>
-      <c r="N33" s="97"/>
-      <c r="O33" s="97"/>
-      <c r="P33" s="97"/>
+      <c r="I33" s="105"/>
+      <c r="J33" s="105"/>
+      <c r="K33" s="105"/>
+      <c r="L33" s="105"/>
+      <c r="M33" s="105"/>
+      <c r="N33" s="105"/>
+      <c r="O33" s="105"/>
+      <c r="P33" s="105"/>
       <c r="Q33" s="62"/>
       <c r="R33" s="62"/>
       <c r="S33" s="51"/>
@@ -2532,13 +2544,13 @@
         <f t="shared" ref="B34:B39" si="1">B24+7</f>
         <v>43739</v>
       </c>
-      <c r="C34" s="69" t="s">
+      <c r="C34" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="D34" s="69"/>
-      <c r="E34" s="69"/>
-      <c r="F34" s="69"/>
-      <c r="G34" s="69"/>
+      <c r="D34" s="86"/>
+      <c r="E34" s="86"/>
+      <c r="F34" s="86"/>
+      <c r="G34" s="86"/>
       <c r="H34" s="62"/>
       <c r="I34" s="62"/>
       <c r="J34" s="62"/>
@@ -2592,13 +2604,13 @@
         <f t="shared" si="1"/>
         <v>43741</v>
       </c>
-      <c r="C36" s="69" t="s">
+      <c r="C36" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="D36" s="69"/>
-      <c r="E36" s="69"/>
-      <c r="F36" s="69"/>
-      <c r="G36" s="69"/>
+      <c r="D36" s="86"/>
+      <c r="E36" s="86"/>
+      <c r="F36" s="86"/>
+      <c r="G36" s="86"/>
       <c r="H36" s="63"/>
       <c r="I36" s="63"/>
       <c r="J36" s="63"/>
@@ -2811,24 +2823,24 @@
         <f>B33+7</f>
         <v>43745</v>
       </c>
-      <c r="C43" s="69" t="s">
+      <c r="C43" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="D43" s="69"/>
-      <c r="E43" s="69"/>
-      <c r="F43" s="69"/>
-      <c r="G43" s="69"/>
-      <c r="H43" s="98" t="s">
+      <c r="D43" s="86"/>
+      <c r="E43" s="86"/>
+      <c r="F43" s="86"/>
+      <c r="G43" s="86"/>
+      <c r="H43" s="106" t="s">
         <v>14</v>
       </c>
-      <c r="I43" s="98"/>
-      <c r="J43" s="98"/>
-      <c r="K43" s="98"/>
-      <c r="L43" s="98"/>
-      <c r="M43" s="98"/>
-      <c r="N43" s="98"/>
-      <c r="O43" s="98"/>
-      <c r="P43" s="98"/>
+      <c r="I43" s="106"/>
+      <c r="J43" s="106"/>
+      <c r="K43" s="106"/>
+      <c r="L43" s="106"/>
+      <c r="M43" s="106"/>
+      <c r="N43" s="106"/>
+      <c r="O43" s="106"/>
+      <c r="P43" s="106"/>
       <c r="Q43" s="20"/>
       <c r="R43" s="20"/>
       <c r="S43" s="51"/>
@@ -2844,22 +2856,22 @@
         <f t="shared" ref="B44:B49" si="2">B34+7</f>
         <v>43746</v>
       </c>
-      <c r="C44" s="69" t="s">
+      <c r="C44" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="D44" s="69"/>
-      <c r="E44" s="69"/>
-      <c r="F44" s="69"/>
-      <c r="G44" s="69"/>
-      <c r="H44" s="82" t="s">
+      <c r="D44" s="86"/>
+      <c r="E44" s="86"/>
+      <c r="F44" s="86"/>
+      <c r="G44" s="86"/>
+      <c r="H44" s="110" t="s">
         <v>58</v>
       </c>
-      <c r="I44" s="83"/>
-      <c r="J44" s="83"/>
-      <c r="K44" s="83"/>
-      <c r="L44" s="83"/>
-      <c r="M44" s="83"/>
-      <c r="N44" s="83"/>
+      <c r="I44" s="97"/>
+      <c r="J44" s="97"/>
+      <c r="K44" s="97"/>
+      <c r="L44" s="97"/>
+      <c r="M44" s="97"/>
+      <c r="N44" s="97"/>
       <c r="O44" s="49"/>
       <c r="P44" s="49"/>
       <c r="Q44" s="49"/>
@@ -2882,17 +2894,17 @@
       <c r="E45" s="20"/>
       <c r="F45" s="20"/>
       <c r="G45" s="20"/>
-      <c r="H45" s="94" t="s">
+      <c r="H45" s="102" t="s">
         <v>58</v>
       </c>
-      <c r="I45" s="95"/>
-      <c r="J45" s="95"/>
-      <c r="K45" s="95"/>
-      <c r="L45" s="95"/>
-      <c r="M45" s="95"/>
-      <c r="N45" s="95"/>
-      <c r="O45" s="95"/>
-      <c r="P45" s="96"/>
+      <c r="I45" s="103"/>
+      <c r="J45" s="103"/>
+      <c r="K45" s="103"/>
+      <c r="L45" s="103"/>
+      <c r="M45" s="103"/>
+      <c r="N45" s="103"/>
+      <c r="O45" s="103"/>
+      <c r="P45" s="104"/>
       <c r="Q45" s="49"/>
       <c r="R45" s="49"/>
       <c r="S45" s="51"/>
@@ -2908,24 +2920,24 @@
         <f t="shared" si="2"/>
         <v>43748</v>
       </c>
-      <c r="C46" s="69" t="s">
+      <c r="C46" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="D46" s="69"/>
-      <c r="E46" s="69"/>
-      <c r="F46" s="69"/>
-      <c r="G46" s="69"/>
-      <c r="H46" s="79" t="s">
+      <c r="D46" s="86"/>
+      <c r="E46" s="86"/>
+      <c r="F46" s="86"/>
+      <c r="G46" s="86"/>
+      <c r="H46" s="88" t="s">
         <v>62</v>
       </c>
-      <c r="I46" s="80"/>
-      <c r="J46" s="80"/>
-      <c r="K46" s="80"/>
-      <c r="L46" s="80"/>
-      <c r="M46" s="80"/>
-      <c r="N46" s="80"/>
-      <c r="O46" s="80"/>
-      <c r="P46" s="81"/>
+      <c r="I46" s="74"/>
+      <c r="J46" s="74"/>
+      <c r="K46" s="74"/>
+      <c r="L46" s="74"/>
+      <c r="M46" s="74"/>
+      <c r="N46" s="74"/>
+      <c r="O46" s="74"/>
+      <c r="P46" s="89"/>
       <c r="Q46" s="20"/>
       <c r="R46" s="20"/>
       <c r="S46" s="51"/>
@@ -3104,11 +3116,11 @@
         <v>5</v>
       </c>
       <c r="G52" s="15"/>
-      <c r="H52" s="84" t="s">
+      <c r="H52" s="111" t="s">
         <v>67</v>
       </c>
-      <c r="I52" s="84"/>
-      <c r="J52" s="84"/>
+      <c r="I52" s="111"/>
+      <c r="J52" s="111"/>
       <c r="K52" s="19"/>
       <c r="L52" s="19"/>
       <c r="M52" s="19"/>
@@ -3128,23 +3140,23 @@
         <f>B43+7</f>
         <v>43752</v>
       </c>
-      <c r="C53" s="69" t="s">
+      <c r="C53" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="D53" s="69"/>
-      <c r="E53" s="69"/>
-      <c r="F53" s="69"/>
-      <c r="G53" s="69"/>
+      <c r="D53" s="86"/>
+      <c r="E53" s="86"/>
+      <c r="F53" s="86"/>
+      <c r="G53" s="86"/>
       <c r="H53" s="65" t="s">
         <v>68</v>
       </c>
-      <c r="I53" s="86" t="s">
+      <c r="I53" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="J53" s="87"/>
-      <c r="K53" s="87"/>
-      <c r="L53" s="87"/>
-      <c r="M53" s="87"/>
+      <c r="J53" s="72"/>
+      <c r="K53" s="72"/>
+      <c r="L53" s="72"/>
+      <c r="M53" s="72"/>
       <c r="N53" s="49"/>
       <c r="O53" s="49"/>
       <c r="P53" s="49"/>
@@ -3163,28 +3175,28 @@
         <f t="shared" ref="B54:B59" si="3">B44+7</f>
         <v>43753</v>
       </c>
-      <c r="C54" s="69" t="s">
+      <c r="C54" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="D54" s="69"/>
-      <c r="E54" s="69"/>
-      <c r="F54" s="69"/>
-      <c r="G54" s="69"/>
-      <c r="H54" s="105" t="s">
+      <c r="D54" s="86"/>
+      <c r="E54" s="86"/>
+      <c r="F54" s="86"/>
+      <c r="G54" s="86"/>
+      <c r="H54" s="92" t="s">
         <v>63</v>
       </c>
-      <c r="I54" s="106"/>
-      <c r="J54" s="106"/>
-      <c r="K54" s="106"/>
-      <c r="L54" s="106"/>
-      <c r="M54" s="106"/>
-      <c r="N54" s="106"/>
-      <c r="O54" s="106"/>
-      <c r="P54" s="106"/>
-      <c r="Q54" s="88" t="s">
+      <c r="I54" s="93"/>
+      <c r="J54" s="93"/>
+      <c r="K54" s="93"/>
+      <c r="L54" s="93"/>
+      <c r="M54" s="93"/>
+      <c r="N54" s="93"/>
+      <c r="O54" s="93"/>
+      <c r="P54" s="93"/>
+      <c r="Q54" s="90" t="s">
         <v>70</v>
       </c>
-      <c r="R54" s="90"/>
+      <c r="R54" s="91"/>
       <c r="S54" s="51"/>
       <c r="T54" s="53" t="s">
         <v>19</v>
@@ -3202,18 +3214,18 @@
       <c r="D55" s="49"/>
       <c r="E55" s="49"/>
       <c r="F55" s="49"/>
-      <c r="G55" s="69" t="s">
+      <c r="G55" s="86" t="s">
         <v>64</v>
       </c>
-      <c r="H55" s="69"/>
-      <c r="I55" s="110" t="s">
+      <c r="H55" s="86"/>
+      <c r="I55" s="112" t="s">
         <v>14</v>
       </c>
-      <c r="J55" s="87"/>
-      <c r="K55" s="87"/>
-      <c r="L55" s="87"/>
-      <c r="M55" s="87"/>
-      <c r="N55" s="87"/>
+      <c r="J55" s="72"/>
+      <c r="K55" s="72"/>
+      <c r="L55" s="72"/>
+      <c r="M55" s="72"/>
+      <c r="N55" s="72"/>
       <c r="O55" s="49"/>
       <c r="P55" s="49"/>
       <c r="Q55" s="49"/>
@@ -3231,21 +3243,21 @@
         <f t="shared" si="3"/>
         <v>43755</v>
       </c>
-      <c r="C56" s="69" t="s">
+      <c r="C56" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="D56" s="69"/>
-      <c r="E56" s="69"/>
-      <c r="F56" s="69"/>
-      <c r="G56" s="69"/>
-      <c r="H56" s="109" t="s">
+      <c r="D56" s="86"/>
+      <c r="E56" s="86"/>
+      <c r="F56" s="86"/>
+      <c r="G56" s="86"/>
+      <c r="H56" s="96" t="s">
         <v>71</v>
       </c>
-      <c r="I56" s="83"/>
-      <c r="J56" s="83"/>
-      <c r="K56" s="83"/>
-      <c r="L56" s="83"/>
-      <c r="M56" s="83"/>
+      <c r="I56" s="97"/>
+      <c r="J56" s="97"/>
+      <c r="K56" s="97"/>
+      <c r="L56" s="97"/>
+      <c r="M56" s="97"/>
       <c r="N56" s="49"/>
       <c r="O56" s="49"/>
       <c r="P56" s="49"/>
@@ -3277,11 +3289,11 @@
       <c r="M57" s="49"/>
       <c r="N57" s="49"/>
       <c r="O57" s="49"/>
-      <c r="P57" s="79" t="s">
+      <c r="P57" s="88" t="s">
         <v>42</v>
       </c>
-      <c r="Q57" s="80"/>
-      <c r="R57" s="81"/>
+      <c r="Q57" s="74"/>
+      <c r="R57" s="89"/>
       <c r="S57" s="51"/>
       <c r="T57" s="51"/>
     </row>
@@ -3295,31 +3307,31 @@
       </c>
       <c r="C58" s="50"/>
       <c r="D58" s="49"/>
-      <c r="E58" s="107" t="s">
+      <c r="E58" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="F58" s="80"/>
-      <c r="G58" s="108"/>
-      <c r="H58" s="69" t="s">
+      <c r="F58" s="74"/>
+      <c r="G58" s="94"/>
+      <c r="H58" s="86" t="s">
         <v>74</v>
       </c>
-      <c r="I58" s="69"/>
-      <c r="J58" s="86" t="s">
+      <c r="I58" s="86"/>
+      <c r="J58" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="K58" s="87"/>
-      <c r="L58" s="87"/>
-      <c r="M58" s="87"/>
-      <c r="N58" s="87"/>
-      <c r="O58" s="87"/>
-      <c r="P58" s="99"/>
+      <c r="K58" s="72"/>
+      <c r="L58" s="72"/>
+      <c r="M58" s="72"/>
+      <c r="N58" s="72"/>
+      <c r="O58" s="72"/>
+      <c r="P58" s="95"/>
       <c r="Q58" s="20"/>
       <c r="R58" s="20"/>
       <c r="S58" s="51"/>
-      <c r="T58" s="112" t="s">
+      <c r="T58" s="75" t="s">
         <v>72</v>
       </c>
-      <c r="U58" s="112"/>
+      <c r="U58" s="75"/>
     </row>
     <row r="59" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
@@ -3346,8 +3358,8 @@
       <c r="Q59" s="20"/>
       <c r="R59" s="20"/>
       <c r="S59" s="51"/>
-      <c r="T59" s="112"/>
-      <c r="U59" s="112"/>
+      <c r="T59" s="75"/>
+      <c r="U59" s="75"/>
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B60"/>
@@ -3368,8 +3380,8 @@
       <c r="Q60"/>
       <c r="R60"/>
       <c r="S60"/>
-      <c r="T60" s="112"/>
-      <c r="U60" s="112"/>
+      <c r="T60" s="75"/>
+      <c r="U60" s="75"/>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
@@ -3443,11 +3455,11 @@
       <c r="E62" s="15"/>
       <c r="F62" s="15"/>
       <c r="G62" s="15"/>
-      <c r="H62" s="84" t="s">
+      <c r="H62" s="111" t="s">
         <v>73</v>
       </c>
-      <c r="I62" s="84"/>
-      <c r="J62" s="84"/>
+      <c r="I62" s="111"/>
+      <c r="J62" s="111"/>
       <c r="K62" s="19"/>
       <c r="L62" s="19"/>
       <c r="M62" s="19"/>
@@ -3467,22 +3479,22 @@
         <f>B53+7</f>
         <v>43759</v>
       </c>
-      <c r="C63" s="69" t="s">
+      <c r="C63" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="D63" s="69"/>
-      <c r="E63" s="69"/>
-      <c r="F63" s="69"/>
-      <c r="G63" s="69"/>
+      <c r="D63" s="86"/>
+      <c r="E63" s="86"/>
+      <c r="F63" s="86"/>
+      <c r="G63" s="86"/>
       <c r="H63" s="67" t="s">
         <v>68</v>
       </c>
-      <c r="I63" s="86" t="s">
+      <c r="I63" s="71" t="s">
         <v>76</v>
       </c>
-      <c r="J63" s="87"/>
-      <c r="K63" s="87"/>
-      <c r="L63" s="87"/>
+      <c r="J63" s="72"/>
+      <c r="K63" s="72"/>
+      <c r="L63" s="72"/>
       <c r="M63" s="49"/>
       <c r="N63" s="49"/>
       <c r="O63" s="49"/>
@@ -3502,22 +3514,22 @@
         <f t="shared" ref="B64:B69" si="4">B54+7</f>
         <v>43760</v>
       </c>
-      <c r="C64" s="69" t="s">
+      <c r="C64" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="D64" s="69"/>
-      <c r="E64" s="69"/>
-      <c r="F64" s="69"/>
-      <c r="G64" s="69"/>
-      <c r="H64" s="107" t="s">
+      <c r="D64" s="86"/>
+      <c r="E64" s="86"/>
+      <c r="F64" s="86"/>
+      <c r="G64" s="86"/>
+      <c r="H64" s="73" t="s">
         <v>85</v>
       </c>
-      <c r="I64" s="80"/>
-      <c r="J64" s="80"/>
-      <c r="K64" s="80"/>
-      <c r="L64" s="80"/>
-      <c r="M64" s="80"/>
-      <c r="N64" s="80"/>
+      <c r="I64" s="74"/>
+      <c r="J64" s="74"/>
+      <c r="K64" s="74"/>
+      <c r="L64" s="74"/>
+      <c r="M64" s="74"/>
+      <c r="N64" s="74"/>
       <c r="O64" s="49"/>
       <c r="P64" s="49"/>
       <c r="Q64" s="49"/>
@@ -3566,25 +3578,25 @@
         <f t="shared" si="4"/>
         <v>43762</v>
       </c>
-      <c r="C66" s="69" t="s">
+      <c r="C66" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="D66" s="69"/>
-      <c r="E66" s="69"/>
-      <c r="F66" s="69"/>
-      <c r="G66" s="69"/>
-      <c r="H66" s="116" t="s">
+      <c r="D66" s="86"/>
+      <c r="E66" s="86"/>
+      <c r="F66" s="86"/>
+      <c r="G66" s="86"/>
+      <c r="H66" s="82" t="s">
         <v>77</v>
       </c>
-      <c r="I66" s="117"/>
-      <c r="J66" s="117"/>
-      <c r="K66" s="117"/>
-      <c r="L66" s="117"/>
-      <c r="M66" s="117"/>
-      <c r="N66" s="117"/>
-      <c r="O66" s="117"/>
-      <c r="P66" s="117"/>
-      <c r="Q66" s="118"/>
+      <c r="I66" s="83"/>
+      <c r="J66" s="83"/>
+      <c r="K66" s="83"/>
+      <c r="L66" s="83"/>
+      <c r="M66" s="83"/>
+      <c r="N66" s="83"/>
+      <c r="O66" s="83"/>
+      <c r="P66" s="83"/>
+      <c r="Q66" s="84"/>
       <c r="R66" s="20"/>
       <c r="S66" s="51"/>
       <c r="T66" s="18" t="s">
@@ -3599,26 +3611,26 @@
         <f t="shared" si="4"/>
         <v>43763</v>
       </c>
-      <c r="C67" s="74" t="s">
+      <c r="C67" s="69" t="s">
         <v>77</v>
       </c>
-      <c r="D67" s="75"/>
-      <c r="E67" s="75"/>
-      <c r="F67" s="75"/>
-      <c r="G67" s="75"/>
-      <c r="H67" s="75"/>
-      <c r="I67" s="75"/>
-      <c r="J67" s="76"/>
+      <c r="D67" s="77"/>
+      <c r="E67" s="77"/>
+      <c r="F67" s="77"/>
+      <c r="G67" s="77"/>
+      <c r="H67" s="77"/>
+      <c r="I67" s="77"/>
+      <c r="J67" s="70"/>
       <c r="K67" s="49"/>
-      <c r="L67" s="75" t="s">
+      <c r="L67" s="77" t="s">
         <v>42</v>
       </c>
-      <c r="M67" s="75"/>
-      <c r="N67" s="75"/>
-      <c r="O67" s="75"/>
-      <c r="P67" s="75"/>
-      <c r="Q67" s="75"/>
-      <c r="R67" s="76"/>
+      <c r="M67" s="77"/>
+      <c r="N67" s="77"/>
+      <c r="O67" s="77"/>
+      <c r="P67" s="77"/>
+      <c r="Q67" s="77"/>
+      <c r="R67" s="70"/>
       <c r="S67" s="51"/>
       <c r="T67" s="51"/>
     </row>
@@ -3630,26 +3642,26 @@
         <f t="shared" si="4"/>
         <v>43764</v>
       </c>
-      <c r="C68" s="74" t="s">
+      <c r="C68" s="69" t="s">
         <v>77</v>
       </c>
-      <c r="D68" s="75"/>
-      <c r="E68" s="75"/>
-      <c r="F68" s="75"/>
-      <c r="G68" s="75"/>
-      <c r="H68" s="75"/>
-      <c r="I68" s="75"/>
-      <c r="J68" s="76"/>
+      <c r="D68" s="77"/>
+      <c r="E68" s="77"/>
+      <c r="F68" s="77"/>
+      <c r="G68" s="77"/>
+      <c r="H68" s="77"/>
+      <c r="I68" s="77"/>
+      <c r="J68" s="70"/>
       <c r="K68" s="49"/>
-      <c r="L68" s="75" t="s">
+      <c r="L68" s="77" t="s">
         <v>42</v>
       </c>
-      <c r="M68" s="75"/>
-      <c r="N68" s="75"/>
-      <c r="O68" s="75"/>
-      <c r="P68" s="75"/>
-      <c r="Q68" s="75"/>
-      <c r="R68" s="76"/>
+      <c r="M68" s="77"/>
+      <c r="N68" s="77"/>
+      <c r="O68" s="77"/>
+      <c r="P68" s="77"/>
+      <c r="Q68" s="77"/>
+      <c r="R68" s="70"/>
       <c r="S68" s="51"/>
       <c r="T68" s="51"/>
     </row>
@@ -3661,24 +3673,24 @@
         <f t="shared" si="4"/>
         <v>43765</v>
       </c>
-      <c r="C69" s="69" t="s">
+      <c r="C69" s="86" t="s">
         <v>81</v>
       </c>
-      <c r="D69" s="69"/>
-      <c r="E69" s="69"/>
-      <c r="F69" s="69"/>
-      <c r="G69" s="69"/>
-      <c r="H69" s="69"/>
-      <c r="I69" s="69"/>
-      <c r="J69" s="69"/>
-      <c r="K69" s="69"/>
-      <c r="L69" s="69"/>
-      <c r="M69" s="69"/>
-      <c r="N69" s="69"/>
-      <c r="O69" s="69"/>
-      <c r="P69" s="69"/>
-      <c r="Q69" s="69"/>
-      <c r="R69" s="69"/>
+      <c r="D69" s="86"/>
+      <c r="E69" s="86"/>
+      <c r="F69" s="86"/>
+      <c r="G69" s="86"/>
+      <c r="H69" s="86"/>
+      <c r="I69" s="86"/>
+      <c r="J69" s="86"/>
+      <c r="K69" s="86"/>
+      <c r="L69" s="86"/>
+      <c r="M69" s="86"/>
+      <c r="N69" s="86"/>
+      <c r="O69" s="86"/>
+      <c r="P69" s="86"/>
+      <c r="Q69" s="86"/>
+      <c r="R69" s="86"/>
       <c r="S69" s="51"/>
       <c r="T69" s="51"/>
     </row>
@@ -3771,27 +3783,27 @@
         <f>C62+1</f>
         <v>7</v>
       </c>
-      <c r="D72" s="85" t="s">
+      <c r="D72" s="81" t="s">
         <v>42</v>
       </c>
-      <c r="E72" s="85"/>
-      <c r="F72" s="85"/>
+      <c r="E72" s="81"/>
+      <c r="F72" s="81"/>
       <c r="G72" s="15"/>
-      <c r="H72" s="78" t="s">
+      <c r="H72" s="115" t="s">
         <v>82</v>
       </c>
-      <c r="I72" s="78"/>
-      <c r="J72" s="78"/>
-      <c r="K72" s="78"/>
+      <c r="I72" s="115"/>
+      <c r="J72" s="115"/>
+      <c r="K72" s="115"/>
       <c r="L72" s="19"/>
-      <c r="M72" s="77" t="s">
+      <c r="M72" s="114" t="s">
         <v>75</v>
       </c>
-      <c r="N72" s="77"/>
-      <c r="O72" s="77"/>
-      <c r="P72" s="77"/>
-      <c r="Q72" s="77"/>
-      <c r="R72" s="77"/>
+      <c r="N72" s="114"/>
+      <c r="O72" s="114"/>
+      <c r="P72" s="114"/>
+      <c r="Q72" s="114"/>
+      <c r="R72" s="114"/>
       <c r="S72" s="51"/>
       <c r="T72" s="51"/>
     </row>
@@ -3805,23 +3817,23 @@
       </c>
       <c r="C73" s="32"/>
       <c r="D73" s="20"/>
-      <c r="E73" s="70" t="s">
+      <c r="E73" s="106" t="s">
         <v>66</v>
       </c>
-      <c r="F73" s="70"/>
-      <c r="G73" s="70"/>
-      <c r="H73" s="70"/>
-      <c r="I73" s="70"/>
-      <c r="J73" s="70"/>
+      <c r="F73" s="106"/>
+      <c r="G73" s="106"/>
+      <c r="H73" s="106"/>
+      <c r="I73" s="106"/>
+      <c r="J73" s="106"/>
       <c r="K73" s="49"/>
-      <c r="L73" s="74" t="s">
+      <c r="L73" s="71" t="s">
         <v>66</v>
       </c>
-      <c r="M73" s="75"/>
-      <c r="N73" s="75"/>
-      <c r="O73" s="75"/>
-      <c r="P73" s="75"/>
-      <c r="Q73" s="76"/>
+      <c r="M73" s="72"/>
+      <c r="N73" s="72"/>
+      <c r="O73" s="72"/>
+      <c r="P73" s="72"/>
+      <c r="Q73" s="95"/>
       <c r="R73" s="49"/>
       <c r="S73" s="51"/>
       <c r="T73" s="30" t="s">
@@ -3836,27 +3848,27 @@
         <f t="shared" ref="B74:B79" si="5">B64+7</f>
         <v>43767</v>
       </c>
-      <c r="C74" s="74" t="s">
+      <c r="C74" s="71" t="s">
         <v>78</v>
       </c>
-      <c r="D74" s="76"/>
-      <c r="E74" s="70" t="s">
+      <c r="D74" s="95"/>
+      <c r="E74" s="106" t="s">
         <v>66</v>
       </c>
-      <c r="F74" s="70"/>
-      <c r="G74" s="70"/>
-      <c r="H74" s="70"/>
-      <c r="I74" s="70"/>
-      <c r="J74" s="70"/>
+      <c r="F74" s="106"/>
+      <c r="G74" s="106"/>
+      <c r="H74" s="106"/>
+      <c r="I74" s="106"/>
+      <c r="J74" s="106"/>
       <c r="K74" s="49"/>
-      <c r="L74" s="74" t="s">
+      <c r="L74" s="71" t="s">
         <v>66</v>
       </c>
-      <c r="M74" s="75"/>
-      <c r="N74" s="75"/>
-      <c r="O74" s="75"/>
-      <c r="P74" s="75"/>
-      <c r="Q74" s="76"/>
+      <c r="M74" s="72"/>
+      <c r="N74" s="72"/>
+      <c r="O74" s="72"/>
+      <c r="P74" s="72"/>
+      <c r="Q74" s="95"/>
       <c r="R74" s="20"/>
       <c r="S74" s="51"/>
       <c r="T74" s="53" t="s">
@@ -3873,23 +3885,23 @@
       </c>
       <c r="C75" s="32"/>
       <c r="D75" s="20"/>
-      <c r="E75" s="70" t="s">
+      <c r="E75" s="106" t="s">
         <v>66</v>
       </c>
-      <c r="F75" s="70"/>
-      <c r="G75" s="70"/>
-      <c r="H75" s="70"/>
-      <c r="I75" s="70"/>
-      <c r="J75" s="70"/>
+      <c r="F75" s="106"/>
+      <c r="G75" s="106"/>
+      <c r="H75" s="106"/>
+      <c r="I75" s="106"/>
+      <c r="J75" s="106"/>
       <c r="K75" s="49"/>
-      <c r="L75" s="74" t="s">
+      <c r="L75" s="71" t="s">
         <v>66</v>
       </c>
-      <c r="M75" s="75"/>
-      <c r="N75" s="75"/>
-      <c r="O75" s="75"/>
-      <c r="P75" s="75"/>
-      <c r="Q75" s="76"/>
+      <c r="M75" s="72"/>
+      <c r="N75" s="72"/>
+      <c r="O75" s="72"/>
+      <c r="P75" s="72"/>
+      <c r="Q75" s="95"/>
       <c r="R75" s="49"/>
       <c r="S75" s="51"/>
       <c r="T75" s="52" t="s">
@@ -3904,24 +3916,24 @@
         <f t="shared" si="5"/>
         <v>43769</v>
       </c>
-      <c r="C76" s="69" t="s">
+      <c r="C76" s="86" t="s">
         <v>79</v>
       </c>
-      <c r="D76" s="69"/>
-      <c r="E76" s="69"/>
-      <c r="F76" s="69"/>
-      <c r="G76" s="69"/>
-      <c r="H76" s="69"/>
-      <c r="I76" s="69"/>
-      <c r="J76" s="69"/>
-      <c r="K76" s="69"/>
-      <c r="L76" s="69"/>
-      <c r="M76" s="69"/>
-      <c r="N76" s="69"/>
-      <c r="O76" s="69"/>
-      <c r="P76" s="69"/>
-      <c r="Q76" s="69"/>
-      <c r="R76" s="69"/>
+      <c r="D76" s="86"/>
+      <c r="E76" s="86"/>
+      <c r="F76" s="86"/>
+      <c r="G76" s="86"/>
+      <c r="H76" s="86"/>
+      <c r="I76" s="86"/>
+      <c r="J76" s="86"/>
+      <c r="K76" s="86"/>
+      <c r="L76" s="86"/>
+      <c r="M76" s="86"/>
+      <c r="N76" s="86"/>
+      <c r="O76" s="86"/>
+      <c r="P76" s="86"/>
+      <c r="Q76" s="86"/>
+      <c r="R76" s="86"/>
       <c r="S76" s="51"/>
       <c r="T76" s="18" t="s">
         <v>21</v>
@@ -3937,23 +3949,23 @@
       </c>
       <c r="C77" s="32"/>
       <c r="D77" s="20"/>
-      <c r="E77" s="70" t="s">
+      <c r="E77" s="105" t="s">
         <v>66</v>
       </c>
-      <c r="F77" s="70"/>
-      <c r="G77" s="70"/>
-      <c r="H77" s="70"/>
-      <c r="I77" s="70"/>
-      <c r="J77" s="70"/>
+      <c r="F77" s="105"/>
+      <c r="G77" s="105"/>
+      <c r="H77" s="105"/>
+      <c r="I77" s="105"/>
+      <c r="J77" s="105"/>
       <c r="K77" s="49"/>
-      <c r="L77" s="74" t="s">
+      <c r="L77" s="119" t="s">
         <v>66</v>
       </c>
-      <c r="M77" s="75"/>
-      <c r="N77" s="75"/>
-      <c r="O77" s="75"/>
-      <c r="P77" s="75"/>
-      <c r="Q77" s="76"/>
+      <c r="M77" s="120"/>
+      <c r="N77" s="120"/>
+      <c r="O77" s="120"/>
+      <c r="P77" s="120"/>
+      <c r="Q77" s="121"/>
       <c r="R77" s="20"/>
       <c r="S77" s="51"/>
       <c r="T77" s="51"/>
@@ -3968,23 +3980,23 @@
       </c>
       <c r="C78" s="50"/>
       <c r="D78" s="49"/>
-      <c r="E78" s="70" t="s">
+      <c r="E78" s="105" t="s">
         <v>66</v>
       </c>
-      <c r="F78" s="70"/>
-      <c r="G78" s="70"/>
-      <c r="H78" s="70"/>
-      <c r="I78" s="70"/>
-      <c r="J78" s="70"/>
+      <c r="F78" s="105"/>
+      <c r="G78" s="105"/>
+      <c r="H78" s="105"/>
+      <c r="I78" s="105"/>
+      <c r="J78" s="105"/>
       <c r="K78" s="49"/>
-      <c r="L78" s="74" t="s">
+      <c r="L78" s="119" t="s">
         <v>66</v>
       </c>
-      <c r="M78" s="75"/>
-      <c r="N78" s="75"/>
-      <c r="O78" s="75"/>
-      <c r="P78" s="75"/>
-      <c r="Q78" s="76"/>
+      <c r="M78" s="120"/>
+      <c r="N78" s="120"/>
+      <c r="O78" s="120"/>
+      <c r="P78" s="120"/>
+      <c r="Q78" s="121"/>
       <c r="R78" s="49"/>
       <c r="S78" s="51"/>
       <c r="T78" s="51"/>
@@ -3997,24 +4009,24 @@
         <f t="shared" si="5"/>
         <v>43772</v>
       </c>
-      <c r="C79" s="69" t="s">
+      <c r="C79" s="86" t="s">
         <v>81</v>
       </c>
-      <c r="D79" s="69"/>
-      <c r="E79" s="69"/>
-      <c r="F79" s="69"/>
-      <c r="G79" s="69"/>
-      <c r="H79" s="69"/>
-      <c r="I79" s="69"/>
-      <c r="J79" s="69"/>
-      <c r="K79" s="69"/>
-      <c r="L79" s="69"/>
-      <c r="M79" s="69"/>
-      <c r="N79" s="69"/>
-      <c r="O79" s="69"/>
-      <c r="P79" s="69"/>
-      <c r="Q79" s="69"/>
-      <c r="R79" s="69"/>
+      <c r="D79" s="86"/>
+      <c r="E79" s="86"/>
+      <c r="F79" s="86"/>
+      <c r="G79" s="86"/>
+      <c r="H79" s="86"/>
+      <c r="I79" s="86"/>
+      <c r="J79" s="86"/>
+      <c r="K79" s="86"/>
+      <c r="L79" s="86"/>
+      <c r="M79" s="86"/>
+      <c r="N79" s="86"/>
+      <c r="O79" s="86"/>
+      <c r="P79" s="86"/>
+      <c r="Q79" s="86"/>
+      <c r="R79" s="86"/>
       <c r="S79" s="51"/>
       <c r="T79" s="51"/>
     </row>
@@ -4088,11 +4100,11 @@
         <f>C72+1</f>
         <v>8</v>
       </c>
-      <c r="D82" s="85" t="s">
+      <c r="D82" s="81" t="s">
         <v>40</v>
       </c>
-      <c r="E82" s="85"/>
-      <c r="F82" s="85"/>
+      <c r="E82" s="81"/>
+      <c r="F82" s="81"/>
       <c r="G82" s="15"/>
       <c r="H82" s="19"/>
       <c r="I82" s="19"/>
@@ -4117,24 +4129,24 @@
         <f>B73+7</f>
         <v>43773</v>
       </c>
-      <c r="C83" s="69" t="s">
+      <c r="C83" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="D83" s="69"/>
-      <c r="E83" s="69"/>
-      <c r="F83" s="69"/>
-      <c r="G83" s="69"/>
-      <c r="H83" s="71" t="s">
+      <c r="D83" s="86"/>
+      <c r="E83" s="86"/>
+      <c r="F83" s="86"/>
+      <c r="G83" s="86"/>
+      <c r="H83" s="88" t="s">
         <v>66</v>
       </c>
-      <c r="I83" s="72"/>
-      <c r="J83" s="72"/>
-      <c r="K83" s="72"/>
-      <c r="L83" s="72"/>
-      <c r="M83" s="72"/>
-      <c r="N83" s="72"/>
-      <c r="O83" s="72"/>
-      <c r="P83" s="104"/>
+      <c r="I83" s="74"/>
+      <c r="J83" s="74"/>
+      <c r="K83" s="74"/>
+      <c r="L83" s="74"/>
+      <c r="M83" s="74"/>
+      <c r="N83" s="74"/>
+      <c r="O83" s="74"/>
+      <c r="P83" s="89"/>
       <c r="Q83" s="20"/>
       <c r="R83" s="20"/>
       <c r="S83" s="51"/>
@@ -4151,26 +4163,28 @@
         <f t="shared" ref="B84:B89" si="6">B74+7</f>
         <v>43774</v>
       </c>
-      <c r="C84" s="69" t="s">
+      <c r="C84" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="D84" s="69"/>
-      <c r="E84" s="69"/>
-      <c r="F84" s="69"/>
-      <c r="G84" s="69"/>
-      <c r="H84" s="69" t="s">
+      <c r="D84" s="86"/>
+      <c r="E84" s="86"/>
+      <c r="F84" s="86"/>
+      <c r="G84" s="86"/>
+      <c r="H84" s="86" t="s">
         <v>44</v>
       </c>
-      <c r="I84" s="69"/>
-      <c r="J84" s="20"/>
-      <c r="K84" s="49"/>
-      <c r="L84" s="49"/>
-      <c r="M84" s="20"/>
-      <c r="N84" s="20"/>
-      <c r="O84" s="49"/>
-      <c r="P84" s="49"/>
-      <c r="Q84" s="20"/>
-      <c r="R84" s="20"/>
+      <c r="I84" s="86"/>
+      <c r="J84" s="88" t="s">
+        <v>66</v>
+      </c>
+      <c r="K84" s="74"/>
+      <c r="L84" s="74"/>
+      <c r="M84" s="74"/>
+      <c r="N84" s="74"/>
+      <c r="O84" s="74"/>
+      <c r="P84" s="74"/>
+      <c r="Q84" s="74"/>
+      <c r="R84" s="89"/>
       <c r="S84" s="51"/>
       <c r="T84" s="53" t="s">
         <v>19</v>
@@ -4187,15 +4201,17 @@
       </c>
       <c r="C85" s="32"/>
       <c r="D85" s="20"/>
-      <c r="E85" s="20"/>
-      <c r="F85" s="20"/>
-      <c r="G85" s="20"/>
-      <c r="H85" s="20"/>
-      <c r="I85" s="20"/>
-      <c r="J85" s="20"/>
-      <c r="K85" s="49"/>
-      <c r="L85" s="49"/>
-      <c r="M85" s="49"/>
+      <c r="E85" s="88" t="s">
+        <v>66</v>
+      </c>
+      <c r="F85" s="74"/>
+      <c r="G85" s="74"/>
+      <c r="H85" s="74"/>
+      <c r="I85" s="74"/>
+      <c r="J85" s="74"/>
+      <c r="K85" s="74"/>
+      <c r="L85" s="74"/>
+      <c r="M85" s="89"/>
       <c r="N85" s="49"/>
       <c r="O85" s="49"/>
       <c r="P85" s="49"/>
@@ -4215,13 +4231,13 @@
         <f t="shared" si="6"/>
         <v>43776</v>
       </c>
-      <c r="C86" s="103" t="s">
+      <c r="C86" s="87" t="s">
         <v>69</v>
       </c>
-      <c r="D86" s="103"/>
-      <c r="E86" s="103"/>
-      <c r="F86" s="103"/>
-      <c r="G86" s="103"/>
+      <c r="D86" s="87"/>
+      <c r="E86" s="87"/>
+      <c r="F86" s="87"/>
+      <c r="G86" s="87"/>
       <c r="H86" s="49"/>
       <c r="I86" s="49"/>
       <c r="J86" s="49"/>
@@ -4303,24 +4319,24 @@
         <f t="shared" si="6"/>
         <v>43779</v>
       </c>
-      <c r="C89" s="69" t="s">
+      <c r="C89" s="86" t="s">
         <v>81</v>
       </c>
-      <c r="D89" s="69"/>
-      <c r="E89" s="69"/>
-      <c r="F89" s="69"/>
-      <c r="G89" s="69"/>
-      <c r="H89" s="69"/>
-      <c r="I89" s="69"/>
-      <c r="J89" s="69"/>
-      <c r="K89" s="69"/>
-      <c r="L89" s="69"/>
-      <c r="M89" s="69"/>
-      <c r="N89" s="69"/>
-      <c r="O89" s="69"/>
-      <c r="P89" s="69"/>
-      <c r="Q89" s="69"/>
-      <c r="R89" s="69"/>
+      <c r="D89" s="86"/>
+      <c r="E89" s="86"/>
+      <c r="F89" s="86"/>
+      <c r="G89" s="86"/>
+      <c r="H89" s="86"/>
+      <c r="I89" s="86"/>
+      <c r="J89" s="86"/>
+      <c r="K89" s="86"/>
+      <c r="L89" s="86"/>
+      <c r="M89" s="86"/>
+      <c r="N89" s="86"/>
+      <c r="O89" s="86"/>
+      <c r="P89" s="86"/>
+      <c r="Q89" s="86"/>
+      <c r="R89" s="86"/>
       <c r="S89" s="51"/>
       <c r="T89" s="51"/>
       <c r="U89" s="54"/>
@@ -4383,7 +4399,7 @@
       <c r="T91" s="51"/>
       <c r="U91" s="54"/>
     </row>
-    <row r="92" spans="1:21" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:21" s="27" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="57">
         <f>A82+7</f>
         <v>43780</v>
@@ -4414,7 +4430,7 @@
       <c r="T92" s="51"/>
       <c r="U92" s="54"/>
     </row>
-    <row r="93" spans="1:21" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:21" s="27" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
         <v>0</v>
       </c>
@@ -4422,22 +4438,24 @@
         <f>B83+7</f>
         <v>43780</v>
       </c>
-      <c r="C93" s="69" t="s">
+      <c r="C93" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="D93" s="69"/>
-      <c r="E93" s="69"/>
-      <c r="F93" s="69"/>
-      <c r="G93" s="69"/>
-      <c r="H93" s="49"/>
-      <c r="I93" s="49"/>
-      <c r="J93" s="49"/>
-      <c r="K93" s="20"/>
-      <c r="L93" s="20"/>
-      <c r="M93" s="20"/>
-      <c r="N93" s="20"/>
-      <c r="O93" s="20"/>
-      <c r="P93" s="20"/>
+      <c r="D93" s="86"/>
+      <c r="E93" s="86"/>
+      <c r="F93" s="86"/>
+      <c r="G93" s="86"/>
+      <c r="H93" s="106" t="s">
+        <v>86</v>
+      </c>
+      <c r="I93" s="106"/>
+      <c r="J93" s="106"/>
+      <c r="K93" s="106"/>
+      <c r="L93" s="106"/>
+      <c r="M93" s="106"/>
+      <c r="N93" s="106"/>
+      <c r="O93" s="106"/>
+      <c r="P93" s="106"/>
       <c r="Q93" s="20"/>
       <c r="R93" s="20"/>
       <c r="S93" s="51"/>
@@ -4446,7 +4464,7 @@
       </c>
       <c r="U93" s="54"/>
     </row>
-    <row r="94" spans="1:21" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:21" s="27" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
         <v>1</v>
       </c>
@@ -4454,22 +4472,24 @@
         <f t="shared" ref="B94:B99" si="7">B84+7</f>
         <v>43781</v>
       </c>
-      <c r="C94" s="69" t="s">
+      <c r="C94" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="D94" s="69"/>
-      <c r="E94" s="69"/>
-      <c r="F94" s="69"/>
-      <c r="G94" s="69"/>
-      <c r="H94" s="20"/>
-      <c r="I94" s="20"/>
-      <c r="J94" s="20"/>
-      <c r="K94" s="49"/>
-      <c r="L94" s="49"/>
-      <c r="M94" s="20"/>
-      <c r="N94" s="20"/>
-      <c r="O94" s="49"/>
-      <c r="P94" s="49"/>
+      <c r="D94" s="86"/>
+      <c r="E94" s="86"/>
+      <c r="F94" s="86"/>
+      <c r="G94" s="86"/>
+      <c r="H94" s="106" t="s">
+        <v>86</v>
+      </c>
+      <c r="I94" s="106"/>
+      <c r="J94" s="106"/>
+      <c r="K94" s="106"/>
+      <c r="L94" s="106"/>
+      <c r="M94" s="106"/>
+      <c r="N94" s="106"/>
+      <c r="O94" s="106"/>
+      <c r="P94" s="106"/>
       <c r="Q94" s="20"/>
       <c r="R94" s="20"/>
       <c r="S94" s="51"/>
@@ -4478,7 +4498,7 @@
       </c>
       <c r="U94" s="54"/>
     </row>
-    <row r="95" spans="1:21" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:21" s="27" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
         <v>2</v>
       </c>
@@ -4508,7 +4528,7 @@
       </c>
       <c r="U95" s="54"/>
     </row>
-    <row r="96" spans="1:21" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:21" s="27" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="s">
         <v>3</v>
       </c>
@@ -4516,18 +4536,20 @@
         <f t="shared" si="7"/>
         <v>43783</v>
       </c>
-      <c r="C96" s="69" t="s">
+      <c r="C96" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="D96" s="69"/>
-      <c r="E96" s="69"/>
-      <c r="F96" s="69"/>
-      <c r="G96" s="69"/>
-      <c r="H96" s="49"/>
-      <c r="I96" s="49"/>
-      <c r="J96" s="49"/>
-      <c r="K96" s="49"/>
-      <c r="L96" s="49"/>
+      <c r="D96" s="86"/>
+      <c r="E96" s="86"/>
+      <c r="F96" s="86"/>
+      <c r="G96" s="86"/>
+      <c r="H96" s="71" t="s">
+        <v>86</v>
+      </c>
+      <c r="I96" s="72"/>
+      <c r="J96" s="72"/>
+      <c r="K96" s="72"/>
+      <c r="L96" s="95"/>
       <c r="M96" s="20"/>
       <c r="N96" s="20"/>
       <c r="O96" s="20"/>
@@ -4540,7 +4562,7 @@
       </c>
       <c r="U96" s="54"/>
     </row>
-    <row r="97" spans="1:21" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:21" s="27" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>4</v>
       </c>
@@ -4604,24 +4626,24 @@
         <f t="shared" si="7"/>
         <v>43786</v>
       </c>
-      <c r="C99" s="69" t="s">
+      <c r="C99" s="86" t="s">
         <v>81</v>
       </c>
-      <c r="D99" s="69"/>
-      <c r="E99" s="69"/>
-      <c r="F99" s="69"/>
-      <c r="G99" s="69"/>
-      <c r="H99" s="69"/>
-      <c r="I99" s="69"/>
-      <c r="J99" s="69"/>
-      <c r="K99" s="69"/>
-      <c r="L99" s="69"/>
-      <c r="M99" s="69"/>
-      <c r="N99" s="69"/>
-      <c r="O99" s="69"/>
-      <c r="P99" s="69"/>
-      <c r="Q99" s="69"/>
-      <c r="R99" s="69"/>
+      <c r="D99" s="86"/>
+      <c r="E99" s="86"/>
+      <c r="F99" s="86"/>
+      <c r="G99" s="86"/>
+      <c r="H99" s="86"/>
+      <c r="I99" s="86"/>
+      <c r="J99" s="86"/>
+      <c r="K99" s="86"/>
+      <c r="L99" s="86"/>
+      <c r="M99" s="86"/>
+      <c r="N99" s="86"/>
+      <c r="O99" s="86"/>
+      <c r="P99" s="86"/>
+      <c r="Q99" s="86"/>
+      <c r="R99" s="86"/>
       <c r="S99" s="51"/>
       <c r="T99" s="51"/>
       <c r="U99" s="54"/>
@@ -4723,13 +4745,13 @@
         <f>B93+7</f>
         <v>43787</v>
       </c>
-      <c r="C103" s="69" t="s">
+      <c r="C103" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="D103" s="69"/>
-      <c r="E103" s="69"/>
-      <c r="F103" s="69"/>
-      <c r="G103" s="69"/>
+      <c r="D103" s="86"/>
+      <c r="E103" s="86"/>
+      <c r="F103" s="86"/>
+      <c r="G103" s="86"/>
       <c r="H103" s="49"/>
       <c r="I103" s="49"/>
       <c r="J103" s="49"/>
@@ -4755,17 +4777,17 @@
         <f t="shared" ref="B104:B109" si="8">B94+7</f>
         <v>43788</v>
       </c>
-      <c r="C104" s="69" t="s">
+      <c r="C104" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="D104" s="69"/>
-      <c r="E104" s="69"/>
-      <c r="F104" s="69"/>
-      <c r="G104" s="69"/>
-      <c r="H104" s="69" t="s">
+      <c r="D104" s="86"/>
+      <c r="E104" s="86"/>
+      <c r="F104" s="86"/>
+      <c r="G104" s="86"/>
+      <c r="H104" s="86" t="s">
         <v>44</v>
       </c>
-      <c r="I104" s="69"/>
+      <c r="I104" s="86"/>
       <c r="J104" s="20"/>
       <c r="K104" s="49"/>
       <c r="L104" s="49"/>
@@ -4819,13 +4841,13 @@
         <f t="shared" si="8"/>
         <v>43790</v>
       </c>
-      <c r="C106" s="69" t="s">
+      <c r="C106" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="D106" s="69"/>
-      <c r="E106" s="69"/>
-      <c r="F106" s="69"/>
-      <c r="G106" s="69"/>
+      <c r="D106" s="86"/>
+      <c r="E106" s="86"/>
+      <c r="F106" s="86"/>
+      <c r="G106" s="86"/>
       <c r="H106" s="49"/>
       <c r="I106" s="49"/>
       <c r="J106" s="49"/>
@@ -4907,24 +4929,24 @@
         <f t="shared" si="8"/>
         <v>43793</v>
       </c>
-      <c r="C109" s="69" t="s">
+      <c r="C109" s="86" t="s">
         <v>81</v>
       </c>
-      <c r="D109" s="69"/>
-      <c r="E109" s="69"/>
-      <c r="F109" s="69"/>
-      <c r="G109" s="69"/>
-      <c r="H109" s="69"/>
-      <c r="I109" s="69"/>
-      <c r="J109" s="69"/>
-      <c r="K109" s="69"/>
-      <c r="L109" s="69"/>
-      <c r="M109" s="69"/>
-      <c r="N109" s="69"/>
-      <c r="O109" s="69"/>
-      <c r="P109" s="69"/>
-      <c r="Q109" s="69"/>
-      <c r="R109" s="69"/>
+      <c r="D109" s="86"/>
+      <c r="E109" s="86"/>
+      <c r="F109" s="86"/>
+      <c r="G109" s="86"/>
+      <c r="H109" s="86"/>
+      <c r="I109" s="86"/>
+      <c r="J109" s="86"/>
+      <c r="K109" s="86"/>
+      <c r="L109" s="86"/>
+      <c r="M109" s="86"/>
+      <c r="N109" s="86"/>
+      <c r="O109" s="86"/>
+      <c r="P109" s="86"/>
+      <c r="Q109" s="86"/>
+      <c r="R109" s="86"/>
       <c r="S109" s="51"/>
       <c r="T109" s="51"/>
       <c r="U109" s="54"/>
@@ -4999,11 +5021,11 @@
         <f>C102+1</f>
         <v>11</v>
       </c>
-      <c r="D112" s="85" t="s">
+      <c r="D112" s="81" t="s">
         <v>43</v>
       </c>
-      <c r="E112" s="85"/>
-      <c r="F112" s="85"/>
+      <c r="E112" s="81"/>
+      <c r="F112" s="81"/>
       <c r="G112" s="15"/>
       <c r="H112" s="15"/>
       <c r="I112" s="15"/>
@@ -5028,13 +5050,13 @@
         <f>B103+7</f>
         <v>43794</v>
       </c>
-      <c r="C113" s="69" t="s">
+      <c r="C113" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="D113" s="69"/>
-      <c r="E113" s="69"/>
-      <c r="F113" s="69"/>
-      <c r="G113" s="69"/>
+      <c r="D113" s="86"/>
+      <c r="E113" s="86"/>
+      <c r="F113" s="86"/>
+      <c r="G113" s="86"/>
       <c r="H113" s="49"/>
       <c r="I113" s="49"/>
       <c r="J113" s="49"/>
@@ -5060,13 +5082,13 @@
         <f t="shared" ref="B114:B119" si="9">B104+7</f>
         <v>43795</v>
       </c>
-      <c r="C114" s="69" t="s">
+      <c r="C114" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="D114" s="69"/>
-      <c r="E114" s="69"/>
-      <c r="F114" s="69"/>
-      <c r="G114" s="69"/>
+      <c r="D114" s="86"/>
+      <c r="E114" s="86"/>
+      <c r="F114" s="86"/>
+      <c r="G114" s="86"/>
       <c r="H114" s="20"/>
       <c r="I114" s="20"/>
       <c r="J114" s="20"/>
@@ -5094,23 +5116,23 @@
       </c>
       <c r="C115" s="32"/>
       <c r="D115" s="20"/>
-      <c r="E115" s="70" t="s">
+      <c r="E115" s="76" t="s">
         <v>65</v>
       </c>
-      <c r="F115" s="70"/>
-      <c r="G115" s="70"/>
-      <c r="H115" s="70"/>
-      <c r="I115" s="70"/>
-      <c r="J115" s="70"/>
+      <c r="F115" s="76"/>
+      <c r="G115" s="76"/>
+      <c r="H115" s="76"/>
+      <c r="I115" s="76"/>
+      <c r="J115" s="76"/>
       <c r="K115" s="49"/>
-      <c r="L115" s="74" t="s">
+      <c r="L115" s="69" t="s">
         <v>65</v>
       </c>
-      <c r="M115" s="75"/>
-      <c r="N115" s="75"/>
-      <c r="O115" s="75"/>
-      <c r="P115" s="75"/>
-      <c r="Q115" s="76"/>
+      <c r="M115" s="77"/>
+      <c r="N115" s="77"/>
+      <c r="O115" s="77"/>
+      <c r="P115" s="77"/>
+      <c r="Q115" s="70"/>
       <c r="R115" s="49"/>
       <c r="S115" s="51"/>
       <c r="T115" s="52" t="s">
@@ -5126,27 +5148,27 @@
         <f t="shared" si="9"/>
         <v>43797</v>
       </c>
-      <c r="C116" s="69" t="s">
+      <c r="C116" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="D116" s="69"/>
-      <c r="E116" s="69"/>
-      <c r="F116" s="69"/>
-      <c r="G116" s="69"/>
-      <c r="H116" s="70" t="s">
+      <c r="D116" s="86"/>
+      <c r="E116" s="86"/>
+      <c r="F116" s="86"/>
+      <c r="G116" s="86"/>
+      <c r="H116" s="76" t="s">
         <v>55</v>
       </c>
-      <c r="I116" s="70"/>
-      <c r="J116" s="70"/>
-      <c r="K116" s="71" t="s">
+      <c r="I116" s="76"/>
+      <c r="J116" s="76"/>
+      <c r="K116" s="78" t="s">
         <v>65</v>
       </c>
-      <c r="L116" s="72"/>
-      <c r="M116" s="72"/>
-      <c r="N116" s="72"/>
-      <c r="O116" s="72"/>
-      <c r="P116" s="72"/>
-      <c r="Q116" s="73"/>
+      <c r="L116" s="79"/>
+      <c r="M116" s="79"/>
+      <c r="N116" s="79"/>
+      <c r="O116" s="79"/>
+      <c r="P116" s="79"/>
+      <c r="Q116" s="113"/>
       <c r="R116" s="20"/>
       <c r="S116" s="51"/>
       <c r="T116" s="18" t="s">
@@ -5164,23 +5186,23 @@
       </c>
       <c r="C117" s="32"/>
       <c r="D117" s="20"/>
-      <c r="E117" s="70" t="s">
+      <c r="E117" s="76" t="s">
         <v>65</v>
       </c>
-      <c r="F117" s="70"/>
-      <c r="G117" s="70"/>
-      <c r="H117" s="70"/>
-      <c r="I117" s="70"/>
-      <c r="J117" s="70"/>
+      <c r="F117" s="76"/>
+      <c r="G117" s="76"/>
+      <c r="H117" s="76"/>
+      <c r="I117" s="76"/>
+      <c r="J117" s="76"/>
       <c r="K117" s="49"/>
-      <c r="L117" s="74" t="s">
+      <c r="L117" s="69" t="s">
         <v>65</v>
       </c>
-      <c r="M117" s="75"/>
-      <c r="N117" s="75"/>
-      <c r="O117" s="75"/>
-      <c r="P117" s="75"/>
-      <c r="Q117" s="76"/>
+      <c r="M117" s="77"/>
+      <c r="N117" s="77"/>
+      <c r="O117" s="77"/>
+      <c r="P117" s="77"/>
+      <c r="Q117" s="70"/>
       <c r="R117" s="20"/>
       <c r="S117" s="51"/>
       <c r="T117" s="51"/>
@@ -5196,23 +5218,23 @@
       </c>
       <c r="C118" s="50"/>
       <c r="D118" s="49"/>
-      <c r="E118" s="70" t="s">
+      <c r="E118" s="76" t="s">
         <v>65</v>
       </c>
-      <c r="F118" s="70"/>
-      <c r="G118" s="70"/>
-      <c r="H118" s="70"/>
-      <c r="I118" s="70"/>
-      <c r="J118" s="70"/>
+      <c r="F118" s="76"/>
+      <c r="G118" s="76"/>
+      <c r="H118" s="76"/>
+      <c r="I118" s="76"/>
+      <c r="J118" s="76"/>
       <c r="K118" s="49"/>
-      <c r="L118" s="74" t="s">
+      <c r="L118" s="69" t="s">
         <v>65</v>
       </c>
-      <c r="M118" s="75"/>
-      <c r="N118" s="75"/>
-      <c r="O118" s="75"/>
-      <c r="P118" s="75"/>
-      <c r="Q118" s="76"/>
+      <c r="M118" s="77"/>
+      <c r="N118" s="77"/>
+      <c r="O118" s="77"/>
+      <c r="P118" s="77"/>
+      <c r="Q118" s="70"/>
       <c r="R118" s="49"/>
       <c r="S118" s="51"/>
       <c r="T118" s="51"/>
@@ -5226,24 +5248,24 @@
         <f t="shared" si="9"/>
         <v>43800</v>
       </c>
-      <c r="C119" s="69" t="s">
+      <c r="C119" s="86" t="s">
         <v>81</v>
       </c>
-      <c r="D119" s="69"/>
-      <c r="E119" s="69"/>
-      <c r="F119" s="69"/>
-      <c r="G119" s="69"/>
-      <c r="H119" s="69"/>
-      <c r="I119" s="69"/>
-      <c r="J119" s="69"/>
-      <c r="K119" s="69"/>
-      <c r="L119" s="69"/>
-      <c r="M119" s="69"/>
-      <c r="N119" s="69"/>
-      <c r="O119" s="69"/>
-      <c r="P119" s="69"/>
-      <c r="Q119" s="69"/>
-      <c r="R119" s="69"/>
+      <c r="D119" s="86"/>
+      <c r="E119" s="86"/>
+      <c r="F119" s="86"/>
+      <c r="G119" s="86"/>
+      <c r="H119" s="86"/>
+      <c r="I119" s="86"/>
+      <c r="J119" s="86"/>
+      <c r="K119" s="86"/>
+      <c r="L119" s="86"/>
+      <c r="M119" s="86"/>
+      <c r="N119" s="86"/>
+      <c r="O119" s="86"/>
+      <c r="P119" s="86"/>
+      <c r="Q119" s="86"/>
+      <c r="R119" s="86"/>
       <c r="S119" s="51"/>
       <c r="T119" s="51"/>
       <c r="U119" s="54"/>
@@ -5318,11 +5340,11 @@
         <f>C112+1</f>
         <v>12</v>
       </c>
-      <c r="D122" s="85" t="s">
+      <c r="D122" s="81" t="s">
         <v>41</v>
       </c>
-      <c r="E122" s="85"/>
-      <c r="F122" s="85"/>
+      <c r="E122" s="81"/>
+      <c r="F122" s="81"/>
       <c r="G122" s="15"/>
       <c r="H122" s="15"/>
       <c r="I122" s="15"/>
@@ -5347,24 +5369,24 @@
         <f>B113+7</f>
         <v>43801</v>
       </c>
-      <c r="C123" s="69" t="s">
+      <c r="C123" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="D123" s="69"/>
-      <c r="E123" s="69"/>
-      <c r="F123" s="69"/>
-      <c r="G123" s="69"/>
-      <c r="H123" s="71" t="s">
+      <c r="D123" s="86"/>
+      <c r="E123" s="86"/>
+      <c r="F123" s="86"/>
+      <c r="G123" s="86"/>
+      <c r="H123" s="78" t="s">
         <v>65</v>
       </c>
-      <c r="I123" s="72"/>
-      <c r="J123" s="72"/>
-      <c r="K123" s="72"/>
-      <c r="L123" s="72"/>
-      <c r="M123" s="72"/>
-      <c r="N123" s="72"/>
-      <c r="O123" s="72"/>
-      <c r="P123" s="104"/>
+      <c r="I123" s="79"/>
+      <c r="J123" s="79"/>
+      <c r="K123" s="79"/>
+      <c r="L123" s="79"/>
+      <c r="M123" s="79"/>
+      <c r="N123" s="79"/>
+      <c r="O123" s="79"/>
+      <c r="P123" s="80"/>
       <c r="Q123" s="20"/>
       <c r="R123" s="20"/>
       <c r="S123" s="51"/>
@@ -5381,17 +5403,17 @@
         <f t="shared" ref="B124:B129" si="10">B114+7</f>
         <v>43802</v>
       </c>
-      <c r="C124" s="69" t="s">
+      <c r="C124" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="D124" s="69"/>
-      <c r="E124" s="69"/>
-      <c r="F124" s="69"/>
-      <c r="G124" s="69"/>
-      <c r="H124" s="69" t="s">
+      <c r="D124" s="86"/>
+      <c r="E124" s="86"/>
+      <c r="F124" s="86"/>
+      <c r="G124" s="86"/>
+      <c r="H124" s="86" t="s">
         <v>44</v>
       </c>
-      <c r="I124" s="69"/>
+      <c r="I124" s="86"/>
       <c r="J124" s="20"/>
       <c r="K124" s="49"/>
       <c r="L124" s="49"/>
@@ -5445,13 +5467,13 @@
         <f t="shared" si="10"/>
         <v>43804</v>
       </c>
-      <c r="C126" s="103" t="s">
+      <c r="C126" s="87" t="s">
         <v>80</v>
       </c>
-      <c r="D126" s="103"/>
-      <c r="E126" s="103"/>
-      <c r="F126" s="103"/>
-      <c r="G126" s="103"/>
+      <c r="D126" s="87"/>
+      <c r="E126" s="87"/>
+      <c r="F126" s="87"/>
+      <c r="G126" s="87"/>
       <c r="H126" s="49"/>
       <c r="I126" s="49"/>
       <c r="J126" s="49"/>
@@ -5533,24 +5555,24 @@
         <f t="shared" si="10"/>
         <v>43807</v>
       </c>
-      <c r="C129" s="69" t="s">
+      <c r="C129" s="86" t="s">
         <v>81</v>
       </c>
-      <c r="D129" s="69"/>
-      <c r="E129" s="69"/>
-      <c r="F129" s="69"/>
-      <c r="G129" s="69"/>
-      <c r="H129" s="69"/>
-      <c r="I129" s="69"/>
-      <c r="J129" s="69"/>
-      <c r="K129" s="69"/>
-      <c r="L129" s="69"/>
-      <c r="M129" s="69"/>
-      <c r="N129" s="69"/>
-      <c r="O129" s="69"/>
-      <c r="P129" s="69"/>
-      <c r="Q129" s="69"/>
-      <c r="R129" s="69"/>
+      <c r="D129" s="86"/>
+      <c r="E129" s="86"/>
+      <c r="F129" s="86"/>
+      <c r="G129" s="86"/>
+      <c r="H129" s="86"/>
+      <c r="I129" s="86"/>
+      <c r="J129" s="86"/>
+      <c r="K129" s="86"/>
+      <c r="L129" s="86"/>
+      <c r="M129" s="86"/>
+      <c r="N129" s="86"/>
+      <c r="O129" s="86"/>
+      <c r="P129" s="86"/>
+      <c r="Q129" s="86"/>
+      <c r="R129" s="86"/>
       <c r="S129" s="51"/>
       <c r="T129" s="51"/>
       <c r="U129" s="54"/>
@@ -5652,13 +5674,13 @@
         <f>B123+7</f>
         <v>43808</v>
       </c>
-      <c r="C133" s="69" t="s">
+      <c r="C133" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="D133" s="69"/>
-      <c r="E133" s="69"/>
-      <c r="F133" s="69"/>
-      <c r="G133" s="69"/>
+      <c r="D133" s="86"/>
+      <c r="E133" s="86"/>
+      <c r="F133" s="86"/>
+      <c r="G133" s="86"/>
       <c r="H133" s="49"/>
       <c r="I133" s="49"/>
       <c r="J133" s="49"/>
@@ -5684,13 +5706,13 @@
         <f t="shared" ref="B134:B139" si="11">B124+7</f>
         <v>43809</v>
       </c>
-      <c r="C134" s="69" t="s">
+      <c r="C134" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="D134" s="69"/>
-      <c r="E134" s="69"/>
-      <c r="F134" s="69"/>
-      <c r="G134" s="69"/>
+      <c r="D134" s="86"/>
+      <c r="E134" s="86"/>
+      <c r="F134" s="86"/>
+      <c r="G134" s="86"/>
       <c r="H134" s="20"/>
       <c r="I134" s="20"/>
       <c r="J134" s="20"/>
@@ -5746,13 +5768,13 @@
         <f t="shared" si="11"/>
         <v>43811</v>
       </c>
-      <c r="C136" s="69" t="s">
+      <c r="C136" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="D136" s="69"/>
-      <c r="E136" s="69"/>
-      <c r="F136" s="69"/>
-      <c r="G136" s="69"/>
+      <c r="D136" s="86"/>
+      <c r="E136" s="86"/>
+      <c r="F136" s="86"/>
+      <c r="G136" s="86"/>
       <c r="H136" s="20"/>
       <c r="I136" s="49"/>
       <c r="J136" s="49"/>
@@ -5834,24 +5856,24 @@
         <f t="shared" si="11"/>
         <v>43814</v>
       </c>
-      <c r="C139" s="69" t="s">
+      <c r="C139" s="86" t="s">
         <v>81</v>
       </c>
-      <c r="D139" s="69"/>
-      <c r="E139" s="69"/>
-      <c r="F139" s="69"/>
-      <c r="G139" s="69"/>
-      <c r="H139" s="69"/>
-      <c r="I139" s="69"/>
-      <c r="J139" s="69"/>
-      <c r="K139" s="69"/>
-      <c r="L139" s="69"/>
-      <c r="M139" s="69"/>
-      <c r="N139" s="69"/>
-      <c r="O139" s="69"/>
-      <c r="P139" s="69"/>
-      <c r="Q139" s="69"/>
-      <c r="R139" s="69"/>
+      <c r="D139" s="86"/>
+      <c r="E139" s="86"/>
+      <c r="F139" s="86"/>
+      <c r="G139" s="86"/>
+      <c r="H139" s="86"/>
+      <c r="I139" s="86"/>
+      <c r="J139" s="86"/>
+      <c r="K139" s="86"/>
+      <c r="L139" s="86"/>
+      <c r="M139" s="86"/>
+      <c r="N139" s="86"/>
+      <c r="O139" s="86"/>
+      <c r="P139" s="86"/>
+      <c r="Q139" s="86"/>
+      <c r="R139" s="86"/>
       <c r="S139" s="51"/>
       <c r="T139" s="51"/>
       <c r="U139" s="54"/>
@@ -5946,19 +5968,19 @@
         <f>C132+1</f>
         <v>14</v>
       </c>
-      <c r="D142" s="85" t="s">
+      <c r="D142" s="81" t="s">
         <v>30</v>
       </c>
-      <c r="E142" s="85"/>
-      <c r="F142" s="85"/>
+      <c r="E142" s="81"/>
+      <c r="F142" s="81"/>
       <c r="G142" s="15"/>
-      <c r="H142" s="85" t="s">
+      <c r="H142" s="81" t="s">
         <v>52</v>
       </c>
-      <c r="I142" s="85"/>
-      <c r="J142" s="85"/>
-      <c r="K142" s="85"/>
-      <c r="L142" s="85"/>
+      <c r="I142" s="81"/>
+      <c r="J142" s="81"/>
+      <c r="K142" s="81"/>
+      <c r="L142" s="81"/>
       <c r="M142" s="19"/>
       <c r="N142" s="19"/>
       <c r="O142" s="19"/>
@@ -5977,11 +5999,11 @@
         <f>B133+7</f>
         <v>43815</v>
       </c>
-      <c r="C143" s="70" t="s">
+      <c r="C143" s="76" t="s">
         <v>55</v>
       </c>
-      <c r="D143" s="70"/>
-      <c r="E143" s="70"/>
+      <c r="D143" s="76"/>
+      <c r="E143" s="76"/>
       <c r="F143" s="20"/>
       <c r="G143" s="20"/>
       <c r="H143" s="20"/>
@@ -6352,24 +6374,24 @@
         <f t="shared" si="13"/>
         <v>43824</v>
       </c>
-      <c r="C155" s="111" t="s">
+      <c r="C155" s="85" t="s">
         <v>53</v>
       </c>
-      <c r="D155" s="111"/>
-      <c r="E155" s="111"/>
-      <c r="F155" s="111"/>
-      <c r="G155" s="111"/>
-      <c r="H155" s="111"/>
-      <c r="I155" s="111"/>
-      <c r="J155" s="111"/>
-      <c r="K155" s="111"/>
-      <c r="L155" s="111"/>
-      <c r="M155" s="111"/>
-      <c r="N155" s="111"/>
-      <c r="O155" s="111"/>
-      <c r="P155" s="111"/>
-      <c r="Q155" s="111"/>
-      <c r="R155" s="111"/>
+      <c r="D155" s="85"/>
+      <c r="E155" s="85"/>
+      <c r="F155" s="85"/>
+      <c r="G155" s="85"/>
+      <c r="H155" s="85"/>
+      <c r="I155" s="85"/>
+      <c r="J155" s="85"/>
+      <c r="K155" s="85"/>
+      <c r="L155" s="85"/>
+      <c r="M155" s="85"/>
+      <c r="N155" s="85"/>
+      <c r="O155" s="85"/>
+      <c r="P155" s="85"/>
+      <c r="Q155" s="85"/>
+      <c r="R155" s="85"/>
       <c r="S155" s="51"/>
       <c r="T155" s="52" t="s">
         <v>20</v>
@@ -6384,22 +6406,22 @@
         <f t="shared" si="13"/>
         <v>43825</v>
       </c>
-      <c r="C156" s="111"/>
-      <c r="D156" s="111"/>
-      <c r="E156" s="111"/>
-      <c r="F156" s="111"/>
-      <c r="G156" s="111"/>
-      <c r="H156" s="111"/>
-      <c r="I156" s="111"/>
-      <c r="J156" s="111"/>
-      <c r="K156" s="111"/>
-      <c r="L156" s="111"/>
-      <c r="M156" s="111"/>
-      <c r="N156" s="111"/>
-      <c r="O156" s="111"/>
-      <c r="P156" s="111"/>
-      <c r="Q156" s="111"/>
-      <c r="R156" s="111"/>
+      <c r="C156" s="85"/>
+      <c r="D156" s="85"/>
+      <c r="E156" s="85"/>
+      <c r="F156" s="85"/>
+      <c r="G156" s="85"/>
+      <c r="H156" s="85"/>
+      <c r="I156" s="85"/>
+      <c r="J156" s="85"/>
+      <c r="K156" s="85"/>
+      <c r="L156" s="85"/>
+      <c r="M156" s="85"/>
+      <c r="N156" s="85"/>
+      <c r="O156" s="85"/>
+      <c r="P156" s="85"/>
+      <c r="Q156" s="85"/>
+      <c r="R156" s="85"/>
       <c r="S156" s="51"/>
       <c r="T156" s="18" t="s">
         <v>21</v>
@@ -6414,22 +6436,22 @@
         <f t="shared" si="13"/>
         <v>43826</v>
       </c>
-      <c r="C157" s="111"/>
-      <c r="D157" s="111"/>
-      <c r="E157" s="111"/>
-      <c r="F157" s="111"/>
-      <c r="G157" s="111"/>
-      <c r="H157" s="111"/>
-      <c r="I157" s="111"/>
-      <c r="J157" s="111"/>
-      <c r="K157" s="111"/>
-      <c r="L157" s="111"/>
-      <c r="M157" s="111"/>
-      <c r="N157" s="111"/>
-      <c r="O157" s="111"/>
-      <c r="P157" s="111"/>
-      <c r="Q157" s="111"/>
-      <c r="R157" s="111"/>
+      <c r="C157" s="85"/>
+      <c r="D157" s="85"/>
+      <c r="E157" s="85"/>
+      <c r="F157" s="85"/>
+      <c r="G157" s="85"/>
+      <c r="H157" s="85"/>
+      <c r="I157" s="85"/>
+      <c r="J157" s="85"/>
+      <c r="K157" s="85"/>
+      <c r="L157" s="85"/>
+      <c r="M157" s="85"/>
+      <c r="N157" s="85"/>
+      <c r="O157" s="85"/>
+      <c r="P157" s="85"/>
+      <c r="Q157" s="85"/>
+      <c r="R157" s="85"/>
       <c r="S157" s="51"/>
       <c r="T157" s="51"/>
       <c r="U157" s="54"/>
@@ -6442,22 +6464,22 @@
         <f t="shared" si="13"/>
         <v>43827</v>
       </c>
-      <c r="C158" s="111"/>
-      <c r="D158" s="111"/>
-      <c r="E158" s="111"/>
-      <c r="F158" s="111"/>
-      <c r="G158" s="111"/>
-      <c r="H158" s="111"/>
-      <c r="I158" s="111"/>
-      <c r="J158" s="111"/>
-      <c r="K158" s="111"/>
-      <c r="L158" s="111"/>
-      <c r="M158" s="111"/>
-      <c r="N158" s="111"/>
-      <c r="O158" s="111"/>
-      <c r="P158" s="111"/>
-      <c r="Q158" s="111"/>
-      <c r="R158" s="111"/>
+      <c r="C158" s="85"/>
+      <c r="D158" s="85"/>
+      <c r="E158" s="85"/>
+      <c r="F158" s="85"/>
+      <c r="G158" s="85"/>
+      <c r="H158" s="85"/>
+      <c r="I158" s="85"/>
+      <c r="J158" s="85"/>
+      <c r="K158" s="85"/>
+      <c r="L158" s="85"/>
+      <c r="M158" s="85"/>
+      <c r="N158" s="85"/>
+      <c r="O158" s="85"/>
+      <c r="P158" s="85"/>
+      <c r="Q158" s="85"/>
+      <c r="R158" s="85"/>
       <c r="S158" s="51"/>
       <c r="T158" s="51"/>
       <c r="U158" s="54"/>
@@ -6470,22 +6492,22 @@
         <f t="shared" si="13"/>
         <v>43828</v>
       </c>
-      <c r="C159" s="111"/>
-      <c r="D159" s="111"/>
-      <c r="E159" s="111"/>
-      <c r="F159" s="111"/>
-      <c r="G159" s="111"/>
-      <c r="H159" s="111"/>
-      <c r="I159" s="111"/>
-      <c r="J159" s="111"/>
-      <c r="K159" s="111"/>
-      <c r="L159" s="111"/>
-      <c r="M159" s="111"/>
-      <c r="N159" s="111"/>
-      <c r="O159" s="111"/>
-      <c r="P159" s="111"/>
-      <c r="Q159" s="111"/>
-      <c r="R159" s="111"/>
+      <c r="C159" s="85"/>
+      <c r="D159" s="85"/>
+      <c r="E159" s="85"/>
+      <c r="F159" s="85"/>
+      <c r="G159" s="85"/>
+      <c r="H159" s="85"/>
+      <c r="I159" s="85"/>
+      <c r="J159" s="85"/>
+      <c r="K159" s="85"/>
+      <c r="L159" s="85"/>
+      <c r="M159" s="85"/>
+      <c r="N159" s="85"/>
+      <c r="O159" s="85"/>
+      <c r="P159" s="85"/>
+      <c r="Q159" s="85"/>
+      <c r="R159" s="85"/>
       <c r="S159" s="51"/>
       <c r="T159" s="51"/>
       <c r="U159" s="54"/>
@@ -6607,24 +6629,24 @@
         <f>B153+7</f>
         <v>43829</v>
       </c>
-      <c r="C163" s="111" t="s">
+      <c r="C163" s="85" t="s">
         <v>54</v>
       </c>
-      <c r="D163" s="111"/>
-      <c r="E163" s="111"/>
-      <c r="F163" s="111"/>
-      <c r="G163" s="111"/>
-      <c r="H163" s="111"/>
-      <c r="I163" s="111"/>
-      <c r="J163" s="111"/>
-      <c r="K163" s="111"/>
-      <c r="L163" s="111"/>
-      <c r="M163" s="111"/>
-      <c r="N163" s="111"/>
-      <c r="O163" s="111"/>
-      <c r="P163" s="111"/>
-      <c r="Q163" s="111"/>
-      <c r="R163" s="111"/>
+      <c r="D163" s="85"/>
+      <c r="E163" s="85"/>
+      <c r="F163" s="85"/>
+      <c r="G163" s="85"/>
+      <c r="H163" s="85"/>
+      <c r="I163" s="85"/>
+      <c r="J163" s="85"/>
+      <c r="K163" s="85"/>
+      <c r="L163" s="85"/>
+      <c r="M163" s="85"/>
+      <c r="N163" s="85"/>
+      <c r="O163" s="85"/>
+      <c r="P163" s="85"/>
+      <c r="Q163" s="85"/>
+      <c r="R163" s="85"/>
       <c r="S163" s="51"/>
       <c r="T163" s="30" t="s">
         <v>22</v>
@@ -6639,22 +6661,22 @@
         <f t="shared" ref="B164:B169" si="14">B154+7</f>
         <v>43830</v>
       </c>
-      <c r="C164" s="111"/>
-      <c r="D164" s="111"/>
-      <c r="E164" s="111"/>
-      <c r="F164" s="111"/>
-      <c r="G164" s="111"/>
-      <c r="H164" s="111"/>
-      <c r="I164" s="111"/>
-      <c r="J164" s="111"/>
-      <c r="K164" s="111"/>
-      <c r="L164" s="111"/>
-      <c r="M164" s="111"/>
-      <c r="N164" s="111"/>
-      <c r="O164" s="111"/>
-      <c r="P164" s="111"/>
-      <c r="Q164" s="111"/>
-      <c r="R164" s="111"/>
+      <c r="C164" s="85"/>
+      <c r="D164" s="85"/>
+      <c r="E164" s="85"/>
+      <c r="F164" s="85"/>
+      <c r="G164" s="85"/>
+      <c r="H164" s="85"/>
+      <c r="I164" s="85"/>
+      <c r="J164" s="85"/>
+      <c r="K164" s="85"/>
+      <c r="L164" s="85"/>
+      <c r="M164" s="85"/>
+      <c r="N164" s="85"/>
+      <c r="O164" s="85"/>
+      <c r="P164" s="85"/>
+      <c r="Q164" s="85"/>
+      <c r="R164" s="85"/>
       <c r="S164" s="51"/>
       <c r="T164" s="53" t="s">
         <v>19</v>
@@ -6669,22 +6691,22 @@
         <f t="shared" si="14"/>
         <v>43831</v>
       </c>
-      <c r="C165" s="111"/>
-      <c r="D165" s="111"/>
-      <c r="E165" s="111"/>
-      <c r="F165" s="111"/>
-      <c r="G165" s="111"/>
-      <c r="H165" s="111"/>
-      <c r="I165" s="111"/>
-      <c r="J165" s="111"/>
-      <c r="K165" s="111"/>
-      <c r="L165" s="111"/>
-      <c r="M165" s="111"/>
-      <c r="N165" s="111"/>
-      <c r="O165" s="111"/>
-      <c r="P165" s="111"/>
-      <c r="Q165" s="111"/>
-      <c r="R165" s="111"/>
+      <c r="C165" s="85"/>
+      <c r="D165" s="85"/>
+      <c r="E165" s="85"/>
+      <c r="F165" s="85"/>
+      <c r="G165" s="85"/>
+      <c r="H165" s="85"/>
+      <c r="I165" s="85"/>
+      <c r="J165" s="85"/>
+      <c r="K165" s="85"/>
+      <c r="L165" s="85"/>
+      <c r="M165" s="85"/>
+      <c r="N165" s="85"/>
+      <c r="O165" s="85"/>
+      <c r="P165" s="85"/>
+      <c r="Q165" s="85"/>
+      <c r="R165" s="85"/>
       <c r="S165" s="51"/>
       <c r="T165" s="52" t="s">
         <v>20</v>
@@ -6701,23 +6723,23 @@
       </c>
       <c r="C166" s="32"/>
       <c r="D166" s="20"/>
-      <c r="E166" s="70" t="s">
+      <c r="E166" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="F166" s="70"/>
-      <c r="G166" s="70"/>
-      <c r="H166" s="70"/>
-      <c r="I166" s="70"/>
-      <c r="J166" s="70"/>
+      <c r="F166" s="76"/>
+      <c r="G166" s="76"/>
+      <c r="H166" s="76"/>
+      <c r="I166" s="76"/>
+      <c r="J166" s="76"/>
       <c r="K166" s="49"/>
-      <c r="L166" s="74" t="s">
+      <c r="L166" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="M166" s="75"/>
-      <c r="N166" s="75"/>
-      <c r="O166" s="75"/>
-      <c r="P166" s="75"/>
-      <c r="Q166" s="76"/>
+      <c r="M166" s="77"/>
+      <c r="N166" s="77"/>
+      <c r="O166" s="77"/>
+      <c r="P166" s="77"/>
+      <c r="Q166" s="70"/>
       <c r="R166" s="20"/>
       <c r="S166" s="51"/>
       <c r="T166" s="18" t="s">
@@ -6735,23 +6757,23 @@
       </c>
       <c r="C167" s="50"/>
       <c r="D167" s="49"/>
-      <c r="E167" s="70" t="s">
+      <c r="E167" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="F167" s="70"/>
-      <c r="G167" s="70"/>
-      <c r="H167" s="70"/>
-      <c r="I167" s="70"/>
-      <c r="J167" s="70"/>
+      <c r="F167" s="76"/>
+      <c r="G167" s="76"/>
+      <c r="H167" s="76"/>
+      <c r="I167" s="76"/>
+      <c r="J167" s="76"/>
       <c r="K167" s="49"/>
-      <c r="L167" s="74" t="s">
+      <c r="L167" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="M167" s="75"/>
-      <c r="N167" s="75"/>
-      <c r="O167" s="75"/>
-      <c r="P167" s="75"/>
-      <c r="Q167" s="76"/>
+      <c r="M167" s="77"/>
+      <c r="N167" s="77"/>
+      <c r="O167" s="77"/>
+      <c r="P167" s="77"/>
+      <c r="Q167" s="70"/>
       <c r="R167" s="49"/>
       <c r="S167" s="51"/>
       <c r="T167" s="51"/>
@@ -6912,23 +6934,23 @@
       </c>
       <c r="C173" s="32"/>
       <c r="D173" s="20"/>
-      <c r="E173" s="70" t="s">
+      <c r="E173" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="F173" s="70"/>
-      <c r="G173" s="70"/>
-      <c r="H173" s="70"/>
-      <c r="I173" s="70"/>
-      <c r="J173" s="70"/>
+      <c r="F173" s="76"/>
+      <c r="G173" s="76"/>
+      <c r="H173" s="76"/>
+      <c r="I173" s="76"/>
+      <c r="J173" s="76"/>
       <c r="K173" s="49"/>
-      <c r="L173" s="74" t="s">
+      <c r="L173" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="M173" s="75"/>
-      <c r="N173" s="75"/>
-      <c r="O173" s="75"/>
-      <c r="P173" s="75"/>
-      <c r="Q173" s="76"/>
+      <c r="M173" s="77"/>
+      <c r="N173" s="77"/>
+      <c r="O173" s="77"/>
+      <c r="P173" s="77"/>
+      <c r="Q173" s="70"/>
       <c r="R173" s="49"/>
       <c r="S173" s="51"/>
       <c r="T173" s="30" t="s">
@@ -6946,23 +6968,23 @@
       </c>
       <c r="C174" s="32"/>
       <c r="D174" s="20"/>
-      <c r="E174" s="70" t="s">
+      <c r="E174" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="F174" s="70"/>
-      <c r="G174" s="70"/>
-      <c r="H174" s="70"/>
-      <c r="I174" s="70"/>
-      <c r="J174" s="70"/>
+      <c r="F174" s="76"/>
+      <c r="G174" s="76"/>
+      <c r="H174" s="76"/>
+      <c r="I174" s="76"/>
+      <c r="J174" s="76"/>
       <c r="K174" s="49"/>
-      <c r="L174" s="74" t="s">
+      <c r="L174" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="M174" s="75"/>
-      <c r="N174" s="75"/>
-      <c r="O174" s="75"/>
-      <c r="P174" s="75"/>
-      <c r="Q174" s="76"/>
+      <c r="M174" s="77"/>
+      <c r="N174" s="77"/>
+      <c r="O174" s="77"/>
+      <c r="P174" s="77"/>
+      <c r="Q174" s="70"/>
       <c r="R174" s="20"/>
       <c r="S174" s="51"/>
       <c r="T174" s="53" t="s">
@@ -6980,23 +7002,23 @@
       </c>
       <c r="C175" s="32"/>
       <c r="D175" s="20"/>
-      <c r="E175" s="70" t="s">
+      <c r="E175" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="F175" s="70"/>
-      <c r="G175" s="70"/>
-      <c r="H175" s="70"/>
-      <c r="I175" s="70"/>
-      <c r="J175" s="70"/>
+      <c r="F175" s="76"/>
+      <c r="G175" s="76"/>
+      <c r="H175" s="76"/>
+      <c r="I175" s="76"/>
+      <c r="J175" s="76"/>
       <c r="K175" s="20"/>
-      <c r="L175" s="74" t="s">
+      <c r="L175" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="M175" s="75"/>
-      <c r="N175" s="75"/>
-      <c r="O175" s="75"/>
-      <c r="P175" s="75"/>
-      <c r="Q175" s="76"/>
+      <c r="M175" s="77"/>
+      <c r="N175" s="77"/>
+      <c r="O175" s="77"/>
+      <c r="P175" s="77"/>
+      <c r="Q175" s="70"/>
       <c r="R175" s="49"/>
       <c r="S175" s="51"/>
       <c r="T175" s="52" t="s">
@@ -7014,23 +7036,23 @@
       </c>
       <c r="C176" s="49"/>
       <c r="D176" s="49"/>
-      <c r="E176" s="70" t="s">
+      <c r="E176" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="F176" s="70"/>
-      <c r="G176" s="70"/>
-      <c r="H176" s="70"/>
-      <c r="I176" s="70"/>
-      <c r="J176" s="70"/>
+      <c r="F176" s="76"/>
+      <c r="G176" s="76"/>
+      <c r="H176" s="76"/>
+      <c r="I176" s="76"/>
+      <c r="J176" s="76"/>
       <c r="K176" s="20"/>
-      <c r="L176" s="74" t="s">
+      <c r="L176" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="M176" s="75"/>
-      <c r="N176" s="75"/>
-      <c r="O176" s="75"/>
-      <c r="P176" s="75"/>
-      <c r="Q176" s="76"/>
+      <c r="M176" s="77"/>
+      <c r="N176" s="77"/>
+      <c r="O176" s="77"/>
+      <c r="P176" s="77"/>
+      <c r="Q176" s="70"/>
       <c r="R176" s="20"/>
       <c r="S176" s="51"/>
       <c r="T176" s="18" t="s">
@@ -7048,23 +7070,23 @@
       </c>
       <c r="C177" s="32"/>
       <c r="D177" s="20"/>
-      <c r="E177" s="70" t="s">
+      <c r="E177" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="F177" s="70"/>
-      <c r="G177" s="70"/>
-      <c r="H177" s="70"/>
-      <c r="I177" s="70"/>
-      <c r="J177" s="70"/>
+      <c r="F177" s="76"/>
+      <c r="G177" s="76"/>
+      <c r="H177" s="76"/>
+      <c r="I177" s="76"/>
+      <c r="J177" s="76"/>
       <c r="K177" s="20"/>
-      <c r="L177" s="74" t="s">
+      <c r="L177" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="M177" s="75"/>
-      <c r="N177" s="75"/>
-      <c r="O177" s="75"/>
-      <c r="P177" s="75"/>
-      <c r="Q177" s="76"/>
+      <c r="M177" s="77"/>
+      <c r="N177" s="77"/>
+      <c r="O177" s="77"/>
+      <c r="P177" s="77"/>
+      <c r="Q177" s="70"/>
       <c r="R177" s="20"/>
       <c r="S177" s="51"/>
       <c r="T177" s="51"/>
@@ -7223,23 +7245,23 @@
       </c>
       <c r="C183" s="32"/>
       <c r="D183" s="20"/>
-      <c r="E183" s="70" t="s">
+      <c r="E183" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="F183" s="70"/>
-      <c r="G183" s="70"/>
-      <c r="H183" s="70"/>
-      <c r="I183" s="70"/>
-      <c r="J183" s="70"/>
+      <c r="F183" s="76"/>
+      <c r="G183" s="76"/>
+      <c r="H183" s="76"/>
+      <c r="I183" s="76"/>
+      <c r="J183" s="76"/>
       <c r="K183" s="49"/>
-      <c r="L183" s="74" t="s">
+      <c r="L183" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="M183" s="75"/>
-      <c r="N183" s="75"/>
-      <c r="O183" s="75"/>
-      <c r="P183" s="75"/>
-      <c r="Q183" s="76"/>
+      <c r="M183" s="77"/>
+      <c r="N183" s="77"/>
+      <c r="O183" s="77"/>
+      <c r="P183" s="77"/>
+      <c r="Q183" s="70"/>
       <c r="R183" s="49"/>
       <c r="S183" s="51"/>
       <c r="T183" s="30" t="s">
@@ -7256,23 +7278,23 @@
       </c>
       <c r="C184" s="32"/>
       <c r="D184" s="20"/>
-      <c r="E184" s="70" t="s">
+      <c r="E184" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="F184" s="70"/>
-      <c r="G184" s="70"/>
-      <c r="H184" s="70"/>
-      <c r="I184" s="70"/>
-      <c r="J184" s="70"/>
+      <c r="F184" s="76"/>
+      <c r="G184" s="76"/>
+      <c r="H184" s="76"/>
+      <c r="I184" s="76"/>
+      <c r="J184" s="76"/>
       <c r="K184" s="49"/>
-      <c r="L184" s="74" t="s">
+      <c r="L184" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="M184" s="75"/>
-      <c r="N184" s="75"/>
-      <c r="O184" s="75"/>
-      <c r="P184" s="75"/>
-      <c r="Q184" s="76"/>
+      <c r="M184" s="77"/>
+      <c r="N184" s="77"/>
+      <c r="O184" s="77"/>
+      <c r="P184" s="77"/>
+      <c r="Q184" s="70"/>
       <c r="R184" s="20"/>
       <c r="S184" s="51"/>
       <c r="T184" s="53" t="s">
@@ -7289,23 +7311,23 @@
       </c>
       <c r="C185" s="32"/>
       <c r="D185" s="20"/>
-      <c r="E185" s="70" t="s">
+      <c r="E185" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="F185" s="70"/>
-      <c r="G185" s="70"/>
-      <c r="H185" s="70"/>
-      <c r="I185" s="70"/>
-      <c r="J185" s="70"/>
+      <c r="F185" s="76"/>
+      <c r="G185" s="76"/>
+      <c r="H185" s="76"/>
+      <c r="I185" s="76"/>
+      <c r="J185" s="76"/>
       <c r="K185" s="20"/>
-      <c r="L185" s="74" t="s">
+      <c r="L185" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="M185" s="75"/>
-      <c r="N185" s="75"/>
-      <c r="O185" s="75"/>
-      <c r="P185" s="75"/>
-      <c r="Q185" s="76"/>
+      <c r="M185" s="77"/>
+      <c r="N185" s="77"/>
+      <c r="O185" s="77"/>
+      <c r="P185" s="77"/>
+      <c r="Q185" s="70"/>
       <c r="R185" s="49"/>
       <c r="S185" s="51"/>
       <c r="T185" s="52" t="s">
@@ -7322,23 +7344,23 @@
       </c>
       <c r="C186" s="49"/>
       <c r="D186" s="49"/>
-      <c r="E186" s="70" t="s">
+      <c r="E186" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="F186" s="70"/>
-      <c r="G186" s="70"/>
-      <c r="H186" s="70"/>
-      <c r="I186" s="70"/>
-      <c r="J186" s="70"/>
+      <c r="F186" s="76"/>
+      <c r="G186" s="76"/>
+      <c r="H186" s="76"/>
+      <c r="I186" s="76"/>
+      <c r="J186" s="76"/>
       <c r="K186" s="20"/>
-      <c r="L186" s="74" t="s">
+      <c r="L186" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="M186" s="75"/>
-      <c r="N186" s="75"/>
-      <c r="O186" s="75"/>
-      <c r="P186" s="75"/>
-      <c r="Q186" s="76"/>
+      <c r="M186" s="77"/>
+      <c r="N186" s="77"/>
+      <c r="O186" s="77"/>
+      <c r="P186" s="77"/>
+      <c r="Q186" s="70"/>
       <c r="R186" s="20"/>
       <c r="S186" s="51"/>
       <c r="T186" s="18" t="s">
@@ -7355,23 +7377,23 @@
       </c>
       <c r="C187" s="32"/>
       <c r="D187" s="20"/>
-      <c r="E187" s="70" t="s">
+      <c r="E187" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="F187" s="70"/>
-      <c r="G187" s="70"/>
-      <c r="H187" s="70"/>
-      <c r="I187" s="70"/>
-      <c r="J187" s="70"/>
+      <c r="F187" s="76"/>
+      <c r="G187" s="76"/>
+      <c r="H187" s="76"/>
+      <c r="I187" s="76"/>
+      <c r="J187" s="76"/>
       <c r="K187" s="20"/>
-      <c r="L187" s="74" t="s">
+      <c r="L187" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="M187" s="75"/>
-      <c r="N187" s="75"/>
-      <c r="O187" s="75"/>
-      <c r="P187" s="75"/>
-      <c r="Q187" s="76"/>
+      <c r="M187" s="77"/>
+      <c r="N187" s="77"/>
+      <c r="O187" s="77"/>
+      <c r="P187" s="77"/>
+      <c r="Q187" s="70"/>
       <c r="R187" s="20"/>
       <c r="S187" s="51"/>
       <c r="T187" s="51"/>
@@ -15801,7 +15823,128 @@
       <c r="T507"/>
     </row>
   </sheetData>
-  <mergeCells count="140">
+  <mergeCells count="145">
+    <mergeCell ref="J84:R84"/>
+    <mergeCell ref="E85:M85"/>
+    <mergeCell ref="H93:P93"/>
+    <mergeCell ref="H94:P94"/>
+    <mergeCell ref="H96:L96"/>
+    <mergeCell ref="C119:R119"/>
+    <mergeCell ref="C129:R129"/>
+    <mergeCell ref="C139:R139"/>
+    <mergeCell ref="C143:E143"/>
+    <mergeCell ref="K116:Q116"/>
+    <mergeCell ref="E115:J115"/>
+    <mergeCell ref="L115:Q115"/>
+    <mergeCell ref="L67:R67"/>
+    <mergeCell ref="L68:R68"/>
+    <mergeCell ref="M72:R72"/>
+    <mergeCell ref="H72:K72"/>
+    <mergeCell ref="C69:R69"/>
+    <mergeCell ref="C79:R79"/>
+    <mergeCell ref="C89:R89"/>
+    <mergeCell ref="C99:R99"/>
+    <mergeCell ref="C109:R109"/>
+    <mergeCell ref="C134:G134"/>
+    <mergeCell ref="C103:G103"/>
+    <mergeCell ref="C104:G104"/>
+    <mergeCell ref="C114:G114"/>
+    <mergeCell ref="C83:G83"/>
+    <mergeCell ref="C84:G84"/>
+    <mergeCell ref="C86:G86"/>
+    <mergeCell ref="C93:G93"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H46:P46"/>
+    <mergeCell ref="H44:N44"/>
+    <mergeCell ref="H52:J52"/>
+    <mergeCell ref="H62:J62"/>
+    <mergeCell ref="D82:F82"/>
+    <mergeCell ref="C53:G53"/>
+    <mergeCell ref="D72:F72"/>
+    <mergeCell ref="L75:Q75"/>
+    <mergeCell ref="I53:M53"/>
+    <mergeCell ref="C67:J67"/>
+    <mergeCell ref="C46:G46"/>
+    <mergeCell ref="C54:G54"/>
+    <mergeCell ref="C56:G56"/>
+    <mergeCell ref="C63:G63"/>
+    <mergeCell ref="C64:G64"/>
+    <mergeCell ref="I55:N55"/>
+    <mergeCell ref="C68:J68"/>
+    <mergeCell ref="C76:R76"/>
+    <mergeCell ref="E78:J78"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="H13:R13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="J14:N14"/>
+    <mergeCell ref="H45:P45"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C43:G43"/>
+    <mergeCell ref="C44:G44"/>
+    <mergeCell ref="H26:L26"/>
+    <mergeCell ref="H43:P43"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="J24:L24"/>
+    <mergeCell ref="H33:P33"/>
+    <mergeCell ref="D32:G32"/>
+    <mergeCell ref="H16:L16"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="H23:R23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C133:G133"/>
+    <mergeCell ref="H124:I124"/>
+    <mergeCell ref="C113:G113"/>
+    <mergeCell ref="C94:G94"/>
+    <mergeCell ref="C96:G96"/>
+    <mergeCell ref="E75:J75"/>
+    <mergeCell ref="E77:J77"/>
+    <mergeCell ref="H116:J116"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="H83:P83"/>
+    <mergeCell ref="P57:R57"/>
+    <mergeCell ref="E73:J73"/>
+    <mergeCell ref="L73:Q73"/>
+    <mergeCell ref="Q54:R54"/>
+    <mergeCell ref="H54:P54"/>
+    <mergeCell ref="C66:G66"/>
+    <mergeCell ref="L74:Q74"/>
+    <mergeCell ref="L77:Q77"/>
+    <mergeCell ref="L78:Q78"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="J58:P58"/>
+    <mergeCell ref="E74:J74"/>
+    <mergeCell ref="H56:M56"/>
+    <mergeCell ref="D122:F122"/>
+    <mergeCell ref="D142:F142"/>
+    <mergeCell ref="H66:Q66"/>
+    <mergeCell ref="E175:J175"/>
+    <mergeCell ref="L175:Q175"/>
+    <mergeCell ref="L167:Q167"/>
+    <mergeCell ref="C155:R159"/>
+    <mergeCell ref="C163:R165"/>
+    <mergeCell ref="E166:J166"/>
+    <mergeCell ref="L166:Q166"/>
+    <mergeCell ref="E167:J167"/>
+    <mergeCell ref="H84:I84"/>
+    <mergeCell ref="H104:I104"/>
+    <mergeCell ref="D112:F112"/>
+    <mergeCell ref="C136:G136"/>
+    <mergeCell ref="C116:G116"/>
+    <mergeCell ref="C123:G123"/>
+    <mergeCell ref="C124:G124"/>
+    <mergeCell ref="C106:G106"/>
+    <mergeCell ref="L173:Q173"/>
+    <mergeCell ref="E174:J174"/>
+    <mergeCell ref="L174:Q174"/>
+    <mergeCell ref="C126:G126"/>
+    <mergeCell ref="H142:L142"/>
     <mergeCell ref="C74:D74"/>
     <mergeCell ref="I63:L63"/>
     <mergeCell ref="H64:N64"/>
@@ -15826,122 +15969,6 @@
     <mergeCell ref="E183:J183"/>
     <mergeCell ref="L183:Q183"/>
     <mergeCell ref="E173:J173"/>
-    <mergeCell ref="D122:F122"/>
-    <mergeCell ref="D142:F142"/>
-    <mergeCell ref="H66:Q66"/>
-    <mergeCell ref="E175:J175"/>
-    <mergeCell ref="L175:Q175"/>
-    <mergeCell ref="L167:Q167"/>
-    <mergeCell ref="C155:R159"/>
-    <mergeCell ref="C163:R165"/>
-    <mergeCell ref="E166:J166"/>
-    <mergeCell ref="L166:Q166"/>
-    <mergeCell ref="E167:J167"/>
-    <mergeCell ref="H84:I84"/>
-    <mergeCell ref="H104:I104"/>
-    <mergeCell ref="D112:F112"/>
-    <mergeCell ref="C136:G136"/>
-    <mergeCell ref="C116:G116"/>
-    <mergeCell ref="C123:G123"/>
-    <mergeCell ref="C124:G124"/>
-    <mergeCell ref="C106:G106"/>
-    <mergeCell ref="L173:Q173"/>
-    <mergeCell ref="E174:J174"/>
-    <mergeCell ref="L174:Q174"/>
-    <mergeCell ref="C126:G126"/>
-    <mergeCell ref="H142:L142"/>
-    <mergeCell ref="C133:G133"/>
-    <mergeCell ref="H124:I124"/>
-    <mergeCell ref="C113:G113"/>
-    <mergeCell ref="C94:G94"/>
-    <mergeCell ref="C96:G96"/>
-    <mergeCell ref="E75:J75"/>
-    <mergeCell ref="E77:J77"/>
-    <mergeCell ref="H116:J116"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="H83:P83"/>
-    <mergeCell ref="P57:R57"/>
-    <mergeCell ref="E73:J73"/>
-    <mergeCell ref="L73:Q73"/>
-    <mergeCell ref="Q54:R54"/>
-    <mergeCell ref="H54:P54"/>
-    <mergeCell ref="C66:G66"/>
-    <mergeCell ref="L74:Q74"/>
-    <mergeCell ref="L77:Q77"/>
-    <mergeCell ref="L78:Q78"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="E58:G58"/>
-    <mergeCell ref="J58:P58"/>
-    <mergeCell ref="E74:J74"/>
-    <mergeCell ref="H56:M56"/>
-    <mergeCell ref="E78:J78"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="H13:R13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="J14:N14"/>
-    <mergeCell ref="H45:P45"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C43:G43"/>
-    <mergeCell ref="C44:G44"/>
-    <mergeCell ref="H26:L26"/>
-    <mergeCell ref="H43:P43"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="J24:L24"/>
-    <mergeCell ref="H33:P33"/>
-    <mergeCell ref="D32:G32"/>
-    <mergeCell ref="H16:L16"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="H23:R23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H46:P46"/>
-    <mergeCell ref="H44:N44"/>
-    <mergeCell ref="H52:J52"/>
-    <mergeCell ref="H62:J62"/>
-    <mergeCell ref="D82:F82"/>
-    <mergeCell ref="C53:G53"/>
-    <mergeCell ref="D72:F72"/>
-    <mergeCell ref="L75:Q75"/>
-    <mergeCell ref="I53:M53"/>
-    <mergeCell ref="C67:J67"/>
-    <mergeCell ref="C46:G46"/>
-    <mergeCell ref="C54:G54"/>
-    <mergeCell ref="C56:G56"/>
-    <mergeCell ref="C63:G63"/>
-    <mergeCell ref="C64:G64"/>
-    <mergeCell ref="I55:N55"/>
-    <mergeCell ref="C68:J68"/>
-    <mergeCell ref="C76:R76"/>
-    <mergeCell ref="C119:R119"/>
-    <mergeCell ref="C129:R129"/>
-    <mergeCell ref="C139:R139"/>
-    <mergeCell ref="C143:E143"/>
-    <mergeCell ref="K116:Q116"/>
-    <mergeCell ref="E115:J115"/>
-    <mergeCell ref="L115:Q115"/>
-    <mergeCell ref="L67:R67"/>
-    <mergeCell ref="L68:R68"/>
-    <mergeCell ref="M72:R72"/>
-    <mergeCell ref="H72:K72"/>
-    <mergeCell ref="C69:R69"/>
-    <mergeCell ref="C79:R79"/>
-    <mergeCell ref="C89:R89"/>
-    <mergeCell ref="C99:R99"/>
-    <mergeCell ref="C109:R109"/>
-    <mergeCell ref="C134:G134"/>
-    <mergeCell ref="C103:G103"/>
-    <mergeCell ref="C104:G104"/>
-    <mergeCell ref="C114:G114"/>
-    <mergeCell ref="C83:G83"/>
-    <mergeCell ref="C84:G84"/>
-    <mergeCell ref="C86:G86"/>
-    <mergeCell ref="C93:G93"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -15969,10 +15996,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="113" t="s">
+      <c r="A2" s="116" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="113"/>
+      <c r="B2" s="116"/>
       <c r="C2" s="41" t="s">
         <v>18</v>
       </c>
@@ -15991,10 +16018,10 @@
       <c r="I2" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="114" t="s">
+      <c r="J2" s="117" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="114"/>
+      <c r="K2" s="117"/>
     </row>
     <row r="3" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
@@ -16009,10 +16036,10 @@
       <c r="I3" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="J3" s="115" t="s">
+      <c r="J3" s="118" t="s">
         <v>60</v>
       </c>
-      <c r="K3" s="115"/>
+      <c r="K3" s="118"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
@@ -16034,10 +16061,10 @@
       <c r="I4" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="J4" s="115" t="s">
+      <c r="J4" s="118" t="s">
         <v>61</v>
       </c>
-      <c r="K4" s="115"/>
+      <c r="K4" s="118"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
@@ -16312,10 +16339,10 @@
       <c r="H22" s="51"/>
     </row>
     <row r="23" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="113" t="s">
+      <c r="A23" s="116" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="113"/>
+      <c r="B23" s="116"/>
       <c r="C23" s="41" t="s">
         <v>18</v>
       </c>
@@ -16520,7 +16547,7 @@
         <v>43929</v>
       </c>
       <c r="D36" s="29"/>
-      <c r="F36" s="111" t="s">
+      <c r="F36" s="85" t="s">
         <v>49</v>
       </c>
     </row>
@@ -16538,7 +16565,7 @@
         <v>43936</v>
       </c>
       <c r="D37" s="44"/>
-      <c r="F37" s="111"/>
+      <c r="F37" s="85"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="23">
@@ -16554,7 +16581,7 @@
         <v>43943</v>
       </c>
       <c r="D38" s="29"/>
-      <c r="F38" s="111"/>
+      <c r="F38" s="85"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="23">

</xml_diff>

<commit_message>
Added some more images for trhe mock-ups and fixed Use Cases with Payment Sys
</commit_message>
<xml_diff>
--- a/Weekly Planner.xlsx
+++ b/Weekly Planner.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20351"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20352"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\SoftwareProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D990BC-FA64-444A-A232-5EDDABBA4A77}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2DB77DF-A779-43F0-9365-1D17C7B3A277}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="88">
   <si>
     <t>Monday</t>
   </si>
@@ -302,6 +302,9 @@
   <si>
     <t>Software Project - Requirements Specifications</t>
   </si>
+  <si>
+    <t>DAD - Project</t>
+  </si>
 </sst>
 </file>
 
@@ -465,7 +468,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -840,6 +843,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -854,7 +899,7 @@
     <xf numFmtId="0" fontId="11" fillId="10" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1032,10 +1077,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="15" xfId="9" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="16" xfId="9" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
@@ -1044,19 +1095,13 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="8" xfId="8" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="10" xfId="9" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="17" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="19" xfId="9" applyBorder="1" applyAlignment="1">
@@ -1065,70 +1110,64 @@
     <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="20" xfId="9" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="29" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="15" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="17" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="16" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="9" fillId="6" borderId="11" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="6" fillId="8" borderId="11" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="8" xfId="8" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="5" borderId="24" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="20" fontId="6" fillId="8" borderId="4" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="30" xfId="9" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="24" xfId="9" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="31" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="8" xfId="8" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="8" xfId="8" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="8" xfId="8" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="29" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
@@ -1140,37 +1179,43 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="20" fontId="6" fillId="11" borderId="4" xfId="10" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="4" fillId="5" borderId="24" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="29" xfId="9" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="9" fillId="6" borderId="11" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="6" fillId="8" borderId="11" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="29" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="8" xfId="8" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="20" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1182,13 +1227,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="33" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="34" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="31" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="35" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="13" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="14" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1491,8 +1554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y507"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q95" sqref="Q95"/>
+    <sheetView tabSelected="1" topLeftCell="A115" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C107" sqref="C107:M107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1875,26 +1938,26 @@
       <c r="B13" s="57">
         <v>43724</v>
       </c>
-      <c r="C13" s="86" t="s">
+      <c r="C13" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="86"/>
-      <c r="E13" s="86"/>
-      <c r="F13" s="86"/>
-      <c r="G13" s="86"/>
-      <c r="H13" s="90" t="s">
+      <c r="D13" s="76"/>
+      <c r="E13" s="76"/>
+      <c r="F13" s="76"/>
+      <c r="G13" s="76"/>
+      <c r="H13" s="89" t="s">
         <v>39</v>
       </c>
-      <c r="I13" s="98"/>
-      <c r="J13" s="98"/>
-      <c r="K13" s="98"/>
-      <c r="L13" s="98"/>
-      <c r="M13" s="98"/>
-      <c r="N13" s="98"/>
-      <c r="O13" s="98"/>
-      <c r="P13" s="98"/>
-      <c r="Q13" s="98"/>
-      <c r="R13" s="91"/>
+      <c r="I13" s="97"/>
+      <c r="J13" s="97"/>
+      <c r="K13" s="97"/>
+      <c r="L13" s="97"/>
+      <c r="M13" s="97"/>
+      <c r="N13" s="97"/>
+      <c r="O13" s="97"/>
+      <c r="P13" s="97"/>
+      <c r="Q13" s="97"/>
+      <c r="R13" s="98"/>
       <c r="S13" s="51"/>
       <c r="T13" s="30" t="s">
         <v>22</v>
@@ -1907,26 +1970,26 @@
       <c r="B14" s="57">
         <v>43725</v>
       </c>
-      <c r="C14" s="86" t="s">
+      <c r="C14" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="86"/>
-      <c r="E14" s="86"/>
-      <c r="F14" s="86"/>
-      <c r="G14" s="86"/>
+      <c r="D14" s="76"/>
+      <c r="E14" s="76"/>
+      <c r="F14" s="76"/>
+      <c r="G14" s="76"/>
       <c r="H14" s="20"/>
       <c r="I14" s="20"/>
-      <c r="J14" s="99" t="s">
+      <c r="J14" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="K14" s="100"/>
-      <c r="L14" s="100"/>
-      <c r="M14" s="100"/>
-      <c r="N14" s="101"/>
-      <c r="O14" s="90" t="s">
+      <c r="K14" s="99"/>
+      <c r="L14" s="99"/>
+      <c r="M14" s="99"/>
+      <c r="N14" s="88"/>
+      <c r="O14" s="89" t="s">
         <v>38</v>
       </c>
-      <c r="P14" s="91"/>
+      <c r="P14" s="98"/>
       <c r="Q14" s="20"/>
       <c r="R14" s="20"/>
       <c r="S14" s="51"/>
@@ -1969,20 +2032,20 @@
       <c r="B16" s="57">
         <v>43727</v>
       </c>
-      <c r="C16" s="86" t="s">
+      <c r="C16" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="86"/>
-      <c r="E16" s="86"/>
-      <c r="F16" s="86"/>
-      <c r="G16" s="86"/>
-      <c r="H16" s="108" t="s">
+      <c r="D16" s="76"/>
+      <c r="E16" s="76"/>
+      <c r="F16" s="76"/>
+      <c r="G16" s="76"/>
+      <c r="H16" s="104" t="s">
         <v>47</v>
       </c>
-      <c r="I16" s="108"/>
-      <c r="J16" s="108"/>
-      <c r="K16" s="108"/>
-      <c r="L16" s="108"/>
+      <c r="I16" s="104"/>
+      <c r="J16" s="104"/>
+      <c r="K16" s="104"/>
+      <c r="L16" s="104"/>
       <c r="M16" s="20"/>
       <c r="N16" s="20"/>
       <c r="O16" s="20"/>
@@ -2187,26 +2250,26 @@
         <f>B13+7</f>
         <v>43731</v>
       </c>
-      <c r="C23" s="86" t="s">
+      <c r="C23" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="86"/>
-      <c r="E23" s="86"/>
-      <c r="F23" s="86"/>
-      <c r="G23" s="86"/>
-      <c r="H23" s="90" t="s">
+      <c r="D23" s="76"/>
+      <c r="E23" s="76"/>
+      <c r="F23" s="76"/>
+      <c r="G23" s="76"/>
+      <c r="H23" s="89" t="s">
         <v>39</v>
       </c>
-      <c r="I23" s="98"/>
-      <c r="J23" s="98"/>
-      <c r="K23" s="98"/>
-      <c r="L23" s="98"/>
-      <c r="M23" s="98"/>
-      <c r="N23" s="98"/>
-      <c r="O23" s="98"/>
-      <c r="P23" s="98"/>
-      <c r="Q23" s="98"/>
-      <c r="R23" s="91"/>
+      <c r="I23" s="97"/>
+      <c r="J23" s="97"/>
+      <c r="K23" s="97"/>
+      <c r="L23" s="97"/>
+      <c r="M23" s="97"/>
+      <c r="N23" s="97"/>
+      <c r="O23" s="97"/>
+      <c r="P23" s="97"/>
+      <c r="Q23" s="97"/>
+      <c r="R23" s="98"/>
       <c r="S23" s="51"/>
       <c r="T23" s="30" t="s">
         <v>22</v>
@@ -2220,30 +2283,30 @@
         <f t="shared" ref="B24:B29" si="0">B14+7</f>
         <v>43732</v>
       </c>
-      <c r="C24" s="86" t="s">
+      <c r="C24" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="86"/>
-      <c r="E24" s="86"/>
-      <c r="F24" s="86"/>
-      <c r="G24" s="86"/>
-      <c r="H24" s="90" t="s">
+      <c r="D24" s="76"/>
+      <c r="E24" s="76"/>
+      <c r="F24" s="76"/>
+      <c r="G24" s="76"/>
+      <c r="H24" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="I24" s="109"/>
-      <c r="J24" s="71" t="s">
+      <c r="I24" s="90"/>
+      <c r="J24" s="73" t="s">
         <v>48</v>
       </c>
-      <c r="K24" s="72"/>
-      <c r="L24" s="95"/>
-      <c r="M24" s="71" t="s">
+      <c r="K24" s="74"/>
+      <c r="L24" s="75"/>
+      <c r="M24" s="73" t="s">
         <v>56</v>
       </c>
-      <c r="N24" s="95"/>
-      <c r="O24" s="99" t="s">
+      <c r="N24" s="75"/>
+      <c r="O24" s="87" t="s">
         <v>38</v>
       </c>
-      <c r="P24" s="101"/>
+      <c r="P24" s="88"/>
       <c r="Q24" s="20"/>
       <c r="R24" s="20"/>
       <c r="S24" s="51"/>
@@ -2288,20 +2351,20 @@
         <f t="shared" si="0"/>
         <v>43734</v>
       </c>
-      <c r="C26" s="86" t="s">
+      <c r="C26" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="D26" s="86"/>
-      <c r="E26" s="86"/>
-      <c r="F26" s="86"/>
-      <c r="G26" s="86"/>
-      <c r="H26" s="105" t="s">
+      <c r="D26" s="76"/>
+      <c r="E26" s="76"/>
+      <c r="F26" s="76"/>
+      <c r="G26" s="76"/>
+      <c r="H26" s="96" t="s">
         <v>57</v>
       </c>
-      <c r="I26" s="105"/>
-      <c r="J26" s="105"/>
-      <c r="K26" s="105"/>
-      <c r="L26" s="105"/>
+      <c r="I26" s="96"/>
+      <c r="J26" s="96"/>
+      <c r="K26" s="96"/>
+      <c r="L26" s="96"/>
       <c r="M26" s="20"/>
       <c r="N26" s="20"/>
       <c r="O26" s="20"/>
@@ -2483,12 +2546,12 @@
         <f>C22+1</f>
         <v>3</v>
       </c>
-      <c r="D32" s="107" t="s">
+      <c r="D32" s="103" t="s">
         <v>46</v>
       </c>
-      <c r="E32" s="107"/>
-      <c r="F32" s="107"/>
-      <c r="G32" s="107"/>
+      <c r="E32" s="103"/>
+      <c r="F32" s="103"/>
+      <c r="G32" s="103"/>
       <c r="H32" s="15"/>
       <c r="I32" s="15"/>
       <c r="J32" s="15"/>
@@ -2511,24 +2574,24 @@
         <f>B23+7</f>
         <v>43738</v>
       </c>
-      <c r="C33" s="86" t="s">
+      <c r="C33" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="D33" s="86"/>
-      <c r="E33" s="86"/>
-      <c r="F33" s="86"/>
-      <c r="G33" s="86"/>
-      <c r="H33" s="105" t="s">
+      <c r="D33" s="76"/>
+      <c r="E33" s="76"/>
+      <c r="F33" s="76"/>
+      <c r="G33" s="76"/>
+      <c r="H33" s="96" t="s">
         <v>14</v>
       </c>
-      <c r="I33" s="105"/>
-      <c r="J33" s="105"/>
-      <c r="K33" s="105"/>
-      <c r="L33" s="105"/>
-      <c r="M33" s="105"/>
-      <c r="N33" s="105"/>
-      <c r="O33" s="105"/>
-      <c r="P33" s="105"/>
+      <c r="I33" s="96"/>
+      <c r="J33" s="96"/>
+      <c r="K33" s="96"/>
+      <c r="L33" s="96"/>
+      <c r="M33" s="96"/>
+      <c r="N33" s="96"/>
+      <c r="O33" s="96"/>
+      <c r="P33" s="96"/>
       <c r="Q33" s="62"/>
       <c r="R33" s="62"/>
       <c r="S33" s="51"/>
@@ -2544,13 +2607,13 @@
         <f t="shared" ref="B34:B39" si="1">B24+7</f>
         <v>43739</v>
       </c>
-      <c r="C34" s="86" t="s">
+      <c r="C34" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="D34" s="86"/>
-      <c r="E34" s="86"/>
-      <c r="F34" s="86"/>
-      <c r="G34" s="86"/>
+      <c r="D34" s="76"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="76"/>
+      <c r="G34" s="76"/>
       <c r="H34" s="62"/>
       <c r="I34" s="62"/>
       <c r="J34" s="62"/>
@@ -2604,13 +2667,13 @@
         <f t="shared" si="1"/>
         <v>43741</v>
       </c>
-      <c r="C36" s="86" t="s">
+      <c r="C36" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="D36" s="86"/>
-      <c r="E36" s="86"/>
-      <c r="F36" s="86"/>
-      <c r="G36" s="86"/>
+      <c r="D36" s="76"/>
+      <c r="E36" s="76"/>
+      <c r="F36" s="76"/>
+      <c r="G36" s="76"/>
       <c r="H36" s="63"/>
       <c r="I36" s="63"/>
       <c r="J36" s="63"/>
@@ -2823,24 +2886,24 @@
         <f>B33+7</f>
         <v>43745</v>
       </c>
-      <c r="C43" s="86" t="s">
+      <c r="C43" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="D43" s="86"/>
-      <c r="E43" s="86"/>
-      <c r="F43" s="86"/>
-      <c r="G43" s="86"/>
-      <c r="H43" s="106" t="s">
+      <c r="D43" s="76"/>
+      <c r="E43" s="76"/>
+      <c r="F43" s="76"/>
+      <c r="G43" s="76"/>
+      <c r="H43" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="I43" s="106"/>
-      <c r="J43" s="106"/>
-      <c r="K43" s="106"/>
-      <c r="L43" s="106"/>
-      <c r="M43" s="106"/>
-      <c r="N43" s="106"/>
-      <c r="O43" s="106"/>
-      <c r="P43" s="106"/>
+      <c r="I43" s="72"/>
+      <c r="J43" s="72"/>
+      <c r="K43" s="72"/>
+      <c r="L43" s="72"/>
+      <c r="M43" s="72"/>
+      <c r="N43" s="72"/>
+      <c r="O43" s="72"/>
+      <c r="P43" s="72"/>
       <c r="Q43" s="20"/>
       <c r="R43" s="20"/>
       <c r="S43" s="51"/>
@@ -2856,22 +2919,22 @@
         <f t="shared" ref="B44:B49" si="2">B34+7</f>
         <v>43746</v>
       </c>
-      <c r="C44" s="86" t="s">
+      <c r="C44" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="D44" s="86"/>
-      <c r="E44" s="86"/>
-      <c r="F44" s="86"/>
-      <c r="G44" s="86"/>
-      <c r="H44" s="110" t="s">
+      <c r="D44" s="76"/>
+      <c r="E44" s="76"/>
+      <c r="F44" s="76"/>
+      <c r="G44" s="76"/>
+      <c r="H44" s="91" t="s">
         <v>58</v>
       </c>
-      <c r="I44" s="97"/>
-      <c r="J44" s="97"/>
-      <c r="K44" s="97"/>
-      <c r="L44" s="97"/>
-      <c r="M44" s="97"/>
-      <c r="N44" s="97"/>
+      <c r="I44" s="92"/>
+      <c r="J44" s="92"/>
+      <c r="K44" s="92"/>
+      <c r="L44" s="92"/>
+      <c r="M44" s="92"/>
+      <c r="N44" s="92"/>
       <c r="O44" s="49"/>
       <c r="P44" s="49"/>
       <c r="Q44" s="49"/>
@@ -2894,17 +2957,17 @@
       <c r="E45" s="20"/>
       <c r="F45" s="20"/>
       <c r="G45" s="20"/>
-      <c r="H45" s="102" t="s">
+      <c r="H45" s="100" t="s">
         <v>58</v>
       </c>
-      <c r="I45" s="103"/>
-      <c r="J45" s="103"/>
-      <c r="K45" s="103"/>
-      <c r="L45" s="103"/>
-      <c r="M45" s="103"/>
-      <c r="N45" s="103"/>
-      <c r="O45" s="103"/>
-      <c r="P45" s="104"/>
+      <c r="I45" s="101"/>
+      <c r="J45" s="101"/>
+      <c r="K45" s="101"/>
+      <c r="L45" s="101"/>
+      <c r="M45" s="101"/>
+      <c r="N45" s="101"/>
+      <c r="O45" s="101"/>
+      <c r="P45" s="102"/>
       <c r="Q45" s="49"/>
       <c r="R45" s="49"/>
       <c r="S45" s="51"/>
@@ -2920,24 +2983,24 @@
         <f t="shared" si="2"/>
         <v>43748</v>
       </c>
-      <c r="C46" s="86" t="s">
+      <c r="C46" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="D46" s="86"/>
-      <c r="E46" s="86"/>
-      <c r="F46" s="86"/>
-      <c r="G46" s="86"/>
-      <c r="H46" s="88" t="s">
+      <c r="D46" s="76"/>
+      <c r="E46" s="76"/>
+      <c r="F46" s="76"/>
+      <c r="G46" s="76"/>
+      <c r="H46" s="69" t="s">
         <v>62</v>
       </c>
-      <c r="I46" s="74"/>
-      <c r="J46" s="74"/>
-      <c r="K46" s="74"/>
-      <c r="L46" s="74"/>
-      <c r="M46" s="74"/>
-      <c r="N46" s="74"/>
-      <c r="O46" s="74"/>
-      <c r="P46" s="89"/>
+      <c r="I46" s="70"/>
+      <c r="J46" s="70"/>
+      <c r="K46" s="70"/>
+      <c r="L46" s="70"/>
+      <c r="M46" s="70"/>
+      <c r="N46" s="70"/>
+      <c r="O46" s="70"/>
+      <c r="P46" s="71"/>
       <c r="Q46" s="20"/>
       <c r="R46" s="20"/>
       <c r="S46" s="51"/>
@@ -3116,11 +3179,11 @@
         <v>5</v>
       </c>
       <c r="G52" s="15"/>
-      <c r="H52" s="111" t="s">
+      <c r="H52" s="93" t="s">
         <v>67</v>
       </c>
-      <c r="I52" s="111"/>
-      <c r="J52" s="111"/>
+      <c r="I52" s="93"/>
+      <c r="J52" s="93"/>
       <c r="K52" s="19"/>
       <c r="L52" s="19"/>
       <c r="M52" s="19"/>
@@ -3140,23 +3203,23 @@
         <f>B43+7</f>
         <v>43752</v>
       </c>
-      <c r="C53" s="86" t="s">
+      <c r="C53" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="D53" s="86"/>
-      <c r="E53" s="86"/>
-      <c r="F53" s="86"/>
-      <c r="G53" s="86"/>
+      <c r="D53" s="76"/>
+      <c r="E53" s="76"/>
+      <c r="F53" s="76"/>
+      <c r="G53" s="76"/>
       <c r="H53" s="65" t="s">
         <v>68</v>
       </c>
-      <c r="I53" s="71" t="s">
+      <c r="I53" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="J53" s="72"/>
-      <c r="K53" s="72"/>
-      <c r="L53" s="72"/>
-      <c r="M53" s="72"/>
+      <c r="J53" s="74"/>
+      <c r="K53" s="74"/>
+      <c r="L53" s="74"/>
+      <c r="M53" s="74"/>
       <c r="N53" s="49"/>
       <c r="O53" s="49"/>
       <c r="P53" s="49"/>
@@ -3175,28 +3238,28 @@
         <f t="shared" ref="B54:B59" si="3">B44+7</f>
         <v>43753</v>
       </c>
-      <c r="C54" s="86" t="s">
+      <c r="C54" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="D54" s="86"/>
-      <c r="E54" s="86"/>
-      <c r="F54" s="86"/>
-      <c r="G54" s="86"/>
-      <c r="H54" s="92" t="s">
+      <c r="D54" s="76"/>
+      <c r="E54" s="76"/>
+      <c r="F54" s="76"/>
+      <c r="G54" s="76"/>
+      <c r="H54" s="105" t="s">
         <v>63</v>
       </c>
-      <c r="I54" s="93"/>
-      <c r="J54" s="93"/>
-      <c r="K54" s="93"/>
-      <c r="L54" s="93"/>
-      <c r="M54" s="93"/>
-      <c r="N54" s="93"/>
-      <c r="O54" s="93"/>
-      <c r="P54" s="93"/>
-      <c r="Q54" s="90" t="s">
+      <c r="I54" s="106"/>
+      <c r="J54" s="106"/>
+      <c r="K54" s="106"/>
+      <c r="L54" s="106"/>
+      <c r="M54" s="106"/>
+      <c r="N54" s="106"/>
+      <c r="O54" s="106"/>
+      <c r="P54" s="106"/>
+      <c r="Q54" s="89" t="s">
         <v>70</v>
       </c>
-      <c r="R54" s="91"/>
+      <c r="R54" s="98"/>
       <c r="S54" s="51"/>
       <c r="T54" s="53" t="s">
         <v>19</v>
@@ -3214,18 +3277,18 @@
       <c r="D55" s="49"/>
       <c r="E55" s="49"/>
       <c r="F55" s="49"/>
-      <c r="G55" s="86" t="s">
+      <c r="G55" s="76" t="s">
         <v>64</v>
       </c>
-      <c r="H55" s="86"/>
-      <c r="I55" s="112" t="s">
+      <c r="H55" s="76"/>
+      <c r="I55" s="95" t="s">
         <v>14</v>
       </c>
-      <c r="J55" s="72"/>
-      <c r="K55" s="72"/>
-      <c r="L55" s="72"/>
-      <c r="M55" s="72"/>
-      <c r="N55" s="72"/>
+      <c r="J55" s="74"/>
+      <c r="K55" s="74"/>
+      <c r="L55" s="74"/>
+      <c r="M55" s="74"/>
+      <c r="N55" s="74"/>
       <c r="O55" s="49"/>
       <c r="P55" s="49"/>
       <c r="Q55" s="49"/>
@@ -3243,21 +3306,21 @@
         <f t="shared" si="3"/>
         <v>43755</v>
       </c>
-      <c r="C56" s="86" t="s">
+      <c r="C56" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="D56" s="86"/>
-      <c r="E56" s="86"/>
-      <c r="F56" s="86"/>
-      <c r="G56" s="86"/>
-      <c r="H56" s="96" t="s">
+      <c r="D56" s="76"/>
+      <c r="E56" s="76"/>
+      <c r="F56" s="76"/>
+      <c r="G56" s="76"/>
+      <c r="H56" s="112" t="s">
         <v>71</v>
       </c>
-      <c r="I56" s="97"/>
-      <c r="J56" s="97"/>
-      <c r="K56" s="97"/>
-      <c r="L56" s="97"/>
-      <c r="M56" s="97"/>
+      <c r="I56" s="92"/>
+      <c r="J56" s="92"/>
+      <c r="K56" s="92"/>
+      <c r="L56" s="92"/>
+      <c r="M56" s="92"/>
       <c r="N56" s="49"/>
       <c r="O56" s="49"/>
       <c r="P56" s="49"/>
@@ -3289,11 +3352,11 @@
       <c r="M57" s="49"/>
       <c r="N57" s="49"/>
       <c r="O57" s="49"/>
-      <c r="P57" s="88" t="s">
+      <c r="P57" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="Q57" s="74"/>
-      <c r="R57" s="89"/>
+      <c r="Q57" s="70"/>
+      <c r="R57" s="71"/>
       <c r="S57" s="51"/>
       <c r="T57" s="51"/>
     </row>
@@ -3307,31 +3370,31 @@
       </c>
       <c r="C58" s="50"/>
       <c r="D58" s="49"/>
-      <c r="E58" s="73" t="s">
+      <c r="E58" s="110" t="s">
         <v>42</v>
       </c>
-      <c r="F58" s="74"/>
-      <c r="G58" s="94"/>
-      <c r="H58" s="86" t="s">
+      <c r="F58" s="70"/>
+      <c r="G58" s="111"/>
+      <c r="H58" s="76" t="s">
         <v>74</v>
       </c>
-      <c r="I58" s="86"/>
-      <c r="J58" s="71" t="s">
+      <c r="I58" s="76"/>
+      <c r="J58" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="K58" s="72"/>
-      <c r="L58" s="72"/>
-      <c r="M58" s="72"/>
-      <c r="N58" s="72"/>
-      <c r="O58" s="72"/>
-      <c r="P58" s="95"/>
+      <c r="K58" s="74"/>
+      <c r="L58" s="74"/>
+      <c r="M58" s="74"/>
+      <c r="N58" s="74"/>
+      <c r="O58" s="74"/>
+      <c r="P58" s="75"/>
       <c r="Q58" s="20"/>
       <c r="R58" s="20"/>
       <c r="S58" s="51"/>
-      <c r="T58" s="75" t="s">
+      <c r="T58" s="114" t="s">
         <v>72</v>
       </c>
-      <c r="U58" s="75"/>
+      <c r="U58" s="114"/>
     </row>
     <row r="59" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
@@ -3358,8 +3421,8 @@
       <c r="Q59" s="20"/>
       <c r="R59" s="20"/>
       <c r="S59" s="51"/>
-      <c r="T59" s="75"/>
-      <c r="U59" s="75"/>
+      <c r="T59" s="114"/>
+      <c r="U59" s="114"/>
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B60"/>
@@ -3380,8 +3443,8 @@
       <c r="Q60"/>
       <c r="R60"/>
       <c r="S60"/>
-      <c r="T60" s="75"/>
-      <c r="U60" s="75"/>
+      <c r="T60" s="114"/>
+      <c r="U60" s="114"/>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
@@ -3455,11 +3518,11 @@
       <c r="E62" s="15"/>
       <c r="F62" s="15"/>
       <c r="G62" s="15"/>
-      <c r="H62" s="111" t="s">
+      <c r="H62" s="93" t="s">
         <v>73</v>
       </c>
-      <c r="I62" s="111"/>
-      <c r="J62" s="111"/>
+      <c r="I62" s="93"/>
+      <c r="J62" s="93"/>
       <c r="K62" s="19"/>
       <c r="L62" s="19"/>
       <c r="M62" s="19"/>
@@ -3479,22 +3542,22 @@
         <f>B53+7</f>
         <v>43759</v>
       </c>
-      <c r="C63" s="86" t="s">
+      <c r="C63" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="D63" s="86"/>
-      <c r="E63" s="86"/>
-      <c r="F63" s="86"/>
-      <c r="G63" s="86"/>
+      <c r="D63" s="76"/>
+      <c r="E63" s="76"/>
+      <c r="F63" s="76"/>
+      <c r="G63" s="76"/>
       <c r="H63" s="67" t="s">
         <v>68</v>
       </c>
-      <c r="I63" s="71" t="s">
+      <c r="I63" s="73" t="s">
         <v>76</v>
       </c>
-      <c r="J63" s="72"/>
-      <c r="K63" s="72"/>
-      <c r="L63" s="72"/>
+      <c r="J63" s="74"/>
+      <c r="K63" s="74"/>
+      <c r="L63" s="74"/>
       <c r="M63" s="49"/>
       <c r="N63" s="49"/>
       <c r="O63" s="49"/>
@@ -3514,22 +3577,22 @@
         <f t="shared" ref="B64:B69" si="4">B54+7</f>
         <v>43760</v>
       </c>
-      <c r="C64" s="86" t="s">
+      <c r="C64" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="D64" s="86"/>
-      <c r="E64" s="86"/>
-      <c r="F64" s="86"/>
-      <c r="G64" s="86"/>
-      <c r="H64" s="73" t="s">
+      <c r="D64" s="76"/>
+      <c r="E64" s="76"/>
+      <c r="F64" s="76"/>
+      <c r="G64" s="76"/>
+      <c r="H64" s="110" t="s">
         <v>85</v>
       </c>
-      <c r="I64" s="74"/>
-      <c r="J64" s="74"/>
-      <c r="K64" s="74"/>
-      <c r="L64" s="74"/>
-      <c r="M64" s="74"/>
-      <c r="N64" s="74"/>
+      <c r="I64" s="70"/>
+      <c r="J64" s="70"/>
+      <c r="K64" s="70"/>
+      <c r="L64" s="70"/>
+      <c r="M64" s="70"/>
+      <c r="N64" s="70"/>
       <c r="O64" s="49"/>
       <c r="P64" s="49"/>
       <c r="Q64" s="49"/>
@@ -3578,25 +3641,25 @@
         <f t="shared" si="4"/>
         <v>43762</v>
       </c>
-      <c r="C66" s="86" t="s">
+      <c r="C66" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="D66" s="86"/>
-      <c r="E66" s="86"/>
-      <c r="F66" s="86"/>
-      <c r="G66" s="86"/>
-      <c r="H66" s="82" t="s">
+      <c r="D66" s="76"/>
+      <c r="E66" s="76"/>
+      <c r="F66" s="76"/>
+      <c r="G66" s="76"/>
+      <c r="H66" s="122" t="s">
         <v>77</v>
       </c>
-      <c r="I66" s="83"/>
-      <c r="J66" s="83"/>
-      <c r="K66" s="83"/>
-      <c r="L66" s="83"/>
-      <c r="M66" s="83"/>
-      <c r="N66" s="83"/>
-      <c r="O66" s="83"/>
-      <c r="P66" s="83"/>
-      <c r="Q66" s="84"/>
+      <c r="I66" s="123"/>
+      <c r="J66" s="123"/>
+      <c r="K66" s="123"/>
+      <c r="L66" s="123"/>
+      <c r="M66" s="123"/>
+      <c r="N66" s="123"/>
+      <c r="O66" s="123"/>
+      <c r="P66" s="123"/>
+      <c r="Q66" s="124"/>
       <c r="R66" s="20"/>
       <c r="S66" s="51"/>
       <c r="T66" s="18" t="s">
@@ -3611,30 +3674,30 @@
         <f t="shared" si="4"/>
         <v>43763</v>
       </c>
-      <c r="C67" s="69" t="s">
+      <c r="C67" s="73" t="s">
         <v>77</v>
       </c>
-      <c r="D67" s="77"/>
-      <c r="E67" s="77"/>
-      <c r="F67" s="77"/>
-      <c r="G67" s="77"/>
-      <c r="H67" s="77"/>
-      <c r="I67" s="77"/>
-      <c r="J67" s="70"/>
+      <c r="D67" s="74"/>
+      <c r="E67" s="74"/>
+      <c r="F67" s="74"/>
+      <c r="G67" s="74"/>
+      <c r="H67" s="74"/>
+      <c r="I67" s="74"/>
+      <c r="J67" s="75"/>
       <c r="K67" s="49"/>
-      <c r="L67" s="77" t="s">
+      <c r="L67" s="74" t="s">
         <v>42</v>
       </c>
-      <c r="M67" s="77"/>
-      <c r="N67" s="77"/>
-      <c r="O67" s="77"/>
-      <c r="P67" s="77"/>
-      <c r="Q67" s="77"/>
-      <c r="R67" s="70"/>
+      <c r="M67" s="74"/>
+      <c r="N67" s="74"/>
+      <c r="O67" s="74"/>
+      <c r="P67" s="74"/>
+      <c r="Q67" s="74"/>
+      <c r="R67" s="75"/>
       <c r="S67" s="51"/>
       <c r="T67" s="51"/>
     </row>
-    <row r="68" spans="1:25" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:25" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>5</v>
       </c>
@@ -3642,30 +3705,26 @@
         <f t="shared" si="4"/>
         <v>43764</v>
       </c>
-      <c r="C68" s="69" t="s">
-        <v>77</v>
-      </c>
-      <c r="D68" s="77"/>
-      <c r="E68" s="77"/>
-      <c r="F68" s="77"/>
-      <c r="G68" s="77"/>
-      <c r="H68" s="77"/>
-      <c r="I68" s="77"/>
-      <c r="J68" s="70"/>
+      <c r="C68" s="50"/>
+      <c r="D68" s="49"/>
+      <c r="E68" s="49"/>
+      <c r="F68" s="49"/>
+      <c r="G68" s="49"/>
+      <c r="H68" s="49"/>
+      <c r="I68" s="49"/>
+      <c r="J68" s="49"/>
       <c r="K68" s="49"/>
-      <c r="L68" s="77" t="s">
-        <v>42</v>
-      </c>
-      <c r="M68" s="77"/>
-      <c r="N68" s="77"/>
-      <c r="O68" s="77"/>
-      <c r="P68" s="77"/>
-      <c r="Q68" s="77"/>
-      <c r="R68" s="70"/>
+      <c r="L68" s="49"/>
+      <c r="M68" s="49"/>
+      <c r="N68" s="49"/>
+      <c r="O68" s="49"/>
+      <c r="P68" s="49"/>
+      <c r="Q68" s="49"/>
+      <c r="R68" s="49"/>
       <c r="S68" s="51"/>
       <c r="T68" s="51"/>
     </row>
-    <row r="69" spans="1:25" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>6</v>
       </c>
@@ -3673,24 +3732,24 @@
         <f t="shared" si="4"/>
         <v>43765</v>
       </c>
-      <c r="C69" s="86" t="s">
+      <c r="C69" s="76" t="s">
         <v>81</v>
       </c>
-      <c r="D69" s="86"/>
-      <c r="E69" s="86"/>
-      <c r="F69" s="86"/>
-      <c r="G69" s="86"/>
-      <c r="H69" s="86"/>
-      <c r="I69" s="86"/>
-      <c r="J69" s="86"/>
-      <c r="K69" s="86"/>
-      <c r="L69" s="86"/>
-      <c r="M69" s="86"/>
-      <c r="N69" s="86"/>
-      <c r="O69" s="86"/>
-      <c r="P69" s="86"/>
-      <c r="Q69" s="86"/>
-      <c r="R69" s="86"/>
+      <c r="D69" s="76"/>
+      <c r="E69" s="76"/>
+      <c r="F69" s="76"/>
+      <c r="G69" s="76"/>
+      <c r="H69" s="76"/>
+      <c r="I69" s="76"/>
+      <c r="J69" s="76"/>
+      <c r="K69" s="76"/>
+      <c r="L69" s="76"/>
+      <c r="M69" s="76"/>
+      <c r="N69" s="76"/>
+      <c r="O69" s="76"/>
+      <c r="P69" s="76"/>
+      <c r="Q69" s="76"/>
+      <c r="R69" s="76"/>
       <c r="S69" s="51"/>
       <c r="T69" s="51"/>
     </row>
@@ -3783,27 +3842,27 @@
         <f>C62+1</f>
         <v>7</v>
       </c>
-      <c r="D72" s="81" t="s">
+      <c r="D72" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="E72" s="81"/>
-      <c r="F72" s="81"/>
+      <c r="E72" s="94"/>
+      <c r="F72" s="94"/>
       <c r="G72" s="15"/>
-      <c r="H72" s="115" t="s">
+      <c r="H72" s="85" t="s">
         <v>82</v>
       </c>
-      <c r="I72" s="115"/>
-      <c r="J72" s="115"/>
-      <c r="K72" s="115"/>
+      <c r="I72" s="85"/>
+      <c r="J72" s="85"/>
+      <c r="K72" s="85"/>
       <c r="L72" s="19"/>
-      <c r="M72" s="114" t="s">
+      <c r="M72" s="84" t="s">
         <v>75</v>
       </c>
-      <c r="N72" s="114"/>
-      <c r="O72" s="114"/>
-      <c r="P72" s="114"/>
-      <c r="Q72" s="114"/>
-      <c r="R72" s="114"/>
+      <c r="N72" s="84"/>
+      <c r="O72" s="84"/>
+      <c r="P72" s="84"/>
+      <c r="Q72" s="84"/>
+      <c r="R72" s="84"/>
       <c r="S72" s="51"/>
       <c r="T72" s="51"/>
     </row>
@@ -3817,23 +3876,23 @@
       </c>
       <c r="C73" s="32"/>
       <c r="D73" s="20"/>
-      <c r="E73" s="106" t="s">
+      <c r="E73" s="72" t="s">
         <v>66</v>
       </c>
-      <c r="F73" s="106"/>
-      <c r="G73" s="106"/>
-      <c r="H73" s="106"/>
-      <c r="I73" s="106"/>
-      <c r="J73" s="106"/>
+      <c r="F73" s="72"/>
+      <c r="G73" s="72"/>
+      <c r="H73" s="72"/>
+      <c r="I73" s="72"/>
+      <c r="J73" s="72"/>
       <c r="K73" s="49"/>
-      <c r="L73" s="71" t="s">
+      <c r="L73" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="M73" s="72"/>
-      <c r="N73" s="72"/>
-      <c r="O73" s="72"/>
-      <c r="P73" s="72"/>
-      <c r="Q73" s="95"/>
+      <c r="M73" s="74"/>
+      <c r="N73" s="74"/>
+      <c r="O73" s="74"/>
+      <c r="P73" s="74"/>
+      <c r="Q73" s="75"/>
       <c r="R73" s="49"/>
       <c r="S73" s="51"/>
       <c r="T73" s="30" t="s">
@@ -3848,27 +3907,27 @@
         <f t="shared" ref="B74:B79" si="5">B64+7</f>
         <v>43767</v>
       </c>
-      <c r="C74" s="71" t="s">
+      <c r="C74" s="73" t="s">
         <v>78</v>
       </c>
-      <c r="D74" s="95"/>
-      <c r="E74" s="106" t="s">
+      <c r="D74" s="75"/>
+      <c r="E74" s="72" t="s">
         <v>66</v>
       </c>
-      <c r="F74" s="106"/>
-      <c r="G74" s="106"/>
-      <c r="H74" s="106"/>
-      <c r="I74" s="106"/>
-      <c r="J74" s="106"/>
+      <c r="F74" s="72"/>
+      <c r="G74" s="72"/>
+      <c r="H74" s="72"/>
+      <c r="I74" s="72"/>
+      <c r="J74" s="72"/>
       <c r="K74" s="49"/>
-      <c r="L74" s="71" t="s">
+      <c r="L74" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="M74" s="72"/>
-      <c r="N74" s="72"/>
-      <c r="O74" s="72"/>
-      <c r="P74" s="72"/>
-      <c r="Q74" s="95"/>
+      <c r="M74" s="74"/>
+      <c r="N74" s="74"/>
+      <c r="O74" s="74"/>
+      <c r="P74" s="74"/>
+      <c r="Q74" s="75"/>
       <c r="R74" s="20"/>
       <c r="S74" s="51"/>
       <c r="T74" s="53" t="s">
@@ -3885,23 +3944,23 @@
       </c>
       <c r="C75" s="32"/>
       <c r="D75" s="20"/>
-      <c r="E75" s="106" t="s">
+      <c r="E75" s="72" t="s">
         <v>66</v>
       </c>
-      <c r="F75" s="106"/>
-      <c r="G75" s="106"/>
-      <c r="H75" s="106"/>
-      <c r="I75" s="106"/>
-      <c r="J75" s="106"/>
+      <c r="F75" s="72"/>
+      <c r="G75" s="72"/>
+      <c r="H75" s="72"/>
+      <c r="I75" s="72"/>
+      <c r="J75" s="72"/>
       <c r="K75" s="49"/>
-      <c r="L75" s="71" t="s">
+      <c r="L75" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="M75" s="72"/>
-      <c r="N75" s="72"/>
-      <c r="O75" s="72"/>
-      <c r="P75" s="72"/>
-      <c r="Q75" s="95"/>
+      <c r="M75" s="74"/>
+      <c r="N75" s="74"/>
+      <c r="O75" s="74"/>
+      <c r="P75" s="74"/>
+      <c r="Q75" s="75"/>
       <c r="R75" s="49"/>
       <c r="S75" s="51"/>
       <c r="T75" s="52" t="s">
@@ -3916,24 +3975,24 @@
         <f t="shared" si="5"/>
         <v>43769</v>
       </c>
-      <c r="C76" s="86" t="s">
+      <c r="C76" s="76" t="s">
         <v>79</v>
       </c>
-      <c r="D76" s="86"/>
-      <c r="E76" s="86"/>
-      <c r="F76" s="86"/>
-      <c r="G76" s="86"/>
-      <c r="H76" s="86"/>
-      <c r="I76" s="86"/>
-      <c r="J76" s="86"/>
-      <c r="K76" s="86"/>
-      <c r="L76" s="86"/>
-      <c r="M76" s="86"/>
-      <c r="N76" s="86"/>
-      <c r="O76" s="86"/>
-      <c r="P76" s="86"/>
-      <c r="Q76" s="86"/>
-      <c r="R76" s="86"/>
+      <c r="D76" s="76"/>
+      <c r="E76" s="76"/>
+      <c r="F76" s="76"/>
+      <c r="G76" s="76"/>
+      <c r="H76" s="76"/>
+      <c r="I76" s="76"/>
+      <c r="J76" s="76"/>
+      <c r="K76" s="76"/>
+      <c r="L76" s="76"/>
+      <c r="M76" s="76"/>
+      <c r="N76" s="76"/>
+      <c r="O76" s="76"/>
+      <c r="P76" s="76"/>
+      <c r="Q76" s="76"/>
+      <c r="R76" s="76"/>
       <c r="S76" s="51"/>
       <c r="T76" s="18" t="s">
         <v>21</v>
@@ -3949,23 +4008,23 @@
       </c>
       <c r="C77" s="32"/>
       <c r="D77" s="20"/>
-      <c r="E77" s="105" t="s">
+      <c r="E77" s="96" t="s">
         <v>66</v>
       </c>
-      <c r="F77" s="105"/>
-      <c r="G77" s="105"/>
-      <c r="H77" s="105"/>
-      <c r="I77" s="105"/>
-      <c r="J77" s="105"/>
+      <c r="F77" s="96"/>
+      <c r="G77" s="96"/>
+      <c r="H77" s="96"/>
+      <c r="I77" s="96"/>
+      <c r="J77" s="96"/>
       <c r="K77" s="49"/>
-      <c r="L77" s="119" t="s">
+      <c r="L77" s="107" t="s">
         <v>66</v>
       </c>
-      <c r="M77" s="120"/>
-      <c r="N77" s="120"/>
-      <c r="O77" s="120"/>
-      <c r="P77" s="120"/>
-      <c r="Q77" s="121"/>
+      <c r="M77" s="108"/>
+      <c r="N77" s="108"/>
+      <c r="O77" s="108"/>
+      <c r="P77" s="108"/>
+      <c r="Q77" s="109"/>
       <c r="R77" s="20"/>
       <c r="S77" s="51"/>
       <c r="T77" s="51"/>
@@ -3980,23 +4039,23 @@
       </c>
       <c r="C78" s="50"/>
       <c r="D78" s="49"/>
-      <c r="E78" s="105" t="s">
+      <c r="E78" s="96" t="s">
         <v>66</v>
       </c>
-      <c r="F78" s="105"/>
-      <c r="G78" s="105"/>
-      <c r="H78" s="105"/>
-      <c r="I78" s="105"/>
-      <c r="J78" s="105"/>
+      <c r="F78" s="96"/>
+      <c r="G78" s="96"/>
+      <c r="H78" s="96"/>
+      <c r="I78" s="96"/>
+      <c r="J78" s="96"/>
       <c r="K78" s="49"/>
-      <c r="L78" s="119" t="s">
+      <c r="L78" s="107" t="s">
         <v>66</v>
       </c>
-      <c r="M78" s="120"/>
-      <c r="N78" s="120"/>
-      <c r="O78" s="120"/>
-      <c r="P78" s="120"/>
-      <c r="Q78" s="121"/>
+      <c r="M78" s="108"/>
+      <c r="N78" s="108"/>
+      <c r="O78" s="108"/>
+      <c r="P78" s="108"/>
+      <c r="Q78" s="109"/>
       <c r="R78" s="49"/>
       <c r="S78" s="51"/>
       <c r="T78" s="51"/>
@@ -4009,24 +4068,24 @@
         <f t="shared" si="5"/>
         <v>43772</v>
       </c>
-      <c r="C79" s="86" t="s">
+      <c r="C79" s="76" t="s">
         <v>81</v>
       </c>
-      <c r="D79" s="86"/>
-      <c r="E79" s="86"/>
-      <c r="F79" s="86"/>
-      <c r="G79" s="86"/>
-      <c r="H79" s="86"/>
-      <c r="I79" s="86"/>
-      <c r="J79" s="86"/>
-      <c r="K79" s="86"/>
-      <c r="L79" s="86"/>
-      <c r="M79" s="86"/>
-      <c r="N79" s="86"/>
-      <c r="O79" s="86"/>
-      <c r="P79" s="86"/>
-      <c r="Q79" s="86"/>
-      <c r="R79" s="86"/>
+      <c r="D79" s="76"/>
+      <c r="E79" s="76"/>
+      <c r="F79" s="76"/>
+      <c r="G79" s="76"/>
+      <c r="H79" s="76"/>
+      <c r="I79" s="76"/>
+      <c r="J79" s="76"/>
+      <c r="K79" s="76"/>
+      <c r="L79" s="76"/>
+      <c r="M79" s="76"/>
+      <c r="N79" s="76"/>
+      <c r="O79" s="76"/>
+      <c r="P79" s="76"/>
+      <c r="Q79" s="76"/>
+      <c r="R79" s="76"/>
       <c r="S79" s="51"/>
       <c r="T79" s="51"/>
     </row>
@@ -4100,11 +4159,11 @@
         <f>C72+1</f>
         <v>8</v>
       </c>
-      <c r="D82" s="81" t="s">
+      <c r="D82" s="94" t="s">
         <v>40</v>
       </c>
-      <c r="E82" s="81"/>
-      <c r="F82" s="81"/>
+      <c r="E82" s="94"/>
+      <c r="F82" s="94"/>
       <c r="G82" s="15"/>
       <c r="H82" s="19"/>
       <c r="I82" s="19"/>
@@ -4129,24 +4188,24 @@
         <f>B73+7</f>
         <v>43773</v>
       </c>
-      <c r="C83" s="86" t="s">
+      <c r="C83" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="D83" s="86"/>
-      <c r="E83" s="86"/>
-      <c r="F83" s="86"/>
-      <c r="G83" s="86"/>
-      <c r="H83" s="88" t="s">
+      <c r="D83" s="76"/>
+      <c r="E83" s="76"/>
+      <c r="F83" s="76"/>
+      <c r="G83" s="76"/>
+      <c r="H83" s="69" t="s">
         <v>66</v>
       </c>
-      <c r="I83" s="74"/>
-      <c r="J83" s="74"/>
-      <c r="K83" s="74"/>
-      <c r="L83" s="74"/>
-      <c r="M83" s="74"/>
-      <c r="N83" s="74"/>
-      <c r="O83" s="74"/>
-      <c r="P83" s="89"/>
+      <c r="I83" s="70"/>
+      <c r="J83" s="70"/>
+      <c r="K83" s="70"/>
+      <c r="L83" s="70"/>
+      <c r="M83" s="70"/>
+      <c r="N83" s="70"/>
+      <c r="O83" s="70"/>
+      <c r="P83" s="71"/>
       <c r="Q83" s="20"/>
       <c r="R83" s="20"/>
       <c r="S83" s="51"/>
@@ -4163,28 +4222,28 @@
         <f t="shared" ref="B84:B89" si="6">B74+7</f>
         <v>43774</v>
       </c>
-      <c r="C84" s="86" t="s">
+      <c r="C84" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="D84" s="86"/>
-      <c r="E84" s="86"/>
-      <c r="F84" s="86"/>
-      <c r="G84" s="86"/>
-      <c r="H84" s="86" t="s">
+      <c r="D84" s="76"/>
+      <c r="E84" s="76"/>
+      <c r="F84" s="76"/>
+      <c r="G84" s="76"/>
+      <c r="H84" s="76" t="s">
         <v>44</v>
       </c>
-      <c r="I84" s="86"/>
-      <c r="J84" s="88" t="s">
+      <c r="I84" s="76"/>
+      <c r="J84" s="69" t="s">
         <v>66</v>
       </c>
-      <c r="K84" s="74"/>
-      <c r="L84" s="74"/>
-      <c r="M84" s="74"/>
-      <c r="N84" s="74"/>
-      <c r="O84" s="74"/>
-      <c r="P84" s="74"/>
-      <c r="Q84" s="74"/>
-      <c r="R84" s="89"/>
+      <c r="K84" s="70"/>
+      <c r="L84" s="70"/>
+      <c r="M84" s="70"/>
+      <c r="N84" s="70"/>
+      <c r="O84" s="70"/>
+      <c r="P84" s="70"/>
+      <c r="Q84" s="70"/>
+      <c r="R84" s="71"/>
       <c r="S84" s="51"/>
       <c r="T84" s="53" t="s">
         <v>19</v>
@@ -4201,17 +4260,17 @@
       </c>
       <c r="C85" s="32"/>
       <c r="D85" s="20"/>
-      <c r="E85" s="88" t="s">
+      <c r="E85" s="69" t="s">
         <v>66</v>
       </c>
-      <c r="F85" s="74"/>
-      <c r="G85" s="74"/>
-      <c r="H85" s="74"/>
-      <c r="I85" s="74"/>
-      <c r="J85" s="74"/>
-      <c r="K85" s="74"/>
-      <c r="L85" s="74"/>
-      <c r="M85" s="89"/>
+      <c r="F85" s="70"/>
+      <c r="G85" s="70"/>
+      <c r="H85" s="70"/>
+      <c r="I85" s="70"/>
+      <c r="J85" s="70"/>
+      <c r="K85" s="70"/>
+      <c r="L85" s="70"/>
+      <c r="M85" s="71"/>
       <c r="N85" s="49"/>
       <c r="O85" s="49"/>
       <c r="P85" s="49"/>
@@ -4231,13 +4290,13 @@
         <f t="shared" si="6"/>
         <v>43776</v>
       </c>
-      <c r="C86" s="87" t="s">
+      <c r="C86" s="86" t="s">
         <v>69</v>
       </c>
-      <c r="D86" s="87"/>
-      <c r="E86" s="87"/>
-      <c r="F86" s="87"/>
-      <c r="G86" s="87"/>
+      <c r="D86" s="86"/>
+      <c r="E86" s="86"/>
+      <c r="F86" s="86"/>
+      <c r="G86" s="86"/>
       <c r="H86" s="49"/>
       <c r="I86" s="49"/>
       <c r="J86" s="49"/>
@@ -4319,24 +4378,24 @@
         <f t="shared" si="6"/>
         <v>43779</v>
       </c>
-      <c r="C89" s="86" t="s">
+      <c r="C89" s="76" t="s">
         <v>81</v>
       </c>
-      <c r="D89" s="86"/>
-      <c r="E89" s="86"/>
-      <c r="F89" s="86"/>
-      <c r="G89" s="86"/>
-      <c r="H89" s="86"/>
-      <c r="I89" s="86"/>
-      <c r="J89" s="86"/>
-      <c r="K89" s="86"/>
-      <c r="L89" s="86"/>
-      <c r="M89" s="86"/>
-      <c r="N89" s="86"/>
-      <c r="O89" s="86"/>
-      <c r="P89" s="86"/>
-      <c r="Q89" s="86"/>
-      <c r="R89" s="86"/>
+      <c r="D89" s="76"/>
+      <c r="E89" s="76"/>
+      <c r="F89" s="76"/>
+      <c r="G89" s="76"/>
+      <c r="H89" s="76"/>
+      <c r="I89" s="76"/>
+      <c r="J89" s="76"/>
+      <c r="K89" s="76"/>
+      <c r="L89" s="76"/>
+      <c r="M89" s="76"/>
+      <c r="N89" s="76"/>
+      <c r="O89" s="76"/>
+      <c r="P89" s="76"/>
+      <c r="Q89" s="76"/>
+      <c r="R89" s="76"/>
       <c r="S89" s="51"/>
       <c r="T89" s="51"/>
       <c r="U89" s="54"/>
@@ -4438,24 +4497,24 @@
         <f>B83+7</f>
         <v>43780</v>
       </c>
-      <c r="C93" s="86" t="s">
+      <c r="C93" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="D93" s="86"/>
-      <c r="E93" s="86"/>
-      <c r="F93" s="86"/>
-      <c r="G93" s="86"/>
-      <c r="H93" s="106" t="s">
+      <c r="D93" s="76"/>
+      <c r="E93" s="76"/>
+      <c r="F93" s="76"/>
+      <c r="G93" s="76"/>
+      <c r="H93" s="72" t="s">
         <v>86</v>
       </c>
-      <c r="I93" s="106"/>
-      <c r="J93" s="106"/>
-      <c r="K93" s="106"/>
-      <c r="L93" s="106"/>
-      <c r="M93" s="106"/>
-      <c r="N93" s="106"/>
-      <c r="O93" s="106"/>
-      <c r="P93" s="106"/>
+      <c r="I93" s="72"/>
+      <c r="J93" s="72"/>
+      <c r="K93" s="72"/>
+      <c r="L93" s="72"/>
+      <c r="M93" s="72"/>
+      <c r="N93" s="72"/>
+      <c r="O93" s="72"/>
+      <c r="P93" s="72"/>
       <c r="Q93" s="20"/>
       <c r="R93" s="20"/>
       <c r="S93" s="51"/>
@@ -4472,24 +4531,24 @@
         <f t="shared" ref="B94:B99" si="7">B84+7</f>
         <v>43781</v>
       </c>
-      <c r="C94" s="86" t="s">
+      <c r="C94" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="D94" s="86"/>
-      <c r="E94" s="86"/>
-      <c r="F94" s="86"/>
-      <c r="G94" s="86"/>
-      <c r="H94" s="106" t="s">
+      <c r="D94" s="76"/>
+      <c r="E94" s="76"/>
+      <c r="F94" s="76"/>
+      <c r="G94" s="76"/>
+      <c r="H94" s="72" t="s">
         <v>86</v>
       </c>
-      <c r="I94" s="106"/>
-      <c r="J94" s="106"/>
-      <c r="K94" s="106"/>
-      <c r="L94" s="106"/>
-      <c r="M94" s="106"/>
-      <c r="N94" s="106"/>
-      <c r="O94" s="106"/>
-      <c r="P94" s="106"/>
+      <c r="I94" s="72"/>
+      <c r="J94" s="72"/>
+      <c r="K94" s="72"/>
+      <c r="L94" s="72"/>
+      <c r="M94" s="72"/>
+      <c r="N94" s="72"/>
+      <c r="O94" s="72"/>
+      <c r="P94" s="72"/>
       <c r="Q94" s="20"/>
       <c r="R94" s="20"/>
       <c r="S94" s="51"/>
@@ -4536,20 +4595,20 @@
         <f t="shared" si="7"/>
         <v>43783</v>
       </c>
-      <c r="C96" s="86" t="s">
+      <c r="C96" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="D96" s="86"/>
-      <c r="E96" s="86"/>
-      <c r="F96" s="86"/>
-      <c r="G96" s="86"/>
-      <c r="H96" s="71" t="s">
+      <c r="D96" s="76"/>
+      <c r="E96" s="76"/>
+      <c r="F96" s="76"/>
+      <c r="G96" s="76"/>
+      <c r="H96" s="73" t="s">
         <v>86</v>
       </c>
-      <c r="I96" s="72"/>
-      <c r="J96" s="72"/>
-      <c r="K96" s="72"/>
-      <c r="L96" s="95"/>
+      <c r="I96" s="74"/>
+      <c r="J96" s="74"/>
+      <c r="K96" s="74"/>
+      <c r="L96" s="75"/>
       <c r="M96" s="20"/>
       <c r="N96" s="20"/>
       <c r="O96" s="20"/>
@@ -4626,24 +4685,24 @@
         <f t="shared" si="7"/>
         <v>43786</v>
       </c>
-      <c r="C99" s="86" t="s">
+      <c r="C99" s="76" t="s">
         <v>81</v>
       </c>
-      <c r="D99" s="86"/>
-      <c r="E99" s="86"/>
-      <c r="F99" s="86"/>
-      <c r="G99" s="86"/>
-      <c r="H99" s="86"/>
-      <c r="I99" s="86"/>
-      <c r="J99" s="86"/>
-      <c r="K99" s="86"/>
-      <c r="L99" s="86"/>
-      <c r="M99" s="86"/>
-      <c r="N99" s="86"/>
-      <c r="O99" s="86"/>
-      <c r="P99" s="86"/>
-      <c r="Q99" s="86"/>
-      <c r="R99" s="86"/>
+      <c r="D99" s="76"/>
+      <c r="E99" s="76"/>
+      <c r="F99" s="76"/>
+      <c r="G99" s="76"/>
+      <c r="H99" s="76"/>
+      <c r="I99" s="76"/>
+      <c r="J99" s="76"/>
+      <c r="K99" s="76"/>
+      <c r="L99" s="76"/>
+      <c r="M99" s="76"/>
+      <c r="N99" s="76"/>
+      <c r="O99" s="76"/>
+      <c r="P99" s="76"/>
+      <c r="Q99" s="76"/>
+      <c r="R99" s="76"/>
       <c r="S99" s="51"/>
       <c r="T99" s="51"/>
       <c r="U99" s="54"/>
@@ -4706,7 +4765,7 @@
       <c r="T101" s="51"/>
       <c r="U101" s="54"/>
     </row>
-    <row r="102" spans="1:21" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:21" s="27" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="57">
         <f>A92+7</f>
         <v>43787</v>
@@ -4737,7 +4796,7 @@
       <c r="T102" s="51"/>
       <c r="U102" s="54"/>
     </row>
-    <row r="103" spans="1:21" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:21" s="27" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="s">
         <v>0</v>
       </c>
@@ -4745,22 +4804,24 @@
         <f>B93+7</f>
         <v>43787</v>
       </c>
-      <c r="C103" s="86" t="s">
+      <c r="C103" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="D103" s="86"/>
-      <c r="E103" s="86"/>
-      <c r="F103" s="86"/>
-      <c r="G103" s="86"/>
-      <c r="H103" s="49"/>
-      <c r="I103" s="49"/>
-      <c r="J103" s="49"/>
-      <c r="K103" s="20"/>
-      <c r="L103" s="20"/>
-      <c r="M103" s="20"/>
-      <c r="N103" s="20"/>
-      <c r="O103" s="20"/>
-      <c r="P103" s="20"/>
+      <c r="D103" s="76"/>
+      <c r="E103" s="76"/>
+      <c r="F103" s="76"/>
+      <c r="G103" s="76"/>
+      <c r="H103" s="72" t="s">
+        <v>86</v>
+      </c>
+      <c r="I103" s="72"/>
+      <c r="J103" s="72"/>
+      <c r="K103" s="72"/>
+      <c r="L103" s="72"/>
+      <c r="M103" s="72"/>
+      <c r="N103" s="72"/>
+      <c r="O103" s="72"/>
+      <c r="P103" s="72"/>
       <c r="Q103" s="20"/>
       <c r="R103" s="20"/>
       <c r="S103" s="51"/>
@@ -4769,7 +4830,7 @@
       </c>
       <c r="U103" s="54"/>
     </row>
-    <row r="104" spans="1:21" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:21" s="27" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
         <v>1</v>
       </c>
@@ -4777,24 +4838,24 @@
         <f t="shared" ref="B104:B109" si="8">B94+7</f>
         <v>43788</v>
       </c>
-      <c r="C104" s="86" t="s">
+      <c r="C104" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="D104" s="86"/>
-      <c r="E104" s="86"/>
-      <c r="F104" s="86"/>
-      <c r="G104" s="86"/>
-      <c r="H104" s="86" t="s">
-        <v>44</v>
-      </c>
-      <c r="I104" s="86"/>
-      <c r="J104" s="20"/>
-      <c r="K104" s="49"/>
-      <c r="L104" s="49"/>
-      <c r="M104" s="20"/>
-      <c r="N104" s="20"/>
-      <c r="O104" s="49"/>
-      <c r="P104" s="49"/>
+      <c r="D104" s="76"/>
+      <c r="E104" s="76"/>
+      <c r="F104" s="76"/>
+      <c r="G104" s="76"/>
+      <c r="H104" s="72" t="s">
+        <v>86</v>
+      </c>
+      <c r="I104" s="72"/>
+      <c r="J104" s="72"/>
+      <c r="K104" s="72"/>
+      <c r="L104" s="72"/>
+      <c r="M104" s="72"/>
+      <c r="N104" s="72"/>
+      <c r="O104" s="72"/>
+      <c r="P104" s="72"/>
       <c r="Q104" s="20"/>
       <c r="R104" s="20"/>
       <c r="S104" s="51"/>
@@ -4803,7 +4864,7 @@
       </c>
       <c r="U104" s="54"/>
     </row>
-    <row r="105" spans="1:21" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:21" s="27" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
         <v>2</v>
       </c>
@@ -4811,17 +4872,19 @@
         <f t="shared" si="8"/>
         <v>43789</v>
       </c>
-      <c r="C105" s="32"/>
-      <c r="D105" s="20"/>
-      <c r="E105" s="20"/>
-      <c r="F105" s="20"/>
-      <c r="G105" s="20"/>
-      <c r="H105" s="20"/>
-      <c r="I105" s="20"/>
-      <c r="J105" s="20"/>
-      <c r="K105" s="49"/>
-      <c r="L105" s="49"/>
-      <c r="M105" s="49"/>
+      <c r="C105" s="119" t="s">
+        <v>86</v>
+      </c>
+      <c r="D105" s="120"/>
+      <c r="E105" s="120"/>
+      <c r="F105" s="120"/>
+      <c r="G105" s="120"/>
+      <c r="H105" s="120"/>
+      <c r="I105" s="120"/>
+      <c r="J105" s="120"/>
+      <c r="K105" s="120"/>
+      <c r="L105" s="120"/>
+      <c r="M105" s="121"/>
       <c r="N105" s="49"/>
       <c r="O105" s="49"/>
       <c r="P105" s="49"/>
@@ -4841,22 +4904,24 @@
         <f t="shared" si="8"/>
         <v>43790</v>
       </c>
-      <c r="C106" s="86" t="s">
+      <c r="C106" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="D106" s="86"/>
-      <c r="E106" s="86"/>
-      <c r="F106" s="86"/>
-      <c r="G106" s="86"/>
-      <c r="H106" s="49"/>
-      <c r="I106" s="49"/>
-      <c r="J106" s="49"/>
-      <c r="K106" s="49"/>
-      <c r="L106" s="49"/>
-      <c r="M106" s="20"/>
-      <c r="N106" s="20"/>
-      <c r="O106" s="20"/>
-      <c r="P106" s="20"/>
+      <c r="D106" s="76"/>
+      <c r="E106" s="76"/>
+      <c r="F106" s="76"/>
+      <c r="G106" s="76"/>
+      <c r="H106" s="78" t="s">
+        <v>87</v>
+      </c>
+      <c r="I106" s="79"/>
+      <c r="J106" s="79"/>
+      <c r="K106" s="79"/>
+      <c r="L106" s="79"/>
+      <c r="M106" s="79"/>
+      <c r="N106" s="79"/>
+      <c r="O106" s="79"/>
+      <c r="P106" s="115"/>
       <c r="Q106" s="20"/>
       <c r="R106" s="20"/>
       <c r="S106" s="51"/>
@@ -4873,17 +4938,19 @@
         <f t="shared" si="8"/>
         <v>43791</v>
       </c>
-      <c r="C107" s="32"/>
-      <c r="D107" s="20"/>
-      <c r="E107" s="20"/>
-      <c r="F107" s="20"/>
-      <c r="G107" s="20"/>
-      <c r="H107" s="20"/>
-      <c r="I107" s="49"/>
-      <c r="J107" s="49"/>
-      <c r="K107" s="49"/>
-      <c r="L107" s="49"/>
-      <c r="M107" s="20"/>
+      <c r="C107" s="125" t="s">
+        <v>87</v>
+      </c>
+      <c r="D107" s="126"/>
+      <c r="E107" s="126"/>
+      <c r="F107" s="126"/>
+      <c r="G107" s="126"/>
+      <c r="H107" s="126"/>
+      <c r="I107" s="126"/>
+      <c r="J107" s="126"/>
+      <c r="K107" s="126"/>
+      <c r="L107" s="126"/>
+      <c r="M107" s="127"/>
       <c r="N107" s="20"/>
       <c r="O107" s="20"/>
       <c r="P107" s="20"/>
@@ -4929,24 +4996,24 @@
         <f t="shared" si="8"/>
         <v>43793</v>
       </c>
-      <c r="C109" s="86" t="s">
+      <c r="C109" s="76" t="s">
         <v>81</v>
       </c>
-      <c r="D109" s="86"/>
-      <c r="E109" s="86"/>
-      <c r="F109" s="86"/>
-      <c r="G109" s="86"/>
-      <c r="H109" s="86"/>
-      <c r="I109" s="86"/>
-      <c r="J109" s="86"/>
-      <c r="K109" s="86"/>
-      <c r="L109" s="86"/>
-      <c r="M109" s="86"/>
-      <c r="N109" s="86"/>
-      <c r="O109" s="86"/>
-      <c r="P109" s="86"/>
-      <c r="Q109" s="86"/>
-      <c r="R109" s="86"/>
+      <c r="D109" s="76"/>
+      <c r="E109" s="76"/>
+      <c r="F109" s="76"/>
+      <c r="G109" s="76"/>
+      <c r="H109" s="76"/>
+      <c r="I109" s="76"/>
+      <c r="J109" s="76"/>
+      <c r="K109" s="76"/>
+      <c r="L109" s="76"/>
+      <c r="M109" s="76"/>
+      <c r="N109" s="76"/>
+      <c r="O109" s="76"/>
+      <c r="P109" s="76"/>
+      <c r="Q109" s="76"/>
+      <c r="R109" s="76"/>
       <c r="S109" s="51"/>
       <c r="T109" s="51"/>
       <c r="U109" s="54"/>
@@ -5021,11 +5088,11 @@
         <f>C102+1</f>
         <v>11</v>
       </c>
-      <c r="D112" s="81" t="s">
+      <c r="D112" s="94" t="s">
         <v>43</v>
       </c>
-      <c r="E112" s="81"/>
-      <c r="F112" s="81"/>
+      <c r="E112" s="94"/>
+      <c r="F112" s="94"/>
       <c r="G112" s="15"/>
       <c r="H112" s="15"/>
       <c r="I112" s="15"/>
@@ -5050,13 +5117,13 @@
         <f>B103+7</f>
         <v>43794</v>
       </c>
-      <c r="C113" s="86" t="s">
+      <c r="C113" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="D113" s="86"/>
-      <c r="E113" s="86"/>
-      <c r="F113" s="86"/>
-      <c r="G113" s="86"/>
+      <c r="D113" s="76"/>
+      <c r="E113" s="76"/>
+      <c r="F113" s="76"/>
+      <c r="G113" s="76"/>
       <c r="H113" s="49"/>
       <c r="I113" s="49"/>
       <c r="J113" s="49"/>
@@ -5082,13 +5149,13 @@
         <f t="shared" ref="B114:B119" si="9">B104+7</f>
         <v>43795</v>
       </c>
-      <c r="C114" s="86" t="s">
+      <c r="C114" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="D114" s="86"/>
-      <c r="E114" s="86"/>
-      <c r="F114" s="86"/>
-      <c r="G114" s="86"/>
+      <c r="D114" s="76"/>
+      <c r="E114" s="76"/>
+      <c r="F114" s="76"/>
+      <c r="G114" s="76"/>
       <c r="H114" s="20"/>
       <c r="I114" s="20"/>
       <c r="J114" s="20"/>
@@ -5116,23 +5183,23 @@
       </c>
       <c r="C115" s="32"/>
       <c r="D115" s="20"/>
-      <c r="E115" s="76" t="s">
+      <c r="E115" s="77" t="s">
         <v>65</v>
       </c>
-      <c r="F115" s="76"/>
-      <c r="G115" s="76"/>
-      <c r="H115" s="76"/>
-      <c r="I115" s="76"/>
-      <c r="J115" s="76"/>
+      <c r="F115" s="77"/>
+      <c r="G115" s="77"/>
+      <c r="H115" s="77"/>
+      <c r="I115" s="77"/>
+      <c r="J115" s="77"/>
       <c r="K115" s="49"/>
-      <c r="L115" s="69" t="s">
+      <c r="L115" s="81" t="s">
         <v>65</v>
       </c>
-      <c r="M115" s="77"/>
-      <c r="N115" s="77"/>
-      <c r="O115" s="77"/>
-      <c r="P115" s="77"/>
-      <c r="Q115" s="70"/>
+      <c r="M115" s="82"/>
+      <c r="N115" s="82"/>
+      <c r="O115" s="82"/>
+      <c r="P115" s="82"/>
+      <c r="Q115" s="83"/>
       <c r="R115" s="49"/>
       <c r="S115" s="51"/>
       <c r="T115" s="52" t="s">
@@ -5148,18 +5215,18 @@
         <f t="shared" si="9"/>
         <v>43797</v>
       </c>
-      <c r="C116" s="86" t="s">
+      <c r="C116" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="D116" s="86"/>
-      <c r="E116" s="86"/>
-      <c r="F116" s="86"/>
-      <c r="G116" s="86"/>
-      <c r="H116" s="76" t="s">
+      <c r="D116" s="76"/>
+      <c r="E116" s="76"/>
+      <c r="F116" s="76"/>
+      <c r="G116" s="76"/>
+      <c r="H116" s="77" t="s">
         <v>55</v>
       </c>
-      <c r="I116" s="76"/>
-      <c r="J116" s="76"/>
+      <c r="I116" s="77"/>
+      <c r="J116" s="77"/>
       <c r="K116" s="78" t="s">
         <v>65</v>
       </c>
@@ -5168,7 +5235,7 @@
       <c r="N116" s="79"/>
       <c r="O116" s="79"/>
       <c r="P116" s="79"/>
-      <c r="Q116" s="113"/>
+      <c r="Q116" s="80"/>
       <c r="R116" s="20"/>
       <c r="S116" s="51"/>
       <c r="T116" s="18" t="s">
@@ -5186,23 +5253,23 @@
       </c>
       <c r="C117" s="32"/>
       <c r="D117" s="20"/>
-      <c r="E117" s="76" t="s">
+      <c r="E117" s="77" t="s">
         <v>65</v>
       </c>
-      <c r="F117" s="76"/>
-      <c r="G117" s="76"/>
-      <c r="H117" s="76"/>
-      <c r="I117" s="76"/>
-      <c r="J117" s="76"/>
+      <c r="F117" s="77"/>
+      <c r="G117" s="77"/>
+      <c r="H117" s="77"/>
+      <c r="I117" s="77"/>
+      <c r="J117" s="77"/>
       <c r="K117" s="49"/>
-      <c r="L117" s="69" t="s">
+      <c r="L117" s="81" t="s">
         <v>65</v>
       </c>
-      <c r="M117" s="77"/>
-      <c r="N117" s="77"/>
-      <c r="O117" s="77"/>
-      <c r="P117" s="77"/>
-      <c r="Q117" s="70"/>
+      <c r="M117" s="82"/>
+      <c r="N117" s="82"/>
+      <c r="O117" s="82"/>
+      <c r="P117" s="82"/>
+      <c r="Q117" s="83"/>
       <c r="R117" s="20"/>
       <c r="S117" s="51"/>
       <c r="T117" s="51"/>
@@ -5218,23 +5285,23 @@
       </c>
       <c r="C118" s="50"/>
       <c r="D118" s="49"/>
-      <c r="E118" s="76" t="s">
+      <c r="E118" s="77" t="s">
         <v>65</v>
       </c>
-      <c r="F118" s="76"/>
-      <c r="G118" s="76"/>
-      <c r="H118" s="76"/>
-      <c r="I118" s="76"/>
-      <c r="J118" s="76"/>
+      <c r="F118" s="77"/>
+      <c r="G118" s="77"/>
+      <c r="H118" s="77"/>
+      <c r="I118" s="77"/>
+      <c r="J118" s="77"/>
       <c r="K118" s="49"/>
-      <c r="L118" s="69" t="s">
+      <c r="L118" s="81" t="s">
         <v>65</v>
       </c>
-      <c r="M118" s="77"/>
-      <c r="N118" s="77"/>
-      <c r="O118" s="77"/>
-      <c r="P118" s="77"/>
-      <c r="Q118" s="70"/>
+      <c r="M118" s="82"/>
+      <c r="N118" s="82"/>
+      <c r="O118" s="82"/>
+      <c r="P118" s="82"/>
+      <c r="Q118" s="83"/>
       <c r="R118" s="49"/>
       <c r="S118" s="51"/>
       <c r="T118" s="51"/>
@@ -5248,24 +5315,24 @@
         <f t="shared" si="9"/>
         <v>43800</v>
       </c>
-      <c r="C119" s="86" t="s">
+      <c r="C119" s="76" t="s">
         <v>81</v>
       </c>
-      <c r="D119" s="86"/>
-      <c r="E119" s="86"/>
-      <c r="F119" s="86"/>
-      <c r="G119" s="86"/>
-      <c r="H119" s="86"/>
-      <c r="I119" s="86"/>
-      <c r="J119" s="86"/>
-      <c r="K119" s="86"/>
-      <c r="L119" s="86"/>
-      <c r="M119" s="86"/>
-      <c r="N119" s="86"/>
-      <c r="O119" s="86"/>
-      <c r="P119" s="86"/>
-      <c r="Q119" s="86"/>
-      <c r="R119" s="86"/>
+      <c r="D119" s="76"/>
+      <c r="E119" s="76"/>
+      <c r="F119" s="76"/>
+      <c r="G119" s="76"/>
+      <c r="H119" s="76"/>
+      <c r="I119" s="76"/>
+      <c r="J119" s="76"/>
+      <c r="K119" s="76"/>
+      <c r="L119" s="76"/>
+      <c r="M119" s="76"/>
+      <c r="N119" s="76"/>
+      <c r="O119" s="76"/>
+      <c r="P119" s="76"/>
+      <c r="Q119" s="76"/>
+      <c r="R119" s="76"/>
       <c r="S119" s="51"/>
       <c r="T119" s="51"/>
       <c r="U119" s="54"/>
@@ -5340,11 +5407,11 @@
         <f>C112+1</f>
         <v>12</v>
       </c>
-      <c r="D122" s="81" t="s">
+      <c r="D122" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="E122" s="81"/>
-      <c r="F122" s="81"/>
+      <c r="E122" s="94"/>
+      <c r="F122" s="94"/>
       <c r="G122" s="15"/>
       <c r="H122" s="15"/>
       <c r="I122" s="15"/>
@@ -5369,13 +5436,13 @@
         <f>B113+7</f>
         <v>43801</v>
       </c>
-      <c r="C123" s="86" t="s">
+      <c r="C123" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="D123" s="86"/>
-      <c r="E123" s="86"/>
-      <c r="F123" s="86"/>
-      <c r="G123" s="86"/>
+      <c r="D123" s="76"/>
+      <c r="E123" s="76"/>
+      <c r="F123" s="76"/>
+      <c r="G123" s="76"/>
       <c r="H123" s="78" t="s">
         <v>65</v>
       </c>
@@ -5386,7 +5453,7 @@
       <c r="M123" s="79"/>
       <c r="N123" s="79"/>
       <c r="O123" s="79"/>
-      <c r="P123" s="80"/>
+      <c r="P123" s="115"/>
       <c r="Q123" s="20"/>
       <c r="R123" s="20"/>
       <c r="S123" s="51"/>
@@ -5403,17 +5470,17 @@
         <f t="shared" ref="B124:B129" si="10">B114+7</f>
         <v>43802</v>
       </c>
-      <c r="C124" s="86" t="s">
+      <c r="C124" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="D124" s="86"/>
-      <c r="E124" s="86"/>
-      <c r="F124" s="86"/>
-      <c r="G124" s="86"/>
-      <c r="H124" s="86" t="s">
+      <c r="D124" s="76"/>
+      <c r="E124" s="76"/>
+      <c r="F124" s="76"/>
+      <c r="G124" s="76"/>
+      <c r="H124" s="76" t="s">
         <v>44</v>
       </c>
-      <c r="I124" s="86"/>
+      <c r="I124" s="76"/>
       <c r="J124" s="20"/>
       <c r="K124" s="49"/>
       <c r="L124" s="49"/>
@@ -5467,13 +5534,13 @@
         <f t="shared" si="10"/>
         <v>43804</v>
       </c>
-      <c r="C126" s="87" t="s">
+      <c r="C126" s="86" t="s">
         <v>80</v>
       </c>
-      <c r="D126" s="87"/>
-      <c r="E126" s="87"/>
-      <c r="F126" s="87"/>
-      <c r="G126" s="87"/>
+      <c r="D126" s="86"/>
+      <c r="E126" s="86"/>
+      <c r="F126" s="86"/>
+      <c r="G126" s="86"/>
       <c r="H126" s="49"/>
       <c r="I126" s="49"/>
       <c r="J126" s="49"/>
@@ -5555,24 +5622,24 @@
         <f t="shared" si="10"/>
         <v>43807</v>
       </c>
-      <c r="C129" s="86" t="s">
+      <c r="C129" s="76" t="s">
         <v>81</v>
       </c>
-      <c r="D129" s="86"/>
-      <c r="E129" s="86"/>
-      <c r="F129" s="86"/>
-      <c r="G129" s="86"/>
-      <c r="H129" s="86"/>
-      <c r="I129" s="86"/>
-      <c r="J129" s="86"/>
-      <c r="K129" s="86"/>
-      <c r="L129" s="86"/>
-      <c r="M129" s="86"/>
-      <c r="N129" s="86"/>
-      <c r="O129" s="86"/>
-      <c r="P129" s="86"/>
-      <c r="Q129" s="86"/>
-      <c r="R129" s="86"/>
+      <c r="D129" s="76"/>
+      <c r="E129" s="76"/>
+      <c r="F129" s="76"/>
+      <c r="G129" s="76"/>
+      <c r="H129" s="76"/>
+      <c r="I129" s="76"/>
+      <c r="J129" s="76"/>
+      <c r="K129" s="76"/>
+      <c r="L129" s="76"/>
+      <c r="M129" s="76"/>
+      <c r="N129" s="76"/>
+      <c r="O129" s="76"/>
+      <c r="P129" s="76"/>
+      <c r="Q129" s="76"/>
+      <c r="R129" s="76"/>
       <c r="S129" s="51"/>
       <c r="T129" s="51"/>
       <c r="U129" s="54"/>
@@ -5674,13 +5741,13 @@
         <f>B123+7</f>
         <v>43808</v>
       </c>
-      <c r="C133" s="86" t="s">
+      <c r="C133" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="D133" s="86"/>
-      <c r="E133" s="86"/>
-      <c r="F133" s="86"/>
-      <c r="G133" s="86"/>
+      <c r="D133" s="76"/>
+      <c r="E133" s="76"/>
+      <c r="F133" s="76"/>
+      <c r="G133" s="76"/>
       <c r="H133" s="49"/>
       <c r="I133" s="49"/>
       <c r="J133" s="49"/>
@@ -5706,13 +5773,13 @@
         <f t="shared" ref="B134:B139" si="11">B124+7</f>
         <v>43809</v>
       </c>
-      <c r="C134" s="86" t="s">
+      <c r="C134" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="D134" s="86"/>
-      <c r="E134" s="86"/>
-      <c r="F134" s="86"/>
-      <c r="G134" s="86"/>
+      <c r="D134" s="76"/>
+      <c r="E134" s="76"/>
+      <c r="F134" s="76"/>
+      <c r="G134" s="76"/>
       <c r="H134" s="20"/>
       <c r="I134" s="20"/>
       <c r="J134" s="20"/>
@@ -5768,13 +5835,13 @@
         <f t="shared" si="11"/>
         <v>43811</v>
       </c>
-      <c r="C136" s="86" t="s">
+      <c r="C136" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="D136" s="86"/>
-      <c r="E136" s="86"/>
-      <c r="F136" s="86"/>
-      <c r="G136" s="86"/>
+      <c r="D136" s="76"/>
+      <c r="E136" s="76"/>
+      <c r="F136" s="76"/>
+      <c r="G136" s="76"/>
       <c r="H136" s="20"/>
       <c r="I136" s="49"/>
       <c r="J136" s="49"/>
@@ -5856,24 +5923,24 @@
         <f t="shared" si="11"/>
         <v>43814</v>
       </c>
-      <c r="C139" s="86" t="s">
+      <c r="C139" s="76" t="s">
         <v>81</v>
       </c>
-      <c r="D139" s="86"/>
-      <c r="E139" s="86"/>
-      <c r="F139" s="86"/>
-      <c r="G139" s="86"/>
-      <c r="H139" s="86"/>
-      <c r="I139" s="86"/>
-      <c r="J139" s="86"/>
-      <c r="K139" s="86"/>
-      <c r="L139" s="86"/>
-      <c r="M139" s="86"/>
-      <c r="N139" s="86"/>
-      <c r="O139" s="86"/>
-      <c r="P139" s="86"/>
-      <c r="Q139" s="86"/>
-      <c r="R139" s="86"/>
+      <c r="D139" s="76"/>
+      <c r="E139" s="76"/>
+      <c r="F139" s="76"/>
+      <c r="G139" s="76"/>
+      <c r="H139" s="76"/>
+      <c r="I139" s="76"/>
+      <c r="J139" s="76"/>
+      <c r="K139" s="76"/>
+      <c r="L139" s="76"/>
+      <c r="M139" s="76"/>
+      <c r="N139" s="76"/>
+      <c r="O139" s="76"/>
+      <c r="P139" s="76"/>
+      <c r="Q139" s="76"/>
+      <c r="R139" s="76"/>
       <c r="S139" s="51"/>
       <c r="T139" s="51"/>
       <c r="U139" s="54"/>
@@ -5968,19 +6035,19 @@
         <f>C132+1</f>
         <v>14</v>
       </c>
-      <c r="D142" s="81" t="s">
+      <c r="D142" s="94" t="s">
         <v>30</v>
       </c>
-      <c r="E142" s="81"/>
-      <c r="F142" s="81"/>
+      <c r="E142" s="94"/>
+      <c r="F142" s="94"/>
       <c r="G142" s="15"/>
-      <c r="H142" s="81" t="s">
+      <c r="H142" s="94" t="s">
         <v>52</v>
       </c>
-      <c r="I142" s="81"/>
-      <c r="J142" s="81"/>
-      <c r="K142" s="81"/>
-      <c r="L142" s="81"/>
+      <c r="I142" s="94"/>
+      <c r="J142" s="94"/>
+      <c r="K142" s="94"/>
+      <c r="L142" s="94"/>
       <c r="M142" s="19"/>
       <c r="N142" s="19"/>
       <c r="O142" s="19"/>
@@ -5999,11 +6066,11 @@
         <f>B133+7</f>
         <v>43815</v>
       </c>
-      <c r="C143" s="76" t="s">
+      <c r="C143" s="77" t="s">
         <v>55</v>
       </c>
-      <c r="D143" s="76"/>
-      <c r="E143" s="76"/>
+      <c r="D143" s="77"/>
+      <c r="E143" s="77"/>
       <c r="F143" s="20"/>
       <c r="G143" s="20"/>
       <c r="H143" s="20"/>
@@ -6374,24 +6441,24 @@
         <f t="shared" si="13"/>
         <v>43824</v>
       </c>
-      <c r="C155" s="85" t="s">
+      <c r="C155" s="113" t="s">
         <v>53</v>
       </c>
-      <c r="D155" s="85"/>
-      <c r="E155" s="85"/>
-      <c r="F155" s="85"/>
-      <c r="G155" s="85"/>
-      <c r="H155" s="85"/>
-      <c r="I155" s="85"/>
-      <c r="J155" s="85"/>
-      <c r="K155" s="85"/>
-      <c r="L155" s="85"/>
-      <c r="M155" s="85"/>
-      <c r="N155" s="85"/>
-      <c r="O155" s="85"/>
-      <c r="P155" s="85"/>
-      <c r="Q155" s="85"/>
-      <c r="R155" s="85"/>
+      <c r="D155" s="113"/>
+      <c r="E155" s="113"/>
+      <c r="F155" s="113"/>
+      <c r="G155" s="113"/>
+      <c r="H155" s="113"/>
+      <c r="I155" s="113"/>
+      <c r="J155" s="113"/>
+      <c r="K155" s="113"/>
+      <c r="L155" s="113"/>
+      <c r="M155" s="113"/>
+      <c r="N155" s="113"/>
+      <c r="O155" s="113"/>
+      <c r="P155" s="113"/>
+      <c r="Q155" s="113"/>
+      <c r="R155" s="113"/>
       <c r="S155" s="51"/>
       <c r="T155" s="52" t="s">
         <v>20</v>
@@ -6406,22 +6473,22 @@
         <f t="shared" si="13"/>
         <v>43825</v>
       </c>
-      <c r="C156" s="85"/>
-      <c r="D156" s="85"/>
-      <c r="E156" s="85"/>
-      <c r="F156" s="85"/>
-      <c r="G156" s="85"/>
-      <c r="H156" s="85"/>
-      <c r="I156" s="85"/>
-      <c r="J156" s="85"/>
-      <c r="K156" s="85"/>
-      <c r="L156" s="85"/>
-      <c r="M156" s="85"/>
-      <c r="N156" s="85"/>
-      <c r="O156" s="85"/>
-      <c r="P156" s="85"/>
-      <c r="Q156" s="85"/>
-      <c r="R156" s="85"/>
+      <c r="C156" s="113"/>
+      <c r="D156" s="113"/>
+      <c r="E156" s="113"/>
+      <c r="F156" s="113"/>
+      <c r="G156" s="113"/>
+      <c r="H156" s="113"/>
+      <c r="I156" s="113"/>
+      <c r="J156" s="113"/>
+      <c r="K156" s="113"/>
+      <c r="L156" s="113"/>
+      <c r="M156" s="113"/>
+      <c r="N156" s="113"/>
+      <c r="O156" s="113"/>
+      <c r="P156" s="113"/>
+      <c r="Q156" s="113"/>
+      <c r="R156" s="113"/>
       <c r="S156" s="51"/>
       <c r="T156" s="18" t="s">
         <v>21</v>
@@ -6436,22 +6503,22 @@
         <f t="shared" si="13"/>
         <v>43826</v>
       </c>
-      <c r="C157" s="85"/>
-      <c r="D157" s="85"/>
-      <c r="E157" s="85"/>
-      <c r="F157" s="85"/>
-      <c r="G157" s="85"/>
-      <c r="H157" s="85"/>
-      <c r="I157" s="85"/>
-      <c r="J157" s="85"/>
-      <c r="K157" s="85"/>
-      <c r="L157" s="85"/>
-      <c r="M157" s="85"/>
-      <c r="N157" s="85"/>
-      <c r="O157" s="85"/>
-      <c r="P157" s="85"/>
-      <c r="Q157" s="85"/>
-      <c r="R157" s="85"/>
+      <c r="C157" s="113"/>
+      <c r="D157" s="113"/>
+      <c r="E157" s="113"/>
+      <c r="F157" s="113"/>
+      <c r="G157" s="113"/>
+      <c r="H157" s="113"/>
+      <c r="I157" s="113"/>
+      <c r="J157" s="113"/>
+      <c r="K157" s="113"/>
+      <c r="L157" s="113"/>
+      <c r="M157" s="113"/>
+      <c r="N157" s="113"/>
+      <c r="O157" s="113"/>
+      <c r="P157" s="113"/>
+      <c r="Q157" s="113"/>
+      <c r="R157" s="113"/>
       <c r="S157" s="51"/>
       <c r="T157" s="51"/>
       <c r="U157" s="54"/>
@@ -6464,22 +6531,22 @@
         <f t="shared" si="13"/>
         <v>43827</v>
       </c>
-      <c r="C158" s="85"/>
-      <c r="D158" s="85"/>
-      <c r="E158" s="85"/>
-      <c r="F158" s="85"/>
-      <c r="G158" s="85"/>
-      <c r="H158" s="85"/>
-      <c r="I158" s="85"/>
-      <c r="J158" s="85"/>
-      <c r="K158" s="85"/>
-      <c r="L158" s="85"/>
-      <c r="M158" s="85"/>
-      <c r="N158" s="85"/>
-      <c r="O158" s="85"/>
-      <c r="P158" s="85"/>
-      <c r="Q158" s="85"/>
-      <c r="R158" s="85"/>
+      <c r="C158" s="113"/>
+      <c r="D158" s="113"/>
+      <c r="E158" s="113"/>
+      <c r="F158" s="113"/>
+      <c r="G158" s="113"/>
+      <c r="H158" s="113"/>
+      <c r="I158" s="113"/>
+      <c r="J158" s="113"/>
+      <c r="K158" s="113"/>
+      <c r="L158" s="113"/>
+      <c r="M158" s="113"/>
+      <c r="N158" s="113"/>
+      <c r="O158" s="113"/>
+      <c r="P158" s="113"/>
+      <c r="Q158" s="113"/>
+      <c r="R158" s="113"/>
       <c r="S158" s="51"/>
       <c r="T158" s="51"/>
       <c r="U158" s="54"/>
@@ -6492,22 +6559,22 @@
         <f t="shared" si="13"/>
         <v>43828</v>
       </c>
-      <c r="C159" s="85"/>
-      <c r="D159" s="85"/>
-      <c r="E159" s="85"/>
-      <c r="F159" s="85"/>
-      <c r="G159" s="85"/>
-      <c r="H159" s="85"/>
-      <c r="I159" s="85"/>
-      <c r="J159" s="85"/>
-      <c r="K159" s="85"/>
-      <c r="L159" s="85"/>
-      <c r="M159" s="85"/>
-      <c r="N159" s="85"/>
-      <c r="O159" s="85"/>
-      <c r="P159" s="85"/>
-      <c r="Q159" s="85"/>
-      <c r="R159" s="85"/>
+      <c r="C159" s="113"/>
+      <c r="D159" s="113"/>
+      <c r="E159" s="113"/>
+      <c r="F159" s="113"/>
+      <c r="G159" s="113"/>
+      <c r="H159" s="113"/>
+      <c r="I159" s="113"/>
+      <c r="J159" s="113"/>
+      <c r="K159" s="113"/>
+      <c r="L159" s="113"/>
+      <c r="M159" s="113"/>
+      <c r="N159" s="113"/>
+      <c r="O159" s="113"/>
+      <c r="P159" s="113"/>
+      <c r="Q159" s="113"/>
+      <c r="R159" s="113"/>
       <c r="S159" s="51"/>
       <c r="T159" s="51"/>
       <c r="U159" s="54"/>
@@ -6629,24 +6696,24 @@
         <f>B153+7</f>
         <v>43829</v>
       </c>
-      <c r="C163" s="85" t="s">
+      <c r="C163" s="113" t="s">
         <v>54</v>
       </c>
-      <c r="D163" s="85"/>
-      <c r="E163" s="85"/>
-      <c r="F163" s="85"/>
-      <c r="G163" s="85"/>
-      <c r="H163" s="85"/>
-      <c r="I163" s="85"/>
-      <c r="J163" s="85"/>
-      <c r="K163" s="85"/>
-      <c r="L163" s="85"/>
-      <c r="M163" s="85"/>
-      <c r="N163" s="85"/>
-      <c r="O163" s="85"/>
-      <c r="P163" s="85"/>
-      <c r="Q163" s="85"/>
-      <c r="R163" s="85"/>
+      <c r="D163" s="113"/>
+      <c r="E163" s="113"/>
+      <c r="F163" s="113"/>
+      <c r="G163" s="113"/>
+      <c r="H163" s="113"/>
+      <c r="I163" s="113"/>
+      <c r="J163" s="113"/>
+      <c r="K163" s="113"/>
+      <c r="L163" s="113"/>
+      <c r="M163" s="113"/>
+      <c r="N163" s="113"/>
+      <c r="O163" s="113"/>
+      <c r="P163" s="113"/>
+      <c r="Q163" s="113"/>
+      <c r="R163" s="113"/>
       <c r="S163" s="51"/>
       <c r="T163" s="30" t="s">
         <v>22</v>
@@ -6661,22 +6728,22 @@
         <f t="shared" ref="B164:B169" si="14">B154+7</f>
         <v>43830</v>
       </c>
-      <c r="C164" s="85"/>
-      <c r="D164" s="85"/>
-      <c r="E164" s="85"/>
-      <c r="F164" s="85"/>
-      <c r="G164" s="85"/>
-      <c r="H164" s="85"/>
-      <c r="I164" s="85"/>
-      <c r="J164" s="85"/>
-      <c r="K164" s="85"/>
-      <c r="L164" s="85"/>
-      <c r="M164" s="85"/>
-      <c r="N164" s="85"/>
-      <c r="O164" s="85"/>
-      <c r="P164" s="85"/>
-      <c r="Q164" s="85"/>
-      <c r="R164" s="85"/>
+      <c r="C164" s="113"/>
+      <c r="D164" s="113"/>
+      <c r="E164" s="113"/>
+      <c r="F164" s="113"/>
+      <c r="G164" s="113"/>
+      <c r="H164" s="113"/>
+      <c r="I164" s="113"/>
+      <c r="J164" s="113"/>
+      <c r="K164" s="113"/>
+      <c r="L164" s="113"/>
+      <c r="M164" s="113"/>
+      <c r="N164" s="113"/>
+      <c r="O164" s="113"/>
+      <c r="P164" s="113"/>
+      <c r="Q164" s="113"/>
+      <c r="R164" s="113"/>
       <c r="S164" s="51"/>
       <c r="T164" s="53" t="s">
         <v>19</v>
@@ -6691,22 +6758,22 @@
         <f t="shared" si="14"/>
         <v>43831</v>
       </c>
-      <c r="C165" s="85"/>
-      <c r="D165" s="85"/>
-      <c r="E165" s="85"/>
-      <c r="F165" s="85"/>
-      <c r="G165" s="85"/>
-      <c r="H165" s="85"/>
-      <c r="I165" s="85"/>
-      <c r="J165" s="85"/>
-      <c r="K165" s="85"/>
-      <c r="L165" s="85"/>
-      <c r="M165" s="85"/>
-      <c r="N165" s="85"/>
-      <c r="O165" s="85"/>
-      <c r="P165" s="85"/>
-      <c r="Q165" s="85"/>
-      <c r="R165" s="85"/>
+      <c r="C165" s="113"/>
+      <c r="D165" s="113"/>
+      <c r="E165" s="113"/>
+      <c r="F165" s="113"/>
+      <c r="G165" s="113"/>
+      <c r="H165" s="113"/>
+      <c r="I165" s="113"/>
+      <c r="J165" s="113"/>
+      <c r="K165" s="113"/>
+      <c r="L165" s="113"/>
+      <c r="M165" s="113"/>
+      <c r="N165" s="113"/>
+      <c r="O165" s="113"/>
+      <c r="P165" s="113"/>
+      <c r="Q165" s="113"/>
+      <c r="R165" s="113"/>
       <c r="S165" s="51"/>
       <c r="T165" s="52" t="s">
         <v>20</v>
@@ -6723,23 +6790,23 @@
       </c>
       <c r="C166" s="32"/>
       <c r="D166" s="20"/>
-      <c r="E166" s="76" t="s">
+      <c r="E166" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="F166" s="76"/>
-      <c r="G166" s="76"/>
-      <c r="H166" s="76"/>
-      <c r="I166" s="76"/>
-      <c r="J166" s="76"/>
+      <c r="F166" s="77"/>
+      <c r="G166" s="77"/>
+      <c r="H166" s="77"/>
+      <c r="I166" s="77"/>
+      <c r="J166" s="77"/>
       <c r="K166" s="49"/>
-      <c r="L166" s="69" t="s">
+      <c r="L166" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="M166" s="77"/>
-      <c r="N166" s="77"/>
-      <c r="O166" s="77"/>
-      <c r="P166" s="77"/>
-      <c r="Q166" s="70"/>
+      <c r="M166" s="82"/>
+      <c r="N166" s="82"/>
+      <c r="O166" s="82"/>
+      <c r="P166" s="82"/>
+      <c r="Q166" s="83"/>
       <c r="R166" s="20"/>
       <c r="S166" s="51"/>
       <c r="T166" s="18" t="s">
@@ -6757,23 +6824,23 @@
       </c>
       <c r="C167" s="50"/>
       <c r="D167" s="49"/>
-      <c r="E167" s="76" t="s">
+      <c r="E167" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="F167" s="76"/>
-      <c r="G167" s="76"/>
-      <c r="H167" s="76"/>
-      <c r="I167" s="76"/>
-      <c r="J167" s="76"/>
+      <c r="F167" s="77"/>
+      <c r="G167" s="77"/>
+      <c r="H167" s="77"/>
+      <c r="I167" s="77"/>
+      <c r="J167" s="77"/>
       <c r="K167" s="49"/>
-      <c r="L167" s="69" t="s">
+      <c r="L167" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="M167" s="77"/>
-      <c r="N167" s="77"/>
-      <c r="O167" s="77"/>
-      <c r="P167" s="77"/>
-      <c r="Q167" s="70"/>
+      <c r="M167" s="82"/>
+      <c r="N167" s="82"/>
+      <c r="O167" s="82"/>
+      <c r="P167" s="82"/>
+      <c r="Q167" s="83"/>
       <c r="R167" s="49"/>
       <c r="S167" s="51"/>
       <c r="T167" s="51"/>
@@ -6934,23 +7001,23 @@
       </c>
       <c r="C173" s="32"/>
       <c r="D173" s="20"/>
-      <c r="E173" s="76" t="s">
+      <c r="E173" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="F173" s="76"/>
-      <c r="G173" s="76"/>
-      <c r="H173" s="76"/>
-      <c r="I173" s="76"/>
-      <c r="J173" s="76"/>
+      <c r="F173" s="77"/>
+      <c r="G173" s="77"/>
+      <c r="H173" s="77"/>
+      <c r="I173" s="77"/>
+      <c r="J173" s="77"/>
       <c r="K173" s="49"/>
-      <c r="L173" s="69" t="s">
+      <c r="L173" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="M173" s="77"/>
-      <c r="N173" s="77"/>
-      <c r="O173" s="77"/>
-      <c r="P173" s="77"/>
-      <c r="Q173" s="70"/>
+      <c r="M173" s="82"/>
+      <c r="N173" s="82"/>
+      <c r="O173" s="82"/>
+      <c r="P173" s="82"/>
+      <c r="Q173" s="83"/>
       <c r="R173" s="49"/>
       <c r="S173" s="51"/>
       <c r="T173" s="30" t="s">
@@ -6968,23 +7035,23 @@
       </c>
       <c r="C174" s="32"/>
       <c r="D174" s="20"/>
-      <c r="E174" s="76" t="s">
+      <c r="E174" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="F174" s="76"/>
-      <c r="G174" s="76"/>
-      <c r="H174" s="76"/>
-      <c r="I174" s="76"/>
-      <c r="J174" s="76"/>
+      <c r="F174" s="77"/>
+      <c r="G174" s="77"/>
+      <c r="H174" s="77"/>
+      <c r="I174" s="77"/>
+      <c r="J174" s="77"/>
       <c r="K174" s="49"/>
-      <c r="L174" s="69" t="s">
+      <c r="L174" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="M174" s="77"/>
-      <c r="N174" s="77"/>
-      <c r="O174" s="77"/>
-      <c r="P174" s="77"/>
-      <c r="Q174" s="70"/>
+      <c r="M174" s="82"/>
+      <c r="N174" s="82"/>
+      <c r="O174" s="82"/>
+      <c r="P174" s="82"/>
+      <c r="Q174" s="83"/>
       <c r="R174" s="20"/>
       <c r="S174" s="51"/>
       <c r="T174" s="53" t="s">
@@ -7002,23 +7069,23 @@
       </c>
       <c r="C175" s="32"/>
       <c r="D175" s="20"/>
-      <c r="E175" s="76" t="s">
+      <c r="E175" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="F175" s="76"/>
-      <c r="G175" s="76"/>
-      <c r="H175" s="76"/>
-      <c r="I175" s="76"/>
-      <c r="J175" s="76"/>
+      <c r="F175" s="77"/>
+      <c r="G175" s="77"/>
+      <c r="H175" s="77"/>
+      <c r="I175" s="77"/>
+      <c r="J175" s="77"/>
       <c r="K175" s="20"/>
-      <c r="L175" s="69" t="s">
+      <c r="L175" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="M175" s="77"/>
-      <c r="N175" s="77"/>
-      <c r="O175" s="77"/>
-      <c r="P175" s="77"/>
-      <c r="Q175" s="70"/>
+      <c r="M175" s="82"/>
+      <c r="N175" s="82"/>
+      <c r="O175" s="82"/>
+      <c r="P175" s="82"/>
+      <c r="Q175" s="83"/>
       <c r="R175" s="49"/>
       <c r="S175" s="51"/>
       <c r="T175" s="52" t="s">
@@ -7036,23 +7103,23 @@
       </c>
       <c r="C176" s="49"/>
       <c r="D176" s="49"/>
-      <c r="E176" s="76" t="s">
+      <c r="E176" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="F176" s="76"/>
-      <c r="G176" s="76"/>
-      <c r="H176" s="76"/>
-      <c r="I176" s="76"/>
-      <c r="J176" s="76"/>
+      <c r="F176" s="77"/>
+      <c r="G176" s="77"/>
+      <c r="H176" s="77"/>
+      <c r="I176" s="77"/>
+      <c r="J176" s="77"/>
       <c r="K176" s="20"/>
-      <c r="L176" s="69" t="s">
+      <c r="L176" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="M176" s="77"/>
-      <c r="N176" s="77"/>
-      <c r="O176" s="77"/>
-      <c r="P176" s="77"/>
-      <c r="Q176" s="70"/>
+      <c r="M176" s="82"/>
+      <c r="N176" s="82"/>
+      <c r="O176" s="82"/>
+      <c r="P176" s="82"/>
+      <c r="Q176" s="83"/>
       <c r="R176" s="20"/>
       <c r="S176" s="51"/>
       <c r="T176" s="18" t="s">
@@ -7070,23 +7137,23 @@
       </c>
       <c r="C177" s="32"/>
       <c r="D177" s="20"/>
-      <c r="E177" s="76" t="s">
+      <c r="E177" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="F177" s="76"/>
-      <c r="G177" s="76"/>
-      <c r="H177" s="76"/>
-      <c r="I177" s="76"/>
-      <c r="J177" s="76"/>
+      <c r="F177" s="77"/>
+      <c r="G177" s="77"/>
+      <c r="H177" s="77"/>
+      <c r="I177" s="77"/>
+      <c r="J177" s="77"/>
       <c r="K177" s="20"/>
-      <c r="L177" s="69" t="s">
+      <c r="L177" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="M177" s="77"/>
-      <c r="N177" s="77"/>
-      <c r="O177" s="77"/>
-      <c r="P177" s="77"/>
-      <c r="Q177" s="70"/>
+      <c r="M177" s="82"/>
+      <c r="N177" s="82"/>
+      <c r="O177" s="82"/>
+      <c r="P177" s="82"/>
+      <c r="Q177" s="83"/>
       <c r="R177" s="20"/>
       <c r="S177" s="51"/>
       <c r="T177" s="51"/>
@@ -7245,23 +7312,23 @@
       </c>
       <c r="C183" s="32"/>
       <c r="D183" s="20"/>
-      <c r="E183" s="76" t="s">
+      <c r="E183" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="F183" s="76"/>
-      <c r="G183" s="76"/>
-      <c r="H183" s="76"/>
-      <c r="I183" s="76"/>
-      <c r="J183" s="76"/>
+      <c r="F183" s="77"/>
+      <c r="G183" s="77"/>
+      <c r="H183" s="77"/>
+      <c r="I183" s="77"/>
+      <c r="J183" s="77"/>
       <c r="K183" s="49"/>
-      <c r="L183" s="69" t="s">
+      <c r="L183" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="M183" s="77"/>
-      <c r="N183" s="77"/>
-      <c r="O183" s="77"/>
-      <c r="P183" s="77"/>
-      <c r="Q183" s="70"/>
+      <c r="M183" s="82"/>
+      <c r="N183" s="82"/>
+      <c r="O183" s="82"/>
+      <c r="P183" s="82"/>
+      <c r="Q183" s="83"/>
       <c r="R183" s="49"/>
       <c r="S183" s="51"/>
       <c r="T183" s="30" t="s">
@@ -7278,23 +7345,23 @@
       </c>
       <c r="C184" s="32"/>
       <c r="D184" s="20"/>
-      <c r="E184" s="76" t="s">
+      <c r="E184" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="F184" s="76"/>
-      <c r="G184" s="76"/>
-      <c r="H184" s="76"/>
-      <c r="I184" s="76"/>
-      <c r="J184" s="76"/>
+      <c r="F184" s="77"/>
+      <c r="G184" s="77"/>
+      <c r="H184" s="77"/>
+      <c r="I184" s="77"/>
+      <c r="J184" s="77"/>
       <c r="K184" s="49"/>
-      <c r="L184" s="69" t="s">
+      <c r="L184" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="M184" s="77"/>
-      <c r="N184" s="77"/>
-      <c r="O184" s="77"/>
-      <c r="P184" s="77"/>
-      <c r="Q184" s="70"/>
+      <c r="M184" s="82"/>
+      <c r="N184" s="82"/>
+      <c r="O184" s="82"/>
+      <c r="P184" s="82"/>
+      <c r="Q184" s="83"/>
       <c r="R184" s="20"/>
       <c r="S184" s="51"/>
       <c r="T184" s="53" t="s">
@@ -7311,23 +7378,23 @@
       </c>
       <c r="C185" s="32"/>
       <c r="D185" s="20"/>
-      <c r="E185" s="76" t="s">
+      <c r="E185" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="F185" s="76"/>
-      <c r="G185" s="76"/>
-      <c r="H185" s="76"/>
-      <c r="I185" s="76"/>
-      <c r="J185" s="76"/>
+      <c r="F185" s="77"/>
+      <c r="G185" s="77"/>
+      <c r="H185" s="77"/>
+      <c r="I185" s="77"/>
+      <c r="J185" s="77"/>
       <c r="K185" s="20"/>
-      <c r="L185" s="69" t="s">
+      <c r="L185" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="M185" s="77"/>
-      <c r="N185" s="77"/>
-      <c r="O185" s="77"/>
-      <c r="P185" s="77"/>
-      <c r="Q185" s="70"/>
+      <c r="M185" s="82"/>
+      <c r="N185" s="82"/>
+      <c r="O185" s="82"/>
+      <c r="P185" s="82"/>
+      <c r="Q185" s="83"/>
       <c r="R185" s="49"/>
       <c r="S185" s="51"/>
       <c r="T185" s="52" t="s">
@@ -7344,23 +7411,23 @@
       </c>
       <c r="C186" s="49"/>
       <c r="D186" s="49"/>
-      <c r="E186" s="76" t="s">
+      <c r="E186" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="F186" s="76"/>
-      <c r="G186" s="76"/>
-      <c r="H186" s="76"/>
-      <c r="I186" s="76"/>
-      <c r="J186" s="76"/>
+      <c r="F186" s="77"/>
+      <c r="G186" s="77"/>
+      <c r="H186" s="77"/>
+      <c r="I186" s="77"/>
+      <c r="J186" s="77"/>
       <c r="K186" s="20"/>
-      <c r="L186" s="69" t="s">
+      <c r="L186" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="M186" s="77"/>
-      <c r="N186" s="77"/>
-      <c r="O186" s="77"/>
-      <c r="P186" s="77"/>
-      <c r="Q186" s="70"/>
+      <c r="M186" s="82"/>
+      <c r="N186" s="82"/>
+      <c r="O186" s="82"/>
+      <c r="P186" s="82"/>
+      <c r="Q186" s="83"/>
       <c r="R186" s="20"/>
       <c r="S186" s="51"/>
       <c r="T186" s="18" t="s">
@@ -7377,23 +7444,23 @@
       </c>
       <c r="C187" s="32"/>
       <c r="D187" s="20"/>
-      <c r="E187" s="76" t="s">
+      <c r="E187" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="F187" s="76"/>
-      <c r="G187" s="76"/>
-      <c r="H187" s="76"/>
-      <c r="I187" s="76"/>
-      <c r="J187" s="76"/>
+      <c r="F187" s="77"/>
+      <c r="G187" s="77"/>
+      <c r="H187" s="77"/>
+      <c r="I187" s="77"/>
+      <c r="J187" s="77"/>
       <c r="K187" s="20"/>
-      <c r="L187" s="69" t="s">
+      <c r="L187" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="M187" s="77"/>
-      <c r="N187" s="77"/>
-      <c r="O187" s="77"/>
-      <c r="P187" s="77"/>
-      <c r="Q187" s="70"/>
+      <c r="M187" s="82"/>
+      <c r="N187" s="82"/>
+      <c r="O187" s="82"/>
+      <c r="P187" s="82"/>
+      <c r="Q187" s="83"/>
       <c r="R187" s="20"/>
       <c r="S187" s="51"/>
       <c r="T187" s="51"/>
@@ -15823,58 +15890,70 @@
       <c r="T507"/>
     </row>
   </sheetData>
-  <mergeCells count="145">
-    <mergeCell ref="J84:R84"/>
-    <mergeCell ref="E85:M85"/>
-    <mergeCell ref="H93:P93"/>
-    <mergeCell ref="H94:P94"/>
-    <mergeCell ref="H96:L96"/>
-    <mergeCell ref="C119:R119"/>
-    <mergeCell ref="C129:R129"/>
-    <mergeCell ref="C139:R139"/>
-    <mergeCell ref="C143:E143"/>
-    <mergeCell ref="K116:Q116"/>
-    <mergeCell ref="E115:J115"/>
-    <mergeCell ref="L115:Q115"/>
-    <mergeCell ref="L67:R67"/>
-    <mergeCell ref="L68:R68"/>
-    <mergeCell ref="M72:R72"/>
-    <mergeCell ref="H72:K72"/>
-    <mergeCell ref="C69:R69"/>
-    <mergeCell ref="C79:R79"/>
-    <mergeCell ref="C89:R89"/>
-    <mergeCell ref="C99:R99"/>
-    <mergeCell ref="C109:R109"/>
-    <mergeCell ref="C134:G134"/>
-    <mergeCell ref="C103:G103"/>
-    <mergeCell ref="C104:G104"/>
-    <mergeCell ref="C114:G114"/>
-    <mergeCell ref="C83:G83"/>
-    <mergeCell ref="C84:G84"/>
-    <mergeCell ref="C86:G86"/>
-    <mergeCell ref="C93:G93"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H46:P46"/>
-    <mergeCell ref="H44:N44"/>
-    <mergeCell ref="H52:J52"/>
-    <mergeCell ref="H62:J62"/>
-    <mergeCell ref="D82:F82"/>
-    <mergeCell ref="C53:G53"/>
-    <mergeCell ref="D72:F72"/>
-    <mergeCell ref="L75:Q75"/>
-    <mergeCell ref="I53:M53"/>
-    <mergeCell ref="C67:J67"/>
-    <mergeCell ref="C46:G46"/>
-    <mergeCell ref="C54:G54"/>
-    <mergeCell ref="C56:G56"/>
-    <mergeCell ref="C63:G63"/>
-    <mergeCell ref="C64:G64"/>
-    <mergeCell ref="I55:N55"/>
-    <mergeCell ref="C68:J68"/>
-    <mergeCell ref="C76:R76"/>
-    <mergeCell ref="E78:J78"/>
-    <mergeCell ref="G55:H55"/>
+  <mergeCells count="147">
+    <mergeCell ref="T58:U60"/>
+    <mergeCell ref="E187:J187"/>
+    <mergeCell ref="L187:Q187"/>
+    <mergeCell ref="E117:J117"/>
+    <mergeCell ref="L117:Q117"/>
+    <mergeCell ref="E118:J118"/>
+    <mergeCell ref="L118:Q118"/>
+    <mergeCell ref="H123:P123"/>
+    <mergeCell ref="E184:J184"/>
+    <mergeCell ref="L184:Q184"/>
+    <mergeCell ref="E185:J185"/>
+    <mergeCell ref="L185:Q185"/>
+    <mergeCell ref="E186:J186"/>
+    <mergeCell ref="L186:Q186"/>
+    <mergeCell ref="E176:J176"/>
+    <mergeCell ref="L176:Q176"/>
+    <mergeCell ref="E177:J177"/>
+    <mergeCell ref="L177:Q177"/>
+    <mergeCell ref="E183:J183"/>
+    <mergeCell ref="L183:Q183"/>
+    <mergeCell ref="E173:J173"/>
+    <mergeCell ref="H103:P103"/>
+    <mergeCell ref="H104:P104"/>
+    <mergeCell ref="E175:J175"/>
+    <mergeCell ref="L175:Q175"/>
+    <mergeCell ref="L167:Q167"/>
+    <mergeCell ref="C155:R159"/>
+    <mergeCell ref="C163:R165"/>
+    <mergeCell ref="E166:J166"/>
+    <mergeCell ref="L166:Q166"/>
+    <mergeCell ref="E167:J167"/>
+    <mergeCell ref="H84:I84"/>
+    <mergeCell ref="D112:F112"/>
+    <mergeCell ref="C136:G136"/>
+    <mergeCell ref="C116:G116"/>
+    <mergeCell ref="C123:G123"/>
+    <mergeCell ref="C124:G124"/>
+    <mergeCell ref="C106:G106"/>
+    <mergeCell ref="L173:Q173"/>
+    <mergeCell ref="E174:J174"/>
+    <mergeCell ref="L174:Q174"/>
+    <mergeCell ref="C126:G126"/>
+    <mergeCell ref="H142:L142"/>
+    <mergeCell ref="C105:M105"/>
+    <mergeCell ref="H106:P106"/>
+    <mergeCell ref="P57:R57"/>
+    <mergeCell ref="E73:J73"/>
+    <mergeCell ref="L73:Q73"/>
+    <mergeCell ref="Q54:R54"/>
+    <mergeCell ref="H54:P54"/>
+    <mergeCell ref="C66:G66"/>
+    <mergeCell ref="L74:Q74"/>
+    <mergeCell ref="L77:Q77"/>
+    <mergeCell ref="L78:Q78"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="J58:P58"/>
+    <mergeCell ref="E74:J74"/>
+    <mergeCell ref="H56:M56"/>
+    <mergeCell ref="H66:Q66"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="I63:L63"/>
+    <mergeCell ref="H64:N64"/>
     <mergeCell ref="H13:R13"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="O14:P14"/>
@@ -15897,78 +15976,68 @@
     <mergeCell ref="C26:G26"/>
     <mergeCell ref="H23:R23"/>
     <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H46:P46"/>
+    <mergeCell ref="H44:N44"/>
+    <mergeCell ref="H52:J52"/>
+    <mergeCell ref="H62:J62"/>
+    <mergeCell ref="D82:F82"/>
+    <mergeCell ref="C53:G53"/>
+    <mergeCell ref="D72:F72"/>
+    <mergeCell ref="L75:Q75"/>
+    <mergeCell ref="I53:M53"/>
+    <mergeCell ref="C67:J67"/>
+    <mergeCell ref="C46:G46"/>
+    <mergeCell ref="C54:G54"/>
+    <mergeCell ref="C56:G56"/>
+    <mergeCell ref="C63:G63"/>
+    <mergeCell ref="C64:G64"/>
+    <mergeCell ref="I55:N55"/>
+    <mergeCell ref="C76:R76"/>
+    <mergeCell ref="E78:J78"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="E75:J75"/>
+    <mergeCell ref="E77:J77"/>
+    <mergeCell ref="L67:R67"/>
+    <mergeCell ref="M72:R72"/>
+    <mergeCell ref="H72:K72"/>
+    <mergeCell ref="C69:R69"/>
+    <mergeCell ref="C79:R79"/>
+    <mergeCell ref="C89:R89"/>
+    <mergeCell ref="C99:R99"/>
+    <mergeCell ref="C109:R109"/>
+    <mergeCell ref="C103:G103"/>
+    <mergeCell ref="C104:G104"/>
+    <mergeCell ref="C83:G83"/>
+    <mergeCell ref="C84:G84"/>
+    <mergeCell ref="C86:G86"/>
+    <mergeCell ref="C93:G93"/>
+    <mergeCell ref="C94:G94"/>
+    <mergeCell ref="C96:G96"/>
+    <mergeCell ref="H83:P83"/>
+    <mergeCell ref="C107:M107"/>
+    <mergeCell ref="J84:R84"/>
+    <mergeCell ref="E85:M85"/>
+    <mergeCell ref="H93:P93"/>
+    <mergeCell ref="H94:P94"/>
+    <mergeCell ref="H96:L96"/>
+    <mergeCell ref="C119:R119"/>
+    <mergeCell ref="C129:R129"/>
+    <mergeCell ref="C139:R139"/>
+    <mergeCell ref="C143:E143"/>
+    <mergeCell ref="K116:Q116"/>
+    <mergeCell ref="E115:J115"/>
+    <mergeCell ref="L115:Q115"/>
+    <mergeCell ref="C134:G134"/>
+    <mergeCell ref="C114:G114"/>
     <mergeCell ref="C133:G133"/>
     <mergeCell ref="H124:I124"/>
     <mergeCell ref="C113:G113"/>
-    <mergeCell ref="C94:G94"/>
-    <mergeCell ref="C96:G96"/>
-    <mergeCell ref="E75:J75"/>
-    <mergeCell ref="E77:J77"/>
     <mergeCell ref="H116:J116"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="H83:P83"/>
-    <mergeCell ref="P57:R57"/>
-    <mergeCell ref="E73:J73"/>
-    <mergeCell ref="L73:Q73"/>
-    <mergeCell ref="Q54:R54"/>
-    <mergeCell ref="H54:P54"/>
-    <mergeCell ref="C66:G66"/>
-    <mergeCell ref="L74:Q74"/>
-    <mergeCell ref="L77:Q77"/>
-    <mergeCell ref="L78:Q78"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="E58:G58"/>
-    <mergeCell ref="J58:P58"/>
-    <mergeCell ref="E74:J74"/>
-    <mergeCell ref="H56:M56"/>
     <mergeCell ref="D122:F122"/>
     <mergeCell ref="D142:F142"/>
-    <mergeCell ref="H66:Q66"/>
-    <mergeCell ref="E175:J175"/>
-    <mergeCell ref="L175:Q175"/>
-    <mergeCell ref="L167:Q167"/>
-    <mergeCell ref="C155:R159"/>
-    <mergeCell ref="C163:R165"/>
-    <mergeCell ref="E166:J166"/>
-    <mergeCell ref="L166:Q166"/>
-    <mergeCell ref="E167:J167"/>
-    <mergeCell ref="H84:I84"/>
-    <mergeCell ref="H104:I104"/>
-    <mergeCell ref="D112:F112"/>
-    <mergeCell ref="C136:G136"/>
-    <mergeCell ref="C116:G116"/>
-    <mergeCell ref="C123:G123"/>
-    <mergeCell ref="C124:G124"/>
-    <mergeCell ref="C106:G106"/>
-    <mergeCell ref="L173:Q173"/>
-    <mergeCell ref="E174:J174"/>
-    <mergeCell ref="L174:Q174"/>
-    <mergeCell ref="C126:G126"/>
-    <mergeCell ref="H142:L142"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="I63:L63"/>
-    <mergeCell ref="H64:N64"/>
-    <mergeCell ref="T58:U60"/>
-    <mergeCell ref="E187:J187"/>
-    <mergeCell ref="L187:Q187"/>
-    <mergeCell ref="E117:J117"/>
-    <mergeCell ref="L117:Q117"/>
-    <mergeCell ref="E118:J118"/>
-    <mergeCell ref="L118:Q118"/>
-    <mergeCell ref="H123:P123"/>
-    <mergeCell ref="E184:J184"/>
-    <mergeCell ref="L184:Q184"/>
-    <mergeCell ref="E185:J185"/>
-    <mergeCell ref="L185:Q185"/>
-    <mergeCell ref="E186:J186"/>
-    <mergeCell ref="L186:Q186"/>
-    <mergeCell ref="E176:J176"/>
-    <mergeCell ref="L176:Q176"/>
-    <mergeCell ref="E177:J177"/>
-    <mergeCell ref="L177:Q177"/>
-    <mergeCell ref="E183:J183"/>
-    <mergeCell ref="L183:Q183"/>
-    <mergeCell ref="E173:J173"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -16547,7 +16616,7 @@
         <v>43929</v>
       </c>
       <c r="D36" s="29"/>
-      <c r="F36" s="85" t="s">
+      <c r="F36" s="113" t="s">
         <v>49</v>
       </c>
     </row>
@@ -16565,7 +16634,7 @@
         <v>43936</v>
       </c>
       <c r="D37" s="44"/>
-      <c r="F37" s="85"/>
+      <c r="F37" s="113"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="23">
@@ -16581,7 +16650,7 @@
         <v>43943</v>
       </c>
       <c r="D38" s="29"/>
-      <c r="F38" s="85"/>
+      <c r="F38" s="113"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="23">

</xml_diff>

<commit_message>
Updated Weekly Planner, Uploading comments from supervisor
</commit_message>
<xml_diff>
--- a/Weekly Planner.xlsx
+++ b/Weekly Planner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\SoftwareProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2DB77DF-A779-43F0-9365-1D17C7B3A277}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246BF56E-0D70-49FA-85C6-F5773F8E342B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="87">
   <si>
     <t>Monday</t>
   </si>
@@ -301,9 +301,6 @@
   </si>
   <si>
     <t>Software Project - Requirements Specifications</t>
-  </si>
-  <si>
-    <t>DAD - Project</t>
   </si>
 </sst>
 </file>
@@ -899,7 +896,7 @@
     <xf numFmtId="0" fontId="11" fillId="10" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1077,6 +1074,54 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="10" xfId="9" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="15" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="17" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="16" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="19" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="20" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="8" xfId="8" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="8" xfId="8" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="6" fillId="8" borderId="4" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="8" xfId="8" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="33" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="34" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1084,9 +1129,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
@@ -1098,91 +1140,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="8" xfId="8" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="10" xfId="9" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="19" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="29" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="15" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="17" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="16" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="9" fillId="6" borderId="11" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="6" fillId="8" borderId="11" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="8" xfId="8" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="4" fillId="5" borderId="24" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="6" fillId="8" borderId="4" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="6" fillId="11" borderId="4" xfId="10" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
@@ -1209,13 +1170,67 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="8" xfId="8" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="20" xfId="9" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="31" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="6" fillId="11" borderId="4" xfId="10" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="5" borderId="24" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="9" fillId="6" borderId="11" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="6" fillId="8" borderId="11" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="29" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1227,31 +1242,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="33" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="34" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="31" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="35" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="13" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="14" xfId="9" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="35" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1554,8 +1545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y507"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C107" sqref="C107:M107"/>
+    <sheetView tabSelected="1" topLeftCell="A112" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C155" sqref="C155:R159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1938,26 +1929,26 @@
       <c r="B13" s="57">
         <v>43724</v>
       </c>
-      <c r="C13" s="76" t="s">
+      <c r="C13" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="76"/>
-      <c r="E13" s="76"/>
-      <c r="F13" s="76"/>
-      <c r="G13" s="76"/>
-      <c r="H13" s="89" t="s">
+      <c r="D13" s="79"/>
+      <c r="E13" s="79"/>
+      <c r="F13" s="79"/>
+      <c r="G13" s="79"/>
+      <c r="H13" s="91" t="s">
         <v>39</v>
       </c>
-      <c r="I13" s="97"/>
-      <c r="J13" s="97"/>
-      <c r="K13" s="97"/>
-      <c r="L13" s="97"/>
-      <c r="M13" s="97"/>
-      <c r="N13" s="97"/>
-      <c r="O13" s="97"/>
-      <c r="P13" s="97"/>
-      <c r="Q13" s="97"/>
-      <c r="R13" s="98"/>
+      <c r="I13" s="105"/>
+      <c r="J13" s="105"/>
+      <c r="K13" s="105"/>
+      <c r="L13" s="105"/>
+      <c r="M13" s="105"/>
+      <c r="N13" s="105"/>
+      <c r="O13" s="105"/>
+      <c r="P13" s="105"/>
+      <c r="Q13" s="105"/>
+      <c r="R13" s="92"/>
       <c r="S13" s="51"/>
       <c r="T13" s="30" t="s">
         <v>22</v>
@@ -1970,26 +1961,26 @@
       <c r="B14" s="57">
         <v>43725</v>
       </c>
-      <c r="C14" s="76" t="s">
+      <c r="C14" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="76"/>
-      <c r="E14" s="76"/>
-      <c r="F14" s="76"/>
-      <c r="G14" s="76"/>
+      <c r="D14" s="79"/>
+      <c r="E14" s="79"/>
+      <c r="F14" s="79"/>
+      <c r="G14" s="79"/>
       <c r="H14" s="20"/>
       <c r="I14" s="20"/>
-      <c r="J14" s="87" t="s">
+      <c r="J14" s="106" t="s">
         <v>45</v>
       </c>
-      <c r="K14" s="99"/>
-      <c r="L14" s="99"/>
-      <c r="M14" s="99"/>
-      <c r="N14" s="88"/>
-      <c r="O14" s="89" t="s">
+      <c r="K14" s="107"/>
+      <c r="L14" s="107"/>
+      <c r="M14" s="107"/>
+      <c r="N14" s="108"/>
+      <c r="O14" s="91" t="s">
         <v>38</v>
       </c>
-      <c r="P14" s="98"/>
+      <c r="P14" s="92"/>
       <c r="Q14" s="20"/>
       <c r="R14" s="20"/>
       <c r="S14" s="51"/>
@@ -2032,20 +2023,20 @@
       <c r="B16" s="57">
         <v>43727</v>
       </c>
-      <c r="C16" s="76" t="s">
+      <c r="C16" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="76"/>
-      <c r="E16" s="76"/>
-      <c r="F16" s="76"/>
-      <c r="G16" s="76"/>
-      <c r="H16" s="104" t="s">
+      <c r="D16" s="79"/>
+      <c r="E16" s="79"/>
+      <c r="F16" s="79"/>
+      <c r="G16" s="79"/>
+      <c r="H16" s="114" t="s">
         <v>47</v>
       </c>
-      <c r="I16" s="104"/>
-      <c r="J16" s="104"/>
-      <c r="K16" s="104"/>
-      <c r="L16" s="104"/>
+      <c r="I16" s="114"/>
+      <c r="J16" s="114"/>
+      <c r="K16" s="114"/>
+      <c r="L16" s="114"/>
       <c r="M16" s="20"/>
       <c r="N16" s="20"/>
       <c r="O16" s="20"/>
@@ -2250,26 +2241,26 @@
         <f>B13+7</f>
         <v>43731</v>
       </c>
-      <c r="C23" s="76" t="s">
+      <c r="C23" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="76"/>
-      <c r="E23" s="76"/>
-      <c r="F23" s="76"/>
-      <c r="G23" s="76"/>
-      <c r="H23" s="89" t="s">
+      <c r="D23" s="79"/>
+      <c r="E23" s="79"/>
+      <c r="F23" s="79"/>
+      <c r="G23" s="79"/>
+      <c r="H23" s="91" t="s">
         <v>39</v>
       </c>
-      <c r="I23" s="97"/>
-      <c r="J23" s="97"/>
-      <c r="K23" s="97"/>
-      <c r="L23" s="97"/>
-      <c r="M23" s="97"/>
-      <c r="N23" s="97"/>
-      <c r="O23" s="97"/>
-      <c r="P23" s="97"/>
-      <c r="Q23" s="97"/>
-      <c r="R23" s="98"/>
+      <c r="I23" s="105"/>
+      <c r="J23" s="105"/>
+      <c r="K23" s="105"/>
+      <c r="L23" s="105"/>
+      <c r="M23" s="105"/>
+      <c r="N23" s="105"/>
+      <c r="O23" s="105"/>
+      <c r="P23" s="105"/>
+      <c r="Q23" s="105"/>
+      <c r="R23" s="92"/>
       <c r="S23" s="51"/>
       <c r="T23" s="30" t="s">
         <v>22</v>
@@ -2283,30 +2274,30 @@
         <f t="shared" ref="B24:B29" si="0">B14+7</f>
         <v>43732</v>
       </c>
-      <c r="C24" s="76" t="s">
+      <c r="C24" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="76"/>
-      <c r="E24" s="76"/>
-      <c r="F24" s="76"/>
-      <c r="G24" s="76"/>
-      <c r="H24" s="89" t="s">
+      <c r="D24" s="79"/>
+      <c r="E24" s="79"/>
+      <c r="F24" s="79"/>
+      <c r="G24" s="79"/>
+      <c r="H24" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="I24" s="90"/>
-      <c r="J24" s="73" t="s">
+      <c r="I24" s="115"/>
+      <c r="J24" s="88" t="s">
         <v>48</v>
       </c>
-      <c r="K24" s="74"/>
-      <c r="L24" s="75"/>
-      <c r="M24" s="73" t="s">
+      <c r="K24" s="89"/>
+      <c r="L24" s="90"/>
+      <c r="M24" s="88" t="s">
         <v>56</v>
       </c>
-      <c r="N24" s="75"/>
-      <c r="O24" s="87" t="s">
+      <c r="N24" s="90"/>
+      <c r="O24" s="106" t="s">
         <v>38</v>
       </c>
-      <c r="P24" s="88"/>
+      <c r="P24" s="108"/>
       <c r="Q24" s="20"/>
       <c r="R24" s="20"/>
       <c r="S24" s="51"/>
@@ -2351,20 +2342,20 @@
         <f t="shared" si="0"/>
         <v>43734</v>
       </c>
-      <c r="C26" s="76" t="s">
+      <c r="C26" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="D26" s="76"/>
-      <c r="E26" s="76"/>
-      <c r="F26" s="76"/>
-      <c r="G26" s="76"/>
-      <c r="H26" s="96" t="s">
+      <c r="D26" s="79"/>
+      <c r="E26" s="79"/>
+      <c r="F26" s="79"/>
+      <c r="G26" s="79"/>
+      <c r="H26" s="112" t="s">
         <v>57</v>
       </c>
-      <c r="I26" s="96"/>
-      <c r="J26" s="96"/>
-      <c r="K26" s="96"/>
-      <c r="L26" s="96"/>
+      <c r="I26" s="112"/>
+      <c r="J26" s="112"/>
+      <c r="K26" s="112"/>
+      <c r="L26" s="112"/>
       <c r="M26" s="20"/>
       <c r="N26" s="20"/>
       <c r="O26" s="20"/>
@@ -2546,12 +2537,12 @@
         <f>C22+1</f>
         <v>3</v>
       </c>
-      <c r="D32" s="103" t="s">
+      <c r="D32" s="113" t="s">
         <v>46</v>
       </c>
-      <c r="E32" s="103"/>
-      <c r="F32" s="103"/>
-      <c r="G32" s="103"/>
+      <c r="E32" s="113"/>
+      <c r="F32" s="113"/>
+      <c r="G32" s="113"/>
       <c r="H32" s="15"/>
       <c r="I32" s="15"/>
       <c r="J32" s="15"/>
@@ -2574,24 +2565,24 @@
         <f>B23+7</f>
         <v>43738</v>
       </c>
-      <c r="C33" s="76" t="s">
+      <c r="C33" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="D33" s="76"/>
-      <c r="E33" s="76"/>
-      <c r="F33" s="76"/>
-      <c r="G33" s="76"/>
-      <c r="H33" s="96" t="s">
+      <c r="D33" s="79"/>
+      <c r="E33" s="79"/>
+      <c r="F33" s="79"/>
+      <c r="G33" s="79"/>
+      <c r="H33" s="112" t="s">
         <v>14</v>
       </c>
-      <c r="I33" s="96"/>
-      <c r="J33" s="96"/>
-      <c r="K33" s="96"/>
-      <c r="L33" s="96"/>
-      <c r="M33" s="96"/>
-      <c r="N33" s="96"/>
-      <c r="O33" s="96"/>
-      <c r="P33" s="96"/>
+      <c r="I33" s="112"/>
+      <c r="J33" s="112"/>
+      <c r="K33" s="112"/>
+      <c r="L33" s="112"/>
+      <c r="M33" s="112"/>
+      <c r="N33" s="112"/>
+      <c r="O33" s="112"/>
+      <c r="P33" s="112"/>
       <c r="Q33" s="62"/>
       <c r="R33" s="62"/>
       <c r="S33" s="51"/>
@@ -2607,13 +2598,13 @@
         <f t="shared" ref="B34:B39" si="1">B24+7</f>
         <v>43739</v>
       </c>
-      <c r="C34" s="76" t="s">
+      <c r="C34" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="D34" s="76"/>
-      <c r="E34" s="76"/>
-      <c r="F34" s="76"/>
-      <c r="G34" s="76"/>
+      <c r="D34" s="79"/>
+      <c r="E34" s="79"/>
+      <c r="F34" s="79"/>
+      <c r="G34" s="79"/>
       <c r="H34" s="62"/>
       <c r="I34" s="62"/>
       <c r="J34" s="62"/>
@@ -2667,13 +2658,13 @@
         <f t="shared" si="1"/>
         <v>43741</v>
       </c>
-      <c r="C36" s="76" t="s">
+      <c r="C36" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="D36" s="76"/>
-      <c r="E36" s="76"/>
-      <c r="F36" s="76"/>
-      <c r="G36" s="76"/>
+      <c r="D36" s="79"/>
+      <c r="E36" s="79"/>
+      <c r="F36" s="79"/>
+      <c r="G36" s="79"/>
       <c r="H36" s="63"/>
       <c r="I36" s="63"/>
       <c r="J36" s="63"/>
@@ -2886,24 +2877,24 @@
         <f>B33+7</f>
         <v>43745</v>
       </c>
-      <c r="C43" s="76" t="s">
+      <c r="C43" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="D43" s="76"/>
-      <c r="E43" s="76"/>
-      <c r="F43" s="76"/>
-      <c r="G43" s="76"/>
-      <c r="H43" s="72" t="s">
+      <c r="D43" s="79"/>
+      <c r="E43" s="79"/>
+      <c r="F43" s="79"/>
+      <c r="G43" s="79"/>
+      <c r="H43" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="I43" s="72"/>
-      <c r="J43" s="72"/>
-      <c r="K43" s="72"/>
-      <c r="L43" s="72"/>
-      <c r="M43" s="72"/>
-      <c r="N43" s="72"/>
-      <c r="O43" s="72"/>
-      <c r="P43" s="72"/>
+      <c r="I43" s="77"/>
+      <c r="J43" s="77"/>
+      <c r="K43" s="77"/>
+      <c r="L43" s="77"/>
+      <c r="M43" s="77"/>
+      <c r="N43" s="77"/>
+      <c r="O43" s="77"/>
+      <c r="P43" s="77"/>
       <c r="Q43" s="20"/>
       <c r="R43" s="20"/>
       <c r="S43" s="51"/>
@@ -2919,22 +2910,22 @@
         <f t="shared" ref="B44:B49" si="2">B34+7</f>
         <v>43746</v>
       </c>
-      <c r="C44" s="76" t="s">
+      <c r="C44" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="D44" s="76"/>
-      <c r="E44" s="76"/>
-      <c r="F44" s="76"/>
-      <c r="G44" s="76"/>
-      <c r="H44" s="91" t="s">
+      <c r="D44" s="79"/>
+      <c r="E44" s="79"/>
+      <c r="F44" s="79"/>
+      <c r="G44" s="79"/>
+      <c r="H44" s="116" t="s">
         <v>58</v>
       </c>
-      <c r="I44" s="92"/>
-      <c r="J44" s="92"/>
-      <c r="K44" s="92"/>
-      <c r="L44" s="92"/>
-      <c r="M44" s="92"/>
-      <c r="N44" s="92"/>
+      <c r="I44" s="101"/>
+      <c r="J44" s="101"/>
+      <c r="K44" s="101"/>
+      <c r="L44" s="101"/>
+      <c r="M44" s="101"/>
+      <c r="N44" s="101"/>
       <c r="O44" s="49"/>
       <c r="P44" s="49"/>
       <c r="Q44" s="49"/>
@@ -2957,17 +2948,17 @@
       <c r="E45" s="20"/>
       <c r="F45" s="20"/>
       <c r="G45" s="20"/>
-      <c r="H45" s="100" t="s">
+      <c r="H45" s="109" t="s">
         <v>58</v>
       </c>
-      <c r="I45" s="101"/>
-      <c r="J45" s="101"/>
-      <c r="K45" s="101"/>
-      <c r="L45" s="101"/>
-      <c r="M45" s="101"/>
-      <c r="N45" s="101"/>
-      <c r="O45" s="101"/>
-      <c r="P45" s="102"/>
+      <c r="I45" s="110"/>
+      <c r="J45" s="110"/>
+      <c r="K45" s="110"/>
+      <c r="L45" s="110"/>
+      <c r="M45" s="110"/>
+      <c r="N45" s="110"/>
+      <c r="O45" s="110"/>
+      <c r="P45" s="111"/>
       <c r="Q45" s="49"/>
       <c r="R45" s="49"/>
       <c r="S45" s="51"/>
@@ -2983,24 +2974,24 @@
         <f t="shared" si="2"/>
         <v>43748</v>
       </c>
-      <c r="C46" s="76" t="s">
+      <c r="C46" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="D46" s="76"/>
-      <c r="E46" s="76"/>
-      <c r="F46" s="76"/>
-      <c r="G46" s="76"/>
-      <c r="H46" s="69" t="s">
+      <c r="D46" s="79"/>
+      <c r="E46" s="79"/>
+      <c r="F46" s="79"/>
+      <c r="G46" s="79"/>
+      <c r="H46" s="85" t="s">
         <v>62</v>
       </c>
-      <c r="I46" s="70"/>
-      <c r="J46" s="70"/>
-      <c r="K46" s="70"/>
-      <c r="L46" s="70"/>
-      <c r="M46" s="70"/>
-      <c r="N46" s="70"/>
-      <c r="O46" s="70"/>
-      <c r="P46" s="71"/>
+      <c r="I46" s="86"/>
+      <c r="J46" s="86"/>
+      <c r="K46" s="86"/>
+      <c r="L46" s="86"/>
+      <c r="M46" s="86"/>
+      <c r="N46" s="86"/>
+      <c r="O46" s="86"/>
+      <c r="P46" s="87"/>
       <c r="Q46" s="20"/>
       <c r="R46" s="20"/>
       <c r="S46" s="51"/>
@@ -3179,11 +3170,11 @@
         <v>5</v>
       </c>
       <c r="G52" s="15"/>
-      <c r="H52" s="93" t="s">
+      <c r="H52" s="117" t="s">
         <v>67</v>
       </c>
-      <c r="I52" s="93"/>
-      <c r="J52" s="93"/>
+      <c r="I52" s="117"/>
+      <c r="J52" s="117"/>
       <c r="K52" s="19"/>
       <c r="L52" s="19"/>
       <c r="M52" s="19"/>
@@ -3203,23 +3194,23 @@
         <f>B43+7</f>
         <v>43752</v>
       </c>
-      <c r="C53" s="76" t="s">
+      <c r="C53" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="D53" s="76"/>
-      <c r="E53" s="76"/>
-      <c r="F53" s="76"/>
-      <c r="G53" s="76"/>
+      <c r="D53" s="79"/>
+      <c r="E53" s="79"/>
+      <c r="F53" s="79"/>
+      <c r="G53" s="79"/>
       <c r="H53" s="65" t="s">
         <v>68</v>
       </c>
-      <c r="I53" s="73" t="s">
+      <c r="I53" s="88" t="s">
         <v>14</v>
       </c>
-      <c r="J53" s="74"/>
-      <c r="K53" s="74"/>
-      <c r="L53" s="74"/>
-      <c r="M53" s="74"/>
+      <c r="J53" s="89"/>
+      <c r="K53" s="89"/>
+      <c r="L53" s="89"/>
+      <c r="M53" s="89"/>
       <c r="N53" s="49"/>
       <c r="O53" s="49"/>
       <c r="P53" s="49"/>
@@ -3238,28 +3229,28 @@
         <f t="shared" ref="B54:B59" si="3">B44+7</f>
         <v>43753</v>
       </c>
-      <c r="C54" s="76" t="s">
+      <c r="C54" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="D54" s="76"/>
-      <c r="E54" s="76"/>
-      <c r="F54" s="76"/>
-      <c r="G54" s="76"/>
-      <c r="H54" s="105" t="s">
+      <c r="D54" s="79"/>
+      <c r="E54" s="79"/>
+      <c r="F54" s="79"/>
+      <c r="G54" s="79"/>
+      <c r="H54" s="93" t="s">
         <v>63</v>
       </c>
-      <c r="I54" s="106"/>
-      <c r="J54" s="106"/>
-      <c r="K54" s="106"/>
-      <c r="L54" s="106"/>
-      <c r="M54" s="106"/>
-      <c r="N54" s="106"/>
-      <c r="O54" s="106"/>
-      <c r="P54" s="106"/>
-      <c r="Q54" s="89" t="s">
+      <c r="I54" s="94"/>
+      <c r="J54" s="94"/>
+      <c r="K54" s="94"/>
+      <c r="L54" s="94"/>
+      <c r="M54" s="94"/>
+      <c r="N54" s="94"/>
+      <c r="O54" s="94"/>
+      <c r="P54" s="94"/>
+      <c r="Q54" s="91" t="s">
         <v>70</v>
       </c>
-      <c r="R54" s="98"/>
+      <c r="R54" s="92"/>
       <c r="S54" s="51"/>
       <c r="T54" s="53" t="s">
         <v>19</v>
@@ -3277,18 +3268,18 @@
       <c r="D55" s="49"/>
       <c r="E55" s="49"/>
       <c r="F55" s="49"/>
-      <c r="G55" s="76" t="s">
+      <c r="G55" s="79" t="s">
         <v>64</v>
       </c>
-      <c r="H55" s="76"/>
-      <c r="I55" s="95" t="s">
+      <c r="H55" s="79"/>
+      <c r="I55" s="118" t="s">
         <v>14</v>
       </c>
-      <c r="J55" s="74"/>
-      <c r="K55" s="74"/>
-      <c r="L55" s="74"/>
-      <c r="M55" s="74"/>
-      <c r="N55" s="74"/>
+      <c r="J55" s="89"/>
+      <c r="K55" s="89"/>
+      <c r="L55" s="89"/>
+      <c r="M55" s="89"/>
+      <c r="N55" s="89"/>
       <c r="O55" s="49"/>
       <c r="P55" s="49"/>
       <c r="Q55" s="49"/>
@@ -3306,21 +3297,21 @@
         <f t="shared" si="3"/>
         <v>43755</v>
       </c>
-      <c r="C56" s="76" t="s">
+      <c r="C56" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="D56" s="76"/>
-      <c r="E56" s="76"/>
-      <c r="F56" s="76"/>
-      <c r="G56" s="76"/>
-      <c r="H56" s="112" t="s">
+      <c r="D56" s="79"/>
+      <c r="E56" s="79"/>
+      <c r="F56" s="79"/>
+      <c r="G56" s="79"/>
+      <c r="H56" s="100" t="s">
         <v>71</v>
       </c>
-      <c r="I56" s="92"/>
-      <c r="J56" s="92"/>
-      <c r="K56" s="92"/>
-      <c r="L56" s="92"/>
-      <c r="M56" s="92"/>
+      <c r="I56" s="101"/>
+      <c r="J56" s="101"/>
+      <c r="K56" s="101"/>
+      <c r="L56" s="101"/>
+      <c r="M56" s="101"/>
       <c r="N56" s="49"/>
       <c r="O56" s="49"/>
       <c r="P56" s="49"/>
@@ -3352,11 +3343,11 @@
       <c r="M57" s="49"/>
       <c r="N57" s="49"/>
       <c r="O57" s="49"/>
-      <c r="P57" s="69" t="s">
+      <c r="P57" s="85" t="s">
         <v>42</v>
       </c>
-      <c r="Q57" s="70"/>
-      <c r="R57" s="71"/>
+      <c r="Q57" s="86"/>
+      <c r="R57" s="87"/>
       <c r="S57" s="51"/>
       <c r="T57" s="51"/>
     </row>
@@ -3370,31 +3361,31 @@
       </c>
       <c r="C58" s="50"/>
       <c r="D58" s="49"/>
-      <c r="E58" s="110" t="s">
+      <c r="E58" s="98" t="s">
         <v>42</v>
       </c>
-      <c r="F58" s="70"/>
-      <c r="G58" s="111"/>
-      <c r="H58" s="76" t="s">
+      <c r="F58" s="86"/>
+      <c r="G58" s="99"/>
+      <c r="H58" s="79" t="s">
         <v>74</v>
       </c>
-      <c r="I58" s="76"/>
-      <c r="J58" s="73" t="s">
+      <c r="I58" s="79"/>
+      <c r="J58" s="88" t="s">
         <v>42</v>
       </c>
-      <c r="K58" s="74"/>
-      <c r="L58" s="74"/>
-      <c r="M58" s="74"/>
-      <c r="N58" s="74"/>
-      <c r="O58" s="74"/>
-      <c r="P58" s="75"/>
+      <c r="K58" s="89"/>
+      <c r="L58" s="89"/>
+      <c r="M58" s="89"/>
+      <c r="N58" s="89"/>
+      <c r="O58" s="89"/>
+      <c r="P58" s="90"/>
       <c r="Q58" s="20"/>
       <c r="R58" s="20"/>
       <c r="S58" s="51"/>
-      <c r="T58" s="114" t="s">
+      <c r="T58" s="69" t="s">
         <v>72</v>
       </c>
-      <c r="U58" s="114"/>
+      <c r="U58" s="69"/>
     </row>
     <row r="59" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
@@ -3421,8 +3412,8 @@
       <c r="Q59" s="20"/>
       <c r="R59" s="20"/>
       <c r="S59" s="51"/>
-      <c r="T59" s="114"/>
-      <c r="U59" s="114"/>
+      <c r="T59" s="69"/>
+      <c r="U59" s="69"/>
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B60"/>
@@ -3443,8 +3434,8 @@
       <c r="Q60"/>
       <c r="R60"/>
       <c r="S60"/>
-      <c r="T60" s="114"/>
-      <c r="U60" s="114"/>
+      <c r="T60" s="69"/>
+      <c r="U60" s="69"/>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
@@ -3518,11 +3509,11 @@
       <c r="E62" s="15"/>
       <c r="F62" s="15"/>
       <c r="G62" s="15"/>
-      <c r="H62" s="93" t="s">
+      <c r="H62" s="117" t="s">
         <v>73</v>
       </c>
-      <c r="I62" s="93"/>
-      <c r="J62" s="93"/>
+      <c r="I62" s="117"/>
+      <c r="J62" s="117"/>
       <c r="K62" s="19"/>
       <c r="L62" s="19"/>
       <c r="M62" s="19"/>
@@ -3542,22 +3533,22 @@
         <f>B53+7</f>
         <v>43759</v>
       </c>
-      <c r="C63" s="76" t="s">
+      <c r="C63" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="D63" s="76"/>
-      <c r="E63" s="76"/>
-      <c r="F63" s="76"/>
-      <c r="G63" s="76"/>
+      <c r="D63" s="79"/>
+      <c r="E63" s="79"/>
+      <c r="F63" s="79"/>
+      <c r="G63" s="79"/>
       <c r="H63" s="67" t="s">
         <v>68</v>
       </c>
-      <c r="I63" s="73" t="s">
+      <c r="I63" s="88" t="s">
         <v>76</v>
       </c>
-      <c r="J63" s="74"/>
-      <c r="K63" s="74"/>
-      <c r="L63" s="74"/>
+      <c r="J63" s="89"/>
+      <c r="K63" s="89"/>
+      <c r="L63" s="89"/>
       <c r="M63" s="49"/>
       <c r="N63" s="49"/>
       <c r="O63" s="49"/>
@@ -3577,22 +3568,22 @@
         <f t="shared" ref="B64:B69" si="4">B54+7</f>
         <v>43760</v>
       </c>
-      <c r="C64" s="76" t="s">
+      <c r="C64" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="D64" s="76"/>
-      <c r="E64" s="76"/>
-      <c r="F64" s="76"/>
-      <c r="G64" s="76"/>
-      <c r="H64" s="110" t="s">
+      <c r="D64" s="79"/>
+      <c r="E64" s="79"/>
+      <c r="F64" s="79"/>
+      <c r="G64" s="79"/>
+      <c r="H64" s="98" t="s">
         <v>85</v>
       </c>
-      <c r="I64" s="70"/>
-      <c r="J64" s="70"/>
-      <c r="K64" s="70"/>
-      <c r="L64" s="70"/>
-      <c r="M64" s="70"/>
-      <c r="N64" s="70"/>
+      <c r="I64" s="86"/>
+      <c r="J64" s="86"/>
+      <c r="K64" s="86"/>
+      <c r="L64" s="86"/>
+      <c r="M64" s="86"/>
+      <c r="N64" s="86"/>
       <c r="O64" s="49"/>
       <c r="P64" s="49"/>
       <c r="Q64" s="49"/>
@@ -3641,25 +3632,25 @@
         <f t="shared" si="4"/>
         <v>43762</v>
       </c>
-      <c r="C66" s="76" t="s">
+      <c r="C66" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="D66" s="76"/>
-      <c r="E66" s="76"/>
-      <c r="F66" s="76"/>
-      <c r="G66" s="76"/>
-      <c r="H66" s="122" t="s">
+      <c r="D66" s="79"/>
+      <c r="E66" s="79"/>
+      <c r="F66" s="79"/>
+      <c r="G66" s="79"/>
+      <c r="H66" s="102" t="s">
         <v>77</v>
       </c>
-      <c r="I66" s="123"/>
-      <c r="J66" s="123"/>
-      <c r="K66" s="123"/>
-      <c r="L66" s="123"/>
-      <c r="M66" s="123"/>
-      <c r="N66" s="123"/>
-      <c r="O66" s="123"/>
-      <c r="P66" s="123"/>
-      <c r="Q66" s="124"/>
+      <c r="I66" s="103"/>
+      <c r="J66" s="103"/>
+      <c r="K66" s="103"/>
+      <c r="L66" s="103"/>
+      <c r="M66" s="103"/>
+      <c r="N66" s="103"/>
+      <c r="O66" s="103"/>
+      <c r="P66" s="103"/>
+      <c r="Q66" s="104"/>
       <c r="R66" s="20"/>
       <c r="S66" s="51"/>
       <c r="T66" s="18" t="s">
@@ -3674,26 +3665,26 @@
         <f t="shared" si="4"/>
         <v>43763</v>
       </c>
-      <c r="C67" s="73" t="s">
+      <c r="C67" s="88" t="s">
         <v>77</v>
       </c>
-      <c r="D67" s="74"/>
-      <c r="E67" s="74"/>
-      <c r="F67" s="74"/>
-      <c r="G67" s="74"/>
-      <c r="H67" s="74"/>
-      <c r="I67" s="74"/>
-      <c r="J67" s="75"/>
+      <c r="D67" s="89"/>
+      <c r="E67" s="89"/>
+      <c r="F67" s="89"/>
+      <c r="G67" s="89"/>
+      <c r="H67" s="89"/>
+      <c r="I67" s="89"/>
+      <c r="J67" s="90"/>
       <c r="K67" s="49"/>
-      <c r="L67" s="74" t="s">
+      <c r="L67" s="89" t="s">
         <v>42</v>
       </c>
-      <c r="M67" s="74"/>
-      <c r="N67" s="74"/>
-      <c r="O67" s="74"/>
-      <c r="P67" s="74"/>
-      <c r="Q67" s="74"/>
-      <c r="R67" s="75"/>
+      <c r="M67" s="89"/>
+      <c r="N67" s="89"/>
+      <c r="O67" s="89"/>
+      <c r="P67" s="89"/>
+      <c r="Q67" s="89"/>
+      <c r="R67" s="90"/>
       <c r="S67" s="51"/>
       <c r="T67" s="51"/>
     </row>
@@ -3732,24 +3723,24 @@
         <f t="shared" si="4"/>
         <v>43765</v>
       </c>
-      <c r="C69" s="76" t="s">
+      <c r="C69" s="79" t="s">
         <v>81</v>
       </c>
-      <c r="D69" s="76"/>
-      <c r="E69" s="76"/>
-      <c r="F69" s="76"/>
-      <c r="G69" s="76"/>
-      <c r="H69" s="76"/>
-      <c r="I69" s="76"/>
-      <c r="J69" s="76"/>
-      <c r="K69" s="76"/>
-      <c r="L69" s="76"/>
-      <c r="M69" s="76"/>
-      <c r="N69" s="76"/>
-      <c r="O69" s="76"/>
-      <c r="P69" s="76"/>
-      <c r="Q69" s="76"/>
-      <c r="R69" s="76"/>
+      <c r="D69" s="79"/>
+      <c r="E69" s="79"/>
+      <c r="F69" s="79"/>
+      <c r="G69" s="79"/>
+      <c r="H69" s="79"/>
+      <c r="I69" s="79"/>
+      <c r="J69" s="79"/>
+      <c r="K69" s="79"/>
+      <c r="L69" s="79"/>
+      <c r="M69" s="79"/>
+      <c r="N69" s="79"/>
+      <c r="O69" s="79"/>
+      <c r="P69" s="79"/>
+      <c r="Q69" s="79"/>
+      <c r="R69" s="79"/>
       <c r="S69" s="51"/>
       <c r="T69" s="51"/>
     </row>
@@ -3842,27 +3833,27 @@
         <f>C62+1</f>
         <v>7</v>
       </c>
-      <c r="D72" s="94" t="s">
+      <c r="D72" s="80" t="s">
         <v>42</v>
       </c>
-      <c r="E72" s="94"/>
-      <c r="F72" s="94"/>
+      <c r="E72" s="80"/>
+      <c r="F72" s="80"/>
       <c r="G72" s="15"/>
-      <c r="H72" s="85" t="s">
+      <c r="H72" s="120" t="s">
         <v>82</v>
       </c>
-      <c r="I72" s="85"/>
-      <c r="J72" s="85"/>
-      <c r="K72" s="85"/>
+      <c r="I72" s="120"/>
+      <c r="J72" s="120"/>
+      <c r="K72" s="120"/>
       <c r="L72" s="19"/>
-      <c r="M72" s="84" t="s">
+      <c r="M72" s="119" t="s">
         <v>75</v>
       </c>
-      <c r="N72" s="84"/>
-      <c r="O72" s="84"/>
-      <c r="P72" s="84"/>
-      <c r="Q72" s="84"/>
-      <c r="R72" s="84"/>
+      <c r="N72" s="119"/>
+      <c r="O72" s="119"/>
+      <c r="P72" s="119"/>
+      <c r="Q72" s="119"/>
+      <c r="R72" s="119"/>
       <c r="S72" s="51"/>
       <c r="T72" s="51"/>
     </row>
@@ -3876,23 +3867,23 @@
       </c>
       <c r="C73" s="32"/>
       <c r="D73" s="20"/>
-      <c r="E73" s="72" t="s">
+      <c r="E73" s="77" t="s">
         <v>66</v>
       </c>
-      <c r="F73" s="72"/>
-      <c r="G73" s="72"/>
-      <c r="H73" s="72"/>
-      <c r="I73" s="72"/>
-      <c r="J73" s="72"/>
+      <c r="F73" s="77"/>
+      <c r="G73" s="77"/>
+      <c r="H73" s="77"/>
+      <c r="I73" s="77"/>
+      <c r="J73" s="77"/>
       <c r="K73" s="49"/>
-      <c r="L73" s="73" t="s">
+      <c r="L73" s="88" t="s">
         <v>66</v>
       </c>
-      <c r="M73" s="74"/>
-      <c r="N73" s="74"/>
-      <c r="O73" s="74"/>
-      <c r="P73" s="74"/>
-      <c r="Q73" s="75"/>
+      <c r="M73" s="89"/>
+      <c r="N73" s="89"/>
+      <c r="O73" s="89"/>
+      <c r="P73" s="89"/>
+      <c r="Q73" s="90"/>
       <c r="R73" s="49"/>
       <c r="S73" s="51"/>
       <c r="T73" s="30" t="s">
@@ -3907,27 +3898,27 @@
         <f t="shared" ref="B74:B79" si="5">B64+7</f>
         <v>43767</v>
       </c>
-      <c r="C74" s="73" t="s">
+      <c r="C74" s="88" t="s">
         <v>78</v>
       </c>
-      <c r="D74" s="75"/>
-      <c r="E74" s="72" t="s">
+      <c r="D74" s="90"/>
+      <c r="E74" s="77" t="s">
         <v>66</v>
       </c>
-      <c r="F74" s="72"/>
-      <c r="G74" s="72"/>
-      <c r="H74" s="72"/>
-      <c r="I74" s="72"/>
-      <c r="J74" s="72"/>
+      <c r="F74" s="77"/>
+      <c r="G74" s="77"/>
+      <c r="H74" s="77"/>
+      <c r="I74" s="77"/>
+      <c r="J74" s="77"/>
       <c r="K74" s="49"/>
-      <c r="L74" s="73" t="s">
+      <c r="L74" s="88" t="s">
         <v>66</v>
       </c>
-      <c r="M74" s="74"/>
-      <c r="N74" s="74"/>
-      <c r="O74" s="74"/>
-      <c r="P74" s="74"/>
-      <c r="Q74" s="75"/>
+      <c r="M74" s="89"/>
+      <c r="N74" s="89"/>
+      <c r="O74" s="89"/>
+      <c r="P74" s="89"/>
+      <c r="Q74" s="90"/>
       <c r="R74" s="20"/>
       <c r="S74" s="51"/>
       <c r="T74" s="53" t="s">
@@ -3944,23 +3935,23 @@
       </c>
       <c r="C75" s="32"/>
       <c r="D75" s="20"/>
-      <c r="E75" s="72" t="s">
+      <c r="E75" s="77" t="s">
         <v>66</v>
       </c>
-      <c r="F75" s="72"/>
-      <c r="G75" s="72"/>
-      <c r="H75" s="72"/>
-      <c r="I75" s="72"/>
-      <c r="J75" s="72"/>
+      <c r="F75" s="77"/>
+      <c r="G75" s="77"/>
+      <c r="H75" s="77"/>
+      <c r="I75" s="77"/>
+      <c r="J75" s="77"/>
       <c r="K75" s="49"/>
-      <c r="L75" s="73" t="s">
+      <c r="L75" s="88" t="s">
         <v>66</v>
       </c>
-      <c r="M75" s="74"/>
-      <c r="N75" s="74"/>
-      <c r="O75" s="74"/>
-      <c r="P75" s="74"/>
-      <c r="Q75" s="75"/>
+      <c r="M75" s="89"/>
+      <c r="N75" s="89"/>
+      <c r="O75" s="89"/>
+      <c r="P75" s="89"/>
+      <c r="Q75" s="90"/>
       <c r="R75" s="49"/>
       <c r="S75" s="51"/>
       <c r="T75" s="52" t="s">
@@ -3975,24 +3966,24 @@
         <f t="shared" si="5"/>
         <v>43769</v>
       </c>
-      <c r="C76" s="76" t="s">
+      <c r="C76" s="79" t="s">
         <v>79</v>
       </c>
-      <c r="D76" s="76"/>
-      <c r="E76" s="76"/>
-      <c r="F76" s="76"/>
-      <c r="G76" s="76"/>
-      <c r="H76" s="76"/>
-      <c r="I76" s="76"/>
-      <c r="J76" s="76"/>
-      <c r="K76" s="76"/>
-      <c r="L76" s="76"/>
-      <c r="M76" s="76"/>
-      <c r="N76" s="76"/>
-      <c r="O76" s="76"/>
-      <c r="P76" s="76"/>
-      <c r="Q76" s="76"/>
-      <c r="R76" s="76"/>
+      <c r="D76" s="79"/>
+      <c r="E76" s="79"/>
+      <c r="F76" s="79"/>
+      <c r="G76" s="79"/>
+      <c r="H76" s="79"/>
+      <c r="I76" s="79"/>
+      <c r="J76" s="79"/>
+      <c r="K76" s="79"/>
+      <c r="L76" s="79"/>
+      <c r="M76" s="79"/>
+      <c r="N76" s="79"/>
+      <c r="O76" s="79"/>
+      <c r="P76" s="79"/>
+      <c r="Q76" s="79"/>
+      <c r="R76" s="79"/>
       <c r="S76" s="51"/>
       <c r="T76" s="18" t="s">
         <v>21</v>
@@ -4008,23 +3999,23 @@
       </c>
       <c r="C77" s="32"/>
       <c r="D77" s="20"/>
-      <c r="E77" s="96" t="s">
+      <c r="E77" s="112" t="s">
         <v>66</v>
       </c>
-      <c r="F77" s="96"/>
-      <c r="G77" s="96"/>
-      <c r="H77" s="96"/>
-      <c r="I77" s="96"/>
-      <c r="J77" s="96"/>
+      <c r="F77" s="112"/>
+      <c r="G77" s="112"/>
+      <c r="H77" s="112"/>
+      <c r="I77" s="112"/>
+      <c r="J77" s="112"/>
       <c r="K77" s="49"/>
-      <c r="L77" s="107" t="s">
+      <c r="L77" s="95" t="s">
         <v>66</v>
       </c>
-      <c r="M77" s="108"/>
-      <c r="N77" s="108"/>
-      <c r="O77" s="108"/>
-      <c r="P77" s="108"/>
-      <c r="Q77" s="109"/>
+      <c r="M77" s="96"/>
+      <c r="N77" s="96"/>
+      <c r="O77" s="96"/>
+      <c r="P77" s="96"/>
+      <c r="Q77" s="97"/>
       <c r="R77" s="20"/>
       <c r="S77" s="51"/>
       <c r="T77" s="51"/>
@@ -4039,23 +4030,23 @@
       </c>
       <c r="C78" s="50"/>
       <c r="D78" s="49"/>
-      <c r="E78" s="96" t="s">
+      <c r="E78" s="112" t="s">
         <v>66</v>
       </c>
-      <c r="F78" s="96"/>
-      <c r="G78" s="96"/>
-      <c r="H78" s="96"/>
-      <c r="I78" s="96"/>
-      <c r="J78" s="96"/>
+      <c r="F78" s="112"/>
+      <c r="G78" s="112"/>
+      <c r="H78" s="112"/>
+      <c r="I78" s="112"/>
+      <c r="J78" s="112"/>
       <c r="K78" s="49"/>
-      <c r="L78" s="107" t="s">
+      <c r="L78" s="95" t="s">
         <v>66</v>
       </c>
-      <c r="M78" s="108"/>
-      <c r="N78" s="108"/>
-      <c r="O78" s="108"/>
-      <c r="P78" s="108"/>
-      <c r="Q78" s="109"/>
+      <c r="M78" s="96"/>
+      <c r="N78" s="96"/>
+      <c r="O78" s="96"/>
+      <c r="P78" s="96"/>
+      <c r="Q78" s="97"/>
       <c r="R78" s="49"/>
       <c r="S78" s="51"/>
       <c r="T78" s="51"/>
@@ -4068,24 +4059,24 @@
         <f t="shared" si="5"/>
         <v>43772</v>
       </c>
-      <c r="C79" s="76" t="s">
+      <c r="C79" s="79" t="s">
         <v>81</v>
       </c>
-      <c r="D79" s="76"/>
-      <c r="E79" s="76"/>
-      <c r="F79" s="76"/>
-      <c r="G79" s="76"/>
-      <c r="H79" s="76"/>
-      <c r="I79" s="76"/>
-      <c r="J79" s="76"/>
-      <c r="K79" s="76"/>
-      <c r="L79" s="76"/>
-      <c r="M79" s="76"/>
-      <c r="N79" s="76"/>
-      <c r="O79" s="76"/>
-      <c r="P79" s="76"/>
-      <c r="Q79" s="76"/>
-      <c r="R79" s="76"/>
+      <c r="D79" s="79"/>
+      <c r="E79" s="79"/>
+      <c r="F79" s="79"/>
+      <c r="G79" s="79"/>
+      <c r="H79" s="79"/>
+      <c r="I79" s="79"/>
+      <c r="J79" s="79"/>
+      <c r="K79" s="79"/>
+      <c r="L79" s="79"/>
+      <c r="M79" s="79"/>
+      <c r="N79" s="79"/>
+      <c r="O79" s="79"/>
+      <c r="P79" s="79"/>
+      <c r="Q79" s="79"/>
+      <c r="R79" s="79"/>
       <c r="S79" s="51"/>
       <c r="T79" s="51"/>
     </row>
@@ -4159,11 +4150,11 @@
         <f>C72+1</f>
         <v>8</v>
       </c>
-      <c r="D82" s="94" t="s">
+      <c r="D82" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="E82" s="94"/>
-      <c r="F82" s="94"/>
+      <c r="E82" s="80"/>
+      <c r="F82" s="80"/>
       <c r="G82" s="15"/>
       <c r="H82" s="19"/>
       <c r="I82" s="19"/>
@@ -4188,24 +4179,24 @@
         <f>B73+7</f>
         <v>43773</v>
       </c>
-      <c r="C83" s="76" t="s">
+      <c r="C83" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="D83" s="76"/>
-      <c r="E83" s="76"/>
-      <c r="F83" s="76"/>
-      <c r="G83" s="76"/>
-      <c r="H83" s="69" t="s">
+      <c r="D83" s="79"/>
+      <c r="E83" s="79"/>
+      <c r="F83" s="79"/>
+      <c r="G83" s="79"/>
+      <c r="H83" s="85" t="s">
         <v>66</v>
       </c>
-      <c r="I83" s="70"/>
-      <c r="J83" s="70"/>
-      <c r="K83" s="70"/>
-      <c r="L83" s="70"/>
-      <c r="M83" s="70"/>
-      <c r="N83" s="70"/>
-      <c r="O83" s="70"/>
-      <c r="P83" s="71"/>
+      <c r="I83" s="86"/>
+      <c r="J83" s="86"/>
+      <c r="K83" s="86"/>
+      <c r="L83" s="86"/>
+      <c r="M83" s="86"/>
+      <c r="N83" s="86"/>
+      <c r="O83" s="86"/>
+      <c r="P83" s="87"/>
       <c r="Q83" s="20"/>
       <c r="R83" s="20"/>
       <c r="S83" s="51"/>
@@ -4222,28 +4213,28 @@
         <f t="shared" ref="B84:B89" si="6">B74+7</f>
         <v>43774</v>
       </c>
-      <c r="C84" s="76" t="s">
+      <c r="C84" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="D84" s="76"/>
-      <c r="E84" s="76"/>
-      <c r="F84" s="76"/>
-      <c r="G84" s="76"/>
-      <c r="H84" s="76" t="s">
+      <c r="D84" s="79"/>
+      <c r="E84" s="79"/>
+      <c r="F84" s="79"/>
+      <c r="G84" s="79"/>
+      <c r="H84" s="79" t="s">
         <v>44</v>
       </c>
-      <c r="I84" s="76"/>
-      <c r="J84" s="69" t="s">
+      <c r="I84" s="79"/>
+      <c r="J84" s="85" t="s">
         <v>66</v>
       </c>
-      <c r="K84" s="70"/>
-      <c r="L84" s="70"/>
-      <c r="M84" s="70"/>
-      <c r="N84" s="70"/>
-      <c r="O84" s="70"/>
-      <c r="P84" s="70"/>
-      <c r="Q84" s="70"/>
-      <c r="R84" s="71"/>
+      <c r="K84" s="86"/>
+      <c r="L84" s="86"/>
+      <c r="M84" s="86"/>
+      <c r="N84" s="86"/>
+      <c r="O84" s="86"/>
+      <c r="P84" s="86"/>
+      <c r="Q84" s="86"/>
+      <c r="R84" s="87"/>
       <c r="S84" s="51"/>
       <c r="T84" s="53" t="s">
         <v>19</v>
@@ -4260,17 +4251,17 @@
       </c>
       <c r="C85" s="32"/>
       <c r="D85" s="20"/>
-      <c r="E85" s="69" t="s">
+      <c r="E85" s="85" t="s">
         <v>66</v>
       </c>
-      <c r="F85" s="70"/>
-      <c r="G85" s="70"/>
-      <c r="H85" s="70"/>
-      <c r="I85" s="70"/>
-      <c r="J85" s="70"/>
-      <c r="K85" s="70"/>
-      <c r="L85" s="70"/>
-      <c r="M85" s="71"/>
+      <c r="F85" s="86"/>
+      <c r="G85" s="86"/>
+      <c r="H85" s="86"/>
+      <c r="I85" s="86"/>
+      <c r="J85" s="86"/>
+      <c r="K85" s="86"/>
+      <c r="L85" s="86"/>
+      <c r="M85" s="87"/>
       <c r="N85" s="49"/>
       <c r="O85" s="49"/>
       <c r="P85" s="49"/>
@@ -4290,13 +4281,13 @@
         <f t="shared" si="6"/>
         <v>43776</v>
       </c>
-      <c r="C86" s="86" t="s">
+      <c r="C86" s="81" t="s">
         <v>69</v>
       </c>
-      <c r="D86" s="86"/>
-      <c r="E86" s="86"/>
-      <c r="F86" s="86"/>
-      <c r="G86" s="86"/>
+      <c r="D86" s="81"/>
+      <c r="E86" s="81"/>
+      <c r="F86" s="81"/>
+      <c r="G86" s="81"/>
       <c r="H86" s="49"/>
       <c r="I86" s="49"/>
       <c r="J86" s="49"/>
@@ -4378,24 +4369,24 @@
         <f t="shared" si="6"/>
         <v>43779</v>
       </c>
-      <c r="C89" s="76" t="s">
+      <c r="C89" s="79" t="s">
         <v>81</v>
       </c>
-      <c r="D89" s="76"/>
-      <c r="E89" s="76"/>
-      <c r="F89" s="76"/>
-      <c r="G89" s="76"/>
-      <c r="H89" s="76"/>
-      <c r="I89" s="76"/>
-      <c r="J89" s="76"/>
-      <c r="K89" s="76"/>
-      <c r="L89" s="76"/>
-      <c r="M89" s="76"/>
-      <c r="N89" s="76"/>
-      <c r="O89" s="76"/>
-      <c r="P89" s="76"/>
-      <c r="Q89" s="76"/>
-      <c r="R89" s="76"/>
+      <c r="D89" s="79"/>
+      <c r="E89" s="79"/>
+      <c r="F89" s="79"/>
+      <c r="G89" s="79"/>
+      <c r="H89" s="79"/>
+      <c r="I89" s="79"/>
+      <c r="J89" s="79"/>
+      <c r="K89" s="79"/>
+      <c r="L89" s="79"/>
+      <c r="M89" s="79"/>
+      <c r="N89" s="79"/>
+      <c r="O89" s="79"/>
+      <c r="P89" s="79"/>
+      <c r="Q89" s="79"/>
+      <c r="R89" s="79"/>
       <c r="S89" s="51"/>
       <c r="T89" s="51"/>
       <c r="U89" s="54"/>
@@ -4497,24 +4488,24 @@
         <f>B83+7</f>
         <v>43780</v>
       </c>
-      <c r="C93" s="76" t="s">
+      <c r="C93" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="D93" s="76"/>
-      <c r="E93" s="76"/>
-      <c r="F93" s="76"/>
-      <c r="G93" s="76"/>
-      <c r="H93" s="72" t="s">
+      <c r="D93" s="79"/>
+      <c r="E93" s="79"/>
+      <c r="F93" s="79"/>
+      <c r="G93" s="79"/>
+      <c r="H93" s="77" t="s">
         <v>86</v>
       </c>
-      <c r="I93" s="72"/>
-      <c r="J93" s="72"/>
-      <c r="K93" s="72"/>
-      <c r="L93" s="72"/>
-      <c r="M93" s="72"/>
-      <c r="N93" s="72"/>
-      <c r="O93" s="72"/>
-      <c r="P93" s="72"/>
+      <c r="I93" s="77"/>
+      <c r="J93" s="77"/>
+      <c r="K93" s="77"/>
+      <c r="L93" s="77"/>
+      <c r="M93" s="77"/>
+      <c r="N93" s="77"/>
+      <c r="O93" s="77"/>
+      <c r="P93" s="77"/>
       <c r="Q93" s="20"/>
       <c r="R93" s="20"/>
       <c r="S93" s="51"/>
@@ -4531,24 +4522,24 @@
         <f t="shared" ref="B94:B99" si="7">B84+7</f>
         <v>43781</v>
       </c>
-      <c r="C94" s="76" t="s">
+      <c r="C94" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="D94" s="76"/>
-      <c r="E94" s="76"/>
-      <c r="F94" s="76"/>
-      <c r="G94" s="76"/>
-      <c r="H94" s="72" t="s">
+      <c r="D94" s="79"/>
+      <c r="E94" s="79"/>
+      <c r="F94" s="79"/>
+      <c r="G94" s="79"/>
+      <c r="H94" s="77" t="s">
         <v>86</v>
       </c>
-      <c r="I94" s="72"/>
-      <c r="J94" s="72"/>
-      <c r="K94" s="72"/>
-      <c r="L94" s="72"/>
-      <c r="M94" s="72"/>
-      <c r="N94" s="72"/>
-      <c r="O94" s="72"/>
-      <c r="P94" s="72"/>
+      <c r="I94" s="77"/>
+      <c r="J94" s="77"/>
+      <c r="K94" s="77"/>
+      <c r="L94" s="77"/>
+      <c r="M94" s="77"/>
+      <c r="N94" s="77"/>
+      <c r="O94" s="77"/>
+      <c r="P94" s="77"/>
       <c r="Q94" s="20"/>
       <c r="R94" s="20"/>
       <c r="S94" s="51"/>
@@ -4595,20 +4586,20 @@
         <f t="shared" si="7"/>
         <v>43783</v>
       </c>
-      <c r="C96" s="76" t="s">
+      <c r="C96" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="D96" s="76"/>
-      <c r="E96" s="76"/>
-      <c r="F96" s="76"/>
-      <c r="G96" s="76"/>
-      <c r="H96" s="73" t="s">
+      <c r="D96" s="79"/>
+      <c r="E96" s="79"/>
+      <c r="F96" s="79"/>
+      <c r="G96" s="79"/>
+      <c r="H96" s="88" t="s">
         <v>86</v>
       </c>
-      <c r="I96" s="74"/>
-      <c r="J96" s="74"/>
-      <c r="K96" s="74"/>
-      <c r="L96" s="75"/>
+      <c r="I96" s="89"/>
+      <c r="J96" s="89"/>
+      <c r="K96" s="89"/>
+      <c r="L96" s="90"/>
       <c r="M96" s="20"/>
       <c r="N96" s="20"/>
       <c r="O96" s="20"/>
@@ -4685,24 +4676,24 @@
         <f t="shared" si="7"/>
         <v>43786</v>
       </c>
-      <c r="C99" s="76" t="s">
+      <c r="C99" s="79" t="s">
         <v>81</v>
       </c>
-      <c r="D99" s="76"/>
-      <c r="E99" s="76"/>
-      <c r="F99" s="76"/>
-      <c r="G99" s="76"/>
-      <c r="H99" s="76"/>
-      <c r="I99" s="76"/>
-      <c r="J99" s="76"/>
-      <c r="K99" s="76"/>
-      <c r="L99" s="76"/>
-      <c r="M99" s="76"/>
-      <c r="N99" s="76"/>
-      <c r="O99" s="76"/>
-      <c r="P99" s="76"/>
-      <c r="Q99" s="76"/>
-      <c r="R99" s="76"/>
+      <c r="D99" s="79"/>
+      <c r="E99" s="79"/>
+      <c r="F99" s="79"/>
+      <c r="G99" s="79"/>
+      <c r="H99" s="79"/>
+      <c r="I99" s="79"/>
+      <c r="J99" s="79"/>
+      <c r="K99" s="79"/>
+      <c r="L99" s="79"/>
+      <c r="M99" s="79"/>
+      <c r="N99" s="79"/>
+      <c r="O99" s="79"/>
+      <c r="P99" s="79"/>
+      <c r="Q99" s="79"/>
+      <c r="R99" s="79"/>
       <c r="S99" s="51"/>
       <c r="T99" s="51"/>
       <c r="U99" s="54"/>
@@ -4804,24 +4795,24 @@
         <f>B93+7</f>
         <v>43787</v>
       </c>
-      <c r="C103" s="76" t="s">
+      <c r="C103" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="D103" s="76"/>
-      <c r="E103" s="76"/>
-      <c r="F103" s="76"/>
-      <c r="G103" s="76"/>
-      <c r="H103" s="72" t="s">
+      <c r="D103" s="79"/>
+      <c r="E103" s="79"/>
+      <c r="F103" s="79"/>
+      <c r="G103" s="79"/>
+      <c r="H103" s="77" t="s">
         <v>86</v>
       </c>
-      <c r="I103" s="72"/>
-      <c r="J103" s="72"/>
-      <c r="K103" s="72"/>
-      <c r="L103" s="72"/>
-      <c r="M103" s="72"/>
-      <c r="N103" s="72"/>
-      <c r="O103" s="72"/>
-      <c r="P103" s="72"/>
+      <c r="I103" s="77"/>
+      <c r="J103" s="77"/>
+      <c r="K103" s="77"/>
+      <c r="L103" s="77"/>
+      <c r="M103" s="77"/>
+      <c r="N103" s="77"/>
+      <c r="O103" s="77"/>
+      <c r="P103" s="77"/>
       <c r="Q103" s="20"/>
       <c r="R103" s="20"/>
       <c r="S103" s="51"/>
@@ -4838,24 +4829,24 @@
         <f t="shared" ref="B104:B109" si="8">B94+7</f>
         <v>43788</v>
       </c>
-      <c r="C104" s="76" t="s">
+      <c r="C104" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="D104" s="76"/>
-      <c r="E104" s="76"/>
-      <c r="F104" s="76"/>
-      <c r="G104" s="76"/>
-      <c r="H104" s="72" t="s">
+      <c r="D104" s="79"/>
+      <c r="E104" s="79"/>
+      <c r="F104" s="79"/>
+      <c r="G104" s="79"/>
+      <c r="H104" s="77" t="s">
         <v>86</v>
       </c>
-      <c r="I104" s="72"/>
-      <c r="J104" s="72"/>
-      <c r="K104" s="72"/>
-      <c r="L104" s="72"/>
-      <c r="M104" s="72"/>
-      <c r="N104" s="72"/>
-      <c r="O104" s="72"/>
-      <c r="P104" s="72"/>
+      <c r="I104" s="77"/>
+      <c r="J104" s="77"/>
+      <c r="K104" s="77"/>
+      <c r="L104" s="77"/>
+      <c r="M104" s="77"/>
+      <c r="N104" s="77"/>
+      <c r="O104" s="77"/>
+      <c r="P104" s="77"/>
       <c r="Q104" s="20"/>
       <c r="R104" s="20"/>
       <c r="S104" s="51"/>
@@ -4864,7 +4855,7 @@
       </c>
       <c r="U104" s="54"/>
     </row>
-    <row r="105" spans="1:21" s="27" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:21" s="27" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
         <v>2</v>
       </c>
@@ -4872,19 +4863,19 @@
         <f t="shared" si="8"/>
         <v>43789</v>
       </c>
-      <c r="C105" s="119" t="s">
+      <c r="C105" s="82" t="s">
         <v>86</v>
       </c>
-      <c r="D105" s="120"/>
-      <c r="E105" s="120"/>
-      <c r="F105" s="120"/>
-      <c r="G105" s="120"/>
-      <c r="H105" s="120"/>
-      <c r="I105" s="120"/>
-      <c r="J105" s="120"/>
-      <c r="K105" s="120"/>
-      <c r="L105" s="120"/>
-      <c r="M105" s="121"/>
+      <c r="D105" s="83"/>
+      <c r="E105" s="83"/>
+      <c r="F105" s="83"/>
+      <c r="G105" s="83"/>
+      <c r="H105" s="83"/>
+      <c r="I105" s="83"/>
+      <c r="J105" s="83"/>
+      <c r="K105" s="83"/>
+      <c r="L105" s="83"/>
+      <c r="M105" s="84"/>
       <c r="N105" s="49"/>
       <c r="O105" s="49"/>
       <c r="P105" s="49"/>
@@ -4896,7 +4887,7 @@
       </c>
       <c r="U105" s="54"/>
     </row>
-    <row r="106" spans="1:21" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:21" s="27" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="s">
         <v>3</v>
       </c>
@@ -4904,24 +4895,24 @@
         <f t="shared" si="8"/>
         <v>43790</v>
       </c>
-      <c r="C106" s="76" t="s">
+      <c r="C106" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="D106" s="76"/>
-      <c r="E106" s="76"/>
-      <c r="F106" s="76"/>
-      <c r="G106" s="76"/>
-      <c r="H106" s="78" t="s">
-        <v>87</v>
-      </c>
-      <c r="I106" s="79"/>
-      <c r="J106" s="79"/>
-      <c r="K106" s="79"/>
-      <c r="L106" s="79"/>
-      <c r="M106" s="79"/>
-      <c r="N106" s="79"/>
-      <c r="O106" s="79"/>
-      <c r="P106" s="115"/>
+      <c r="D106" s="79"/>
+      <c r="E106" s="79"/>
+      <c r="F106" s="79"/>
+      <c r="G106" s="79"/>
+      <c r="H106" s="77" t="s">
+        <v>86</v>
+      </c>
+      <c r="I106" s="77"/>
+      <c r="J106" s="77"/>
+      <c r="K106" s="77"/>
+      <c r="L106" s="77"/>
+      <c r="M106" s="77"/>
+      <c r="N106" s="77"/>
+      <c r="O106" s="77"/>
+      <c r="P106" s="77"/>
       <c r="Q106" s="20"/>
       <c r="R106" s="20"/>
       <c r="S106" s="51"/>
@@ -4930,7 +4921,7 @@
       </c>
       <c r="U106" s="54"/>
     </row>
-    <row r="107" spans="1:21" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:21" s="27" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
         <v>4</v>
       </c>
@@ -4939,18 +4930,18 @@
         <v>43791</v>
       </c>
       <c r="C107" s="125" t="s">
-        <v>87</v>
-      </c>
-      <c r="D107" s="126"/>
-      <c r="E107" s="126"/>
-      <c r="F107" s="126"/>
-      <c r="G107" s="126"/>
-      <c r="H107" s="126"/>
-      <c r="I107" s="126"/>
-      <c r="J107" s="126"/>
-      <c r="K107" s="126"/>
-      <c r="L107" s="126"/>
-      <c r="M107" s="127"/>
+        <v>86</v>
+      </c>
+      <c r="D107" s="110"/>
+      <c r="E107" s="110"/>
+      <c r="F107" s="110"/>
+      <c r="G107" s="110"/>
+      <c r="H107" s="110"/>
+      <c r="I107" s="110"/>
+      <c r="J107" s="110"/>
+      <c r="K107" s="110"/>
+      <c r="L107" s="110"/>
+      <c r="M107" s="111"/>
       <c r="N107" s="20"/>
       <c r="O107" s="20"/>
       <c r="P107" s="20"/>
@@ -4996,24 +4987,24 @@
         <f t="shared" si="8"/>
         <v>43793</v>
       </c>
-      <c r="C109" s="76" t="s">
+      <c r="C109" s="79" t="s">
         <v>81</v>
       </c>
-      <c r="D109" s="76"/>
-      <c r="E109" s="76"/>
-      <c r="F109" s="76"/>
-      <c r="G109" s="76"/>
-      <c r="H109" s="76"/>
-      <c r="I109" s="76"/>
-      <c r="J109" s="76"/>
-      <c r="K109" s="76"/>
-      <c r="L109" s="76"/>
-      <c r="M109" s="76"/>
-      <c r="N109" s="76"/>
-      <c r="O109" s="76"/>
-      <c r="P109" s="76"/>
-      <c r="Q109" s="76"/>
-      <c r="R109" s="76"/>
+      <c r="D109" s="79"/>
+      <c r="E109" s="79"/>
+      <c r="F109" s="79"/>
+      <c r="G109" s="79"/>
+      <c r="H109" s="79"/>
+      <c r="I109" s="79"/>
+      <c r="J109" s="79"/>
+      <c r="K109" s="79"/>
+      <c r="L109" s="79"/>
+      <c r="M109" s="79"/>
+      <c r="N109" s="79"/>
+      <c r="O109" s="79"/>
+      <c r="P109" s="79"/>
+      <c r="Q109" s="79"/>
+      <c r="R109" s="79"/>
       <c r="S109" s="51"/>
       <c r="T109" s="51"/>
       <c r="U109" s="54"/>
@@ -5076,7 +5067,7 @@
       <c r="T111" s="51"/>
       <c r="U111" s="54"/>
     </row>
-    <row r="112" spans="1:21" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:21" s="27" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="57">
         <f>A102+7</f>
         <v>43794</v>
@@ -5088,11 +5079,11 @@
         <f>C102+1</f>
         <v>11</v>
       </c>
-      <c r="D112" s="94" t="s">
+      <c r="D112" s="80" t="s">
         <v>43</v>
       </c>
-      <c r="E112" s="94"/>
-      <c r="F112" s="94"/>
+      <c r="E112" s="80"/>
+      <c r="F112" s="80"/>
       <c r="G112" s="15"/>
       <c r="H112" s="15"/>
       <c r="I112" s="15"/>
@@ -5109,7 +5100,7 @@
       <c r="T112" s="51"/>
       <c r="U112" s="54"/>
     </row>
-    <row r="113" spans="1:21" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:21" s="27" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="3" t="s">
         <v>0</v>
       </c>
@@ -5117,19 +5108,21 @@
         <f>B103+7</f>
         <v>43794</v>
       </c>
-      <c r="C113" s="76" t="s">
+      <c r="C113" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="D113" s="76"/>
-      <c r="E113" s="76"/>
-      <c r="F113" s="76"/>
-      <c r="G113" s="76"/>
-      <c r="H113" s="49"/>
-      <c r="I113" s="49"/>
-      <c r="J113" s="49"/>
-      <c r="K113" s="20"/>
-      <c r="L113" s="20"/>
-      <c r="M113" s="20"/>
+      <c r="D113" s="79"/>
+      <c r="E113" s="79"/>
+      <c r="F113" s="79"/>
+      <c r="G113" s="79"/>
+      <c r="H113" s="77" t="s">
+        <v>86</v>
+      </c>
+      <c r="I113" s="77"/>
+      <c r="J113" s="77"/>
+      <c r="K113" s="77"/>
+      <c r="L113" s="77"/>
+      <c r="M113" s="77"/>
       <c r="N113" s="20"/>
       <c r="O113" s="20"/>
       <c r="P113" s="20"/>
@@ -5141,7 +5134,7 @@
       </c>
       <c r="U113" s="54"/>
     </row>
-    <row r="114" spans="1:21" s="27" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:21" s="27" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="3" t="s">
         <v>1</v>
       </c>
@@ -5149,19 +5142,21 @@
         <f t="shared" ref="B114:B119" si="9">B104+7</f>
         <v>43795</v>
       </c>
-      <c r="C114" s="76" t="s">
+      <c r="C114" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="D114" s="76"/>
-      <c r="E114" s="76"/>
-      <c r="F114" s="76"/>
-      <c r="G114" s="76"/>
-      <c r="H114" s="20"/>
-      <c r="I114" s="20"/>
-      <c r="J114" s="20"/>
-      <c r="K114" s="49"/>
-      <c r="L114" s="49"/>
-      <c r="M114" s="20"/>
+      <c r="D114" s="79"/>
+      <c r="E114" s="79"/>
+      <c r="F114" s="79"/>
+      <c r="G114" s="79"/>
+      <c r="H114" s="77" t="s">
+        <v>86</v>
+      </c>
+      <c r="I114" s="77"/>
+      <c r="J114" s="77"/>
+      <c r="K114" s="77"/>
+      <c r="L114" s="77"/>
+      <c r="M114" s="77"/>
       <c r="N114" s="20"/>
       <c r="O114" s="49"/>
       <c r="P114" s="49"/>
@@ -5183,23 +5178,23 @@
       </c>
       <c r="C115" s="32"/>
       <c r="D115" s="20"/>
-      <c r="E115" s="77" t="s">
-        <v>65</v>
-      </c>
-      <c r="F115" s="77"/>
-      <c r="G115" s="77"/>
-      <c r="H115" s="77"/>
-      <c r="I115" s="77"/>
-      <c r="J115" s="77"/>
+      <c r="E115" s="70" t="s">
+        <v>86</v>
+      </c>
+      <c r="F115" s="70"/>
+      <c r="G115" s="70"/>
+      <c r="H115" s="70"/>
+      <c r="I115" s="70"/>
+      <c r="J115" s="70"/>
       <c r="K115" s="49"/>
-      <c r="L115" s="81" t="s">
-        <v>65</v>
-      </c>
-      <c r="M115" s="82"/>
-      <c r="N115" s="82"/>
-      <c r="O115" s="82"/>
-      <c r="P115" s="82"/>
-      <c r="Q115" s="83"/>
+      <c r="L115" s="71" t="s">
+        <v>86</v>
+      </c>
+      <c r="M115" s="72"/>
+      <c r="N115" s="72"/>
+      <c r="O115" s="72"/>
+      <c r="P115" s="72"/>
+      <c r="Q115" s="73"/>
       <c r="R115" s="49"/>
       <c r="S115" s="51"/>
       <c r="T115" s="52" t="s">
@@ -5215,27 +5210,27 @@
         <f t="shared" si="9"/>
         <v>43797</v>
       </c>
-      <c r="C116" s="76" t="s">
+      <c r="C116" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="D116" s="76"/>
-      <c r="E116" s="76"/>
-      <c r="F116" s="76"/>
-      <c r="G116" s="76"/>
-      <c r="H116" s="77" t="s">
+      <c r="D116" s="79"/>
+      <c r="E116" s="79"/>
+      <c r="F116" s="79"/>
+      <c r="G116" s="79"/>
+      <c r="H116" s="70" t="s">
         <v>55</v>
       </c>
-      <c r="I116" s="77"/>
-      <c r="J116" s="77"/>
-      <c r="K116" s="78" t="s">
-        <v>65</v>
-      </c>
-      <c r="L116" s="79"/>
-      <c r="M116" s="79"/>
-      <c r="N116" s="79"/>
-      <c r="O116" s="79"/>
-      <c r="P116" s="79"/>
-      <c r="Q116" s="80"/>
+      <c r="I116" s="70"/>
+      <c r="J116" s="70"/>
+      <c r="K116" s="74" t="s">
+        <v>86</v>
+      </c>
+      <c r="L116" s="75"/>
+      <c r="M116" s="75"/>
+      <c r="N116" s="75"/>
+      <c r="O116" s="75"/>
+      <c r="P116" s="75"/>
+      <c r="Q116" s="121"/>
       <c r="R116" s="20"/>
       <c r="S116" s="51"/>
       <c r="T116" s="18" t="s">
@@ -5243,7 +5238,7 @@
       </c>
       <c r="U116" s="54"/>
     </row>
-    <row r="117" spans="1:21" s="27" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:21" s="27" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
         <v>4</v>
       </c>
@@ -5253,29 +5248,25 @@
       </c>
       <c r="C117" s="32"/>
       <c r="D117" s="20"/>
-      <c r="E117" s="77" t="s">
-        <v>65</v>
-      </c>
-      <c r="F117" s="77"/>
-      <c r="G117" s="77"/>
-      <c r="H117" s="77"/>
-      <c r="I117" s="77"/>
-      <c r="J117" s="77"/>
-      <c r="K117" s="49"/>
-      <c r="L117" s="81" t="s">
-        <v>65</v>
-      </c>
-      <c r="M117" s="82"/>
-      <c r="N117" s="82"/>
-      <c r="O117" s="82"/>
-      <c r="P117" s="82"/>
-      <c r="Q117" s="83"/>
+      <c r="E117" s="49"/>
+      <c r="F117" s="49"/>
+      <c r="G117" s="49"/>
+      <c r="H117" s="20"/>
+      <c r="I117" s="20"/>
+      <c r="J117" s="20"/>
+      <c r="K117" s="20"/>
+      <c r="L117" s="49"/>
+      <c r="M117" s="49"/>
+      <c r="N117" s="49"/>
+      <c r="O117" s="20"/>
+      <c r="P117" s="20"/>
+      <c r="Q117" s="20"/>
       <c r="R117" s="20"/>
       <c r="S117" s="51"/>
       <c r="T117" s="51"/>
       <c r="U117" s="54"/>
     </row>
-    <row r="118" spans="1:21" s="27" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:21" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
         <v>5</v>
       </c>
@@ -5285,29 +5276,25 @@
       </c>
       <c r="C118" s="50"/>
       <c r="D118" s="49"/>
-      <c r="E118" s="77" t="s">
-        <v>65</v>
-      </c>
-      <c r="F118" s="77"/>
-      <c r="G118" s="77"/>
-      <c r="H118" s="77"/>
-      <c r="I118" s="77"/>
-      <c r="J118" s="77"/>
-      <c r="K118" s="49"/>
-      <c r="L118" s="81" t="s">
-        <v>65</v>
-      </c>
-      <c r="M118" s="82"/>
-      <c r="N118" s="82"/>
-      <c r="O118" s="82"/>
-      <c r="P118" s="82"/>
-      <c r="Q118" s="83"/>
-      <c r="R118" s="49"/>
+      <c r="E118" s="49"/>
+      <c r="F118" s="49"/>
+      <c r="G118" s="49"/>
+      <c r="H118" s="20"/>
+      <c r="I118" s="20"/>
+      <c r="J118" s="20"/>
+      <c r="K118" s="20"/>
+      <c r="L118" s="49"/>
+      <c r="M118" s="49"/>
+      <c r="N118" s="49"/>
+      <c r="O118" s="20"/>
+      <c r="P118" s="20"/>
+      <c r="Q118" s="20"/>
+      <c r="R118" s="20"/>
       <c r="S118" s="51"/>
       <c r="T118" s="51"/>
       <c r="U118" s="54"/>
     </row>
-    <row r="119" spans="1:21" s="27" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:21" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
         <v>6</v>
       </c>
@@ -5315,24 +5302,24 @@
         <f t="shared" si="9"/>
         <v>43800</v>
       </c>
-      <c r="C119" s="76" t="s">
+      <c r="C119" s="79" t="s">
         <v>81</v>
       </c>
-      <c r="D119" s="76"/>
-      <c r="E119" s="76"/>
-      <c r="F119" s="76"/>
-      <c r="G119" s="76"/>
-      <c r="H119" s="76"/>
-      <c r="I119" s="76"/>
-      <c r="J119" s="76"/>
-      <c r="K119" s="76"/>
-      <c r="L119" s="76"/>
-      <c r="M119" s="76"/>
-      <c r="N119" s="76"/>
-      <c r="O119" s="76"/>
-      <c r="P119" s="76"/>
-      <c r="Q119" s="76"/>
-      <c r="R119" s="76"/>
+      <c r="D119" s="79"/>
+      <c r="E119" s="79"/>
+      <c r="F119" s="79"/>
+      <c r="G119" s="79"/>
+      <c r="H119" s="79"/>
+      <c r="I119" s="79"/>
+      <c r="J119" s="79"/>
+      <c r="K119" s="79"/>
+      <c r="L119" s="79"/>
+      <c r="M119" s="79"/>
+      <c r="N119" s="79"/>
+      <c r="O119" s="79"/>
+      <c r="P119" s="79"/>
+      <c r="Q119" s="79"/>
+      <c r="R119" s="79"/>
       <c r="S119" s="51"/>
       <c r="T119" s="51"/>
       <c r="U119" s="54"/>
@@ -5407,11 +5394,11 @@
         <f>C112+1</f>
         <v>12</v>
       </c>
-      <c r="D122" s="94" t="s">
+      <c r="D122" s="80" t="s">
         <v>41</v>
       </c>
-      <c r="E122" s="94"/>
-      <c r="F122" s="94"/>
+      <c r="E122" s="80"/>
+      <c r="F122" s="80"/>
       <c r="G122" s="15"/>
       <c r="H122" s="15"/>
       <c r="I122" s="15"/>
@@ -5436,24 +5423,24 @@
         <f>B113+7</f>
         <v>43801</v>
       </c>
-      <c r="C123" s="76" t="s">
+      <c r="C123" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="D123" s="76"/>
-      <c r="E123" s="76"/>
-      <c r="F123" s="76"/>
-      <c r="G123" s="76"/>
-      <c r="H123" s="78" t="s">
+      <c r="D123" s="79"/>
+      <c r="E123" s="79"/>
+      <c r="F123" s="79"/>
+      <c r="G123" s="79"/>
+      <c r="H123" s="74" t="s">
         <v>65</v>
       </c>
-      <c r="I123" s="79"/>
-      <c r="J123" s="79"/>
-      <c r="K123" s="79"/>
-      <c r="L123" s="79"/>
-      <c r="M123" s="79"/>
-      <c r="N123" s="79"/>
-      <c r="O123" s="79"/>
-      <c r="P123" s="115"/>
+      <c r="I123" s="75"/>
+      <c r="J123" s="75"/>
+      <c r="K123" s="75"/>
+      <c r="L123" s="75"/>
+      <c r="M123" s="75"/>
+      <c r="N123" s="75"/>
+      <c r="O123" s="75"/>
+      <c r="P123" s="76"/>
       <c r="Q123" s="20"/>
       <c r="R123" s="20"/>
       <c r="S123" s="51"/>
@@ -5470,24 +5457,24 @@
         <f t="shared" ref="B124:B129" si="10">B114+7</f>
         <v>43802</v>
       </c>
-      <c r="C124" s="76" t="s">
+      <c r="C124" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="D124" s="76"/>
-      <c r="E124" s="76"/>
-      <c r="F124" s="76"/>
-      <c r="G124" s="76"/>
-      <c r="H124" s="76" t="s">
-        <v>44</v>
-      </c>
-      <c r="I124" s="76"/>
-      <c r="J124" s="20"/>
-      <c r="K124" s="49"/>
-      <c r="L124" s="49"/>
-      <c r="M124" s="20"/>
-      <c r="N124" s="20"/>
-      <c r="O124" s="49"/>
-      <c r="P124" s="49"/>
+      <c r="D124" s="79"/>
+      <c r="E124" s="79"/>
+      <c r="F124" s="79"/>
+      <c r="G124" s="79"/>
+      <c r="H124" s="74" t="s">
+        <v>65</v>
+      </c>
+      <c r="I124" s="75"/>
+      <c r="J124" s="75"/>
+      <c r="K124" s="75"/>
+      <c r="L124" s="75"/>
+      <c r="M124" s="75"/>
+      <c r="N124" s="75"/>
+      <c r="O124" s="75"/>
+      <c r="P124" s="76"/>
       <c r="Q124" s="20"/>
       <c r="R124" s="20"/>
       <c r="S124" s="51"/>
@@ -5504,15 +5491,17 @@
         <f t="shared" si="10"/>
         <v>43803</v>
       </c>
-      <c r="C125" s="32"/>
-      <c r="D125" s="20"/>
-      <c r="E125" s="20"/>
-      <c r="F125" s="20"/>
-      <c r="G125" s="20"/>
-      <c r="H125" s="20"/>
-      <c r="I125" s="20"/>
-      <c r="J125" s="20"/>
-      <c r="K125" s="49"/>
+      <c r="C125" s="74" t="s">
+        <v>65</v>
+      </c>
+      <c r="D125" s="75"/>
+      <c r="E125" s="75"/>
+      <c r="F125" s="75"/>
+      <c r="G125" s="75"/>
+      <c r="H125" s="75"/>
+      <c r="I125" s="75"/>
+      <c r="J125" s="75"/>
+      <c r="K125" s="76"/>
       <c r="L125" s="49"/>
       <c r="M125" s="49"/>
       <c r="N125" s="49"/>
@@ -5534,13 +5523,13 @@
         <f t="shared" si="10"/>
         <v>43804</v>
       </c>
-      <c r="C126" s="86" t="s">
+      <c r="C126" s="81" t="s">
         <v>80</v>
       </c>
-      <c r="D126" s="86"/>
-      <c r="E126" s="86"/>
-      <c r="F126" s="86"/>
-      <c r="G126" s="86"/>
+      <c r="D126" s="81"/>
+      <c r="E126" s="81"/>
+      <c r="F126" s="81"/>
+      <c r="G126" s="81"/>
       <c r="H126" s="49"/>
       <c r="I126" s="49"/>
       <c r="J126" s="49"/>
@@ -5622,24 +5611,24 @@
         <f t="shared" si="10"/>
         <v>43807</v>
       </c>
-      <c r="C129" s="76" t="s">
+      <c r="C129" s="79" t="s">
         <v>81</v>
       </c>
-      <c r="D129" s="76"/>
-      <c r="E129" s="76"/>
-      <c r="F129" s="76"/>
-      <c r="G129" s="76"/>
-      <c r="H129" s="76"/>
-      <c r="I129" s="76"/>
-      <c r="J129" s="76"/>
-      <c r="K129" s="76"/>
-      <c r="L129" s="76"/>
-      <c r="M129" s="76"/>
-      <c r="N129" s="76"/>
-      <c r="O129" s="76"/>
-      <c r="P129" s="76"/>
-      <c r="Q129" s="76"/>
-      <c r="R129" s="76"/>
+      <c r="D129" s="79"/>
+      <c r="E129" s="79"/>
+      <c r="F129" s="79"/>
+      <c r="G129" s="79"/>
+      <c r="H129" s="79"/>
+      <c r="I129" s="79"/>
+      <c r="J129" s="79"/>
+      <c r="K129" s="79"/>
+      <c r="L129" s="79"/>
+      <c r="M129" s="79"/>
+      <c r="N129" s="79"/>
+      <c r="O129" s="79"/>
+      <c r="P129" s="79"/>
+      <c r="Q129" s="79"/>
+      <c r="R129" s="79"/>
       <c r="S129" s="51"/>
       <c r="T129" s="51"/>
       <c r="U129" s="54"/>
@@ -5741,13 +5730,13 @@
         <f>B123+7</f>
         <v>43808</v>
       </c>
-      <c r="C133" s="76" t="s">
+      <c r="C133" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="D133" s="76"/>
-      <c r="E133" s="76"/>
-      <c r="F133" s="76"/>
-      <c r="G133" s="76"/>
+      <c r="D133" s="79"/>
+      <c r="E133" s="79"/>
+      <c r="F133" s="79"/>
+      <c r="G133" s="79"/>
       <c r="H133" s="49"/>
       <c r="I133" s="49"/>
       <c r="J133" s="49"/>
@@ -5773,13 +5762,13 @@
         <f t="shared" ref="B134:B139" si="11">B124+7</f>
         <v>43809</v>
       </c>
-      <c r="C134" s="76" t="s">
+      <c r="C134" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="D134" s="76"/>
-      <c r="E134" s="76"/>
-      <c r="F134" s="76"/>
-      <c r="G134" s="76"/>
+      <c r="D134" s="79"/>
+      <c r="E134" s="79"/>
+      <c r="F134" s="79"/>
+      <c r="G134" s="79"/>
       <c r="H134" s="20"/>
       <c r="I134" s="20"/>
       <c r="J134" s="20"/>
@@ -5835,13 +5824,13 @@
         <f t="shared" si="11"/>
         <v>43811</v>
       </c>
-      <c r="C136" s="76" t="s">
+      <c r="C136" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="D136" s="76"/>
-      <c r="E136" s="76"/>
-      <c r="F136" s="76"/>
-      <c r="G136" s="76"/>
+      <c r="D136" s="79"/>
+      <c r="E136" s="79"/>
+      <c r="F136" s="79"/>
+      <c r="G136" s="79"/>
       <c r="H136" s="20"/>
       <c r="I136" s="49"/>
       <c r="J136" s="49"/>
@@ -5923,24 +5912,24 @@
         <f t="shared" si="11"/>
         <v>43814</v>
       </c>
-      <c r="C139" s="76" t="s">
+      <c r="C139" s="79" t="s">
         <v>81</v>
       </c>
-      <c r="D139" s="76"/>
-      <c r="E139" s="76"/>
-      <c r="F139" s="76"/>
-      <c r="G139" s="76"/>
-      <c r="H139" s="76"/>
-      <c r="I139" s="76"/>
-      <c r="J139" s="76"/>
-      <c r="K139" s="76"/>
-      <c r="L139" s="76"/>
-      <c r="M139" s="76"/>
-      <c r="N139" s="76"/>
-      <c r="O139" s="76"/>
-      <c r="P139" s="76"/>
-      <c r="Q139" s="76"/>
-      <c r="R139" s="76"/>
+      <c r="D139" s="79"/>
+      <c r="E139" s="79"/>
+      <c r="F139" s="79"/>
+      <c r="G139" s="79"/>
+      <c r="H139" s="79"/>
+      <c r="I139" s="79"/>
+      <c r="J139" s="79"/>
+      <c r="K139" s="79"/>
+      <c r="L139" s="79"/>
+      <c r="M139" s="79"/>
+      <c r="N139" s="79"/>
+      <c r="O139" s="79"/>
+      <c r="P139" s="79"/>
+      <c r="Q139" s="79"/>
+      <c r="R139" s="79"/>
       <c r="S139" s="51"/>
       <c r="T139" s="51"/>
       <c r="U139" s="54"/>
@@ -6035,19 +6024,19 @@
         <f>C132+1</f>
         <v>14</v>
       </c>
-      <c r="D142" s="94" t="s">
+      <c r="D142" s="80" t="s">
         <v>30</v>
       </c>
-      <c r="E142" s="94"/>
-      <c r="F142" s="94"/>
+      <c r="E142" s="80"/>
+      <c r="F142" s="80"/>
       <c r="G142" s="15"/>
-      <c r="H142" s="94" t="s">
+      <c r="H142" s="80" t="s">
         <v>52</v>
       </c>
-      <c r="I142" s="94"/>
-      <c r="J142" s="94"/>
-      <c r="K142" s="94"/>
-      <c r="L142" s="94"/>
+      <c r="I142" s="80"/>
+      <c r="J142" s="80"/>
+      <c r="K142" s="80"/>
+      <c r="L142" s="80"/>
       <c r="M142" s="19"/>
       <c r="N142" s="19"/>
       <c r="O142" s="19"/>
@@ -6066,11 +6055,11 @@
         <f>B133+7</f>
         <v>43815</v>
       </c>
-      <c r="C143" s="77" t="s">
+      <c r="C143" s="70" t="s">
         <v>55</v>
       </c>
-      <c r="D143" s="77"/>
-      <c r="E143" s="77"/>
+      <c r="D143" s="70"/>
+      <c r="E143" s="70"/>
       <c r="F143" s="20"/>
       <c r="G143" s="20"/>
       <c r="H143" s="20"/>
@@ -6441,24 +6430,24 @@
         <f t="shared" si="13"/>
         <v>43824</v>
       </c>
-      <c r="C155" s="113" t="s">
+      <c r="C155" s="78" t="s">
         <v>53</v>
       </c>
-      <c r="D155" s="113"/>
-      <c r="E155" s="113"/>
-      <c r="F155" s="113"/>
-      <c r="G155" s="113"/>
-      <c r="H155" s="113"/>
-      <c r="I155" s="113"/>
-      <c r="J155" s="113"/>
-      <c r="K155" s="113"/>
-      <c r="L155" s="113"/>
-      <c r="M155" s="113"/>
-      <c r="N155" s="113"/>
-      <c r="O155" s="113"/>
-      <c r="P155" s="113"/>
-      <c r="Q155" s="113"/>
-      <c r="R155" s="113"/>
+      <c r="D155" s="78"/>
+      <c r="E155" s="78"/>
+      <c r="F155" s="78"/>
+      <c r="G155" s="78"/>
+      <c r="H155" s="78"/>
+      <c r="I155" s="78"/>
+      <c r="J155" s="78"/>
+      <c r="K155" s="78"/>
+      <c r="L155" s="78"/>
+      <c r="M155" s="78"/>
+      <c r="N155" s="78"/>
+      <c r="O155" s="78"/>
+      <c r="P155" s="78"/>
+      <c r="Q155" s="78"/>
+      <c r="R155" s="78"/>
       <c r="S155" s="51"/>
       <c r="T155" s="52" t="s">
         <v>20</v>
@@ -6473,22 +6462,22 @@
         <f t="shared" si="13"/>
         <v>43825</v>
       </c>
-      <c r="C156" s="113"/>
-      <c r="D156" s="113"/>
-      <c r="E156" s="113"/>
-      <c r="F156" s="113"/>
-      <c r="G156" s="113"/>
-      <c r="H156" s="113"/>
-      <c r="I156" s="113"/>
-      <c r="J156" s="113"/>
-      <c r="K156" s="113"/>
-      <c r="L156" s="113"/>
-      <c r="M156" s="113"/>
-      <c r="N156" s="113"/>
-      <c r="O156" s="113"/>
-      <c r="P156" s="113"/>
-      <c r="Q156" s="113"/>
-      <c r="R156" s="113"/>
+      <c r="C156" s="78"/>
+      <c r="D156" s="78"/>
+      <c r="E156" s="78"/>
+      <c r="F156" s="78"/>
+      <c r="G156" s="78"/>
+      <c r="H156" s="78"/>
+      <c r="I156" s="78"/>
+      <c r="J156" s="78"/>
+      <c r="K156" s="78"/>
+      <c r="L156" s="78"/>
+      <c r="M156" s="78"/>
+      <c r="N156" s="78"/>
+      <c r="O156" s="78"/>
+      <c r="P156" s="78"/>
+      <c r="Q156" s="78"/>
+      <c r="R156" s="78"/>
       <c r="S156" s="51"/>
       <c r="T156" s="18" t="s">
         <v>21</v>
@@ -6503,22 +6492,22 @@
         <f t="shared" si="13"/>
         <v>43826</v>
       </c>
-      <c r="C157" s="113"/>
-      <c r="D157" s="113"/>
-      <c r="E157" s="113"/>
-      <c r="F157" s="113"/>
-      <c r="G157" s="113"/>
-      <c r="H157" s="113"/>
-      <c r="I157" s="113"/>
-      <c r="J157" s="113"/>
-      <c r="K157" s="113"/>
-      <c r="L157" s="113"/>
-      <c r="M157" s="113"/>
-      <c r="N157" s="113"/>
-      <c r="O157" s="113"/>
-      <c r="P157" s="113"/>
-      <c r="Q157" s="113"/>
-      <c r="R157" s="113"/>
+      <c r="C157" s="78"/>
+      <c r="D157" s="78"/>
+      <c r="E157" s="78"/>
+      <c r="F157" s="78"/>
+      <c r="G157" s="78"/>
+      <c r="H157" s="78"/>
+      <c r="I157" s="78"/>
+      <c r="J157" s="78"/>
+      <c r="K157" s="78"/>
+      <c r="L157" s="78"/>
+      <c r="M157" s="78"/>
+      <c r="N157" s="78"/>
+      <c r="O157" s="78"/>
+      <c r="P157" s="78"/>
+      <c r="Q157" s="78"/>
+      <c r="R157" s="78"/>
       <c r="S157" s="51"/>
       <c r="T157" s="51"/>
       <c r="U157" s="54"/>
@@ -6531,22 +6520,22 @@
         <f t="shared" si="13"/>
         <v>43827</v>
       </c>
-      <c r="C158" s="113"/>
-      <c r="D158" s="113"/>
-      <c r="E158" s="113"/>
-      <c r="F158" s="113"/>
-      <c r="G158" s="113"/>
-      <c r="H158" s="113"/>
-      <c r="I158" s="113"/>
-      <c r="J158" s="113"/>
-      <c r="K158" s="113"/>
-      <c r="L158" s="113"/>
-      <c r="M158" s="113"/>
-      <c r="N158" s="113"/>
-      <c r="O158" s="113"/>
-      <c r="P158" s="113"/>
-      <c r="Q158" s="113"/>
-      <c r="R158" s="113"/>
+      <c r="C158" s="78"/>
+      <c r="D158" s="78"/>
+      <c r="E158" s="78"/>
+      <c r="F158" s="78"/>
+      <c r="G158" s="78"/>
+      <c r="H158" s="78"/>
+      <c r="I158" s="78"/>
+      <c r="J158" s="78"/>
+      <c r="K158" s="78"/>
+      <c r="L158" s="78"/>
+      <c r="M158" s="78"/>
+      <c r="N158" s="78"/>
+      <c r="O158" s="78"/>
+      <c r="P158" s="78"/>
+      <c r="Q158" s="78"/>
+      <c r="R158" s="78"/>
       <c r="S158" s="51"/>
       <c r="T158" s="51"/>
       <c r="U158" s="54"/>
@@ -6559,22 +6548,22 @@
         <f t="shared" si="13"/>
         <v>43828</v>
       </c>
-      <c r="C159" s="113"/>
-      <c r="D159" s="113"/>
-      <c r="E159" s="113"/>
-      <c r="F159" s="113"/>
-      <c r="G159" s="113"/>
-      <c r="H159" s="113"/>
-      <c r="I159" s="113"/>
-      <c r="J159" s="113"/>
-      <c r="K159" s="113"/>
-      <c r="L159" s="113"/>
-      <c r="M159" s="113"/>
-      <c r="N159" s="113"/>
-      <c r="O159" s="113"/>
-      <c r="P159" s="113"/>
-      <c r="Q159" s="113"/>
-      <c r="R159" s="113"/>
+      <c r="C159" s="78"/>
+      <c r="D159" s="78"/>
+      <c r="E159" s="78"/>
+      <c r="F159" s="78"/>
+      <c r="G159" s="78"/>
+      <c r="H159" s="78"/>
+      <c r="I159" s="78"/>
+      <c r="J159" s="78"/>
+      <c r="K159" s="78"/>
+      <c r="L159" s="78"/>
+      <c r="M159" s="78"/>
+      <c r="N159" s="78"/>
+      <c r="O159" s="78"/>
+      <c r="P159" s="78"/>
+      <c r="Q159" s="78"/>
+      <c r="R159" s="78"/>
       <c r="S159" s="51"/>
       <c r="T159" s="51"/>
       <c r="U159" s="54"/>
@@ -6696,24 +6685,24 @@
         <f>B153+7</f>
         <v>43829</v>
       </c>
-      <c r="C163" s="113" t="s">
+      <c r="C163" s="78" t="s">
         <v>54</v>
       </c>
-      <c r="D163" s="113"/>
-      <c r="E163" s="113"/>
-      <c r="F163" s="113"/>
-      <c r="G163" s="113"/>
-      <c r="H163" s="113"/>
-      <c r="I163" s="113"/>
-      <c r="J163" s="113"/>
-      <c r="K163" s="113"/>
-      <c r="L163" s="113"/>
-      <c r="M163" s="113"/>
-      <c r="N163" s="113"/>
-      <c r="O163" s="113"/>
-      <c r="P163" s="113"/>
-      <c r="Q163" s="113"/>
-      <c r="R163" s="113"/>
+      <c r="D163" s="78"/>
+      <c r="E163" s="78"/>
+      <c r="F163" s="78"/>
+      <c r="G163" s="78"/>
+      <c r="H163" s="78"/>
+      <c r="I163" s="78"/>
+      <c r="J163" s="78"/>
+      <c r="K163" s="78"/>
+      <c r="L163" s="78"/>
+      <c r="M163" s="78"/>
+      <c r="N163" s="78"/>
+      <c r="O163" s="78"/>
+      <c r="P163" s="78"/>
+      <c r="Q163" s="78"/>
+      <c r="R163" s="78"/>
       <c r="S163" s="51"/>
       <c r="T163" s="30" t="s">
         <v>22</v>
@@ -6728,22 +6717,22 @@
         <f t="shared" ref="B164:B169" si="14">B154+7</f>
         <v>43830</v>
       </c>
-      <c r="C164" s="113"/>
-      <c r="D164" s="113"/>
-      <c r="E164" s="113"/>
-      <c r="F164" s="113"/>
-      <c r="G164" s="113"/>
-      <c r="H164" s="113"/>
-      <c r="I164" s="113"/>
-      <c r="J164" s="113"/>
-      <c r="K164" s="113"/>
-      <c r="L164" s="113"/>
-      <c r="M164" s="113"/>
-      <c r="N164" s="113"/>
-      <c r="O164" s="113"/>
-      <c r="P164" s="113"/>
-      <c r="Q164" s="113"/>
-      <c r="R164" s="113"/>
+      <c r="C164" s="78"/>
+      <c r="D164" s="78"/>
+      <c r="E164" s="78"/>
+      <c r="F164" s="78"/>
+      <c r="G164" s="78"/>
+      <c r="H164" s="78"/>
+      <c r="I164" s="78"/>
+      <c r="J164" s="78"/>
+      <c r="K164" s="78"/>
+      <c r="L164" s="78"/>
+      <c r="M164" s="78"/>
+      <c r="N164" s="78"/>
+      <c r="O164" s="78"/>
+      <c r="P164" s="78"/>
+      <c r="Q164" s="78"/>
+      <c r="R164" s="78"/>
       <c r="S164" s="51"/>
       <c r="T164" s="53" t="s">
         <v>19</v>
@@ -6758,22 +6747,22 @@
         <f t="shared" si="14"/>
         <v>43831</v>
       </c>
-      <c r="C165" s="113"/>
-      <c r="D165" s="113"/>
-      <c r="E165" s="113"/>
-      <c r="F165" s="113"/>
-      <c r="G165" s="113"/>
-      <c r="H165" s="113"/>
-      <c r="I165" s="113"/>
-      <c r="J165" s="113"/>
-      <c r="K165" s="113"/>
-      <c r="L165" s="113"/>
-      <c r="M165" s="113"/>
-      <c r="N165" s="113"/>
-      <c r="O165" s="113"/>
-      <c r="P165" s="113"/>
-      <c r="Q165" s="113"/>
-      <c r="R165" s="113"/>
+      <c r="C165" s="78"/>
+      <c r="D165" s="78"/>
+      <c r="E165" s="78"/>
+      <c r="F165" s="78"/>
+      <c r="G165" s="78"/>
+      <c r="H165" s="78"/>
+      <c r="I165" s="78"/>
+      <c r="J165" s="78"/>
+      <c r="K165" s="78"/>
+      <c r="L165" s="78"/>
+      <c r="M165" s="78"/>
+      <c r="N165" s="78"/>
+      <c r="O165" s="78"/>
+      <c r="P165" s="78"/>
+      <c r="Q165" s="78"/>
+      <c r="R165" s="78"/>
       <c r="S165" s="51"/>
       <c r="T165" s="52" t="s">
         <v>20</v>
@@ -6790,23 +6779,23 @@
       </c>
       <c r="C166" s="32"/>
       <c r="D166" s="20"/>
-      <c r="E166" s="77" t="s">
+      <c r="E166" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="F166" s="77"/>
-      <c r="G166" s="77"/>
-      <c r="H166" s="77"/>
-      <c r="I166" s="77"/>
-      <c r="J166" s="77"/>
+      <c r="F166" s="70"/>
+      <c r="G166" s="70"/>
+      <c r="H166" s="70"/>
+      <c r="I166" s="70"/>
+      <c r="J166" s="70"/>
       <c r="K166" s="49"/>
-      <c r="L166" s="81" t="s">
+      <c r="L166" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="M166" s="82"/>
-      <c r="N166" s="82"/>
-      <c r="O166" s="82"/>
-      <c r="P166" s="82"/>
-      <c r="Q166" s="83"/>
+      <c r="M166" s="72"/>
+      <c r="N166" s="72"/>
+      <c r="O166" s="72"/>
+      <c r="P166" s="72"/>
+      <c r="Q166" s="73"/>
       <c r="R166" s="20"/>
       <c r="S166" s="51"/>
       <c r="T166" s="18" t="s">
@@ -6824,23 +6813,23 @@
       </c>
       <c r="C167" s="50"/>
       <c r="D167" s="49"/>
-      <c r="E167" s="77" t="s">
+      <c r="E167" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="F167" s="77"/>
-      <c r="G167" s="77"/>
-      <c r="H167" s="77"/>
-      <c r="I167" s="77"/>
-      <c r="J167" s="77"/>
+      <c r="F167" s="70"/>
+      <c r="G167" s="70"/>
+      <c r="H167" s="70"/>
+      <c r="I167" s="70"/>
+      <c r="J167" s="70"/>
       <c r="K167" s="49"/>
-      <c r="L167" s="81" t="s">
+      <c r="L167" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="M167" s="82"/>
-      <c r="N167" s="82"/>
-      <c r="O167" s="82"/>
-      <c r="P167" s="82"/>
-      <c r="Q167" s="83"/>
+      <c r="M167" s="72"/>
+      <c r="N167" s="72"/>
+      <c r="O167" s="72"/>
+      <c r="P167" s="72"/>
+      <c r="Q167" s="73"/>
       <c r="R167" s="49"/>
       <c r="S167" s="51"/>
       <c r="T167" s="51"/>
@@ -7001,23 +6990,23 @@
       </c>
       <c r="C173" s="32"/>
       <c r="D173" s="20"/>
-      <c r="E173" s="77" t="s">
+      <c r="E173" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="F173" s="77"/>
-      <c r="G173" s="77"/>
-      <c r="H173" s="77"/>
-      <c r="I173" s="77"/>
-      <c r="J173" s="77"/>
+      <c r="F173" s="70"/>
+      <c r="G173" s="70"/>
+      <c r="H173" s="70"/>
+      <c r="I173" s="70"/>
+      <c r="J173" s="70"/>
       <c r="K173" s="49"/>
-      <c r="L173" s="81" t="s">
+      <c r="L173" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="M173" s="82"/>
-      <c r="N173" s="82"/>
-      <c r="O173" s="82"/>
-      <c r="P173" s="82"/>
-      <c r="Q173" s="83"/>
+      <c r="M173" s="72"/>
+      <c r="N173" s="72"/>
+      <c r="O173" s="72"/>
+      <c r="P173" s="72"/>
+      <c r="Q173" s="73"/>
       <c r="R173" s="49"/>
       <c r="S173" s="51"/>
       <c r="T173" s="30" t="s">
@@ -7035,23 +7024,23 @@
       </c>
       <c r="C174" s="32"/>
       <c r="D174" s="20"/>
-      <c r="E174" s="77" t="s">
+      <c r="E174" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="F174" s="77"/>
-      <c r="G174" s="77"/>
-      <c r="H174" s="77"/>
-      <c r="I174" s="77"/>
-      <c r="J174" s="77"/>
+      <c r="F174" s="70"/>
+      <c r="G174" s="70"/>
+      <c r="H174" s="70"/>
+      <c r="I174" s="70"/>
+      <c r="J174" s="70"/>
       <c r="K174" s="49"/>
-      <c r="L174" s="81" t="s">
+      <c r="L174" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="M174" s="82"/>
-      <c r="N174" s="82"/>
-      <c r="O174" s="82"/>
-      <c r="P174" s="82"/>
-      <c r="Q174" s="83"/>
+      <c r="M174" s="72"/>
+      <c r="N174" s="72"/>
+      <c r="O174" s="72"/>
+      <c r="P174" s="72"/>
+      <c r="Q174" s="73"/>
       <c r="R174" s="20"/>
       <c r="S174" s="51"/>
       <c r="T174" s="53" t="s">
@@ -7069,23 +7058,23 @@
       </c>
       <c r="C175" s="32"/>
       <c r="D175" s="20"/>
-      <c r="E175" s="77" t="s">
+      <c r="E175" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="F175" s="77"/>
-      <c r="G175" s="77"/>
-      <c r="H175" s="77"/>
-      <c r="I175" s="77"/>
-      <c r="J175" s="77"/>
+      <c r="F175" s="70"/>
+      <c r="G175" s="70"/>
+      <c r="H175" s="70"/>
+      <c r="I175" s="70"/>
+      <c r="J175" s="70"/>
       <c r="K175" s="20"/>
-      <c r="L175" s="81" t="s">
+      <c r="L175" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="M175" s="82"/>
-      <c r="N175" s="82"/>
-      <c r="O175" s="82"/>
-      <c r="P175" s="82"/>
-      <c r="Q175" s="83"/>
+      <c r="M175" s="72"/>
+      <c r="N175" s="72"/>
+      <c r="O175" s="72"/>
+      <c r="P175" s="72"/>
+      <c r="Q175" s="73"/>
       <c r="R175" s="49"/>
       <c r="S175" s="51"/>
       <c r="T175" s="52" t="s">
@@ -7103,23 +7092,23 @@
       </c>
       <c r="C176" s="49"/>
       <c r="D176" s="49"/>
-      <c r="E176" s="77" t="s">
+      <c r="E176" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="F176" s="77"/>
-      <c r="G176" s="77"/>
-      <c r="H176" s="77"/>
-      <c r="I176" s="77"/>
-      <c r="J176" s="77"/>
+      <c r="F176" s="70"/>
+      <c r="G176" s="70"/>
+      <c r="H176" s="70"/>
+      <c r="I176" s="70"/>
+      <c r="J176" s="70"/>
       <c r="K176" s="20"/>
-      <c r="L176" s="81" t="s">
+      <c r="L176" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="M176" s="82"/>
-      <c r="N176" s="82"/>
-      <c r="O176" s="82"/>
-      <c r="P176" s="82"/>
-      <c r="Q176" s="83"/>
+      <c r="M176" s="72"/>
+      <c r="N176" s="72"/>
+      <c r="O176" s="72"/>
+      <c r="P176" s="72"/>
+      <c r="Q176" s="73"/>
       <c r="R176" s="20"/>
       <c r="S176" s="51"/>
       <c r="T176" s="18" t="s">
@@ -7137,23 +7126,23 @@
       </c>
       <c r="C177" s="32"/>
       <c r="D177" s="20"/>
-      <c r="E177" s="77" t="s">
+      <c r="E177" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="F177" s="77"/>
-      <c r="G177" s="77"/>
-      <c r="H177" s="77"/>
-      <c r="I177" s="77"/>
-      <c r="J177" s="77"/>
+      <c r="F177" s="70"/>
+      <c r="G177" s="70"/>
+      <c r="H177" s="70"/>
+      <c r="I177" s="70"/>
+      <c r="J177" s="70"/>
       <c r="K177" s="20"/>
-      <c r="L177" s="81" t="s">
+      <c r="L177" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="M177" s="82"/>
-      <c r="N177" s="82"/>
-      <c r="O177" s="82"/>
-      <c r="P177" s="82"/>
-      <c r="Q177" s="83"/>
+      <c r="M177" s="72"/>
+      <c r="N177" s="72"/>
+      <c r="O177" s="72"/>
+      <c r="P177" s="72"/>
+      <c r="Q177" s="73"/>
       <c r="R177" s="20"/>
       <c r="S177" s="51"/>
       <c r="T177" s="51"/>
@@ -7312,23 +7301,23 @@
       </c>
       <c r="C183" s="32"/>
       <c r="D183" s="20"/>
-      <c r="E183" s="77" t="s">
+      <c r="E183" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="F183" s="77"/>
-      <c r="G183" s="77"/>
-      <c r="H183" s="77"/>
-      <c r="I183" s="77"/>
-      <c r="J183" s="77"/>
+      <c r="F183" s="70"/>
+      <c r="G183" s="70"/>
+      <c r="H183" s="70"/>
+      <c r="I183" s="70"/>
+      <c r="J183" s="70"/>
       <c r="K183" s="49"/>
-      <c r="L183" s="81" t="s">
+      <c r="L183" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="M183" s="82"/>
-      <c r="N183" s="82"/>
-      <c r="O183" s="82"/>
-      <c r="P183" s="82"/>
-      <c r="Q183" s="83"/>
+      <c r="M183" s="72"/>
+      <c r="N183" s="72"/>
+      <c r="O183" s="72"/>
+      <c r="P183" s="72"/>
+      <c r="Q183" s="73"/>
       <c r="R183" s="49"/>
       <c r="S183" s="51"/>
       <c r="T183" s="30" t="s">
@@ -7345,23 +7334,23 @@
       </c>
       <c r="C184" s="32"/>
       <c r="D184" s="20"/>
-      <c r="E184" s="77" t="s">
+      <c r="E184" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="F184" s="77"/>
-      <c r="G184" s="77"/>
-      <c r="H184" s="77"/>
-      <c r="I184" s="77"/>
-      <c r="J184" s="77"/>
+      <c r="F184" s="70"/>
+      <c r="G184" s="70"/>
+      <c r="H184" s="70"/>
+      <c r="I184" s="70"/>
+      <c r="J184" s="70"/>
       <c r="K184" s="49"/>
-      <c r="L184" s="81" t="s">
+      <c r="L184" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="M184" s="82"/>
-      <c r="N184" s="82"/>
-      <c r="O184" s="82"/>
-      <c r="P184" s="82"/>
-      <c r="Q184" s="83"/>
+      <c r="M184" s="72"/>
+      <c r="N184" s="72"/>
+      <c r="O184" s="72"/>
+      <c r="P184" s="72"/>
+      <c r="Q184" s="73"/>
       <c r="R184" s="20"/>
       <c r="S184" s="51"/>
       <c r="T184" s="53" t="s">
@@ -7378,23 +7367,23 @@
       </c>
       <c r="C185" s="32"/>
       <c r="D185" s="20"/>
-      <c r="E185" s="77" t="s">
+      <c r="E185" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="F185" s="77"/>
-      <c r="G185" s="77"/>
-      <c r="H185" s="77"/>
-      <c r="I185" s="77"/>
-      <c r="J185" s="77"/>
+      <c r="F185" s="70"/>
+      <c r="G185" s="70"/>
+      <c r="H185" s="70"/>
+      <c r="I185" s="70"/>
+      <c r="J185" s="70"/>
       <c r="K185" s="20"/>
-      <c r="L185" s="81" t="s">
+      <c r="L185" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="M185" s="82"/>
-      <c r="N185" s="82"/>
-      <c r="O185" s="82"/>
-      <c r="P185" s="82"/>
-      <c r="Q185" s="83"/>
+      <c r="M185" s="72"/>
+      <c r="N185" s="72"/>
+      <c r="O185" s="72"/>
+      <c r="P185" s="72"/>
+      <c r="Q185" s="73"/>
       <c r="R185" s="49"/>
       <c r="S185" s="51"/>
       <c r="T185" s="52" t="s">
@@ -7411,23 +7400,23 @@
       </c>
       <c r="C186" s="49"/>
       <c r="D186" s="49"/>
-      <c r="E186" s="77" t="s">
+      <c r="E186" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="F186" s="77"/>
-      <c r="G186" s="77"/>
-      <c r="H186" s="77"/>
-      <c r="I186" s="77"/>
-      <c r="J186" s="77"/>
+      <c r="F186" s="70"/>
+      <c r="G186" s="70"/>
+      <c r="H186" s="70"/>
+      <c r="I186" s="70"/>
+      <c r="J186" s="70"/>
       <c r="K186" s="20"/>
-      <c r="L186" s="81" t="s">
+      <c r="L186" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="M186" s="82"/>
-      <c r="N186" s="82"/>
-      <c r="O186" s="82"/>
-      <c r="P186" s="82"/>
-      <c r="Q186" s="83"/>
+      <c r="M186" s="72"/>
+      <c r="N186" s="72"/>
+      <c r="O186" s="72"/>
+      <c r="P186" s="72"/>
+      <c r="Q186" s="73"/>
       <c r="R186" s="20"/>
       <c r="S186" s="51"/>
       <c r="T186" s="18" t="s">
@@ -7444,23 +7433,23 @@
       </c>
       <c r="C187" s="32"/>
       <c r="D187" s="20"/>
-      <c r="E187" s="77" t="s">
+      <c r="E187" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="F187" s="77"/>
-      <c r="G187" s="77"/>
-      <c r="H187" s="77"/>
-      <c r="I187" s="77"/>
-      <c r="J187" s="77"/>
+      <c r="F187" s="70"/>
+      <c r="G187" s="70"/>
+      <c r="H187" s="70"/>
+      <c r="I187" s="70"/>
+      <c r="J187" s="70"/>
       <c r="K187" s="20"/>
-      <c r="L187" s="81" t="s">
+      <c r="L187" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="M187" s="82"/>
-      <c r="N187" s="82"/>
-      <c r="O187" s="82"/>
-      <c r="P187" s="82"/>
-      <c r="Q187" s="83"/>
+      <c r="M187" s="72"/>
+      <c r="N187" s="72"/>
+      <c r="O187" s="72"/>
+      <c r="P187" s="72"/>
+      <c r="Q187" s="73"/>
       <c r="R187" s="20"/>
       <c r="S187" s="51"/>
       <c r="T187" s="51"/>
@@ -15890,70 +15879,65 @@
       <c r="T507"/>
     </row>
   </sheetData>
-  <mergeCells count="147">
-    <mergeCell ref="T58:U60"/>
-    <mergeCell ref="E187:J187"/>
-    <mergeCell ref="L187:Q187"/>
-    <mergeCell ref="E117:J117"/>
-    <mergeCell ref="L117:Q117"/>
-    <mergeCell ref="E118:J118"/>
-    <mergeCell ref="L118:Q118"/>
-    <mergeCell ref="H123:P123"/>
-    <mergeCell ref="E184:J184"/>
-    <mergeCell ref="L184:Q184"/>
-    <mergeCell ref="E185:J185"/>
-    <mergeCell ref="L185:Q185"/>
-    <mergeCell ref="E186:J186"/>
-    <mergeCell ref="L186:Q186"/>
-    <mergeCell ref="E176:J176"/>
-    <mergeCell ref="L176:Q176"/>
-    <mergeCell ref="E177:J177"/>
-    <mergeCell ref="L177:Q177"/>
-    <mergeCell ref="E183:J183"/>
-    <mergeCell ref="L183:Q183"/>
-    <mergeCell ref="E173:J173"/>
-    <mergeCell ref="H103:P103"/>
-    <mergeCell ref="H104:P104"/>
-    <mergeCell ref="E175:J175"/>
-    <mergeCell ref="L175:Q175"/>
-    <mergeCell ref="L167:Q167"/>
-    <mergeCell ref="C155:R159"/>
-    <mergeCell ref="C163:R165"/>
-    <mergeCell ref="E166:J166"/>
-    <mergeCell ref="L166:Q166"/>
-    <mergeCell ref="E167:J167"/>
-    <mergeCell ref="H84:I84"/>
-    <mergeCell ref="D112:F112"/>
-    <mergeCell ref="C136:G136"/>
-    <mergeCell ref="C116:G116"/>
-    <mergeCell ref="C123:G123"/>
-    <mergeCell ref="C124:G124"/>
-    <mergeCell ref="C106:G106"/>
-    <mergeCell ref="L173:Q173"/>
-    <mergeCell ref="E174:J174"/>
-    <mergeCell ref="L174:Q174"/>
-    <mergeCell ref="C126:G126"/>
-    <mergeCell ref="H142:L142"/>
-    <mergeCell ref="C105:M105"/>
-    <mergeCell ref="H106:P106"/>
-    <mergeCell ref="P57:R57"/>
-    <mergeCell ref="E73:J73"/>
-    <mergeCell ref="L73:Q73"/>
-    <mergeCell ref="Q54:R54"/>
-    <mergeCell ref="H54:P54"/>
-    <mergeCell ref="C66:G66"/>
-    <mergeCell ref="L74:Q74"/>
-    <mergeCell ref="L77:Q77"/>
-    <mergeCell ref="L78:Q78"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="E58:G58"/>
-    <mergeCell ref="J58:P58"/>
-    <mergeCell ref="E74:J74"/>
-    <mergeCell ref="H56:M56"/>
-    <mergeCell ref="H66:Q66"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="I63:L63"/>
-    <mergeCell ref="H64:N64"/>
+  <mergeCells count="146">
+    <mergeCell ref="C143:E143"/>
+    <mergeCell ref="K116:Q116"/>
+    <mergeCell ref="E115:J115"/>
+    <mergeCell ref="L115:Q115"/>
+    <mergeCell ref="C134:G134"/>
+    <mergeCell ref="C114:G114"/>
+    <mergeCell ref="C133:G133"/>
+    <mergeCell ref="C113:G113"/>
+    <mergeCell ref="H116:J116"/>
+    <mergeCell ref="D122:F122"/>
+    <mergeCell ref="D142:F142"/>
+    <mergeCell ref="H124:P124"/>
+    <mergeCell ref="C125:K125"/>
+    <mergeCell ref="H113:M113"/>
+    <mergeCell ref="H114:M114"/>
+    <mergeCell ref="C79:R79"/>
+    <mergeCell ref="C89:R89"/>
+    <mergeCell ref="C99:R99"/>
+    <mergeCell ref="C109:R109"/>
+    <mergeCell ref="C103:G103"/>
+    <mergeCell ref="C104:G104"/>
+    <mergeCell ref="C83:G83"/>
+    <mergeCell ref="C84:G84"/>
+    <mergeCell ref="C86:G86"/>
+    <mergeCell ref="C93:G93"/>
+    <mergeCell ref="C94:G94"/>
+    <mergeCell ref="C96:G96"/>
+    <mergeCell ref="H83:P83"/>
+    <mergeCell ref="C107:M107"/>
+    <mergeCell ref="J84:R84"/>
+    <mergeCell ref="E85:M85"/>
+    <mergeCell ref="H93:P93"/>
+    <mergeCell ref="H94:P94"/>
+    <mergeCell ref="H96:L96"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H46:P46"/>
+    <mergeCell ref="H44:N44"/>
+    <mergeCell ref="H52:J52"/>
+    <mergeCell ref="H62:J62"/>
+    <mergeCell ref="D82:F82"/>
+    <mergeCell ref="C53:G53"/>
+    <mergeCell ref="D72:F72"/>
+    <mergeCell ref="L75:Q75"/>
+    <mergeCell ref="I53:M53"/>
+    <mergeCell ref="C67:J67"/>
+    <mergeCell ref="C46:G46"/>
+    <mergeCell ref="C54:G54"/>
+    <mergeCell ref="C56:G56"/>
+    <mergeCell ref="C63:G63"/>
+    <mergeCell ref="C64:G64"/>
+    <mergeCell ref="I55:N55"/>
+    <mergeCell ref="C76:R76"/>
+    <mergeCell ref="E78:J78"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="E75:J75"/>
+    <mergeCell ref="E77:J77"/>
+    <mergeCell ref="L67:R67"/>
+    <mergeCell ref="M72:R72"/>
     <mergeCell ref="H13:R13"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="O14:P14"/>
@@ -15978,66 +15962,70 @@
     <mergeCell ref="C24:G24"/>
     <mergeCell ref="C34:G34"/>
     <mergeCell ref="O24:P24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H46:P46"/>
-    <mergeCell ref="H44:N44"/>
-    <mergeCell ref="H52:J52"/>
-    <mergeCell ref="H62:J62"/>
-    <mergeCell ref="D82:F82"/>
-    <mergeCell ref="C53:G53"/>
-    <mergeCell ref="D72:F72"/>
-    <mergeCell ref="L75:Q75"/>
-    <mergeCell ref="I53:M53"/>
-    <mergeCell ref="C67:J67"/>
-    <mergeCell ref="C46:G46"/>
-    <mergeCell ref="C54:G54"/>
-    <mergeCell ref="C56:G56"/>
-    <mergeCell ref="C63:G63"/>
-    <mergeCell ref="C64:G64"/>
-    <mergeCell ref="I55:N55"/>
-    <mergeCell ref="C76:R76"/>
-    <mergeCell ref="E78:J78"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="E75:J75"/>
-    <mergeCell ref="E77:J77"/>
-    <mergeCell ref="L67:R67"/>
-    <mergeCell ref="M72:R72"/>
+    <mergeCell ref="P57:R57"/>
+    <mergeCell ref="E73:J73"/>
+    <mergeCell ref="L73:Q73"/>
+    <mergeCell ref="Q54:R54"/>
+    <mergeCell ref="H54:P54"/>
+    <mergeCell ref="C66:G66"/>
+    <mergeCell ref="L74:Q74"/>
+    <mergeCell ref="L77:Q77"/>
+    <mergeCell ref="L78:Q78"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="J58:P58"/>
+    <mergeCell ref="E74:J74"/>
+    <mergeCell ref="H56:M56"/>
+    <mergeCell ref="H66:Q66"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="I63:L63"/>
+    <mergeCell ref="H64:N64"/>
     <mergeCell ref="H72:K72"/>
     <mergeCell ref="C69:R69"/>
-    <mergeCell ref="C79:R79"/>
-    <mergeCell ref="C89:R89"/>
-    <mergeCell ref="C99:R99"/>
-    <mergeCell ref="C109:R109"/>
-    <mergeCell ref="C103:G103"/>
-    <mergeCell ref="C104:G104"/>
-    <mergeCell ref="C83:G83"/>
-    <mergeCell ref="C84:G84"/>
-    <mergeCell ref="C86:G86"/>
-    <mergeCell ref="C93:G93"/>
-    <mergeCell ref="C94:G94"/>
-    <mergeCell ref="C96:G96"/>
-    <mergeCell ref="H83:P83"/>
-    <mergeCell ref="C107:M107"/>
-    <mergeCell ref="J84:R84"/>
-    <mergeCell ref="E85:M85"/>
-    <mergeCell ref="H93:P93"/>
-    <mergeCell ref="H94:P94"/>
-    <mergeCell ref="H96:L96"/>
+    <mergeCell ref="L175:Q175"/>
+    <mergeCell ref="L167:Q167"/>
+    <mergeCell ref="C155:R159"/>
+    <mergeCell ref="C163:R165"/>
+    <mergeCell ref="E166:J166"/>
+    <mergeCell ref="L166:Q166"/>
+    <mergeCell ref="E167:J167"/>
+    <mergeCell ref="H84:I84"/>
+    <mergeCell ref="D112:F112"/>
+    <mergeCell ref="C136:G136"/>
+    <mergeCell ref="C116:G116"/>
+    <mergeCell ref="C123:G123"/>
+    <mergeCell ref="C124:G124"/>
+    <mergeCell ref="C106:G106"/>
+    <mergeCell ref="L173:Q173"/>
+    <mergeCell ref="E174:J174"/>
+    <mergeCell ref="L174:Q174"/>
+    <mergeCell ref="C126:G126"/>
+    <mergeCell ref="H142:L142"/>
+    <mergeCell ref="C105:M105"/>
+    <mergeCell ref="H106:P106"/>
     <mergeCell ref="C119:R119"/>
     <mergeCell ref="C129:R129"/>
     <mergeCell ref="C139:R139"/>
-    <mergeCell ref="C143:E143"/>
-    <mergeCell ref="K116:Q116"/>
-    <mergeCell ref="E115:J115"/>
-    <mergeCell ref="L115:Q115"/>
-    <mergeCell ref="C134:G134"/>
-    <mergeCell ref="C114:G114"/>
-    <mergeCell ref="C133:G133"/>
-    <mergeCell ref="H124:I124"/>
-    <mergeCell ref="C113:G113"/>
-    <mergeCell ref="H116:J116"/>
-    <mergeCell ref="D122:F122"/>
-    <mergeCell ref="D142:F142"/>
+    <mergeCell ref="T58:U60"/>
+    <mergeCell ref="E187:J187"/>
+    <mergeCell ref="L187:Q187"/>
+    <mergeCell ref="H123:P123"/>
+    <mergeCell ref="E184:J184"/>
+    <mergeCell ref="L184:Q184"/>
+    <mergeCell ref="E185:J185"/>
+    <mergeCell ref="L185:Q185"/>
+    <mergeCell ref="E186:J186"/>
+    <mergeCell ref="L186:Q186"/>
+    <mergeCell ref="E176:J176"/>
+    <mergeCell ref="L176:Q176"/>
+    <mergeCell ref="E177:J177"/>
+    <mergeCell ref="L177:Q177"/>
+    <mergeCell ref="E183:J183"/>
+    <mergeCell ref="L183:Q183"/>
+    <mergeCell ref="E173:J173"/>
+    <mergeCell ref="H103:P103"/>
+    <mergeCell ref="H104:P104"/>
+    <mergeCell ref="E175:J175"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -16065,10 +16053,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="116" t="s">
+      <c r="A2" s="122" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="116"/>
+      <c r="B2" s="122"/>
       <c r="C2" s="41" t="s">
         <v>18</v>
       </c>
@@ -16087,10 +16075,10 @@
       <c r="I2" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="117" t="s">
+      <c r="J2" s="123" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="117"/>
+      <c r="K2" s="123"/>
     </row>
     <row r="3" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
@@ -16105,10 +16093,10 @@
       <c r="I3" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="J3" s="118" t="s">
+      <c r="J3" s="124" t="s">
         <v>60</v>
       </c>
-      <c r="K3" s="118"/>
+      <c r="K3" s="124"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
@@ -16130,10 +16118,10 @@
       <c r="I4" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="J4" s="118" t="s">
+      <c r="J4" s="124" t="s">
         <v>61</v>
       </c>
-      <c r="K4" s="118"/>
+      <c r="K4" s="124"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
@@ -16408,10 +16396,10 @@
       <c r="H22" s="51"/>
     </row>
     <row r="23" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="116" t="s">
+      <c r="A23" s="122" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="116"/>
+      <c r="B23" s="122"/>
       <c r="C23" s="41" t="s">
         <v>18</v>
       </c>
@@ -16616,7 +16604,7 @@
         <v>43929</v>
       </c>
       <c r="D36" s="29"/>
-      <c r="F36" s="113" t="s">
+      <c r="F36" s="78" t="s">
         <v>49</v>
       </c>
     </row>
@@ -16634,7 +16622,7 @@
         <v>43936</v>
       </c>
       <c r="D37" s="44"/>
-      <c r="F37" s="113"/>
+      <c r="F37" s="78"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="23">
@@ -16650,7 +16638,7 @@
         <v>43943</v>
       </c>
       <c r="D38" s="29"/>
-      <c r="F38" s="113"/>
+      <c r="F38" s="78"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="23">

</xml_diff>

<commit_message>
Created November's Reflective Journal and updated Weekly Planner
</commit_message>
<xml_diff>
--- a/Weekly Planner.xlsx
+++ b/Weekly Planner.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\SoftwareProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246BF56E-0D70-49FA-85C6-F5773F8E342B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59DFA32-7E8E-4BD0-BF38-B3488EE39FC7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Weekly Planner" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="90">
   <si>
     <t>Monday</t>
   </si>
@@ -302,12 +302,21 @@
   <si>
     <t>Software Project - Requirements Specifications</t>
   </si>
+  <si>
+    <t>Software Project - Prototype</t>
+  </si>
+  <si>
+    <t>DAD - Project</t>
+  </si>
+  <si>
+    <t>SP - Montly journal</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -400,6 +409,15 @@
       <u val="double"/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -896,7 +914,7 @@
     <xf numFmtId="0" fontId="11" fillId="10" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1074,31 +1092,34 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="12" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="13" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="14" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="10" xfId="9" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="15" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="17" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="16" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="19" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="20" xfId="9" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="8" xfId="8" applyAlignment="1">
@@ -1110,7 +1131,10 @@
     <xf numFmtId="20" fontId="6" fillId="8" borderId="4" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="8" xfId="8" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="1" applyBorder="1" applyAlignment="1">
@@ -1120,15 +1144,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="34" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
@@ -1182,6 +1197,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="31" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="20" fontId="6" fillId="8" borderId="11" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1227,10 +1245,22 @@
     <xf numFmtId="20" fontId="9" fillId="6" borderId="11" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="6" fillId="8" borderId="11" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="8" xfId="8" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="29" xfId="9" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="35" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="10" xfId="9" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="6" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="4" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="5" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1242,7 +1272,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="35" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1545,8 +1575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y507"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C155" sqref="C155:R159"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J116" sqref="J116:N116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1929,14 +1959,14 @@
       <c r="B13" s="57">
         <v>43724</v>
       </c>
-      <c r="C13" s="79" t="s">
+      <c r="C13" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="79"/>
-      <c r="E13" s="79"/>
-      <c r="F13" s="79"/>
-      <c r="G13" s="79"/>
-      <c r="H13" s="91" t="s">
+      <c r="D13" s="80"/>
+      <c r="E13" s="80"/>
+      <c r="F13" s="80"/>
+      <c r="G13" s="80"/>
+      <c r="H13" s="90" t="s">
         <v>39</v>
       </c>
       <c r="I13" s="105"/>
@@ -1948,7 +1978,7 @@
       <c r="O13" s="105"/>
       <c r="P13" s="105"/>
       <c r="Q13" s="105"/>
-      <c r="R13" s="92"/>
+      <c r="R13" s="91"/>
       <c r="S13" s="51"/>
       <c r="T13" s="30" t="s">
         <v>22</v>
@@ -1961,13 +1991,13 @@
       <c r="B14" s="57">
         <v>43725</v>
       </c>
-      <c r="C14" s="79" t="s">
+      <c r="C14" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="79"/>
-      <c r="E14" s="79"/>
-      <c r="F14" s="79"/>
-      <c r="G14" s="79"/>
+      <c r="D14" s="80"/>
+      <c r="E14" s="80"/>
+      <c r="F14" s="80"/>
+      <c r="G14" s="80"/>
       <c r="H14" s="20"/>
       <c r="I14" s="20"/>
       <c r="J14" s="106" t="s">
@@ -1977,10 +2007,10 @@
       <c r="L14" s="107"/>
       <c r="M14" s="107"/>
       <c r="N14" s="108"/>
-      <c r="O14" s="91" t="s">
+      <c r="O14" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="P14" s="92"/>
+      <c r="P14" s="91"/>
       <c r="Q14" s="20"/>
       <c r="R14" s="20"/>
       <c r="S14" s="51"/>
@@ -2023,13 +2053,13 @@
       <c r="B16" s="57">
         <v>43727</v>
       </c>
-      <c r="C16" s="79" t="s">
+      <c r="C16" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="79"/>
-      <c r="E16" s="79"/>
-      <c r="F16" s="79"/>
-      <c r="G16" s="79"/>
+      <c r="D16" s="80"/>
+      <c r="E16" s="80"/>
+      <c r="F16" s="80"/>
+      <c r="G16" s="80"/>
       <c r="H16" s="114" t="s">
         <v>47</v>
       </c>
@@ -2241,14 +2271,14 @@
         <f>B13+7</f>
         <v>43731</v>
       </c>
-      <c r="C23" s="79" t="s">
+      <c r="C23" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="79"/>
-      <c r="E23" s="79"/>
-      <c r="F23" s="79"/>
-      <c r="G23" s="79"/>
-      <c r="H23" s="91" t="s">
+      <c r="D23" s="80"/>
+      <c r="E23" s="80"/>
+      <c r="F23" s="80"/>
+      <c r="G23" s="80"/>
+      <c r="H23" s="90" t="s">
         <v>39</v>
       </c>
       <c r="I23" s="105"/>
@@ -2260,7 +2290,7 @@
       <c r="O23" s="105"/>
       <c r="P23" s="105"/>
       <c r="Q23" s="105"/>
-      <c r="R23" s="92"/>
+      <c r="R23" s="91"/>
       <c r="S23" s="51"/>
       <c r="T23" s="30" t="s">
         <v>22</v>
@@ -2274,26 +2304,26 @@
         <f t="shared" ref="B24:B29" si="0">B14+7</f>
         <v>43732</v>
       </c>
-      <c r="C24" s="79" t="s">
+      <c r="C24" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="79"/>
-      <c r="E24" s="79"/>
-      <c r="F24" s="79"/>
-      <c r="G24" s="79"/>
-      <c r="H24" s="91" t="s">
+      <c r="D24" s="80"/>
+      <c r="E24" s="80"/>
+      <c r="F24" s="80"/>
+      <c r="G24" s="80"/>
+      <c r="H24" s="90" t="s">
         <v>44</v>
       </c>
       <c r="I24" s="115"/>
-      <c r="J24" s="88" t="s">
+      <c r="J24" s="87" t="s">
         <v>48</v>
       </c>
-      <c r="K24" s="89"/>
-      <c r="L24" s="90"/>
-      <c r="M24" s="88" t="s">
+      <c r="K24" s="88"/>
+      <c r="L24" s="89"/>
+      <c r="M24" s="87" t="s">
         <v>56</v>
       </c>
-      <c r="N24" s="90"/>
+      <c r="N24" s="89"/>
       <c r="O24" s="106" t="s">
         <v>38</v>
       </c>
@@ -2342,13 +2372,13 @@
         <f t="shared" si="0"/>
         <v>43734</v>
       </c>
-      <c r="C26" s="79" t="s">
+      <c r="C26" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="D26" s="79"/>
-      <c r="E26" s="79"/>
-      <c r="F26" s="79"/>
-      <c r="G26" s="79"/>
+      <c r="D26" s="80"/>
+      <c r="E26" s="80"/>
+      <c r="F26" s="80"/>
+      <c r="G26" s="80"/>
       <c r="H26" s="112" t="s">
         <v>57</v>
       </c>
@@ -2565,13 +2595,13 @@
         <f>B23+7</f>
         <v>43738</v>
       </c>
-      <c r="C33" s="79" t="s">
+      <c r="C33" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="D33" s="79"/>
-      <c r="E33" s="79"/>
-      <c r="F33" s="79"/>
-      <c r="G33" s="79"/>
+      <c r="D33" s="80"/>
+      <c r="E33" s="80"/>
+      <c r="F33" s="80"/>
+      <c r="G33" s="80"/>
       <c r="H33" s="112" t="s">
         <v>14</v>
       </c>
@@ -2598,13 +2628,13 @@
         <f t="shared" ref="B34:B39" si="1">B24+7</f>
         <v>43739</v>
       </c>
-      <c r="C34" s="79" t="s">
+      <c r="C34" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="D34" s="79"/>
-      <c r="E34" s="79"/>
-      <c r="F34" s="79"/>
-      <c r="G34" s="79"/>
+      <c r="D34" s="80"/>
+      <c r="E34" s="80"/>
+      <c r="F34" s="80"/>
+      <c r="G34" s="80"/>
       <c r="H34" s="62"/>
       <c r="I34" s="62"/>
       <c r="J34" s="62"/>
@@ -2658,13 +2688,13 @@
         <f t="shared" si="1"/>
         <v>43741</v>
       </c>
-      <c r="C36" s="79" t="s">
+      <c r="C36" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="D36" s="79"/>
-      <c r="E36" s="79"/>
-      <c r="F36" s="79"/>
-      <c r="G36" s="79"/>
+      <c r="D36" s="80"/>
+      <c r="E36" s="80"/>
+      <c r="F36" s="80"/>
+      <c r="G36" s="80"/>
       <c r="H36" s="63"/>
       <c r="I36" s="63"/>
       <c r="J36" s="63"/>
@@ -2877,24 +2907,24 @@
         <f>B33+7</f>
         <v>43745</v>
       </c>
-      <c r="C43" s="79" t="s">
+      <c r="C43" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="D43" s="79"/>
-      <c r="E43" s="79"/>
-      <c r="F43" s="79"/>
-      <c r="G43" s="79"/>
-      <c r="H43" s="77" t="s">
+      <c r="D43" s="80"/>
+      <c r="E43" s="80"/>
+      <c r="F43" s="80"/>
+      <c r="G43" s="80"/>
+      <c r="H43" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="I43" s="77"/>
-      <c r="J43" s="77"/>
-      <c r="K43" s="77"/>
-      <c r="L43" s="77"/>
-      <c r="M43" s="77"/>
-      <c r="N43" s="77"/>
-      <c r="O43" s="77"/>
-      <c r="P43" s="77"/>
+      <c r="I43" s="75"/>
+      <c r="J43" s="75"/>
+      <c r="K43" s="75"/>
+      <c r="L43" s="75"/>
+      <c r="M43" s="75"/>
+      <c r="N43" s="75"/>
+      <c r="O43" s="75"/>
+      <c r="P43" s="75"/>
       <c r="Q43" s="20"/>
       <c r="R43" s="20"/>
       <c r="S43" s="51"/>
@@ -2910,22 +2940,22 @@
         <f t="shared" ref="B44:B49" si="2">B34+7</f>
         <v>43746</v>
       </c>
-      <c r="C44" s="79" t="s">
+      <c r="C44" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="D44" s="79"/>
-      <c r="E44" s="79"/>
-      <c r="F44" s="79"/>
-      <c r="G44" s="79"/>
+      <c r="D44" s="80"/>
+      <c r="E44" s="80"/>
+      <c r="F44" s="80"/>
+      <c r="G44" s="80"/>
       <c r="H44" s="116" t="s">
         <v>58</v>
       </c>
-      <c r="I44" s="101"/>
-      <c r="J44" s="101"/>
-      <c r="K44" s="101"/>
-      <c r="L44" s="101"/>
-      <c r="M44" s="101"/>
-      <c r="N44" s="101"/>
+      <c r="I44" s="100"/>
+      <c r="J44" s="100"/>
+      <c r="K44" s="100"/>
+      <c r="L44" s="100"/>
+      <c r="M44" s="100"/>
+      <c r="N44" s="100"/>
       <c r="O44" s="49"/>
       <c r="P44" s="49"/>
       <c r="Q44" s="49"/>
@@ -2974,24 +3004,24 @@
         <f t="shared" si="2"/>
         <v>43748</v>
       </c>
-      <c r="C46" s="79" t="s">
+      <c r="C46" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="D46" s="79"/>
-      <c r="E46" s="79"/>
-      <c r="F46" s="79"/>
-      <c r="G46" s="79"/>
-      <c r="H46" s="85" t="s">
+      <c r="D46" s="80"/>
+      <c r="E46" s="80"/>
+      <c r="F46" s="80"/>
+      <c r="G46" s="80"/>
+      <c r="H46" s="76" t="s">
         <v>62</v>
       </c>
-      <c r="I46" s="86"/>
-      <c r="J46" s="86"/>
-      <c r="K46" s="86"/>
-      <c r="L46" s="86"/>
-      <c r="M46" s="86"/>
-      <c r="N46" s="86"/>
-      <c r="O46" s="86"/>
-      <c r="P46" s="87"/>
+      <c r="I46" s="77"/>
+      <c r="J46" s="77"/>
+      <c r="K46" s="77"/>
+      <c r="L46" s="77"/>
+      <c r="M46" s="77"/>
+      <c r="N46" s="77"/>
+      <c r="O46" s="77"/>
+      <c r="P46" s="78"/>
       <c r="Q46" s="20"/>
       <c r="R46" s="20"/>
       <c r="S46" s="51"/>
@@ -3194,23 +3224,23 @@
         <f>B43+7</f>
         <v>43752</v>
       </c>
-      <c r="C53" s="79" t="s">
+      <c r="C53" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="D53" s="79"/>
-      <c r="E53" s="79"/>
-      <c r="F53" s="79"/>
-      <c r="G53" s="79"/>
+      <c r="D53" s="80"/>
+      <c r="E53" s="80"/>
+      <c r="F53" s="80"/>
+      <c r="G53" s="80"/>
       <c r="H53" s="65" t="s">
         <v>68</v>
       </c>
-      <c r="I53" s="88" t="s">
+      <c r="I53" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="J53" s="89"/>
-      <c r="K53" s="89"/>
-      <c r="L53" s="89"/>
-      <c r="M53" s="89"/>
+      <c r="J53" s="88"/>
+      <c r="K53" s="88"/>
+      <c r="L53" s="88"/>
+      <c r="M53" s="88"/>
       <c r="N53" s="49"/>
       <c r="O53" s="49"/>
       <c r="P53" s="49"/>
@@ -3229,28 +3259,28 @@
         <f t="shared" ref="B54:B59" si="3">B44+7</f>
         <v>43753</v>
       </c>
-      <c r="C54" s="79" t="s">
+      <c r="C54" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="D54" s="79"/>
-      <c r="E54" s="79"/>
-      <c r="F54" s="79"/>
-      <c r="G54" s="79"/>
-      <c r="H54" s="93" t="s">
+      <c r="D54" s="80"/>
+      <c r="E54" s="80"/>
+      <c r="F54" s="80"/>
+      <c r="G54" s="80"/>
+      <c r="H54" s="92" t="s">
         <v>63</v>
       </c>
-      <c r="I54" s="94"/>
-      <c r="J54" s="94"/>
-      <c r="K54" s="94"/>
-      <c r="L54" s="94"/>
-      <c r="M54" s="94"/>
-      <c r="N54" s="94"/>
-      <c r="O54" s="94"/>
-      <c r="P54" s="94"/>
-      <c r="Q54" s="91" t="s">
+      <c r="I54" s="93"/>
+      <c r="J54" s="93"/>
+      <c r="K54" s="93"/>
+      <c r="L54" s="93"/>
+      <c r="M54" s="93"/>
+      <c r="N54" s="93"/>
+      <c r="O54" s="93"/>
+      <c r="P54" s="93"/>
+      <c r="Q54" s="90" t="s">
         <v>70</v>
       </c>
-      <c r="R54" s="92"/>
+      <c r="R54" s="91"/>
       <c r="S54" s="51"/>
       <c r="T54" s="53" t="s">
         <v>19</v>
@@ -3268,18 +3298,18 @@
       <c r="D55" s="49"/>
       <c r="E55" s="49"/>
       <c r="F55" s="49"/>
-      <c r="G55" s="79" t="s">
+      <c r="G55" s="80" t="s">
         <v>64</v>
       </c>
-      <c r="H55" s="79"/>
+      <c r="H55" s="80"/>
       <c r="I55" s="118" t="s">
         <v>14</v>
       </c>
-      <c r="J55" s="89"/>
-      <c r="K55" s="89"/>
-      <c r="L55" s="89"/>
-      <c r="M55" s="89"/>
-      <c r="N55" s="89"/>
+      <c r="J55" s="88"/>
+      <c r="K55" s="88"/>
+      <c r="L55" s="88"/>
+      <c r="M55" s="88"/>
+      <c r="N55" s="88"/>
       <c r="O55" s="49"/>
       <c r="P55" s="49"/>
       <c r="Q55" s="49"/>
@@ -3297,21 +3327,21 @@
         <f t="shared" si="3"/>
         <v>43755</v>
       </c>
-      <c r="C56" s="79" t="s">
+      <c r="C56" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="D56" s="79"/>
-      <c r="E56" s="79"/>
-      <c r="F56" s="79"/>
-      <c r="G56" s="79"/>
-      <c r="H56" s="100" t="s">
+      <c r="D56" s="80"/>
+      <c r="E56" s="80"/>
+      <c r="F56" s="80"/>
+      <c r="G56" s="80"/>
+      <c r="H56" s="99" t="s">
         <v>71</v>
       </c>
-      <c r="I56" s="101"/>
-      <c r="J56" s="101"/>
-      <c r="K56" s="101"/>
-      <c r="L56" s="101"/>
-      <c r="M56" s="101"/>
+      <c r="I56" s="100"/>
+      <c r="J56" s="100"/>
+      <c r="K56" s="100"/>
+      <c r="L56" s="100"/>
+      <c r="M56" s="100"/>
       <c r="N56" s="49"/>
       <c r="O56" s="49"/>
       <c r="P56" s="49"/>
@@ -3343,11 +3373,11 @@
       <c r="M57" s="49"/>
       <c r="N57" s="49"/>
       <c r="O57" s="49"/>
-      <c r="P57" s="85" t="s">
+      <c r="P57" s="76" t="s">
         <v>42</v>
       </c>
-      <c r="Q57" s="86"/>
-      <c r="R57" s="87"/>
+      <c r="Q57" s="77"/>
+      <c r="R57" s="78"/>
       <c r="S57" s="51"/>
       <c r="T57" s="51"/>
     </row>
@@ -3361,31 +3391,31 @@
       </c>
       <c r="C58" s="50"/>
       <c r="D58" s="49"/>
-      <c r="E58" s="98" t="s">
+      <c r="E58" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="F58" s="86"/>
-      <c r="G58" s="99"/>
-      <c r="H58" s="79" t="s">
+      <c r="F58" s="77"/>
+      <c r="G58" s="98"/>
+      <c r="H58" s="80" t="s">
         <v>74</v>
       </c>
-      <c r="I58" s="79"/>
-      <c r="J58" s="88" t="s">
+      <c r="I58" s="80"/>
+      <c r="J58" s="87" t="s">
         <v>42</v>
       </c>
-      <c r="K58" s="89"/>
-      <c r="L58" s="89"/>
-      <c r="M58" s="89"/>
-      <c r="N58" s="89"/>
-      <c r="O58" s="89"/>
-      <c r="P58" s="90"/>
+      <c r="K58" s="88"/>
+      <c r="L58" s="88"/>
+      <c r="M58" s="88"/>
+      <c r="N58" s="88"/>
+      <c r="O58" s="88"/>
+      <c r="P58" s="89"/>
       <c r="Q58" s="20"/>
       <c r="R58" s="20"/>
       <c r="S58" s="51"/>
-      <c r="T58" s="69" t="s">
+      <c r="T58" s="73" t="s">
         <v>72</v>
       </c>
-      <c r="U58" s="69"/>
+      <c r="U58" s="73"/>
     </row>
     <row r="59" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
@@ -3412,8 +3442,8 @@
       <c r="Q59" s="20"/>
       <c r="R59" s="20"/>
       <c r="S59" s="51"/>
-      <c r="T59" s="69"/>
-      <c r="U59" s="69"/>
+      <c r="T59" s="73"/>
+      <c r="U59" s="73"/>
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B60"/>
@@ -3434,8 +3464,8 @@
       <c r="Q60"/>
       <c r="R60"/>
       <c r="S60"/>
-      <c r="T60" s="69"/>
-      <c r="U60" s="69"/>
+      <c r="T60" s="73"/>
+      <c r="U60" s="73"/>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
@@ -3533,22 +3563,22 @@
         <f>B53+7</f>
         <v>43759</v>
       </c>
-      <c r="C63" s="79" t="s">
+      <c r="C63" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="D63" s="79"/>
-      <c r="E63" s="79"/>
-      <c r="F63" s="79"/>
-      <c r="G63" s="79"/>
+      <c r="D63" s="80"/>
+      <c r="E63" s="80"/>
+      <c r="F63" s="80"/>
+      <c r="G63" s="80"/>
       <c r="H63" s="67" t="s">
         <v>68</v>
       </c>
-      <c r="I63" s="88" t="s">
+      <c r="I63" s="87" t="s">
         <v>76</v>
       </c>
-      <c r="J63" s="89"/>
-      <c r="K63" s="89"/>
-      <c r="L63" s="89"/>
+      <c r="J63" s="88"/>
+      <c r="K63" s="88"/>
+      <c r="L63" s="88"/>
       <c r="M63" s="49"/>
       <c r="N63" s="49"/>
       <c r="O63" s="49"/>
@@ -3568,22 +3598,22 @@
         <f t="shared" ref="B64:B69" si="4">B54+7</f>
         <v>43760</v>
       </c>
-      <c r="C64" s="79" t="s">
+      <c r="C64" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="D64" s="79"/>
-      <c r="E64" s="79"/>
-      <c r="F64" s="79"/>
-      <c r="G64" s="79"/>
-      <c r="H64" s="98" t="s">
+      <c r="D64" s="80"/>
+      <c r="E64" s="80"/>
+      <c r="F64" s="80"/>
+      <c r="G64" s="80"/>
+      <c r="H64" s="97" t="s">
         <v>85</v>
       </c>
-      <c r="I64" s="86"/>
-      <c r="J64" s="86"/>
-      <c r="K64" s="86"/>
-      <c r="L64" s="86"/>
-      <c r="M64" s="86"/>
-      <c r="N64" s="86"/>
+      <c r="I64" s="77"/>
+      <c r="J64" s="77"/>
+      <c r="K64" s="77"/>
+      <c r="L64" s="77"/>
+      <c r="M64" s="77"/>
+      <c r="N64" s="77"/>
       <c r="O64" s="49"/>
       <c r="P64" s="49"/>
       <c r="Q64" s="49"/>
@@ -3632,25 +3662,25 @@
         <f t="shared" si="4"/>
         <v>43762</v>
       </c>
-      <c r="C66" s="79" t="s">
+      <c r="C66" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="D66" s="79"/>
-      <c r="E66" s="79"/>
-      <c r="F66" s="79"/>
-      <c r="G66" s="79"/>
-      <c r="H66" s="102" t="s">
+      <c r="D66" s="80"/>
+      <c r="E66" s="80"/>
+      <c r="F66" s="80"/>
+      <c r="G66" s="80"/>
+      <c r="H66" s="101" t="s">
         <v>77</v>
       </c>
-      <c r="I66" s="103"/>
-      <c r="J66" s="103"/>
-      <c r="K66" s="103"/>
-      <c r="L66" s="103"/>
-      <c r="M66" s="103"/>
-      <c r="N66" s="103"/>
-      <c r="O66" s="103"/>
-      <c r="P66" s="103"/>
-      <c r="Q66" s="104"/>
+      <c r="I66" s="102"/>
+      <c r="J66" s="102"/>
+      <c r="K66" s="102"/>
+      <c r="L66" s="102"/>
+      <c r="M66" s="102"/>
+      <c r="N66" s="102"/>
+      <c r="O66" s="102"/>
+      <c r="P66" s="102"/>
+      <c r="Q66" s="103"/>
       <c r="R66" s="20"/>
       <c r="S66" s="51"/>
       <c r="T66" s="18" t="s">
@@ -3665,26 +3695,26 @@
         <f t="shared" si="4"/>
         <v>43763</v>
       </c>
-      <c r="C67" s="88" t="s">
+      <c r="C67" s="87" t="s">
         <v>77</v>
       </c>
-      <c r="D67" s="89"/>
-      <c r="E67" s="89"/>
-      <c r="F67" s="89"/>
-      <c r="G67" s="89"/>
-      <c r="H67" s="89"/>
-      <c r="I67" s="89"/>
-      <c r="J67" s="90"/>
+      <c r="D67" s="88"/>
+      <c r="E67" s="88"/>
+      <c r="F67" s="88"/>
+      <c r="G67" s="88"/>
+      <c r="H67" s="88"/>
+      <c r="I67" s="88"/>
+      <c r="J67" s="89"/>
       <c r="K67" s="49"/>
-      <c r="L67" s="89" t="s">
+      <c r="L67" s="88" t="s">
         <v>42</v>
       </c>
-      <c r="M67" s="89"/>
-      <c r="N67" s="89"/>
-      <c r="O67" s="89"/>
-      <c r="P67" s="89"/>
-      <c r="Q67" s="89"/>
-      <c r="R67" s="90"/>
+      <c r="M67" s="88"/>
+      <c r="N67" s="88"/>
+      <c r="O67" s="88"/>
+      <c r="P67" s="88"/>
+      <c r="Q67" s="88"/>
+      <c r="R67" s="89"/>
       <c r="S67" s="51"/>
       <c r="T67" s="51"/>
     </row>
@@ -3723,24 +3753,24 @@
         <f t="shared" si="4"/>
         <v>43765</v>
       </c>
-      <c r="C69" s="79" t="s">
+      <c r="C69" s="80" t="s">
         <v>81</v>
       </c>
-      <c r="D69" s="79"/>
-      <c r="E69" s="79"/>
-      <c r="F69" s="79"/>
-      <c r="G69" s="79"/>
-      <c r="H69" s="79"/>
-      <c r="I69" s="79"/>
-      <c r="J69" s="79"/>
-      <c r="K69" s="79"/>
-      <c r="L69" s="79"/>
-      <c r="M69" s="79"/>
-      <c r="N69" s="79"/>
-      <c r="O69" s="79"/>
-      <c r="P69" s="79"/>
-      <c r="Q69" s="79"/>
-      <c r="R69" s="79"/>
+      <c r="D69" s="80"/>
+      <c r="E69" s="80"/>
+      <c r="F69" s="80"/>
+      <c r="G69" s="80"/>
+      <c r="H69" s="80"/>
+      <c r="I69" s="80"/>
+      <c r="J69" s="80"/>
+      <c r="K69" s="80"/>
+      <c r="L69" s="80"/>
+      <c r="M69" s="80"/>
+      <c r="N69" s="80"/>
+      <c r="O69" s="80"/>
+      <c r="P69" s="80"/>
+      <c r="Q69" s="80"/>
+      <c r="R69" s="80"/>
       <c r="S69" s="51"/>
       <c r="T69" s="51"/>
     </row>
@@ -3833,18 +3863,18 @@
         <f>C62+1</f>
         <v>7</v>
       </c>
-      <c r="D72" s="80" t="s">
+      <c r="D72" s="81" t="s">
         <v>42</v>
       </c>
-      <c r="E72" s="80"/>
-      <c r="F72" s="80"/>
+      <c r="E72" s="81"/>
+      <c r="F72" s="81"/>
       <c r="G72" s="15"/>
-      <c r="H72" s="120" t="s">
+      <c r="H72" s="104" t="s">
         <v>82</v>
       </c>
-      <c r="I72" s="120"/>
-      <c r="J72" s="120"/>
-      <c r="K72" s="120"/>
+      <c r="I72" s="104"/>
+      <c r="J72" s="104"/>
+      <c r="K72" s="104"/>
       <c r="L72" s="19"/>
       <c r="M72" s="119" t="s">
         <v>75</v>
@@ -3867,23 +3897,23 @@
       </c>
       <c r="C73" s="32"/>
       <c r="D73" s="20"/>
-      <c r="E73" s="77" t="s">
+      <c r="E73" s="75" t="s">
         <v>66</v>
       </c>
-      <c r="F73" s="77"/>
-      <c r="G73" s="77"/>
-      <c r="H73" s="77"/>
-      <c r="I73" s="77"/>
-      <c r="J73" s="77"/>
+      <c r="F73" s="75"/>
+      <c r="G73" s="75"/>
+      <c r="H73" s="75"/>
+      <c r="I73" s="75"/>
+      <c r="J73" s="75"/>
       <c r="K73" s="49"/>
-      <c r="L73" s="88" t="s">
+      <c r="L73" s="87" t="s">
         <v>66</v>
       </c>
-      <c r="M73" s="89"/>
-      <c r="N73" s="89"/>
-      <c r="O73" s="89"/>
-      <c r="P73" s="89"/>
-      <c r="Q73" s="90"/>
+      <c r="M73" s="88"/>
+      <c r="N73" s="88"/>
+      <c r="O73" s="88"/>
+      <c r="P73" s="88"/>
+      <c r="Q73" s="89"/>
       <c r="R73" s="49"/>
       <c r="S73" s="51"/>
       <c r="T73" s="30" t="s">
@@ -3898,27 +3928,27 @@
         <f t="shared" ref="B74:B79" si="5">B64+7</f>
         <v>43767</v>
       </c>
-      <c r="C74" s="88" t="s">
+      <c r="C74" s="87" t="s">
         <v>78</v>
       </c>
-      <c r="D74" s="90"/>
-      <c r="E74" s="77" t="s">
+      <c r="D74" s="89"/>
+      <c r="E74" s="75" t="s">
         <v>66</v>
       </c>
-      <c r="F74" s="77"/>
-      <c r="G74" s="77"/>
-      <c r="H74" s="77"/>
-      <c r="I74" s="77"/>
-      <c r="J74" s="77"/>
+      <c r="F74" s="75"/>
+      <c r="G74" s="75"/>
+      <c r="H74" s="75"/>
+      <c r="I74" s="75"/>
+      <c r="J74" s="75"/>
       <c r="K74" s="49"/>
-      <c r="L74" s="88" t="s">
+      <c r="L74" s="87" t="s">
         <v>66</v>
       </c>
-      <c r="M74" s="89"/>
-      <c r="N74" s="89"/>
-      <c r="O74" s="89"/>
-      <c r="P74" s="89"/>
-      <c r="Q74" s="90"/>
+      <c r="M74" s="88"/>
+      <c r="N74" s="88"/>
+      <c r="O74" s="88"/>
+      <c r="P74" s="88"/>
+      <c r="Q74" s="89"/>
       <c r="R74" s="20"/>
       <c r="S74" s="51"/>
       <c r="T74" s="53" t="s">
@@ -3935,23 +3965,23 @@
       </c>
       <c r="C75" s="32"/>
       <c r="D75" s="20"/>
-      <c r="E75" s="77" t="s">
+      <c r="E75" s="75" t="s">
         <v>66</v>
       </c>
-      <c r="F75" s="77"/>
-      <c r="G75" s="77"/>
-      <c r="H75" s="77"/>
-      <c r="I75" s="77"/>
-      <c r="J75" s="77"/>
+      <c r="F75" s="75"/>
+      <c r="G75" s="75"/>
+      <c r="H75" s="75"/>
+      <c r="I75" s="75"/>
+      <c r="J75" s="75"/>
       <c r="K75" s="49"/>
-      <c r="L75" s="88" t="s">
+      <c r="L75" s="87" t="s">
         <v>66</v>
       </c>
-      <c r="M75" s="89"/>
-      <c r="N75" s="89"/>
-      <c r="O75" s="89"/>
-      <c r="P75" s="89"/>
-      <c r="Q75" s="90"/>
+      <c r="M75" s="88"/>
+      <c r="N75" s="88"/>
+      <c r="O75" s="88"/>
+      <c r="P75" s="88"/>
+      <c r="Q75" s="89"/>
       <c r="R75" s="49"/>
       <c r="S75" s="51"/>
       <c r="T75" s="52" t="s">
@@ -3966,24 +3996,24 @@
         <f t="shared" si="5"/>
         <v>43769</v>
       </c>
-      <c r="C76" s="79" t="s">
+      <c r="C76" s="80" t="s">
         <v>79</v>
       </c>
-      <c r="D76" s="79"/>
-      <c r="E76" s="79"/>
-      <c r="F76" s="79"/>
-      <c r="G76" s="79"/>
-      <c r="H76" s="79"/>
-      <c r="I76" s="79"/>
-      <c r="J76" s="79"/>
-      <c r="K76" s="79"/>
-      <c r="L76" s="79"/>
-      <c r="M76" s="79"/>
-      <c r="N76" s="79"/>
-      <c r="O76" s="79"/>
-      <c r="P76" s="79"/>
-      <c r="Q76" s="79"/>
-      <c r="R76" s="79"/>
+      <c r="D76" s="80"/>
+      <c r="E76" s="80"/>
+      <c r="F76" s="80"/>
+      <c r="G76" s="80"/>
+      <c r="H76" s="80"/>
+      <c r="I76" s="80"/>
+      <c r="J76" s="80"/>
+      <c r="K76" s="80"/>
+      <c r="L76" s="80"/>
+      <c r="M76" s="80"/>
+      <c r="N76" s="80"/>
+      <c r="O76" s="80"/>
+      <c r="P76" s="80"/>
+      <c r="Q76" s="80"/>
+      <c r="R76" s="80"/>
       <c r="S76" s="51"/>
       <c r="T76" s="18" t="s">
         <v>21</v>
@@ -4008,14 +4038,14 @@
       <c r="I77" s="112"/>
       <c r="J77" s="112"/>
       <c r="K77" s="49"/>
-      <c r="L77" s="95" t="s">
+      <c r="L77" s="94" t="s">
         <v>66</v>
       </c>
-      <c r="M77" s="96"/>
-      <c r="N77" s="96"/>
-      <c r="O77" s="96"/>
-      <c r="P77" s="96"/>
-      <c r="Q77" s="97"/>
+      <c r="M77" s="95"/>
+      <c r="N77" s="95"/>
+      <c r="O77" s="95"/>
+      <c r="P77" s="95"/>
+      <c r="Q77" s="96"/>
       <c r="R77" s="20"/>
       <c r="S77" s="51"/>
       <c r="T77" s="51"/>
@@ -4039,14 +4069,14 @@
       <c r="I78" s="112"/>
       <c r="J78" s="112"/>
       <c r="K78" s="49"/>
-      <c r="L78" s="95" t="s">
+      <c r="L78" s="94" t="s">
         <v>66</v>
       </c>
-      <c r="M78" s="96"/>
-      <c r="N78" s="96"/>
-      <c r="O78" s="96"/>
-      <c r="P78" s="96"/>
-      <c r="Q78" s="97"/>
+      <c r="M78" s="95"/>
+      <c r="N78" s="95"/>
+      <c r="O78" s="95"/>
+      <c r="P78" s="95"/>
+      <c r="Q78" s="96"/>
       <c r="R78" s="49"/>
       <c r="S78" s="51"/>
       <c r="T78" s="51"/>
@@ -4059,24 +4089,24 @@
         <f t="shared" si="5"/>
         <v>43772</v>
       </c>
-      <c r="C79" s="79" t="s">
+      <c r="C79" s="80" t="s">
         <v>81</v>
       </c>
-      <c r="D79" s="79"/>
-      <c r="E79" s="79"/>
-      <c r="F79" s="79"/>
-      <c r="G79" s="79"/>
-      <c r="H79" s="79"/>
-      <c r="I79" s="79"/>
-      <c r="J79" s="79"/>
-      <c r="K79" s="79"/>
-      <c r="L79" s="79"/>
-      <c r="M79" s="79"/>
-      <c r="N79" s="79"/>
-      <c r="O79" s="79"/>
-      <c r="P79" s="79"/>
-      <c r="Q79" s="79"/>
-      <c r="R79" s="79"/>
+      <c r="D79" s="80"/>
+      <c r="E79" s="80"/>
+      <c r="F79" s="80"/>
+      <c r="G79" s="80"/>
+      <c r="H79" s="80"/>
+      <c r="I79" s="80"/>
+      <c r="J79" s="80"/>
+      <c r="K79" s="80"/>
+      <c r="L79" s="80"/>
+      <c r="M79" s="80"/>
+      <c r="N79" s="80"/>
+      <c r="O79" s="80"/>
+      <c r="P79" s="80"/>
+      <c r="Q79" s="80"/>
+      <c r="R79" s="80"/>
       <c r="S79" s="51"/>
       <c r="T79" s="51"/>
     </row>
@@ -4150,11 +4180,11 @@
         <f>C72+1</f>
         <v>8</v>
       </c>
-      <c r="D82" s="80" t="s">
+      <c r="D82" s="81" t="s">
         <v>40</v>
       </c>
-      <c r="E82" s="80"/>
-      <c r="F82" s="80"/>
+      <c r="E82" s="81"/>
+      <c r="F82" s="81"/>
       <c r="G82" s="15"/>
       <c r="H82" s="19"/>
       <c r="I82" s="19"/>
@@ -4179,24 +4209,24 @@
         <f>B73+7</f>
         <v>43773</v>
       </c>
-      <c r="C83" s="79" t="s">
+      <c r="C83" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="D83" s="79"/>
-      <c r="E83" s="79"/>
-      <c r="F83" s="79"/>
-      <c r="G83" s="79"/>
-      <c r="H83" s="85" t="s">
+      <c r="D83" s="80"/>
+      <c r="E83" s="80"/>
+      <c r="F83" s="80"/>
+      <c r="G83" s="80"/>
+      <c r="H83" s="76" t="s">
         <v>66</v>
       </c>
-      <c r="I83" s="86"/>
-      <c r="J83" s="86"/>
-      <c r="K83" s="86"/>
-      <c r="L83" s="86"/>
-      <c r="M83" s="86"/>
-      <c r="N83" s="86"/>
-      <c r="O83" s="86"/>
-      <c r="P83" s="87"/>
+      <c r="I83" s="77"/>
+      <c r="J83" s="77"/>
+      <c r="K83" s="77"/>
+      <c r="L83" s="77"/>
+      <c r="M83" s="77"/>
+      <c r="N83" s="77"/>
+      <c r="O83" s="77"/>
+      <c r="P83" s="78"/>
       <c r="Q83" s="20"/>
       <c r="R83" s="20"/>
       <c r="S83" s="51"/>
@@ -4213,28 +4243,28 @@
         <f t="shared" ref="B84:B89" si="6">B74+7</f>
         <v>43774</v>
       </c>
-      <c r="C84" s="79" t="s">
+      <c r="C84" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="D84" s="79"/>
-      <c r="E84" s="79"/>
-      <c r="F84" s="79"/>
-      <c r="G84" s="79"/>
-      <c r="H84" s="79" t="s">
+      <c r="D84" s="80"/>
+      <c r="E84" s="80"/>
+      <c r="F84" s="80"/>
+      <c r="G84" s="80"/>
+      <c r="H84" s="80" t="s">
         <v>44</v>
       </c>
-      <c r="I84" s="79"/>
-      <c r="J84" s="85" t="s">
+      <c r="I84" s="80"/>
+      <c r="J84" s="76" t="s">
         <v>66</v>
       </c>
-      <c r="K84" s="86"/>
-      <c r="L84" s="86"/>
-      <c r="M84" s="86"/>
-      <c r="N84" s="86"/>
-      <c r="O84" s="86"/>
-      <c r="P84" s="86"/>
-      <c r="Q84" s="86"/>
-      <c r="R84" s="87"/>
+      <c r="K84" s="77"/>
+      <c r="L84" s="77"/>
+      <c r="M84" s="77"/>
+      <c r="N84" s="77"/>
+      <c r="O84" s="77"/>
+      <c r="P84" s="77"/>
+      <c r="Q84" s="77"/>
+      <c r="R84" s="78"/>
       <c r="S84" s="51"/>
       <c r="T84" s="53" t="s">
         <v>19</v>
@@ -4251,17 +4281,17 @@
       </c>
       <c r="C85" s="32"/>
       <c r="D85" s="20"/>
-      <c r="E85" s="85" t="s">
+      <c r="E85" s="76" t="s">
         <v>66</v>
       </c>
-      <c r="F85" s="86"/>
-      <c r="G85" s="86"/>
-      <c r="H85" s="86"/>
-      <c r="I85" s="86"/>
-      <c r="J85" s="86"/>
-      <c r="K85" s="86"/>
-      <c r="L85" s="86"/>
-      <c r="M85" s="87"/>
+      <c r="F85" s="77"/>
+      <c r="G85" s="77"/>
+      <c r="H85" s="77"/>
+      <c r="I85" s="77"/>
+      <c r="J85" s="77"/>
+      <c r="K85" s="77"/>
+      <c r="L85" s="77"/>
+      <c r="M85" s="78"/>
       <c r="N85" s="49"/>
       <c r="O85" s="49"/>
       <c r="P85" s="49"/>
@@ -4281,13 +4311,13 @@
         <f t="shared" si="6"/>
         <v>43776</v>
       </c>
-      <c r="C86" s="81" t="s">
+      <c r="C86" s="120" t="s">
         <v>69</v>
       </c>
-      <c r="D86" s="81"/>
-      <c r="E86" s="81"/>
-      <c r="F86" s="81"/>
-      <c r="G86" s="81"/>
+      <c r="D86" s="120"/>
+      <c r="E86" s="120"/>
+      <c r="F86" s="120"/>
+      <c r="G86" s="120"/>
       <c r="H86" s="49"/>
       <c r="I86" s="49"/>
       <c r="J86" s="49"/>
@@ -4369,24 +4399,24 @@
         <f t="shared" si="6"/>
         <v>43779</v>
       </c>
-      <c r="C89" s="79" t="s">
+      <c r="C89" s="80" t="s">
         <v>81</v>
       </c>
-      <c r="D89" s="79"/>
-      <c r="E89" s="79"/>
-      <c r="F89" s="79"/>
-      <c r="G89" s="79"/>
-      <c r="H89" s="79"/>
-      <c r="I89" s="79"/>
-      <c r="J89" s="79"/>
-      <c r="K89" s="79"/>
-      <c r="L89" s="79"/>
-      <c r="M89" s="79"/>
-      <c r="N89" s="79"/>
-      <c r="O89" s="79"/>
-      <c r="P89" s="79"/>
-      <c r="Q89" s="79"/>
-      <c r="R89" s="79"/>
+      <c r="D89" s="80"/>
+      <c r="E89" s="80"/>
+      <c r="F89" s="80"/>
+      <c r="G89" s="80"/>
+      <c r="H89" s="80"/>
+      <c r="I89" s="80"/>
+      <c r="J89" s="80"/>
+      <c r="K89" s="80"/>
+      <c r="L89" s="80"/>
+      <c r="M89" s="80"/>
+      <c r="N89" s="80"/>
+      <c r="O89" s="80"/>
+      <c r="P89" s="80"/>
+      <c r="Q89" s="80"/>
+      <c r="R89" s="80"/>
       <c r="S89" s="51"/>
       <c r="T89" s="51"/>
       <c r="U89" s="54"/>
@@ -4488,24 +4518,24 @@
         <f>B83+7</f>
         <v>43780</v>
       </c>
-      <c r="C93" s="79" t="s">
+      <c r="C93" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="D93" s="79"/>
-      <c r="E93" s="79"/>
-      <c r="F93" s="79"/>
-      <c r="G93" s="79"/>
-      <c r="H93" s="77" t="s">
+      <c r="D93" s="80"/>
+      <c r="E93" s="80"/>
+      <c r="F93" s="80"/>
+      <c r="G93" s="80"/>
+      <c r="H93" s="75" t="s">
         <v>86</v>
       </c>
-      <c r="I93" s="77"/>
-      <c r="J93" s="77"/>
-      <c r="K93" s="77"/>
-      <c r="L93" s="77"/>
-      <c r="M93" s="77"/>
-      <c r="N93" s="77"/>
-      <c r="O93" s="77"/>
-      <c r="P93" s="77"/>
+      <c r="I93" s="75"/>
+      <c r="J93" s="75"/>
+      <c r="K93" s="75"/>
+      <c r="L93" s="75"/>
+      <c r="M93" s="75"/>
+      <c r="N93" s="75"/>
+      <c r="O93" s="75"/>
+      <c r="P93" s="75"/>
       <c r="Q93" s="20"/>
       <c r="R93" s="20"/>
       <c r="S93" s="51"/>
@@ -4522,24 +4552,24 @@
         <f t="shared" ref="B94:B99" si="7">B84+7</f>
         <v>43781</v>
       </c>
-      <c r="C94" s="79" t="s">
+      <c r="C94" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="D94" s="79"/>
-      <c r="E94" s="79"/>
-      <c r="F94" s="79"/>
-      <c r="G94" s="79"/>
-      <c r="H94" s="77" t="s">
+      <c r="D94" s="80"/>
+      <c r="E94" s="80"/>
+      <c r="F94" s="80"/>
+      <c r="G94" s="80"/>
+      <c r="H94" s="75" t="s">
         <v>86</v>
       </c>
-      <c r="I94" s="77"/>
-      <c r="J94" s="77"/>
-      <c r="K94" s="77"/>
-      <c r="L94" s="77"/>
-      <c r="M94" s="77"/>
-      <c r="N94" s="77"/>
-      <c r="O94" s="77"/>
-      <c r="P94" s="77"/>
+      <c r="I94" s="75"/>
+      <c r="J94" s="75"/>
+      <c r="K94" s="75"/>
+      <c r="L94" s="75"/>
+      <c r="M94" s="75"/>
+      <c r="N94" s="75"/>
+      <c r="O94" s="75"/>
+      <c r="P94" s="75"/>
       <c r="Q94" s="20"/>
       <c r="R94" s="20"/>
       <c r="S94" s="51"/>
@@ -4586,20 +4616,20 @@
         <f t="shared" si="7"/>
         <v>43783</v>
       </c>
-      <c r="C96" s="79" t="s">
+      <c r="C96" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="D96" s="79"/>
-      <c r="E96" s="79"/>
-      <c r="F96" s="79"/>
-      <c r="G96" s="79"/>
-      <c r="H96" s="88" t="s">
+      <c r="D96" s="80"/>
+      <c r="E96" s="80"/>
+      <c r="F96" s="80"/>
+      <c r="G96" s="80"/>
+      <c r="H96" s="87" t="s">
         <v>86</v>
       </c>
-      <c r="I96" s="89"/>
-      <c r="J96" s="89"/>
-      <c r="K96" s="89"/>
-      <c r="L96" s="90"/>
+      <c r="I96" s="88"/>
+      <c r="J96" s="88"/>
+      <c r="K96" s="88"/>
+      <c r="L96" s="89"/>
       <c r="M96" s="20"/>
       <c r="N96" s="20"/>
       <c r="O96" s="20"/>
@@ -4676,24 +4706,24 @@
         <f t="shared" si="7"/>
         <v>43786</v>
       </c>
-      <c r="C99" s="79" t="s">
+      <c r="C99" s="80" t="s">
         <v>81</v>
       </c>
-      <c r="D99" s="79"/>
-      <c r="E99" s="79"/>
-      <c r="F99" s="79"/>
-      <c r="G99" s="79"/>
-      <c r="H99" s="79"/>
-      <c r="I99" s="79"/>
-      <c r="J99" s="79"/>
-      <c r="K99" s="79"/>
-      <c r="L99" s="79"/>
-      <c r="M99" s="79"/>
-      <c r="N99" s="79"/>
-      <c r="O99" s="79"/>
-      <c r="P99" s="79"/>
-      <c r="Q99" s="79"/>
-      <c r="R99" s="79"/>
+      <c r="D99" s="80"/>
+      <c r="E99" s="80"/>
+      <c r="F99" s="80"/>
+      <c r="G99" s="80"/>
+      <c r="H99" s="80"/>
+      <c r="I99" s="80"/>
+      <c r="J99" s="80"/>
+      <c r="K99" s="80"/>
+      <c r="L99" s="80"/>
+      <c r="M99" s="80"/>
+      <c r="N99" s="80"/>
+      <c r="O99" s="80"/>
+      <c r="P99" s="80"/>
+      <c r="Q99" s="80"/>
+      <c r="R99" s="80"/>
       <c r="S99" s="51"/>
       <c r="T99" s="51"/>
       <c r="U99" s="54"/>
@@ -4795,24 +4825,24 @@
         <f>B93+7</f>
         <v>43787</v>
       </c>
-      <c r="C103" s="79" t="s">
+      <c r="C103" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="D103" s="79"/>
-      <c r="E103" s="79"/>
-      <c r="F103" s="79"/>
-      <c r="G103" s="79"/>
-      <c r="H103" s="77" t="s">
+      <c r="D103" s="80"/>
+      <c r="E103" s="80"/>
+      <c r="F103" s="80"/>
+      <c r="G103" s="80"/>
+      <c r="H103" s="75" t="s">
         <v>86</v>
       </c>
-      <c r="I103" s="77"/>
-      <c r="J103" s="77"/>
-      <c r="K103" s="77"/>
-      <c r="L103" s="77"/>
-      <c r="M103" s="77"/>
-      <c r="N103" s="77"/>
-      <c r="O103" s="77"/>
-      <c r="P103" s="77"/>
+      <c r="I103" s="75"/>
+      <c r="J103" s="75"/>
+      <c r="K103" s="75"/>
+      <c r="L103" s="75"/>
+      <c r="M103" s="75"/>
+      <c r="N103" s="75"/>
+      <c r="O103" s="75"/>
+      <c r="P103" s="75"/>
       <c r="Q103" s="20"/>
       <c r="R103" s="20"/>
       <c r="S103" s="51"/>
@@ -4829,24 +4859,24 @@
         <f t="shared" ref="B104:B109" si="8">B94+7</f>
         <v>43788</v>
       </c>
-      <c r="C104" s="79" t="s">
+      <c r="C104" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="D104" s="79"/>
-      <c r="E104" s="79"/>
-      <c r="F104" s="79"/>
-      <c r="G104" s="79"/>
-      <c r="H104" s="77" t="s">
+      <c r="D104" s="80"/>
+      <c r="E104" s="80"/>
+      <c r="F104" s="80"/>
+      <c r="G104" s="80"/>
+      <c r="H104" s="75" t="s">
         <v>86</v>
       </c>
-      <c r="I104" s="77"/>
-      <c r="J104" s="77"/>
-      <c r="K104" s="77"/>
-      <c r="L104" s="77"/>
-      <c r="M104" s="77"/>
-      <c r="N104" s="77"/>
-      <c r="O104" s="77"/>
-      <c r="P104" s="77"/>
+      <c r="I104" s="75"/>
+      <c r="J104" s="75"/>
+      <c r="K104" s="75"/>
+      <c r="L104" s="75"/>
+      <c r="M104" s="75"/>
+      <c r="N104" s="75"/>
+      <c r="O104" s="75"/>
+      <c r="P104" s="75"/>
       <c r="Q104" s="20"/>
       <c r="R104" s="20"/>
       <c r="S104" s="51"/>
@@ -4863,19 +4893,19 @@
         <f t="shared" si="8"/>
         <v>43789</v>
       </c>
-      <c r="C105" s="82" t="s">
+      <c r="C105" s="84" t="s">
         <v>86</v>
       </c>
-      <c r="D105" s="83"/>
-      <c r="E105" s="83"/>
-      <c r="F105" s="83"/>
-      <c r="G105" s="83"/>
-      <c r="H105" s="83"/>
-      <c r="I105" s="83"/>
-      <c r="J105" s="83"/>
-      <c r="K105" s="83"/>
-      <c r="L105" s="83"/>
-      <c r="M105" s="84"/>
+      <c r="D105" s="85"/>
+      <c r="E105" s="85"/>
+      <c r="F105" s="85"/>
+      <c r="G105" s="85"/>
+      <c r="H105" s="85"/>
+      <c r="I105" s="85"/>
+      <c r="J105" s="85"/>
+      <c r="K105" s="85"/>
+      <c r="L105" s="85"/>
+      <c r="M105" s="86"/>
       <c r="N105" s="49"/>
       <c r="O105" s="49"/>
       <c r="P105" s="49"/>
@@ -4895,24 +4925,24 @@
         <f t="shared" si="8"/>
         <v>43790</v>
       </c>
-      <c r="C106" s="79" t="s">
+      <c r="C106" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="D106" s="79"/>
-      <c r="E106" s="79"/>
-      <c r="F106" s="79"/>
-      <c r="G106" s="79"/>
-      <c r="H106" s="77" t="s">
+      <c r="D106" s="80"/>
+      <c r="E106" s="80"/>
+      <c r="F106" s="80"/>
+      <c r="G106" s="80"/>
+      <c r="H106" s="75" t="s">
         <v>86</v>
       </c>
-      <c r="I106" s="77"/>
-      <c r="J106" s="77"/>
-      <c r="K106" s="77"/>
-      <c r="L106" s="77"/>
-      <c r="M106" s="77"/>
-      <c r="N106" s="77"/>
-      <c r="O106" s="77"/>
-      <c r="P106" s="77"/>
+      <c r="I106" s="75"/>
+      <c r="J106" s="75"/>
+      <c r="K106" s="75"/>
+      <c r="L106" s="75"/>
+      <c r="M106" s="75"/>
+      <c r="N106" s="75"/>
+      <c r="O106" s="75"/>
+      <c r="P106" s="75"/>
       <c r="Q106" s="20"/>
       <c r="R106" s="20"/>
       <c r="S106" s="51"/>
@@ -4929,7 +4959,7 @@
         <f t="shared" si="8"/>
         <v>43791</v>
       </c>
-      <c r="C107" s="125" t="s">
+      <c r="C107" s="121" t="s">
         <v>86</v>
       </c>
       <c r="D107" s="110"/>
@@ -4987,24 +5017,24 @@
         <f t="shared" si="8"/>
         <v>43793</v>
       </c>
-      <c r="C109" s="79" t="s">
+      <c r="C109" s="80" t="s">
         <v>81</v>
       </c>
-      <c r="D109" s="79"/>
-      <c r="E109" s="79"/>
-      <c r="F109" s="79"/>
-      <c r="G109" s="79"/>
-      <c r="H109" s="79"/>
-      <c r="I109" s="79"/>
-      <c r="J109" s="79"/>
-      <c r="K109" s="79"/>
-      <c r="L109" s="79"/>
-      <c r="M109" s="79"/>
-      <c r="N109" s="79"/>
-      <c r="O109" s="79"/>
-      <c r="P109" s="79"/>
-      <c r="Q109" s="79"/>
-      <c r="R109" s="79"/>
+      <c r="D109" s="80"/>
+      <c r="E109" s="80"/>
+      <c r="F109" s="80"/>
+      <c r="G109" s="80"/>
+      <c r="H109" s="80"/>
+      <c r="I109" s="80"/>
+      <c r="J109" s="80"/>
+      <c r="K109" s="80"/>
+      <c r="L109" s="80"/>
+      <c r="M109" s="80"/>
+      <c r="N109" s="80"/>
+      <c r="O109" s="80"/>
+      <c r="P109" s="80"/>
+      <c r="Q109" s="80"/>
+      <c r="R109" s="80"/>
       <c r="S109" s="51"/>
       <c r="T109" s="51"/>
       <c r="U109" s="54"/>
@@ -5079,11 +5109,11 @@
         <f>C102+1</f>
         <v>11</v>
       </c>
-      <c r="D112" s="80" t="s">
+      <c r="D112" s="81" t="s">
         <v>43</v>
       </c>
-      <c r="E112" s="80"/>
-      <c r="F112" s="80"/>
+      <c r="E112" s="81"/>
+      <c r="F112" s="81"/>
       <c r="G112" s="15"/>
       <c r="H112" s="15"/>
       <c r="I112" s="15"/>
@@ -5108,21 +5138,21 @@
         <f>B103+7</f>
         <v>43794</v>
       </c>
-      <c r="C113" s="79" t="s">
+      <c r="C113" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="D113" s="79"/>
-      <c r="E113" s="79"/>
-      <c r="F113" s="79"/>
-      <c r="G113" s="79"/>
-      <c r="H113" s="77" t="s">
+      <c r="D113" s="80"/>
+      <c r="E113" s="80"/>
+      <c r="F113" s="80"/>
+      <c r="G113" s="80"/>
+      <c r="H113" s="75" t="s">
         <v>86</v>
       </c>
-      <c r="I113" s="77"/>
-      <c r="J113" s="77"/>
-      <c r="K113" s="77"/>
-      <c r="L113" s="77"/>
-      <c r="M113" s="77"/>
+      <c r="I113" s="75"/>
+      <c r="J113" s="75"/>
+      <c r="K113" s="75"/>
+      <c r="L113" s="75"/>
+      <c r="M113" s="75"/>
       <c r="N113" s="20"/>
       <c r="O113" s="20"/>
       <c r="P113" s="20"/>
@@ -5142,21 +5172,21 @@
         <f t="shared" ref="B114:B119" si="9">B104+7</f>
         <v>43795</v>
       </c>
-      <c r="C114" s="79" t="s">
+      <c r="C114" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="D114" s="79"/>
-      <c r="E114" s="79"/>
-      <c r="F114" s="79"/>
-      <c r="G114" s="79"/>
-      <c r="H114" s="77" t="s">
+      <c r="D114" s="80"/>
+      <c r="E114" s="80"/>
+      <c r="F114" s="80"/>
+      <c r="G114" s="80"/>
+      <c r="H114" s="75" t="s">
         <v>86</v>
       </c>
-      <c r="I114" s="77"/>
-      <c r="J114" s="77"/>
-      <c r="K114" s="77"/>
-      <c r="L114" s="77"/>
-      <c r="M114" s="77"/>
+      <c r="I114" s="75"/>
+      <c r="J114" s="75"/>
+      <c r="K114" s="75"/>
+      <c r="L114" s="75"/>
+      <c r="M114" s="75"/>
       <c r="N114" s="20"/>
       <c r="O114" s="49"/>
       <c r="P114" s="49"/>
@@ -5176,26 +5206,24 @@
         <f t="shared" si="9"/>
         <v>43796</v>
       </c>
-      <c r="C115" s="32"/>
-      <c r="D115" s="20"/>
-      <c r="E115" s="70" t="s">
+      <c r="C115" s="50"/>
+      <c r="D115" s="49"/>
+      <c r="E115" s="49"/>
+      <c r="F115" s="49"/>
+      <c r="G115" s="49"/>
+      <c r="H115" s="20"/>
+      <c r="I115" s="76" t="s">
         <v>86</v>
       </c>
-      <c r="F115" s="70"/>
-      <c r="G115" s="70"/>
-      <c r="H115" s="70"/>
-      <c r="I115" s="70"/>
-      <c r="J115" s="70"/>
-      <c r="K115" s="49"/>
-      <c r="L115" s="71" t="s">
-        <v>86</v>
-      </c>
-      <c r="M115" s="72"/>
-      <c r="N115" s="72"/>
-      <c r="O115" s="72"/>
-      <c r="P115" s="72"/>
-      <c r="Q115" s="73"/>
-      <c r="R115" s="49"/>
+      <c r="J115" s="77"/>
+      <c r="K115" s="77"/>
+      <c r="L115" s="77"/>
+      <c r="M115" s="77"/>
+      <c r="N115" s="77"/>
+      <c r="O115" s="77"/>
+      <c r="P115" s="77"/>
+      <c r="Q115" s="77"/>
+      <c r="R115" s="78"/>
       <c r="S115" s="51"/>
       <c r="T115" s="52" t="s">
         <v>20</v>
@@ -5210,27 +5238,27 @@
         <f t="shared" si="9"/>
         <v>43797</v>
       </c>
-      <c r="C116" s="79" t="s">
+      <c r="C116" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="D116" s="79"/>
-      <c r="E116" s="79"/>
-      <c r="F116" s="79"/>
-      <c r="G116" s="79"/>
-      <c r="H116" s="70" t="s">
-        <v>55</v>
-      </c>
-      <c r="I116" s="70"/>
-      <c r="J116" s="70"/>
-      <c r="K116" s="74" t="s">
-        <v>86</v>
-      </c>
-      <c r="L116" s="75"/>
-      <c r="M116" s="75"/>
-      <c r="N116" s="75"/>
-      <c r="O116" s="75"/>
-      <c r="P116" s="75"/>
-      <c r="Q116" s="121"/>
+      <c r="D116" s="80"/>
+      <c r="E116" s="80"/>
+      <c r="F116" s="80"/>
+      <c r="G116" s="80"/>
+      <c r="H116" s="87" t="s">
+        <v>89</v>
+      </c>
+      <c r="I116" s="89"/>
+      <c r="J116" s="76" t="s">
+        <v>65</v>
+      </c>
+      <c r="K116" s="77"/>
+      <c r="L116" s="77"/>
+      <c r="M116" s="77"/>
+      <c r="N116" s="78"/>
+      <c r="O116" s="20"/>
+      <c r="P116" s="20"/>
+      <c r="Q116" s="20"/>
       <c r="R116" s="20"/>
       <c r="S116" s="51"/>
       <c r="T116" s="18" t="s">
@@ -5302,24 +5330,24 @@
         <f t="shared" si="9"/>
         <v>43800</v>
       </c>
-      <c r="C119" s="79" t="s">
+      <c r="C119" s="80" t="s">
         <v>81</v>
       </c>
-      <c r="D119" s="79"/>
-      <c r="E119" s="79"/>
-      <c r="F119" s="79"/>
-      <c r="G119" s="79"/>
-      <c r="H119" s="79"/>
-      <c r="I119" s="79"/>
-      <c r="J119" s="79"/>
-      <c r="K119" s="79"/>
-      <c r="L119" s="79"/>
-      <c r="M119" s="79"/>
-      <c r="N119" s="79"/>
-      <c r="O119" s="79"/>
-      <c r="P119" s="79"/>
-      <c r="Q119" s="79"/>
-      <c r="R119" s="79"/>
+      <c r="D119" s="80"/>
+      <c r="E119" s="80"/>
+      <c r="F119" s="80"/>
+      <c r="G119" s="80"/>
+      <c r="H119" s="80"/>
+      <c r="I119" s="80"/>
+      <c r="J119" s="80"/>
+      <c r="K119" s="80"/>
+      <c r="L119" s="80"/>
+      <c r="M119" s="80"/>
+      <c r="N119" s="80"/>
+      <c r="O119" s="80"/>
+      <c r="P119" s="80"/>
+      <c r="Q119" s="80"/>
+      <c r="R119" s="80"/>
       <c r="S119" s="51"/>
       <c r="T119" s="51"/>
       <c r="U119" s="54"/>
@@ -5394,11 +5422,11 @@
         <f>C112+1</f>
         <v>12</v>
       </c>
-      <c r="D122" s="80" t="s">
+      <c r="D122" s="104" t="s">
         <v>41</v>
       </c>
-      <c r="E122" s="80"/>
-      <c r="F122" s="80"/>
+      <c r="E122" s="104"/>
+      <c r="F122" s="104"/>
       <c r="G122" s="15"/>
       <c r="H122" s="15"/>
       <c r="I122" s="15"/>
@@ -5419,28 +5447,28 @@
       <c r="A123" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B123" s="57">
+      <c r="B123" s="69">
         <f>B113+7</f>
         <v>43801</v>
       </c>
-      <c r="C123" s="79" t="s">
+      <c r="C123" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="D123" s="79"/>
-      <c r="E123" s="79"/>
-      <c r="F123" s="79"/>
-      <c r="G123" s="79"/>
+      <c r="D123" s="82"/>
+      <c r="E123" s="82"/>
+      <c r="F123" s="82"/>
+      <c r="G123" s="82"/>
       <c r="H123" s="74" t="s">
-        <v>65</v>
-      </c>
-      <c r="I123" s="75"/>
-      <c r="J123" s="75"/>
-      <c r="K123" s="75"/>
-      <c r="L123" s="75"/>
-      <c r="M123" s="75"/>
-      <c r="N123" s="75"/>
-      <c r="O123" s="75"/>
-      <c r="P123" s="76"/>
+        <v>87</v>
+      </c>
+      <c r="I123" s="74"/>
+      <c r="J123" s="74"/>
+      <c r="K123" s="74"/>
+      <c r="L123" s="74"/>
+      <c r="M123" s="74"/>
+      <c r="N123" s="74"/>
+      <c r="O123" s="74"/>
+      <c r="P123" s="74"/>
       <c r="Q123" s="20"/>
       <c r="R123" s="20"/>
       <c r="S123" s="51"/>
@@ -5453,28 +5481,28 @@
       <c r="A124" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B124" s="57">
+      <c r="B124" s="69">
         <f t="shared" ref="B124:B129" si="10">B114+7</f>
         <v>43802</v>
       </c>
-      <c r="C124" s="79" t="s">
+      <c r="C124" s="82" t="s">
         <v>37</v>
       </c>
-      <c r="D124" s="79"/>
-      <c r="E124" s="79"/>
-      <c r="F124" s="79"/>
-      <c r="G124" s="79"/>
+      <c r="D124" s="82"/>
+      <c r="E124" s="82"/>
+      <c r="F124" s="82"/>
+      <c r="G124" s="82"/>
       <c r="H124" s="74" t="s">
         <v>65</v>
       </c>
-      <c r="I124" s="75"/>
-      <c r="J124" s="75"/>
-      <c r="K124" s="75"/>
-      <c r="L124" s="75"/>
-      <c r="M124" s="75"/>
-      <c r="N124" s="75"/>
-      <c r="O124" s="75"/>
-      <c r="P124" s="76"/>
+      <c r="I124" s="74"/>
+      <c r="J124" s="74"/>
+      <c r="K124" s="74"/>
+      <c r="L124" s="74"/>
+      <c r="M124" s="74"/>
+      <c r="N124" s="74"/>
+      <c r="O124" s="74"/>
+      <c r="P124" s="74"/>
       <c r="Q124" s="20"/>
       <c r="R124" s="20"/>
       <c r="S124" s="51"/>
@@ -5487,26 +5515,28 @@
       <c r="A125" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B125" s="57">
+      <c r="B125" s="69">
         <f t="shared" si="10"/>
         <v>43803</v>
       </c>
       <c r="C125" s="74" t="s">
         <v>65</v>
       </c>
-      <c r="D125" s="75"/>
-      <c r="E125" s="75"/>
-      <c r="F125" s="75"/>
-      <c r="G125" s="75"/>
-      <c r="H125" s="75"/>
-      <c r="I125" s="75"/>
-      <c r="J125" s="75"/>
-      <c r="K125" s="76"/>
+      <c r="D125" s="74"/>
+      <c r="E125" s="74"/>
+      <c r="F125" s="74"/>
+      <c r="G125" s="74"/>
+      <c r="H125" s="74"/>
+      <c r="I125" s="74"/>
+      <c r="J125" s="74"/>
+      <c r="K125" s="74"/>
       <c r="L125" s="49"/>
-      <c r="M125" s="49"/>
-      <c r="N125" s="49"/>
-      <c r="O125" s="49"/>
-      <c r="P125" s="49"/>
+      <c r="M125" s="74" t="s">
+        <v>65</v>
+      </c>
+      <c r="N125" s="74"/>
+      <c r="O125" s="74"/>
+      <c r="P125" s="74"/>
       <c r="Q125" s="49"/>
       <c r="R125" s="49"/>
       <c r="S125" s="51"/>
@@ -5519,17 +5549,17 @@
       <c r="A126" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B126" s="57">
+      <c r="B126" s="69">
         <f t="shared" si="10"/>
         <v>43804</v>
       </c>
-      <c r="C126" s="81" t="s">
+      <c r="C126" s="83" t="s">
         <v>80</v>
       </c>
-      <c r="D126" s="81"/>
-      <c r="E126" s="81"/>
-      <c r="F126" s="81"/>
-      <c r="G126" s="81"/>
+      <c r="D126" s="83"/>
+      <c r="E126" s="83"/>
+      <c r="F126" s="83"/>
+      <c r="G126" s="83"/>
       <c r="H126" s="49"/>
       <c r="I126" s="49"/>
       <c r="J126" s="49"/>
@@ -5611,24 +5641,24 @@
         <f t="shared" si="10"/>
         <v>43807</v>
       </c>
-      <c r="C129" s="79" t="s">
+      <c r="C129" s="80" t="s">
         <v>81</v>
       </c>
-      <c r="D129" s="79"/>
-      <c r="E129" s="79"/>
-      <c r="F129" s="79"/>
-      <c r="G129" s="79"/>
-      <c r="H129" s="79"/>
-      <c r="I129" s="79"/>
-      <c r="J129" s="79"/>
-      <c r="K129" s="79"/>
-      <c r="L129" s="79"/>
-      <c r="M129" s="79"/>
-      <c r="N129" s="79"/>
-      <c r="O129" s="79"/>
-      <c r="P129" s="79"/>
-      <c r="Q129" s="79"/>
-      <c r="R129" s="79"/>
+      <c r="D129" s="80"/>
+      <c r="E129" s="80"/>
+      <c r="F129" s="80"/>
+      <c r="G129" s="80"/>
+      <c r="H129" s="80"/>
+      <c r="I129" s="80"/>
+      <c r="J129" s="80"/>
+      <c r="K129" s="80"/>
+      <c r="L129" s="80"/>
+      <c r="M129" s="80"/>
+      <c r="N129" s="80"/>
+      <c r="O129" s="80"/>
+      <c r="P129" s="80"/>
+      <c r="Q129" s="80"/>
+      <c r="R129" s="80"/>
       <c r="S129" s="51"/>
       <c r="T129" s="51"/>
       <c r="U129" s="54"/>
@@ -5730,22 +5760,24 @@
         <f>B123+7</f>
         <v>43808</v>
       </c>
-      <c r="C133" s="79" t="s">
+      <c r="C133" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="D133" s="79"/>
-      <c r="E133" s="79"/>
-      <c r="F133" s="79"/>
-      <c r="G133" s="79"/>
-      <c r="H133" s="49"/>
-      <c r="I133" s="49"/>
-      <c r="J133" s="49"/>
-      <c r="K133" s="20"/>
-      <c r="L133" s="20"/>
-      <c r="M133" s="20"/>
-      <c r="N133" s="20"/>
-      <c r="O133" s="20"/>
-      <c r="P133" s="20"/>
+      <c r="D133" s="80"/>
+      <c r="E133" s="80"/>
+      <c r="F133" s="80"/>
+      <c r="G133" s="80"/>
+      <c r="H133" s="74" t="s">
+        <v>87</v>
+      </c>
+      <c r="I133" s="74"/>
+      <c r="J133" s="74"/>
+      <c r="K133" s="74"/>
+      <c r="L133" s="74"/>
+      <c r="M133" s="74"/>
+      <c r="N133" s="74"/>
+      <c r="O133" s="74"/>
+      <c r="P133" s="74"/>
       <c r="Q133" s="20"/>
       <c r="R133" s="20"/>
       <c r="S133" s="51"/>
@@ -5762,22 +5794,24 @@
         <f t="shared" ref="B134:B139" si="11">B124+7</f>
         <v>43809</v>
       </c>
-      <c r="C134" s="79" t="s">
+      <c r="C134" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="D134" s="79"/>
-      <c r="E134" s="79"/>
-      <c r="F134" s="79"/>
-      <c r="G134" s="79"/>
-      <c r="H134" s="20"/>
-      <c r="I134" s="20"/>
-      <c r="J134" s="20"/>
-      <c r="K134" s="49"/>
-      <c r="L134" s="49"/>
-      <c r="M134" s="20"/>
-      <c r="N134" s="20"/>
-      <c r="O134" s="49"/>
-      <c r="P134" s="49"/>
+      <c r="D134" s="80"/>
+      <c r="E134" s="80"/>
+      <c r="F134" s="80"/>
+      <c r="G134" s="80"/>
+      <c r="H134" s="74" t="s">
+        <v>66</v>
+      </c>
+      <c r="I134" s="74"/>
+      <c r="J134" s="74"/>
+      <c r="K134" s="74"/>
+      <c r="L134" s="74"/>
+      <c r="M134" s="74"/>
+      <c r="N134" s="74"/>
+      <c r="O134" s="74"/>
+      <c r="P134" s="74"/>
       <c r="Q134" s="20"/>
       <c r="R134" s="20"/>
       <c r="S134" s="51"/>
@@ -5794,20 +5828,24 @@
         <f t="shared" si="11"/>
         <v>43810</v>
       </c>
-      <c r="C135" s="32"/>
-      <c r="D135" s="20"/>
-      <c r="E135" s="20"/>
-      <c r="F135" s="20"/>
-      <c r="G135" s="20"/>
-      <c r="H135" s="20"/>
-      <c r="I135" s="20"/>
-      <c r="J135" s="20"/>
-      <c r="K135" s="49"/>
+      <c r="C135" s="123" t="s">
+        <v>66</v>
+      </c>
+      <c r="D135" s="124"/>
+      <c r="E135" s="124"/>
+      <c r="F135" s="124"/>
+      <c r="G135" s="124"/>
+      <c r="H135" s="124"/>
+      <c r="I135" s="124"/>
+      <c r="J135" s="124"/>
+      <c r="K135" s="125"/>
       <c r="L135" s="49"/>
-      <c r="M135" s="49"/>
-      <c r="N135" s="49"/>
-      <c r="O135" s="49"/>
-      <c r="P135" s="49"/>
+      <c r="M135" s="74" t="s">
+        <v>66</v>
+      </c>
+      <c r="N135" s="74"/>
+      <c r="O135" s="74"/>
+      <c r="P135" s="74"/>
       <c r="Q135" s="49"/>
       <c r="R135" s="49"/>
       <c r="S135" s="51"/>
@@ -5824,21 +5862,21 @@
         <f t="shared" si="11"/>
         <v>43811</v>
       </c>
-      <c r="C136" s="79" t="s">
-        <v>37</v>
-      </c>
-      <c r="D136" s="79"/>
-      <c r="E136" s="79"/>
-      <c r="F136" s="79"/>
-      <c r="G136" s="79"/>
+      <c r="C136" s="80" t="s">
+        <v>69</v>
+      </c>
+      <c r="D136" s="80"/>
+      <c r="E136" s="80"/>
+      <c r="F136" s="80"/>
+      <c r="G136" s="80"/>
       <c r="H136" s="20"/>
       <c r="I136" s="49"/>
       <c r="J136" s="49"/>
       <c r="K136" s="49"/>
       <c r="L136" s="49"/>
-      <c r="M136" s="20"/>
-      <c r="N136" s="20"/>
-      <c r="O136" s="20"/>
+      <c r="M136" s="49"/>
+      <c r="N136" s="49"/>
+      <c r="O136" s="49"/>
       <c r="P136" s="20"/>
       <c r="Q136" s="20"/>
       <c r="R136" s="20"/>
@@ -5866,10 +5904,10 @@
       <c r="J137" s="20"/>
       <c r="K137" s="49"/>
       <c r="L137" s="49"/>
-      <c r="M137" s="20"/>
-      <c r="N137" s="20"/>
-      <c r="O137" s="20"/>
-      <c r="P137" s="20"/>
+      <c r="M137" s="49"/>
+      <c r="N137" s="49"/>
+      <c r="O137" s="49"/>
+      <c r="P137" s="49"/>
       <c r="Q137" s="20"/>
       <c r="R137" s="20"/>
       <c r="S137" s="51"/>
@@ -5912,24 +5950,24 @@
         <f t="shared" si="11"/>
         <v>43814</v>
       </c>
-      <c r="C139" s="79" t="s">
+      <c r="C139" s="80" t="s">
         <v>81</v>
       </c>
-      <c r="D139" s="79"/>
-      <c r="E139" s="79"/>
-      <c r="F139" s="79"/>
-      <c r="G139" s="79"/>
-      <c r="H139" s="79"/>
-      <c r="I139" s="79"/>
-      <c r="J139" s="79"/>
-      <c r="K139" s="79"/>
-      <c r="L139" s="79"/>
-      <c r="M139" s="79"/>
-      <c r="N139" s="79"/>
-      <c r="O139" s="79"/>
-      <c r="P139" s="79"/>
-      <c r="Q139" s="79"/>
-      <c r="R139" s="79"/>
+      <c r="D139" s="80"/>
+      <c r="E139" s="80"/>
+      <c r="F139" s="80"/>
+      <c r="G139" s="80"/>
+      <c r="H139" s="80"/>
+      <c r="I139" s="80"/>
+      <c r="J139" s="80"/>
+      <c r="K139" s="80"/>
+      <c r="L139" s="80"/>
+      <c r="M139" s="80"/>
+      <c r="N139" s="80"/>
+      <c r="O139" s="80"/>
+      <c r="P139" s="80"/>
+      <c r="Q139" s="80"/>
+      <c r="R139" s="80"/>
       <c r="S139" s="51"/>
       <c r="T139" s="51"/>
       <c r="U139" s="54"/>
@@ -6024,19 +6062,19 @@
         <f>C132+1</f>
         <v>14</v>
       </c>
-      <c r="D142" s="80" t="s">
+      <c r="D142" s="81" t="s">
         <v>30</v>
       </c>
-      <c r="E142" s="80"/>
-      <c r="F142" s="80"/>
+      <c r="E142" s="81"/>
+      <c r="F142" s="81"/>
       <c r="G142" s="15"/>
-      <c r="H142" s="80" t="s">
+      <c r="H142" s="81" t="s">
         <v>52</v>
       </c>
-      <c r="I142" s="80"/>
-      <c r="J142" s="80"/>
-      <c r="K142" s="80"/>
-      <c r="L142" s="80"/>
+      <c r="I142" s="81"/>
+      <c r="J142" s="81"/>
+      <c r="K142" s="81"/>
+      <c r="L142" s="81"/>
       <c r="M142" s="19"/>
       <c r="N142" s="19"/>
       <c r="O142" s="19"/>
@@ -6055,22 +6093,22 @@
         <f>B133+7</f>
         <v>43815</v>
       </c>
-      <c r="C143" s="70" t="s">
+      <c r="C143" s="122" t="s">
         <v>55</v>
       </c>
-      <c r="D143" s="70"/>
-      <c r="E143" s="70"/>
-      <c r="F143" s="20"/>
-      <c r="G143" s="20"/>
-      <c r="H143" s="20"/>
+      <c r="D143" s="122"/>
+      <c r="E143" s="122"/>
+      <c r="F143" s="49"/>
+      <c r="G143" s="49"/>
+      <c r="H143" s="49"/>
       <c r="I143" s="49"/>
       <c r="J143" s="49"/>
-      <c r="K143" s="49"/>
-      <c r="L143" s="49"/>
-      <c r="M143" s="49"/>
-      <c r="N143" s="49"/>
-      <c r="O143" s="49"/>
-      <c r="P143" s="49"/>
+      <c r="K143" s="20"/>
+      <c r="L143" s="20"/>
+      <c r="M143" s="20"/>
+      <c r="N143" s="20"/>
+      <c r="O143" s="20"/>
+      <c r="P143" s="20"/>
       <c r="Q143" s="49"/>
       <c r="R143" s="49"/>
       <c r="S143" s="51"/>
@@ -6087,20 +6125,22 @@
         <f t="shared" ref="B144:B149" si="12">B134+7</f>
         <v>43816</v>
       </c>
-      <c r="C144" s="32"/>
-      <c r="D144" s="20"/>
-      <c r="E144" s="20"/>
-      <c r="F144" s="20"/>
-      <c r="G144" s="20"/>
-      <c r="H144" s="20"/>
-      <c r="I144" s="20"/>
-      <c r="J144" s="20"/>
-      <c r="K144" s="49"/>
-      <c r="L144" s="49"/>
-      <c r="M144" s="20"/>
-      <c r="N144" s="20"/>
-      <c r="O144" s="20"/>
-      <c r="P144" s="20"/>
+      <c r="C144" s="70" t="s">
+        <v>88</v>
+      </c>
+      <c r="D144" s="71"/>
+      <c r="E144" s="71"/>
+      <c r="F144" s="71"/>
+      <c r="G144" s="71"/>
+      <c r="H144" s="71"/>
+      <c r="I144" s="71"/>
+      <c r="J144" s="71"/>
+      <c r="K144" s="71"/>
+      <c r="L144" s="71"/>
+      <c r="M144" s="71"/>
+      <c r="N144" s="71"/>
+      <c r="O144" s="71"/>
+      <c r="P144" s="72"/>
       <c r="Q144" s="20"/>
       <c r="R144" s="20"/>
       <c r="S144" s="51"/>
@@ -6117,20 +6157,22 @@
         <f t="shared" si="12"/>
         <v>43817</v>
       </c>
-      <c r="C145" s="32"/>
-      <c r="D145" s="20"/>
-      <c r="E145" s="20"/>
-      <c r="F145" s="20"/>
-      <c r="G145" s="20"/>
-      <c r="H145" s="20"/>
-      <c r="I145" s="20"/>
-      <c r="J145" s="20"/>
-      <c r="K145" s="49"/>
-      <c r="L145" s="49"/>
-      <c r="M145" s="49"/>
-      <c r="N145" s="49"/>
-      <c r="O145" s="49"/>
-      <c r="P145" s="49"/>
+      <c r="C145" s="70" t="s">
+        <v>88</v>
+      </c>
+      <c r="D145" s="71"/>
+      <c r="E145" s="71"/>
+      <c r="F145" s="71"/>
+      <c r="G145" s="71"/>
+      <c r="H145" s="71"/>
+      <c r="I145" s="71"/>
+      <c r="J145" s="71"/>
+      <c r="K145" s="71"/>
+      <c r="L145" s="71"/>
+      <c r="M145" s="71"/>
+      <c r="N145" s="71"/>
+      <c r="O145" s="71"/>
+      <c r="P145" s="72"/>
       <c r="Q145" s="49"/>
       <c r="R145" s="49"/>
       <c r="S145" s="51"/>
@@ -6147,20 +6189,22 @@
         <f t="shared" si="12"/>
         <v>43818</v>
       </c>
-      <c r="C146" s="49"/>
-      <c r="D146" s="49"/>
-      <c r="E146" s="49"/>
-      <c r="F146" s="49"/>
-      <c r="G146" s="49"/>
-      <c r="H146" s="49"/>
-      <c r="I146" s="49"/>
-      <c r="J146" s="49"/>
-      <c r="K146" s="49"/>
-      <c r="L146" s="49"/>
-      <c r="M146" s="20"/>
-      <c r="N146" s="20"/>
-      <c r="O146" s="20"/>
-      <c r="P146" s="20"/>
+      <c r="C146" s="70" t="s">
+        <v>88</v>
+      </c>
+      <c r="D146" s="71"/>
+      <c r="E146" s="71"/>
+      <c r="F146" s="71"/>
+      <c r="G146" s="71"/>
+      <c r="H146" s="71"/>
+      <c r="I146" s="71"/>
+      <c r="J146" s="71"/>
+      <c r="K146" s="71"/>
+      <c r="L146" s="71"/>
+      <c r="M146" s="71"/>
+      <c r="N146" s="71"/>
+      <c r="O146" s="71"/>
+      <c r="P146" s="72"/>
       <c r="Q146" s="20"/>
       <c r="R146" s="20"/>
       <c r="S146" s="51"/>
@@ -6177,20 +6221,22 @@
         <f t="shared" si="12"/>
         <v>43819</v>
       </c>
-      <c r="C147" s="20"/>
-      <c r="D147" s="20"/>
-      <c r="E147" s="20"/>
-      <c r="F147" s="20"/>
-      <c r="G147" s="20"/>
-      <c r="H147" s="20"/>
-      <c r="I147" s="49"/>
-      <c r="J147" s="49"/>
-      <c r="K147" s="49"/>
-      <c r="L147" s="49"/>
-      <c r="M147" s="20"/>
-      <c r="N147" s="20"/>
-      <c r="O147" s="20"/>
-      <c r="P147" s="20"/>
+      <c r="C147" s="70" t="s">
+        <v>88</v>
+      </c>
+      <c r="D147" s="71"/>
+      <c r="E147" s="71"/>
+      <c r="F147" s="71"/>
+      <c r="G147" s="71"/>
+      <c r="H147" s="71"/>
+      <c r="I147" s="71"/>
+      <c r="J147" s="71"/>
+      <c r="K147" s="71"/>
+      <c r="L147" s="71"/>
+      <c r="M147" s="71"/>
+      <c r="N147" s="71"/>
+      <c r="O147" s="71"/>
+      <c r="P147" s="72"/>
       <c r="Q147" s="20"/>
       <c r="R147" s="20"/>
       <c r="S147" s="51"/>
@@ -6205,20 +6251,22 @@
         <f t="shared" si="12"/>
         <v>43820</v>
       </c>
-      <c r="C148" s="50"/>
-      <c r="D148" s="49"/>
-      <c r="E148" s="49"/>
-      <c r="F148" s="49"/>
-      <c r="G148" s="49"/>
-      <c r="H148" s="49"/>
-      <c r="I148" s="49"/>
-      <c r="J148" s="49"/>
-      <c r="K148" s="49"/>
-      <c r="L148" s="49"/>
-      <c r="M148" s="49"/>
-      <c r="N148" s="49"/>
-      <c r="O148" s="49"/>
-      <c r="P148" s="49"/>
+      <c r="C148" s="70" t="s">
+        <v>88</v>
+      </c>
+      <c r="D148" s="71"/>
+      <c r="E148" s="71"/>
+      <c r="F148" s="71"/>
+      <c r="G148" s="71"/>
+      <c r="H148" s="71"/>
+      <c r="I148" s="71"/>
+      <c r="J148" s="71"/>
+      <c r="K148" s="71"/>
+      <c r="L148" s="71"/>
+      <c r="M148" s="71"/>
+      <c r="N148" s="71"/>
+      <c r="O148" s="71"/>
+      <c r="P148" s="72"/>
       <c r="Q148" s="49"/>
       <c r="R148" s="49"/>
       <c r="S148" s="51"/>
@@ -6370,20 +6418,22 @@
         <f>B143+7</f>
         <v>43822</v>
       </c>
-      <c r="C153" s="32"/>
-      <c r="D153" s="20"/>
-      <c r="E153" s="20"/>
-      <c r="F153" s="20"/>
-      <c r="G153" s="20"/>
-      <c r="H153" s="20"/>
-      <c r="I153" s="49"/>
-      <c r="J153" s="49"/>
-      <c r="K153" s="49"/>
-      <c r="L153" s="49"/>
-      <c r="M153" s="49"/>
-      <c r="N153" s="49"/>
-      <c r="O153" s="49"/>
-      <c r="P153" s="49"/>
+      <c r="C153" s="70" t="s">
+        <v>88</v>
+      </c>
+      <c r="D153" s="71"/>
+      <c r="E153" s="71"/>
+      <c r="F153" s="71"/>
+      <c r="G153" s="71"/>
+      <c r="H153" s="71"/>
+      <c r="I153" s="71"/>
+      <c r="J153" s="71"/>
+      <c r="K153" s="71"/>
+      <c r="L153" s="71"/>
+      <c r="M153" s="71"/>
+      <c r="N153" s="71"/>
+      <c r="O153" s="71"/>
+      <c r="P153" s="72"/>
       <c r="Q153" s="49"/>
       <c r="R153" s="49"/>
       <c r="S153" s="51"/>
@@ -6400,20 +6450,22 @@
         <f t="shared" ref="B154:B159" si="13">B144+7</f>
         <v>43823</v>
       </c>
-      <c r="C154" s="32"/>
-      <c r="D154" s="20"/>
-      <c r="E154" s="20"/>
-      <c r="F154" s="20"/>
-      <c r="G154" s="20"/>
-      <c r="H154" s="20"/>
-      <c r="I154" s="20"/>
-      <c r="J154" s="20"/>
-      <c r="K154" s="49"/>
-      <c r="L154" s="49"/>
-      <c r="M154" s="20"/>
-      <c r="N154" s="20"/>
-      <c r="O154" s="20"/>
-      <c r="P154" s="20"/>
+      <c r="C154" s="70" t="s">
+        <v>88</v>
+      </c>
+      <c r="D154" s="71"/>
+      <c r="E154" s="71"/>
+      <c r="F154" s="71"/>
+      <c r="G154" s="71"/>
+      <c r="H154" s="71"/>
+      <c r="I154" s="71"/>
+      <c r="J154" s="71"/>
+      <c r="K154" s="71"/>
+      <c r="L154" s="71"/>
+      <c r="M154" s="71"/>
+      <c r="N154" s="71"/>
+      <c r="O154" s="71"/>
+      <c r="P154" s="72"/>
       <c r="Q154" s="20"/>
       <c r="R154" s="20"/>
       <c r="S154" s="51"/>
@@ -6430,24 +6482,24 @@
         <f t="shared" si="13"/>
         <v>43824</v>
       </c>
-      <c r="C155" s="78" t="s">
+      <c r="C155" s="79" t="s">
         <v>53</v>
       </c>
-      <c r="D155" s="78"/>
-      <c r="E155" s="78"/>
-      <c r="F155" s="78"/>
-      <c r="G155" s="78"/>
-      <c r="H155" s="78"/>
-      <c r="I155" s="78"/>
-      <c r="J155" s="78"/>
-      <c r="K155" s="78"/>
-      <c r="L155" s="78"/>
-      <c r="M155" s="78"/>
-      <c r="N155" s="78"/>
-      <c r="O155" s="78"/>
-      <c r="P155" s="78"/>
-      <c r="Q155" s="78"/>
-      <c r="R155" s="78"/>
+      <c r="D155" s="79"/>
+      <c r="E155" s="79"/>
+      <c r="F155" s="79"/>
+      <c r="G155" s="79"/>
+      <c r="H155" s="79"/>
+      <c r="I155" s="79"/>
+      <c r="J155" s="79"/>
+      <c r="K155" s="79"/>
+      <c r="L155" s="79"/>
+      <c r="M155" s="79"/>
+      <c r="N155" s="79"/>
+      <c r="O155" s="79"/>
+      <c r="P155" s="79"/>
+      <c r="Q155" s="79"/>
+      <c r="R155" s="79"/>
       <c r="S155" s="51"/>
       <c r="T155" s="52" t="s">
         <v>20</v>
@@ -6462,22 +6514,22 @@
         <f t="shared" si="13"/>
         <v>43825</v>
       </c>
-      <c r="C156" s="78"/>
-      <c r="D156" s="78"/>
-      <c r="E156" s="78"/>
-      <c r="F156" s="78"/>
-      <c r="G156" s="78"/>
-      <c r="H156" s="78"/>
-      <c r="I156" s="78"/>
-      <c r="J156" s="78"/>
-      <c r="K156" s="78"/>
-      <c r="L156" s="78"/>
-      <c r="M156" s="78"/>
-      <c r="N156" s="78"/>
-      <c r="O156" s="78"/>
-      <c r="P156" s="78"/>
-      <c r="Q156" s="78"/>
-      <c r="R156" s="78"/>
+      <c r="C156" s="79"/>
+      <c r="D156" s="79"/>
+      <c r="E156" s="79"/>
+      <c r="F156" s="79"/>
+      <c r="G156" s="79"/>
+      <c r="H156" s="79"/>
+      <c r="I156" s="79"/>
+      <c r="J156" s="79"/>
+      <c r="K156" s="79"/>
+      <c r="L156" s="79"/>
+      <c r="M156" s="79"/>
+      <c r="N156" s="79"/>
+      <c r="O156" s="79"/>
+      <c r="P156" s="79"/>
+      <c r="Q156" s="79"/>
+      <c r="R156" s="79"/>
       <c r="S156" s="51"/>
       <c r="T156" s="18" t="s">
         <v>21</v>
@@ -6492,22 +6544,22 @@
         <f t="shared" si="13"/>
         <v>43826</v>
       </c>
-      <c r="C157" s="78"/>
-      <c r="D157" s="78"/>
-      <c r="E157" s="78"/>
-      <c r="F157" s="78"/>
-      <c r="G157" s="78"/>
-      <c r="H157" s="78"/>
-      <c r="I157" s="78"/>
-      <c r="J157" s="78"/>
-      <c r="K157" s="78"/>
-      <c r="L157" s="78"/>
-      <c r="M157" s="78"/>
-      <c r="N157" s="78"/>
-      <c r="O157" s="78"/>
-      <c r="P157" s="78"/>
-      <c r="Q157" s="78"/>
-      <c r="R157" s="78"/>
+      <c r="C157" s="79"/>
+      <c r="D157" s="79"/>
+      <c r="E157" s="79"/>
+      <c r="F157" s="79"/>
+      <c r="G157" s="79"/>
+      <c r="H157" s="79"/>
+      <c r="I157" s="79"/>
+      <c r="J157" s="79"/>
+      <c r="K157" s="79"/>
+      <c r="L157" s="79"/>
+      <c r="M157" s="79"/>
+      <c r="N157" s="79"/>
+      <c r="O157" s="79"/>
+      <c r="P157" s="79"/>
+      <c r="Q157" s="79"/>
+      <c r="R157" s="79"/>
       <c r="S157" s="51"/>
       <c r="T157" s="51"/>
       <c r="U157" s="54"/>
@@ -6520,22 +6572,22 @@
         <f t="shared" si="13"/>
         <v>43827</v>
       </c>
-      <c r="C158" s="78"/>
-      <c r="D158" s="78"/>
-      <c r="E158" s="78"/>
-      <c r="F158" s="78"/>
-      <c r="G158" s="78"/>
-      <c r="H158" s="78"/>
-      <c r="I158" s="78"/>
-      <c r="J158" s="78"/>
-      <c r="K158" s="78"/>
-      <c r="L158" s="78"/>
-      <c r="M158" s="78"/>
-      <c r="N158" s="78"/>
-      <c r="O158" s="78"/>
-      <c r="P158" s="78"/>
-      <c r="Q158" s="78"/>
-      <c r="R158" s="78"/>
+      <c r="C158" s="79"/>
+      <c r="D158" s="79"/>
+      <c r="E158" s="79"/>
+      <c r="F158" s="79"/>
+      <c r="G158" s="79"/>
+      <c r="H158" s="79"/>
+      <c r="I158" s="79"/>
+      <c r="J158" s="79"/>
+      <c r="K158" s="79"/>
+      <c r="L158" s="79"/>
+      <c r="M158" s="79"/>
+      <c r="N158" s="79"/>
+      <c r="O158" s="79"/>
+      <c r="P158" s="79"/>
+      <c r="Q158" s="79"/>
+      <c r="R158" s="79"/>
       <c r="S158" s="51"/>
       <c r="T158" s="51"/>
       <c r="U158" s="54"/>
@@ -6548,22 +6600,22 @@
         <f t="shared" si="13"/>
         <v>43828</v>
       </c>
-      <c r="C159" s="78"/>
-      <c r="D159" s="78"/>
-      <c r="E159" s="78"/>
-      <c r="F159" s="78"/>
-      <c r="G159" s="78"/>
-      <c r="H159" s="78"/>
-      <c r="I159" s="78"/>
-      <c r="J159" s="78"/>
-      <c r="K159" s="78"/>
-      <c r="L159" s="78"/>
-      <c r="M159" s="78"/>
-      <c r="N159" s="78"/>
-      <c r="O159" s="78"/>
-      <c r="P159" s="78"/>
-      <c r="Q159" s="78"/>
-      <c r="R159" s="78"/>
+      <c r="C159" s="79"/>
+      <c r="D159" s="79"/>
+      <c r="E159" s="79"/>
+      <c r="F159" s="79"/>
+      <c r="G159" s="79"/>
+      <c r="H159" s="79"/>
+      <c r="I159" s="79"/>
+      <c r="J159" s="79"/>
+      <c r="K159" s="79"/>
+      <c r="L159" s="79"/>
+      <c r="M159" s="79"/>
+      <c r="N159" s="79"/>
+      <c r="O159" s="79"/>
+      <c r="P159" s="79"/>
+      <c r="Q159" s="79"/>
+      <c r="R159" s="79"/>
       <c r="S159" s="51"/>
       <c r="T159" s="51"/>
       <c r="U159" s="54"/>
@@ -6685,24 +6737,24 @@
         <f>B153+7</f>
         <v>43829</v>
       </c>
-      <c r="C163" s="78" t="s">
+      <c r="C163" s="79" t="s">
         <v>54</v>
       </c>
-      <c r="D163" s="78"/>
-      <c r="E163" s="78"/>
-      <c r="F163" s="78"/>
-      <c r="G163" s="78"/>
-      <c r="H163" s="78"/>
-      <c r="I163" s="78"/>
-      <c r="J163" s="78"/>
-      <c r="K163" s="78"/>
-      <c r="L163" s="78"/>
-      <c r="M163" s="78"/>
-      <c r="N163" s="78"/>
-      <c r="O163" s="78"/>
-      <c r="P163" s="78"/>
-      <c r="Q163" s="78"/>
-      <c r="R163" s="78"/>
+      <c r="D163" s="79"/>
+      <c r="E163" s="79"/>
+      <c r="F163" s="79"/>
+      <c r="G163" s="79"/>
+      <c r="H163" s="79"/>
+      <c r="I163" s="79"/>
+      <c r="J163" s="79"/>
+      <c r="K163" s="79"/>
+      <c r="L163" s="79"/>
+      <c r="M163" s="79"/>
+      <c r="N163" s="79"/>
+      <c r="O163" s="79"/>
+      <c r="P163" s="79"/>
+      <c r="Q163" s="79"/>
+      <c r="R163" s="79"/>
       <c r="S163" s="51"/>
       <c r="T163" s="30" t="s">
         <v>22</v>
@@ -6717,29 +6769,29 @@
         <f t="shared" ref="B164:B169" si="14">B154+7</f>
         <v>43830</v>
       </c>
-      <c r="C164" s="78"/>
-      <c r="D164" s="78"/>
-      <c r="E164" s="78"/>
-      <c r="F164" s="78"/>
-      <c r="G164" s="78"/>
-      <c r="H164" s="78"/>
-      <c r="I164" s="78"/>
-      <c r="J164" s="78"/>
-      <c r="K164" s="78"/>
-      <c r="L164" s="78"/>
-      <c r="M164" s="78"/>
-      <c r="N164" s="78"/>
-      <c r="O164" s="78"/>
-      <c r="P164" s="78"/>
-      <c r="Q164" s="78"/>
-      <c r="R164" s="78"/>
+      <c r="C164" s="79"/>
+      <c r="D164" s="79"/>
+      <c r="E164" s="79"/>
+      <c r="F164" s="79"/>
+      <c r="G164" s="79"/>
+      <c r="H164" s="79"/>
+      <c r="I164" s="79"/>
+      <c r="J164" s="79"/>
+      <c r="K164" s="79"/>
+      <c r="L164" s="79"/>
+      <c r="M164" s="79"/>
+      <c r="N164" s="79"/>
+      <c r="O164" s="79"/>
+      <c r="P164" s="79"/>
+      <c r="Q164" s="79"/>
+      <c r="R164" s="79"/>
       <c r="S164" s="51"/>
       <c r="T164" s="53" t="s">
         <v>19</v>
       </c>
       <c r="U164" s="54"/>
     </row>
-    <row r="165" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
         <v>2</v>
       </c>
@@ -6747,29 +6799,29 @@
         <f t="shared" si="14"/>
         <v>43831</v>
       </c>
-      <c r="C165" s="78"/>
-      <c r="D165" s="78"/>
-      <c r="E165" s="78"/>
-      <c r="F165" s="78"/>
-      <c r="G165" s="78"/>
-      <c r="H165" s="78"/>
-      <c r="I165" s="78"/>
-      <c r="J165" s="78"/>
-      <c r="K165" s="78"/>
-      <c r="L165" s="78"/>
-      <c r="M165" s="78"/>
-      <c r="N165" s="78"/>
-      <c r="O165" s="78"/>
-      <c r="P165" s="78"/>
-      <c r="Q165" s="78"/>
-      <c r="R165" s="78"/>
+      <c r="C165" s="79"/>
+      <c r="D165" s="79"/>
+      <c r="E165" s="79"/>
+      <c r="F165" s="79"/>
+      <c r="G165" s="79"/>
+      <c r="H165" s="79"/>
+      <c r="I165" s="79"/>
+      <c r="J165" s="79"/>
+      <c r="K165" s="79"/>
+      <c r="L165" s="79"/>
+      <c r="M165" s="79"/>
+      <c r="N165" s="79"/>
+      <c r="O165" s="79"/>
+      <c r="P165" s="79"/>
+      <c r="Q165" s="79"/>
+      <c r="R165" s="79"/>
       <c r="S165" s="51"/>
       <c r="T165" s="52" t="s">
         <v>20</v>
       </c>
       <c r="U165" s="54"/>
     </row>
-    <row r="166" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
         <v>3</v>
       </c>
@@ -6777,25 +6829,23 @@
         <f t="shared" si="14"/>
         <v>43832</v>
       </c>
-      <c r="C166" s="32"/>
-      <c r="D166" s="20"/>
-      <c r="E166" s="70" t="s">
-        <v>7</v>
-      </c>
-      <c r="F166" s="70"/>
-      <c r="G166" s="70"/>
-      <c r="H166" s="70"/>
-      <c r="I166" s="70"/>
-      <c r="J166" s="70"/>
-      <c r="K166" s="49"/>
-      <c r="L166" s="71" t="s">
-        <v>7</v>
-      </c>
-      <c r="M166" s="72"/>
-      <c r="N166" s="72"/>
-      <c r="O166" s="72"/>
+      <c r="C166" s="70" t="s">
+        <v>88</v>
+      </c>
+      <c r="D166" s="71"/>
+      <c r="E166" s="71"/>
+      <c r="F166" s="71"/>
+      <c r="G166" s="71"/>
+      <c r="H166" s="71"/>
+      <c r="I166" s="71"/>
+      <c r="J166" s="71"/>
+      <c r="K166" s="71"/>
+      <c r="L166" s="71"/>
+      <c r="M166" s="71"/>
+      <c r="N166" s="71"/>
+      <c r="O166" s="71"/>
       <c r="P166" s="72"/>
-      <c r="Q166" s="73"/>
+      <c r="Q166" s="49"/>
       <c r="R166" s="20"/>
       <c r="S166" s="51"/>
       <c r="T166" s="18" t="s">
@@ -6803,7 +6853,7 @@
       </c>
       <c r="U166" s="54"/>
     </row>
-    <row r="167" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
         <v>4</v>
       </c>
@@ -6811,31 +6861,29 @@
         <f t="shared" si="14"/>
         <v>43833</v>
       </c>
-      <c r="C167" s="50"/>
-      <c r="D167" s="49"/>
-      <c r="E167" s="70" t="s">
-        <v>7</v>
-      </c>
-      <c r="F167" s="70"/>
-      <c r="G167" s="70"/>
-      <c r="H167" s="70"/>
-      <c r="I167" s="70"/>
-      <c r="J167" s="70"/>
-      <c r="K167" s="49"/>
-      <c r="L167" s="71" t="s">
-        <v>7</v>
-      </c>
-      <c r="M167" s="72"/>
-      <c r="N167" s="72"/>
-      <c r="O167" s="72"/>
+      <c r="C167" s="70" t="s">
+        <v>88</v>
+      </c>
+      <c r="D167" s="71"/>
+      <c r="E167" s="71"/>
+      <c r="F167" s="71"/>
+      <c r="G167" s="71"/>
+      <c r="H167" s="71"/>
+      <c r="I167" s="71"/>
+      <c r="J167" s="71"/>
+      <c r="K167" s="71"/>
+      <c r="L167" s="71"/>
+      <c r="M167" s="71"/>
+      <c r="N167" s="71"/>
+      <c r="O167" s="71"/>
       <c r="P167" s="72"/>
-      <c r="Q167" s="73"/>
+      <c r="Q167" s="49"/>
       <c r="R167" s="49"/>
       <c r="S167" s="51"/>
       <c r="T167" s="51"/>
       <c r="U167" s="54"/>
     </row>
-    <row r="168" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
         <v>5</v>
       </c>
@@ -6843,20 +6891,22 @@
         <f t="shared" si="14"/>
         <v>43834</v>
       </c>
-      <c r="C168" s="50"/>
-      <c r="D168" s="49"/>
-      <c r="E168" s="49"/>
-      <c r="F168" s="49"/>
-      <c r="G168" s="49"/>
-      <c r="H168" s="49"/>
-      <c r="I168" s="49"/>
-      <c r="J168" s="49"/>
-      <c r="K168" s="49"/>
-      <c r="L168" s="49"/>
-      <c r="M168" s="49"/>
-      <c r="N168" s="49"/>
-      <c r="O168" s="49"/>
-      <c r="P168" s="49"/>
+      <c r="C168" s="70" t="s">
+        <v>88</v>
+      </c>
+      <c r="D168" s="71"/>
+      <c r="E168" s="71"/>
+      <c r="F168" s="71"/>
+      <c r="G168" s="71"/>
+      <c r="H168" s="71"/>
+      <c r="I168" s="71"/>
+      <c r="J168" s="71"/>
+      <c r="K168" s="71"/>
+      <c r="L168" s="71"/>
+      <c r="M168" s="71"/>
+      <c r="N168" s="71"/>
+      <c r="O168" s="71"/>
+      <c r="P168" s="72"/>
       <c r="Q168" s="49"/>
       <c r="R168" s="49"/>
       <c r="S168" s="51"/>
@@ -6949,7 +6999,7 @@
       <c r="T171" s="51"/>
       <c r="U171" s="54"/>
     </row>
-    <row r="172" spans="1:21" s="38" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:21" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A172" s="57">
         <f>A162+7</f>
         <v>43836</v>
@@ -6980,7 +7030,7 @@
       <c r="T172" s="51"/>
       <c r="U172" s="54"/>
     </row>
-    <row r="173" spans="1:21" s="38" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:21" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A173" s="3" t="s">
         <v>0</v>
       </c>
@@ -6988,25 +7038,23 @@
         <f>B163+7</f>
         <v>43836</v>
       </c>
-      <c r="C173" s="32"/>
-      <c r="D173" s="20"/>
-      <c r="E173" s="70" t="s">
-        <v>7</v>
-      </c>
-      <c r="F173" s="70"/>
-      <c r="G173" s="70"/>
-      <c r="H173" s="70"/>
-      <c r="I173" s="70"/>
-      <c r="J173" s="70"/>
-      <c r="K173" s="49"/>
-      <c r="L173" s="71" t="s">
-        <v>7</v>
-      </c>
-      <c r="M173" s="72"/>
-      <c r="N173" s="72"/>
-      <c r="O173" s="72"/>
+      <c r="C173" s="70" t="s">
+        <v>88</v>
+      </c>
+      <c r="D173" s="71"/>
+      <c r="E173" s="71"/>
+      <c r="F173" s="71"/>
+      <c r="G173" s="71"/>
+      <c r="H173" s="71"/>
+      <c r="I173" s="71"/>
+      <c r="J173" s="71"/>
+      <c r="K173" s="71"/>
+      <c r="L173" s="71"/>
+      <c r="M173" s="71"/>
+      <c r="N173" s="71"/>
+      <c r="O173" s="71"/>
       <c r="P173" s="72"/>
-      <c r="Q173" s="73"/>
+      <c r="Q173" s="49"/>
       <c r="R173" s="49"/>
       <c r="S173" s="51"/>
       <c r="T173" s="30" t="s">
@@ -7014,7 +7062,7 @@
       </c>
       <c r="U173" s="54"/>
     </row>
-    <row r="174" spans="1:21" s="38" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:21" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A174" s="3" t="s">
         <v>1</v>
       </c>
@@ -7022,33 +7070,31 @@
         <f t="shared" ref="B174:B179" si="15">B164+7</f>
         <v>43837</v>
       </c>
-      <c r="C174" s="32"/>
-      <c r="D174" s="20"/>
-      <c r="E174" s="70" t="s">
-        <v>7</v>
-      </c>
-      <c r="F174" s="70"/>
-      <c r="G174" s="70"/>
-      <c r="H174" s="70"/>
-      <c r="I174" s="70"/>
-      <c r="J174" s="70"/>
-      <c r="K174" s="49"/>
-      <c r="L174" s="71" t="s">
-        <v>7</v>
-      </c>
-      <c r="M174" s="72"/>
-      <c r="N174" s="72"/>
-      <c r="O174" s="72"/>
+      <c r="C174" s="70" t="s">
+        <v>88</v>
+      </c>
+      <c r="D174" s="71"/>
+      <c r="E174" s="71"/>
+      <c r="F174" s="71"/>
+      <c r="G174" s="71"/>
+      <c r="H174" s="71"/>
+      <c r="I174" s="71"/>
+      <c r="J174" s="71"/>
+      <c r="K174" s="71"/>
+      <c r="L174" s="71"/>
+      <c r="M174" s="71"/>
+      <c r="N174" s="71"/>
+      <c r="O174" s="71"/>
       <c r="P174" s="72"/>
-      <c r="Q174" s="73"/>
-      <c r="R174" s="20"/>
+      <c r="Q174" s="49"/>
+      <c r="R174" s="49"/>
       <c r="S174" s="51"/>
       <c r="T174" s="53" t="s">
         <v>19</v>
       </c>
       <c r="U174" s="54"/>
     </row>
-    <row r="175" spans="1:21" s="38" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:21" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A175" s="3" t="s">
         <v>2</v>
       </c>
@@ -7056,25 +7102,23 @@
         <f t="shared" si="15"/>
         <v>43838</v>
       </c>
-      <c r="C175" s="32"/>
-      <c r="D175" s="20"/>
-      <c r="E175" s="70" t="s">
-        <v>7</v>
-      </c>
-      <c r="F175" s="70"/>
-      <c r="G175" s="70"/>
-      <c r="H175" s="70"/>
-      <c r="I175" s="70"/>
-      <c r="J175" s="70"/>
-      <c r="K175" s="20"/>
-      <c r="L175" s="71" t="s">
-        <v>7</v>
-      </c>
-      <c r="M175" s="72"/>
-      <c r="N175" s="72"/>
-      <c r="O175" s="72"/>
+      <c r="C175" s="70" t="s">
+        <v>88</v>
+      </c>
+      <c r="D175" s="71"/>
+      <c r="E175" s="71"/>
+      <c r="F175" s="71"/>
+      <c r="G175" s="71"/>
+      <c r="H175" s="71"/>
+      <c r="I175" s="71"/>
+      <c r="J175" s="71"/>
+      <c r="K175" s="71"/>
+      <c r="L175" s="71"/>
+      <c r="M175" s="71"/>
+      <c r="N175" s="71"/>
+      <c r="O175" s="71"/>
       <c r="P175" s="72"/>
-      <c r="Q175" s="73"/>
+      <c r="Q175" s="49"/>
       <c r="R175" s="49"/>
       <c r="S175" s="51"/>
       <c r="T175" s="52" t="s">
@@ -7082,7 +7126,7 @@
       </c>
       <c r="U175" s="54"/>
     </row>
-    <row r="176" spans="1:21" s="38" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:21" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A176" s="3" t="s">
         <v>3</v>
       </c>
@@ -7090,33 +7134,31 @@
         <f t="shared" si="15"/>
         <v>43839</v>
       </c>
-      <c r="C176" s="49"/>
-      <c r="D176" s="49"/>
-      <c r="E176" s="70" t="s">
-        <v>7</v>
-      </c>
-      <c r="F176" s="70"/>
-      <c r="G176" s="70"/>
-      <c r="H176" s="70"/>
-      <c r="I176" s="70"/>
-      <c r="J176" s="70"/>
-      <c r="K176" s="20"/>
-      <c r="L176" s="71" t="s">
-        <v>7</v>
-      </c>
-      <c r="M176" s="72"/>
-      <c r="N176" s="72"/>
-      <c r="O176" s="72"/>
+      <c r="C176" s="70" t="s">
+        <v>88</v>
+      </c>
+      <c r="D176" s="71"/>
+      <c r="E176" s="71"/>
+      <c r="F176" s="71"/>
+      <c r="G176" s="71"/>
+      <c r="H176" s="71"/>
+      <c r="I176" s="71"/>
+      <c r="J176" s="71"/>
+      <c r="K176" s="71"/>
+      <c r="L176" s="71"/>
+      <c r="M176" s="71"/>
+      <c r="N176" s="71"/>
+      <c r="O176" s="71"/>
       <c r="P176" s="72"/>
-      <c r="Q176" s="73"/>
-      <c r="R176" s="20"/>
+      <c r="Q176" s="49"/>
+      <c r="R176" s="49"/>
       <c r="S176" s="51"/>
       <c r="T176" s="18" t="s">
         <v>21</v>
       </c>
       <c r="U176" s="54"/>
     </row>
-    <row r="177" spans="1:21" s="38" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:21" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
         <v>4</v>
       </c>
@@ -7124,31 +7166,29 @@
         <f t="shared" si="15"/>
         <v>43840</v>
       </c>
-      <c r="C177" s="32"/>
-      <c r="D177" s="20"/>
-      <c r="E177" s="70" t="s">
-        <v>7</v>
-      </c>
-      <c r="F177" s="70"/>
-      <c r="G177" s="70"/>
-      <c r="H177" s="70"/>
-      <c r="I177" s="70"/>
-      <c r="J177" s="70"/>
-      <c r="K177" s="20"/>
-      <c r="L177" s="71" t="s">
-        <v>7</v>
-      </c>
-      <c r="M177" s="72"/>
-      <c r="N177" s="72"/>
-      <c r="O177" s="72"/>
+      <c r="C177" s="70" t="s">
+        <v>88</v>
+      </c>
+      <c r="D177" s="71"/>
+      <c r="E177" s="71"/>
+      <c r="F177" s="71"/>
+      <c r="G177" s="71"/>
+      <c r="H177" s="71"/>
+      <c r="I177" s="71"/>
+      <c r="J177" s="71"/>
+      <c r="K177" s="71"/>
+      <c r="L177" s="71"/>
+      <c r="M177" s="71"/>
+      <c r="N177" s="71"/>
+      <c r="O177" s="71"/>
       <c r="P177" s="72"/>
-      <c r="Q177" s="73"/>
-      <c r="R177" s="20"/>
+      <c r="Q177" s="49"/>
+      <c r="R177" s="49"/>
       <c r="S177" s="51"/>
       <c r="T177" s="51"/>
       <c r="U177" s="54"/>
     </row>
-    <row r="178" spans="1:21" s="38" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:21" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A178" s="3" t="s">
         <v>5</v>
       </c>
@@ -7156,20 +7196,22 @@
         <f t="shared" si="15"/>
         <v>43841</v>
       </c>
-      <c r="C178" s="50"/>
-      <c r="D178" s="49"/>
-      <c r="E178" s="49"/>
-      <c r="F178" s="49"/>
-      <c r="G178" s="49"/>
-      <c r="H178" s="49"/>
-      <c r="I178" s="49"/>
-      <c r="J178" s="49"/>
-      <c r="K178" s="49"/>
-      <c r="L178" s="49"/>
-      <c r="M178" s="49"/>
-      <c r="N178" s="49"/>
-      <c r="O178" s="49"/>
-      <c r="P178" s="49"/>
+      <c r="C178" s="70" t="s">
+        <v>88</v>
+      </c>
+      <c r="D178" s="71"/>
+      <c r="E178" s="71"/>
+      <c r="F178" s="71"/>
+      <c r="G178" s="71"/>
+      <c r="H178" s="71"/>
+      <c r="I178" s="71"/>
+      <c r="J178" s="71"/>
+      <c r="K178" s="71"/>
+      <c r="L178" s="71"/>
+      <c r="M178" s="71"/>
+      <c r="N178" s="71"/>
+      <c r="O178" s="71"/>
+      <c r="P178" s="72"/>
       <c r="Q178" s="49"/>
       <c r="R178" s="49"/>
       <c r="S178" s="51"/>
@@ -7261,7 +7303,7 @@
       <c r="S181" s="51"/>
       <c r="T181" s="51"/>
     </row>
-    <row r="182" spans="1:21" s="38" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:21" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A182" s="57">
         <f>A172+7</f>
         <v>43843</v>
@@ -7291,7 +7333,7 @@
       <c r="S182" s="51"/>
       <c r="T182" s="51"/>
     </row>
-    <row r="183" spans="1:21" s="38" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:21" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A183" s="3" t="s">
         <v>0</v>
       </c>
@@ -7299,32 +7341,30 @@
         <f>B173+7</f>
         <v>43843</v>
       </c>
-      <c r="C183" s="32"/>
-      <c r="D183" s="20"/>
-      <c r="E183" s="70" t="s">
-        <v>7</v>
-      </c>
-      <c r="F183" s="70"/>
-      <c r="G183" s="70"/>
-      <c r="H183" s="70"/>
-      <c r="I183" s="70"/>
-      <c r="J183" s="70"/>
-      <c r="K183" s="49"/>
-      <c r="L183" s="71" t="s">
-        <v>7</v>
-      </c>
-      <c r="M183" s="72"/>
-      <c r="N183" s="72"/>
-      <c r="O183" s="72"/>
+      <c r="C183" s="70" t="s">
+        <v>88</v>
+      </c>
+      <c r="D183" s="71"/>
+      <c r="E183" s="71"/>
+      <c r="F183" s="71"/>
+      <c r="G183" s="71"/>
+      <c r="H183" s="71"/>
+      <c r="I183" s="71"/>
+      <c r="J183" s="71"/>
+      <c r="K183" s="71"/>
+      <c r="L183" s="71"/>
+      <c r="M183" s="71"/>
+      <c r="N183" s="71"/>
+      <c r="O183" s="71"/>
       <c r="P183" s="72"/>
-      <c r="Q183" s="73"/>
+      <c r="Q183" s="49"/>
       <c r="R183" s="49"/>
       <c r="S183" s="51"/>
       <c r="T183" s="30" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="184" spans="1:21" s="38" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:21" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A184" s="3" t="s">
         <v>1</v>
       </c>
@@ -7332,32 +7372,30 @@
         <f t="shared" ref="B184:B189" si="16">B174+7</f>
         <v>43844</v>
       </c>
-      <c r="C184" s="32"/>
-      <c r="D184" s="20"/>
-      <c r="E184" s="70" t="s">
-        <v>7</v>
-      </c>
-      <c r="F184" s="70"/>
-      <c r="G184" s="70"/>
-      <c r="H184" s="70"/>
-      <c r="I184" s="70"/>
-      <c r="J184" s="70"/>
-      <c r="K184" s="49"/>
-      <c r="L184" s="71" t="s">
-        <v>7</v>
-      </c>
-      <c r="M184" s="72"/>
-      <c r="N184" s="72"/>
-      <c r="O184" s="72"/>
+      <c r="C184" s="70" t="s">
+        <v>88</v>
+      </c>
+      <c r="D184" s="71"/>
+      <c r="E184" s="71"/>
+      <c r="F184" s="71"/>
+      <c r="G184" s="71"/>
+      <c r="H184" s="71"/>
+      <c r="I184" s="71"/>
+      <c r="J184" s="71"/>
+      <c r="K184" s="71"/>
+      <c r="L184" s="71"/>
+      <c r="M184" s="71"/>
+      <c r="N184" s="71"/>
+      <c r="O184" s="71"/>
       <c r="P184" s="72"/>
-      <c r="Q184" s="73"/>
-      <c r="R184" s="20"/>
+      <c r="Q184" s="49"/>
+      <c r="R184" s="49"/>
       <c r="S184" s="51"/>
       <c r="T184" s="53" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="185" spans="1:21" s="38" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:21" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A185" s="3" t="s">
         <v>2</v>
       </c>
@@ -7365,32 +7403,30 @@
         <f t="shared" si="16"/>
         <v>43845</v>
       </c>
-      <c r="C185" s="32"/>
-      <c r="D185" s="20"/>
-      <c r="E185" s="70" t="s">
-        <v>7</v>
-      </c>
-      <c r="F185" s="70"/>
-      <c r="G185" s="70"/>
-      <c r="H185" s="70"/>
-      <c r="I185" s="70"/>
-      <c r="J185" s="70"/>
-      <c r="K185" s="20"/>
-      <c r="L185" s="71" t="s">
-        <v>7</v>
-      </c>
-      <c r="M185" s="72"/>
-      <c r="N185" s="72"/>
-      <c r="O185" s="72"/>
+      <c r="C185" s="70" t="s">
+        <v>88</v>
+      </c>
+      <c r="D185" s="71"/>
+      <c r="E185" s="71"/>
+      <c r="F185" s="71"/>
+      <c r="G185" s="71"/>
+      <c r="H185" s="71"/>
+      <c r="I185" s="71"/>
+      <c r="J185" s="71"/>
+      <c r="K185" s="71"/>
+      <c r="L185" s="71"/>
+      <c r="M185" s="71"/>
+      <c r="N185" s="71"/>
+      <c r="O185" s="71"/>
       <c r="P185" s="72"/>
-      <c r="Q185" s="73"/>
+      <c r="Q185" s="49"/>
       <c r="R185" s="49"/>
       <c r="S185" s="51"/>
       <c r="T185" s="52" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="186" spans="1:21" s="38" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:21" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A186" s="3" t="s">
         <v>3</v>
       </c>
@@ -7398,32 +7434,28 @@
         <f t="shared" si="16"/>
         <v>43846</v>
       </c>
-      <c r="C186" s="49"/>
+      <c r="C186" s="50"/>
       <c r="D186" s="49"/>
-      <c r="E186" s="70" t="s">
-        <v>7</v>
-      </c>
-      <c r="F186" s="70"/>
-      <c r="G186" s="70"/>
-      <c r="H186" s="70"/>
-      <c r="I186" s="70"/>
-      <c r="J186" s="70"/>
-      <c r="K186" s="20"/>
-      <c r="L186" s="71" t="s">
-        <v>7</v>
-      </c>
-      <c r="M186" s="72"/>
-      <c r="N186" s="72"/>
-      <c r="O186" s="72"/>
-      <c r="P186" s="72"/>
-      <c r="Q186" s="73"/>
-      <c r="R186" s="20"/>
+      <c r="E186" s="49"/>
+      <c r="F186" s="49"/>
+      <c r="G186" s="49"/>
+      <c r="H186" s="49"/>
+      <c r="I186" s="49"/>
+      <c r="J186" s="49"/>
+      <c r="K186" s="49"/>
+      <c r="L186" s="49"/>
+      <c r="M186" s="49"/>
+      <c r="N186" s="49"/>
+      <c r="O186" s="49"/>
+      <c r="P186" s="49"/>
+      <c r="Q186" s="49"/>
+      <c r="R186" s="49"/>
       <c r="S186" s="51"/>
       <c r="T186" s="18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="187" spans="1:21" s="38" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:21" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A187" s="3" t="s">
         <v>4</v>
       </c>
@@ -7431,30 +7463,26 @@
         <f t="shared" si="16"/>
         <v>43847</v>
       </c>
-      <c r="C187" s="32"/>
-      <c r="D187" s="20"/>
-      <c r="E187" s="70" t="s">
-        <v>7</v>
-      </c>
-      <c r="F187" s="70"/>
-      <c r="G187" s="70"/>
-      <c r="H187" s="70"/>
-      <c r="I187" s="70"/>
-      <c r="J187" s="70"/>
-      <c r="K187" s="20"/>
-      <c r="L187" s="71" t="s">
-        <v>7</v>
-      </c>
-      <c r="M187" s="72"/>
-      <c r="N187" s="72"/>
-      <c r="O187" s="72"/>
-      <c r="P187" s="72"/>
-      <c r="Q187" s="73"/>
-      <c r="R187" s="20"/>
+      <c r="C187" s="50"/>
+      <c r="D187" s="49"/>
+      <c r="E187" s="49"/>
+      <c r="F187" s="49"/>
+      <c r="G187" s="49"/>
+      <c r="H187" s="49"/>
+      <c r="I187" s="49"/>
+      <c r="J187" s="49"/>
+      <c r="K187" s="49"/>
+      <c r="L187" s="49"/>
+      <c r="M187" s="49"/>
+      <c r="N187" s="49"/>
+      <c r="O187" s="49"/>
+      <c r="P187" s="49"/>
+      <c r="Q187" s="49"/>
+      <c r="R187" s="49"/>
       <c r="S187" s="51"/>
       <c r="T187" s="51"/>
     </row>
-    <row r="188" spans="1:21" s="38" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:21" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A188" s="3" t="s">
         <v>5</v>
       </c>
@@ -15879,41 +15907,25 @@
       <c r="T507"/>
     </row>
   </sheetData>
-  <mergeCells count="146">
+  <mergeCells count="145">
+    <mergeCell ref="H96:L96"/>
     <mergeCell ref="C143:E143"/>
-    <mergeCell ref="K116:Q116"/>
-    <mergeCell ref="E115:J115"/>
-    <mergeCell ref="L115:Q115"/>
     <mergeCell ref="C134:G134"/>
     <mergeCell ref="C114:G114"/>
     <mergeCell ref="C133:G133"/>
     <mergeCell ref="C113:G113"/>
-    <mergeCell ref="H116:J116"/>
     <mergeCell ref="D122:F122"/>
     <mergeCell ref="D142:F142"/>
     <mergeCell ref="H124:P124"/>
     <mergeCell ref="C125:K125"/>
     <mergeCell ref="H113:M113"/>
     <mergeCell ref="H114:M114"/>
-    <mergeCell ref="C79:R79"/>
-    <mergeCell ref="C89:R89"/>
-    <mergeCell ref="C99:R99"/>
-    <mergeCell ref="C109:R109"/>
-    <mergeCell ref="C103:G103"/>
-    <mergeCell ref="C104:G104"/>
-    <mergeCell ref="C83:G83"/>
-    <mergeCell ref="C84:G84"/>
-    <mergeCell ref="C86:G86"/>
-    <mergeCell ref="C93:G93"/>
-    <mergeCell ref="C94:G94"/>
-    <mergeCell ref="C96:G96"/>
-    <mergeCell ref="H83:P83"/>
-    <mergeCell ref="C107:M107"/>
-    <mergeCell ref="J84:R84"/>
-    <mergeCell ref="E85:M85"/>
-    <mergeCell ref="H93:P93"/>
-    <mergeCell ref="H94:P94"/>
-    <mergeCell ref="H96:L96"/>
+    <mergeCell ref="H133:P133"/>
+    <mergeCell ref="C135:K135"/>
+    <mergeCell ref="M135:P135"/>
+    <mergeCell ref="H116:I116"/>
+    <mergeCell ref="J116:N116"/>
+    <mergeCell ref="H134:P134"/>
     <mergeCell ref="H24:I24"/>
     <mergeCell ref="H46:P46"/>
     <mergeCell ref="H44:N44"/>
@@ -15982,13 +15994,8 @@
     <mergeCell ref="H64:N64"/>
     <mergeCell ref="H72:K72"/>
     <mergeCell ref="C69:R69"/>
-    <mergeCell ref="L175:Q175"/>
-    <mergeCell ref="L167:Q167"/>
     <mergeCell ref="C155:R159"/>
     <mergeCell ref="C163:R165"/>
-    <mergeCell ref="E166:J166"/>
-    <mergeCell ref="L166:Q166"/>
-    <mergeCell ref="E167:J167"/>
     <mergeCell ref="H84:I84"/>
     <mergeCell ref="D112:F112"/>
     <mergeCell ref="C136:G136"/>
@@ -15996,9 +16003,6 @@
     <mergeCell ref="C123:G123"/>
     <mergeCell ref="C124:G124"/>
     <mergeCell ref="C106:G106"/>
-    <mergeCell ref="L173:Q173"/>
-    <mergeCell ref="E174:J174"/>
-    <mergeCell ref="L174:Q174"/>
     <mergeCell ref="C126:G126"/>
     <mergeCell ref="H142:L142"/>
     <mergeCell ref="C105:M105"/>
@@ -16006,26 +16010,49 @@
     <mergeCell ref="C119:R119"/>
     <mergeCell ref="C129:R129"/>
     <mergeCell ref="C139:R139"/>
+    <mergeCell ref="C89:R89"/>
+    <mergeCell ref="C99:R99"/>
+    <mergeCell ref="C109:R109"/>
+    <mergeCell ref="C103:G103"/>
+    <mergeCell ref="C104:G104"/>
+    <mergeCell ref="C84:G84"/>
+    <mergeCell ref="C86:G86"/>
+    <mergeCell ref="C93:G93"/>
+    <mergeCell ref="C144:P144"/>
+    <mergeCell ref="C145:P145"/>
+    <mergeCell ref="C146:P146"/>
+    <mergeCell ref="C147:P147"/>
+    <mergeCell ref="C148:P148"/>
+    <mergeCell ref="C153:P153"/>
+    <mergeCell ref="C154:P154"/>
     <mergeCell ref="T58:U60"/>
-    <mergeCell ref="E187:J187"/>
-    <mergeCell ref="L187:Q187"/>
     <mergeCell ref="H123:P123"/>
-    <mergeCell ref="E184:J184"/>
-    <mergeCell ref="L184:Q184"/>
-    <mergeCell ref="E185:J185"/>
-    <mergeCell ref="L185:Q185"/>
-    <mergeCell ref="E186:J186"/>
-    <mergeCell ref="L186:Q186"/>
-    <mergeCell ref="E176:J176"/>
-    <mergeCell ref="L176:Q176"/>
-    <mergeCell ref="E177:J177"/>
-    <mergeCell ref="L177:Q177"/>
-    <mergeCell ref="E183:J183"/>
-    <mergeCell ref="L183:Q183"/>
-    <mergeCell ref="E173:J173"/>
     <mergeCell ref="H103:P103"/>
     <mergeCell ref="H104:P104"/>
-    <mergeCell ref="E175:J175"/>
+    <mergeCell ref="I115:R115"/>
+    <mergeCell ref="M125:P125"/>
+    <mergeCell ref="C79:R79"/>
+    <mergeCell ref="C83:G83"/>
+    <mergeCell ref="C94:G94"/>
+    <mergeCell ref="C96:G96"/>
+    <mergeCell ref="H83:P83"/>
+    <mergeCell ref="C107:M107"/>
+    <mergeCell ref="J84:R84"/>
+    <mergeCell ref="E85:M85"/>
+    <mergeCell ref="H93:P93"/>
+    <mergeCell ref="H94:P94"/>
+    <mergeCell ref="C183:P183"/>
+    <mergeCell ref="C184:P184"/>
+    <mergeCell ref="C185:P185"/>
+    <mergeCell ref="C166:P166"/>
+    <mergeCell ref="C167:P167"/>
+    <mergeCell ref="C168:P168"/>
+    <mergeCell ref="C173:P173"/>
+    <mergeCell ref="C174:P174"/>
+    <mergeCell ref="C175:P175"/>
+    <mergeCell ref="C176:P176"/>
+    <mergeCell ref="C177:P177"/>
+    <mergeCell ref="C178:P178"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -16036,8 +16063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:K43"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16053,10 +16080,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="122" t="s">
+      <c r="A2" s="126" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="122"/>
+      <c r="B2" s="126"/>
       <c r="C2" s="41" t="s">
         <v>18</v>
       </c>
@@ -16075,10 +16102,10 @@
       <c r="I2" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="123" t="s">
+      <c r="J2" s="127" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="123"/>
+      <c r="K2" s="127"/>
     </row>
     <row r="3" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
@@ -16093,10 +16120,10 @@
       <c r="I3" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="J3" s="124" t="s">
+      <c r="J3" s="128" t="s">
         <v>60</v>
       </c>
-      <c r="K3" s="124"/>
+      <c r="K3" s="128"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
@@ -16118,10 +16145,10 @@
       <c r="I4" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="J4" s="124" t="s">
+      <c r="J4" s="128" t="s">
         <v>61</v>
       </c>
-      <c r="K4" s="124"/>
+      <c r="K4" s="128"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
@@ -16220,8 +16247,11 @@
         <v>43408</v>
       </c>
       <c r="D11" s="29"/>
-      <c r="F11" s="56" t="s">
+      <c r="F11" s="129" t="s">
         <v>83</v>
+      </c>
+      <c r="G11" s="53" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -16252,7 +16282,9 @@
       <c r="D13" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="56"/>
+      <c r="E13" s="53" t="s">
+        <v>34</v>
+      </c>
       <c r="G13" s="56"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -16269,6 +16301,9 @@
       <c r="D14" s="56" t="s">
         <v>15</v>
       </c>
+      <c r="E14" s="53" t="s">
+        <v>34</v>
+      </c>
       <c r="F14" s="56" t="s">
         <v>10</v>
       </c>
@@ -16285,6 +16320,9 @@
         <v>43436</v>
       </c>
       <c r="D15" s="29"/>
+      <c r="F15" s="56" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
@@ -16396,10 +16434,10 @@
       <c r="H22" s="51"/>
     </row>
     <row r="23" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="122" t="s">
+      <c r="A23" s="126" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="122"/>
+      <c r="B23" s="126"/>
       <c r="C23" s="41" t="s">
         <v>18</v>
       </c>
@@ -16604,7 +16642,7 @@
         <v>43929</v>
       </c>
       <c r="D36" s="29"/>
-      <c r="F36" s="78" t="s">
+      <c r="F36" s="79" t="s">
         <v>49</v>
       </c>
     </row>
@@ -16622,7 +16660,7 @@
         <v>43936</v>
       </c>
       <c r="D37" s="44"/>
-      <c r="F37" s="78"/>
+      <c r="F37" s="79"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="23">
@@ -16638,7 +16676,7 @@
         <v>43943</v>
       </c>
       <c r="D38" s="29"/>
-      <c r="F38" s="78"/>
+      <c r="F38" s="79"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="23">

</xml_diff>